<commit_message>
Fix grid colours on other tabs
</commit_message>
<xml_diff>
--- a/MUSCCArm.xlsx
+++ b/MUSCCArm.xlsx
@@ -6283,15 +6283,129 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="225" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="118" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="119" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="110" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="129" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="130" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="126" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="133" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="113" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="120" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="161" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="162" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="187" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="163" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="188" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="137" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="167" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="194" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="195" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6301,12 +6415,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="205" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="137" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6334,112 +6442,7 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="120" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="167" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="194" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="187" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="188" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="113" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="129" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="130" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="126" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="133" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="119" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="110" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="118" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6450,9 +6453,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7210,7 +7210,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7437,7 +7436,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7509,7 +7507,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7635,7 +7632,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9308,7 +9304,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9380,7 +9375,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9427,7 +9421,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9495,7 +9488,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9722,7 +9714,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9794,7 +9785,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9920,7 +9910,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11593,7 +11582,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11665,7 +11653,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11712,7 +11699,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11796,7 +11782,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12549,7 +12534,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12773,7 +12757,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13526,7 +13509,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15595,6 +15577,150 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -15863,7 +15989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD792"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16173,21 +16299,21 @@
       <c r="E10" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="628" t="str">
+      <c r="F10" s="578" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="628"/>
+      <c r="G10" s="578"/>
       <c r="H10" s="45"/>
       <c r="I10" s="45"/>
       <c r="J10" s="165" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="621" t="str">
+      <c r="K10" s="579" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="621"/>
+      <c r="L10" s="579"/>
       <c r="M10" s="362"/>
       <c r="O10" s="14"/>
       <c r="Q10" s="2" t="s">
@@ -16230,21 +16356,21 @@
       <c r="E11" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="622" t="str">
+      <c r="F11" s="580" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="622"/>
+      <c r="G11" s="580"/>
       <c r="H11" s="45"/>
       <c r="I11" s="45"/>
       <c r="J11" s="165" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="622" t="str">
+      <c r="K11" s="580" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="622"/>
+      <c r="L11" s="580"/>
       <c r="M11" s="362"/>
       <c r="O11" s="14"/>
       <c r="Q11" s="2" t="s">
@@ -16287,21 +16413,21 @@
       <c r="E12" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="622" t="str">
+      <c r="F12" s="580" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="622"/>
+      <c r="G12" s="580"/>
       <c r="H12" s="45"/>
       <c r="I12" s="45"/>
       <c r="J12" s="165" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="629" t="str">
+      <c r="K12" s="581" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="629"/>
+      <c r="L12" s="581"/>
       <c r="M12" s="362"/>
       <c r="O12" s="14"/>
       <c r="Q12" s="2" t="s">
@@ -16344,21 +16470,21 @@
       <c r="E13" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="623" t="str">
+      <c r="F13" s="582" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="623"/>
+      <c r="G13" s="582"/>
       <c r="H13" s="45"/>
       <c r="I13" s="45"/>
       <c r="J13" s="165" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="623" t="str">
+      <c r="K13" s="582" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="623"/>
+      <c r="L13" s="582"/>
       <c r="M13" s="362"/>
       <c r="O13" s="14"/>
       <c r="Q13" s="2" t="s">
@@ -16481,21 +16607,21 @@
       <c r="E16" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="628" t="str">
+      <c r="F16" s="578" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="628"/>
+      <c r="G16" s="578"/>
       <c r="H16" s="45"/>
       <c r="I16" s="45"/>
       <c r="J16" s="165" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="630" t="str">
+      <c r="K16" s="583" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="630"/>
+      <c r="L16" s="583"/>
       <c r="M16" s="362"/>
       <c r="O16" s="14"/>
       <c r="P16" s="53" t="s">
@@ -16525,21 +16651,21 @@
       <c r="E17" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="622" t="str">
+      <c r="F17" s="580" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="622"/>
+      <c r="G17" s="580"/>
       <c r="H17" s="45"/>
       <c r="I17" s="45"/>
       <c r="J17" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="623" t="str">
+      <c r="K17" s="582" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="623"/>
+      <c r="L17" s="582"/>
       <c r="M17" s="362"/>
       <c r="O17" s="14"/>
       <c r="Q17" s="2" t="s">
@@ -16582,21 +16708,21 @@
       <c r="E18" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="623" t="str">
+      <c r="F18" s="582" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="623"/>
+      <c r="G18" s="582"/>
       <c r="H18" s="45"/>
       <c r="I18" s="45"/>
       <c r="J18" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="K18" s="623" t="str">
+      <c r="K18" s="582" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="623"/>
+      <c r="L18" s="582"/>
       <c r="M18" s="362"/>
       <c r="O18" s="14"/>
       <c r="Q18" s="2" t="s">
@@ -16644,11 +16770,11 @@
       <c r="J19" s="165" t="s">
         <v>36</v>
       </c>
-      <c r="K19" s="623" t="str">
+      <c r="K19" s="582" t="str">
         <f>IF(V20="","",V20)</f>
         <v/>
       </c>
-      <c r="L19" s="623"/>
+      <c r="L19" s="582"/>
       <c r="M19" s="362"/>
       <c r="O19" s="14"/>
       <c r="Q19" s="2" t="s">
@@ -16723,11 +16849,11 @@
       <c r="E21" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="628" t="str">
+      <c r="F21" s="578" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="628"/>
+      <c r="G21" s="578"/>
       <c r="H21" s="45"/>
       <c r="I21" s="45"/>
       <c r="J21" s="76" t="s">
@@ -16767,21 +16893,21 @@
       <c r="E22" s="165" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="629" t="str">
+      <c r="F22" s="581" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="629"/>
+      <c r="G22" s="581"/>
       <c r="H22" s="45"/>
       <c r="I22" s="45"/>
       <c r="J22" s="165" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="628" t="str">
+      <c r="K22" s="578" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="628"/>
+      <c r="L22" s="578"/>
       <c r="M22" s="362"/>
       <c r="O22" s="14"/>
       <c r="Q22" s="2" t="s">
@@ -16826,11 +16952,11 @@
       <c r="J23" s="165" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="622" t="str">
+      <c r="K23" s="580" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="622"/>
+      <c r="L23" s="580"/>
       <c r="M23" s="362"/>
       <c r="O23" s="14"/>
       <c r="Q23" s="2" t="s">
@@ -16873,21 +16999,21 @@
       <c r="E24" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="621" t="str">
+      <c r="F24" s="579" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="621"/>
+      <c r="G24" s="579"/>
       <c r="H24" s="45"/>
       <c r="I24" s="45"/>
       <c r="J24" s="165" t="s">
         <v>44</v>
       </c>
-      <c r="K24" s="622" t="str">
+      <c r="K24" s="580" t="str">
         <f>IF(V25="","",V25)</f>
         <v/>
       </c>
-      <c r="L24" s="622"/>
+      <c r="L24" s="580"/>
       <c r="M24" s="362"/>
       <c r="O24" s="14"/>
       <c r="P24" s="53" t="s">
@@ -16925,11 +17051,11 @@
       <c r="E25" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="623" t="str">
+      <c r="F25" s="582" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="623"/>
+      <c r="G25" s="582"/>
       <c r="H25" s="45"/>
       <c r="I25" s="45"/>
       <c r="J25" s="45"/>
@@ -16977,11 +17103,11 @@
       <c r="E26" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="623" t="str">
+      <c r="F26" s="582" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="623"/>
+      <c r="G26" s="582"/>
       <c r="H26" s="45"/>
       <c r="I26" s="45"/>
       <c r="J26" s="363" t="s">
@@ -17030,11 +17156,11 @@
       <c r="J27" s="165" t="s">
         <v>47</v>
       </c>
-      <c r="K27" s="628" t="str">
+      <c r="K27" s="578" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="628"/>
+      <c r="L27" s="578"/>
       <c r="M27" s="362"/>
       <c r="O27" s="14"/>
       <c r="Q27" s="2" t="s">
@@ -17072,21 +17198,21 @@
       <c r="E28" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="F28" s="621" t="str">
+      <c r="F28" s="579" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="621"/>
+      <c r="G28" s="579"/>
       <c r="H28" s="45"/>
       <c r="I28" s="45"/>
       <c r="J28" s="165" t="s">
         <v>48</v>
       </c>
-      <c r="K28" s="622" t="str">
+      <c r="K28" s="580" t="str">
         <f>IF(V29="","",V29)</f>
         <v/>
       </c>
-      <c r="L28" s="622"/>
+      <c r="L28" s="580"/>
       <c r="M28" s="362"/>
       <c r="O28" s="14"/>
       <c r="P28" s="53" t="s">
@@ -17115,11 +17241,11 @@
       <c r="E29" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="623" t="str">
+      <c r="F29" s="582" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="623"/>
+      <c r="G29" s="582"/>
       <c r="H29" s="45"/>
       <c r="I29" s="45"/>
       <c r="J29" s="45"/>
@@ -17167,11 +17293,11 @@
       <c r="E30" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="623" t="str">
+      <c r="F30" s="582" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="623"/>
+      <c r="G30" s="582"/>
       <c r="H30" s="45"/>
       <c r="I30" s="45"/>
       <c r="J30" s="45"/>
@@ -17286,11 +17412,11 @@
       <c r="E33" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="628" t="str">
+      <c r="F33" s="578" t="str">
         <f>IF(R34="","",R34)</f>
         <v/>
       </c>
-      <c r="G33" s="628"/>
+      <c r="G33" s="578"/>
       <c r="H33" s="45"/>
       <c r="I33" s="45"/>
       <c r="J33" s="76" t="s">
@@ -17327,21 +17453,21 @@
       <c r="E34" s="165" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="629" t="str">
+      <c r="F34" s="581" t="str">
         <f>IF(R35="","",R35)</f>
         <v/>
       </c>
-      <c r="G34" s="629"/>
+      <c r="G34" s="581"/>
       <c r="H34" s="45"/>
       <c r="I34" s="45"/>
       <c r="J34" s="165" t="s">
         <v>41</v>
       </c>
-      <c r="K34" s="628" t="str">
+      <c r="K34" s="578" t="str">
         <f>IF(V35="","",V35)</f>
         <v/>
       </c>
-      <c r="L34" s="628"/>
+      <c r="L34" s="578"/>
       <c r="M34" s="362"/>
       <c r="O34" s="14"/>
       <c r="Q34" s="2" t="s">
@@ -17386,11 +17512,11 @@
       <c r="J35" s="165" t="s">
         <v>43</v>
       </c>
-      <c r="K35" s="622" t="str">
+      <c r="K35" s="580" t="str">
         <f>IF(V36="","",V36)</f>
         <v/>
       </c>
-      <c r="L35" s="622"/>
+      <c r="L35" s="580"/>
       <c r="M35" s="362"/>
       <c r="O35" s="14"/>
       <c r="Q35" s="2" t="s">
@@ -17433,21 +17559,21 @@
       <c r="E36" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="F36" s="621" t="str">
+      <c r="F36" s="579" t="str">
         <f>IF(R37="","",R37)</f>
         <v/>
       </c>
-      <c r="G36" s="621"/>
+      <c r="G36" s="579"/>
       <c r="H36" s="45"/>
       <c r="I36" s="45"/>
       <c r="J36" s="165" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="622" t="str">
+      <c r="K36" s="580" t="str">
         <f>IF(V37="","",V37)</f>
         <v/>
       </c>
-      <c r="L36" s="622"/>
+      <c r="L36" s="580"/>
       <c r="M36" s="362"/>
       <c r="O36" s="14"/>
       <c r="P36" s="53" t="s">
@@ -17485,11 +17611,11 @@
       <c r="E37" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="F37" s="623" t="str">
+      <c r="F37" s="582" t="str">
         <f>IF(R38="","",R38)</f>
         <v/>
       </c>
-      <c r="G37" s="623"/>
+      <c r="G37" s="582"/>
       <c r="H37" s="45"/>
       <c r="I37" s="45"/>
       <c r="J37" s="45"/>
@@ -17537,11 +17663,11 @@
       <c r="E38" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="623" t="str">
+      <c r="F38" s="582" t="str">
         <f>IF(R39="","",R39)</f>
         <v/>
       </c>
-      <c r="G38" s="623"/>
+      <c r="G38" s="582"/>
       <c r="H38" s="45"/>
       <c r="I38" s="45"/>
       <c r="J38" s="363" t="s">
@@ -17588,11 +17714,11 @@
       <c r="J39" s="165" t="s">
         <v>47</v>
       </c>
-      <c r="K39" s="628" t="str">
+      <c r="K39" s="578" t="str">
         <f>IF(V40="","",V40)</f>
         <v/>
       </c>
-      <c r="L39" s="628"/>
+      <c r="L39" s="578"/>
       <c r="M39" s="362"/>
       <c r="O39" s="14"/>
       <c r="Q39" s="2" t="s">
@@ -17630,21 +17756,21 @@
       <c r="E40" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="F40" s="621" t="str">
+      <c r="F40" s="579" t="str">
         <f>IF(R41="","",R41)</f>
         <v/>
       </c>
-      <c r="G40" s="621"/>
+      <c r="G40" s="579"/>
       <c r="H40" s="45"/>
       <c r="I40" s="45"/>
       <c r="J40" s="165" t="s">
         <v>48</v>
       </c>
-      <c r="K40" s="622" t="str">
+      <c r="K40" s="580" t="str">
         <f>IF(V41="","",V41)</f>
         <v/>
       </c>
-      <c r="L40" s="622"/>
+      <c r="L40" s="580"/>
       <c r="M40" s="362"/>
       <c r="O40" s="14"/>
       <c r="P40" s="53" t="s">
@@ -17682,11 +17808,11 @@
       <c r="E41" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="623" t="str">
+      <c r="F41" s="582" t="str">
         <f>IF(R42="","",R42)</f>
         <v/>
       </c>
-      <c r="G41" s="623"/>
+      <c r="G41" s="582"/>
       <c r="H41" s="45"/>
       <c r="I41" s="45"/>
       <c r="J41" s="45"/>
@@ -17734,11 +17860,11 @@
       <c r="E42" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="623" t="str">
+      <c r="F42" s="582" t="str">
         <f>IF(R43="","",R43)</f>
         <v/>
       </c>
-      <c r="G42" s="623"/>
+      <c r="G42" s="582"/>
       <c r="H42" s="45"/>
       <c r="I42" s="45"/>
       <c r="J42" s="45"/>
@@ -18496,10 +18622,10 @@
       <c r="I69" s="349"/>
       <c r="J69" s="349"/>
       <c r="K69" s="349"/>
-      <c r="L69" s="624" t="s">
+      <c r="L69" s="584" t="s">
         <v>86</v>
       </c>
-      <c r="M69" s="625"/>
+      <c r="M69" s="585"/>
       <c r="O69" s="59"/>
       <c r="P69" s="18" t="s">
         <v>87</v>
@@ -20131,24 +20257,24 @@
       <c r="P107" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="Q107" s="626" t="str">
+      <c r="Q107" s="586" t="str">
         <f>IF(Q106&lt;&gt;"",Q106,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R107" s="626"/>
-      <c r="S107" s="626"/>
-      <c r="T107" s="627" t="str">
+      <c r="R107" s="586"/>
+      <c r="S107" s="586"/>
+      <c r="T107" s="587" t="str">
         <f>IF(T106&lt;&gt;"",T106,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v>Auto 2</v>
       </c>
-      <c r="U107" s="627"/>
-      <c r="V107" s="627"/>
-      <c r="W107" s="627" t="str">
+      <c r="U107" s="587"/>
+      <c r="V107" s="587"/>
+      <c r="W107" s="587" t="str">
         <f>IF(W106&lt;&gt;"",W106,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v>High Level</v>
       </c>
-      <c r="X107" s="627"/>
-      <c r="Y107" s="627"/>
+      <c r="X107" s="587"/>
+      <c r="Y107" s="587"/>
       <c r="AA107" s="2" t="s">
         <v>113</v>
       </c>
@@ -22142,24 +22268,24 @@
       <c r="P139" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="Q139" s="626" t="str">
+      <c r="Q139" s="586" t="str">
         <f>IF(Q138&lt;&gt;"",Q138,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R139" s="626"/>
-      <c r="S139" s="626"/>
-      <c r="T139" s="627" t="str">
+      <c r="R139" s="586"/>
+      <c r="S139" s="586"/>
+      <c r="T139" s="587" t="str">
         <f>IF(T138&lt;&gt;"",T138,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v>Auto 2</v>
       </c>
-      <c r="U139" s="627"/>
-      <c r="V139" s="627"/>
-      <c r="W139" s="627" t="str">
+      <c r="U139" s="587"/>
+      <c r="V139" s="587"/>
+      <c r="W139" s="587" t="str">
         <f>IF(W138&lt;&gt;"",W138,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v>High Level</v>
       </c>
-      <c r="X139" s="627"/>
-      <c r="Y139" s="627"/>
+      <c r="X139" s="587"/>
+      <c r="Y139" s="587"/>
       <c r="AA139" s="2" t="str">
         <f>$W$139&amp;" Mag 2"</f>
         <v>High Level Mag 2</v>
@@ -24502,10 +24628,10 @@
       <c r="P181" s="138"/>
       <c r="Q181" s="140"/>
       <c r="R181" s="131"/>
-      <c r="T181" s="603" t="s">
+      <c r="T181" s="588" t="s">
         <v>247</v>
       </c>
-      <c r="U181" s="603"/>
+      <c r="U181" s="588"/>
       <c r="W181" s="2" t="s">
         <v>201</v>
       </c>
@@ -24876,7 +25002,7 @@
       <c r="K190" s="373"/>
       <c r="L190" s="373"/>
       <c r="M190" s="377"/>
-      <c r="O190" s="611" t="str">
+      <c r="O190" s="589" t="str">
         <f>$Q$107</f>
         <v>Auto 1</v>
       </c>
@@ -24926,7 +25052,7 @@
       <c r="K191" s="373"/>
       <c r="L191" s="373"/>
       <c r="M191" s="353"/>
-      <c r="O191" s="611"/>
+      <c r="O191" s="589"/>
       <c r="P191" s="147" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -24972,7 +25098,7 @@
       <c r="K192" s="138"/>
       <c r="L192" s="138"/>
       <c r="M192" s="353"/>
-      <c r="O192" s="611"/>
+      <c r="O192" s="589"/>
       <c r="P192" s="147" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -25018,7 +25144,7 @@
       <c r="K193" s="138"/>
       <c r="L193" s="138"/>
       <c r="M193" s="353"/>
-      <c r="O193" s="611"/>
+      <c r="O193" s="589"/>
       <c r="P193" s="147" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -25061,7 +25187,7 @@
       <c r="K194" s="138"/>
       <c r="L194" s="138"/>
       <c r="M194" s="353"/>
-      <c r="O194" s="611"/>
+      <c r="O194" s="589"/>
       <c r="P194" s="137" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -25104,7 +25230,7 @@
       <c r="K195" s="138"/>
       <c r="L195" s="138"/>
       <c r="M195" s="353"/>
-      <c r="O195" s="611" t="str">
+      <c r="O195" s="589" t="str">
         <f>$T$107</f>
         <v>Auto 2</v>
       </c>
@@ -25150,7 +25276,7 @@
       <c r="K196" s="355"/>
       <c r="L196" s="355"/>
       <c r="M196" s="356"/>
-      <c r="O196" s="611"/>
+      <c r="O196" s="589"/>
       <c r="P196" s="147" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -25195,7 +25321,7 @@
         <f>IF($X$7="","",$X$7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="O197" s="611"/>
+      <c r="O197" s="589"/>
       <c r="P197" s="147" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -25240,7 +25366,7 @@
         <f>IF($R$13="","",$R$13)</f>
         <v/>
       </c>
-      <c r="O198" s="611"/>
+      <c r="O198" s="589"/>
       <c r="P198" s="147" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -25286,7 +25412,7 @@
         <f>$H$2</f>
         <v>Medical University of South Carolina</v>
       </c>
-      <c r="O199" s="611"/>
+      <c r="O199" s="589"/>
       <c r="P199" s="137" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -25335,7 +25461,7 @@
         <f>$H$5</f>
         <v>Fluoroscopy System Compliance Inspection</v>
       </c>
-      <c r="O200" s="611" t="str">
+      <c r="O200" s="589" t="str">
         <f>$W$107</f>
         <v>High Level</v>
       </c>
@@ -25384,7 +25510,7 @@
       <c r="K201" s="349"/>
       <c r="L201" s="349"/>
       <c r="M201" s="350"/>
-      <c r="O201" s="611"/>
+      <c r="O201" s="589"/>
       <c r="P201" s="147" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -25418,24 +25544,24 @@
       <c r="B202" s="351"/>
       <c r="C202" s="401"/>
       <c r="D202" s="373"/>
-      <c r="E202" s="614" t="s">
+      <c r="E202" s="590" t="s">
         <v>264</v>
       </c>
-      <c r="F202" s="615" t="s">
+      <c r="F202" s="591" t="s">
         <v>265</v>
       </c>
-      <c r="G202" s="616" t="s">
+      <c r="G202" s="592" t="s">
         <v>266</v>
       </c>
-      <c r="H202" s="617" t="str">
+      <c r="H202" s="593" t="str">
         <f>R276</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="I202" s="618" t="str">
+      <c r="I202" s="594" t="str">
         <f>S276</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="J202" s="619" t="s">
+      <c r="J202" s="595" t="s">
         <v>267</v>
       </c>
       <c r="K202" s="138" t="s">
@@ -25444,10 +25570,10 @@
       <c r="L202" s="138" t="s">
         <v>269</v>
       </c>
-      <c r="M202" s="620" t="s">
+      <c r="M202" s="596" t="s">
         <v>270</v>
       </c>
-      <c r="O202" s="611"/>
+      <c r="O202" s="589"/>
       <c r="P202" s="147" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -25485,12 +25611,12 @@
       <c r="D203" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="E203" s="614"/>
-      <c r="F203" s="615"/>
-      <c r="G203" s="616"/>
-      <c r="H203" s="617"/>
-      <c r="I203" s="618"/>
-      <c r="J203" s="619"/>
+      <c r="E203" s="590"/>
+      <c r="F203" s="591"/>
+      <c r="G203" s="592"/>
+      <c r="H203" s="593"/>
+      <c r="I203" s="594"/>
+      <c r="J203" s="595"/>
       <c r="K203" s="138" t="str">
         <f>U277</f>
         <v>mGy/min</v>
@@ -25499,8 +25625,8 @@
         <f>V277</f>
         <v>mGy/min</v>
       </c>
-      <c r="M203" s="620"/>
-      <c r="O203" s="611"/>
+      <c r="M203" s="596"/>
+      <c r="O203" s="589"/>
       <c r="P203" s="147" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -25576,7 +25702,7 @@
         <f t="shared" si="30"/>
         <v/>
       </c>
-      <c r="O204" s="611"/>
+      <c r="O204" s="589"/>
       <c r="P204" s="137" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -26235,7 +26361,7 @@
       <c r="K214" s="373"/>
       <c r="L214" s="373"/>
       <c r="M214" s="353"/>
-      <c r="O214" s="611" t="str">
+      <c r="O214" s="589" t="str">
         <f>$Q$139</f>
         <v>Auto 1</v>
       </c>
@@ -26285,7 +26411,7 @@
       <c r="K215" s="422"/>
       <c r="L215" s="422"/>
       <c r="M215" s="423"/>
-      <c r="O215" s="611"/>
+      <c r="O215" s="589"/>
       <c r="P215" s="147" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -26335,7 +26461,7 @@
       <c r="K216" s="373"/>
       <c r="L216" s="373"/>
       <c r="M216" s="353"/>
-      <c r="O216" s="611"/>
+      <c r="O216" s="589"/>
       <c r="P216" s="147" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -26381,7 +26507,7 @@
       <c r="K217" s="373"/>
       <c r="L217" s="373"/>
       <c r="M217" s="377"/>
-      <c r="O217" s="611"/>
+      <c r="O217" s="589"/>
       <c r="P217" s="147" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -26429,7 +26555,7 @@
       <c r="K218" s="373"/>
       <c r="L218" s="373"/>
       <c r="M218" s="377"/>
-      <c r="O218" s="611"/>
+      <c r="O218" s="589"/>
       <c r="P218" s="137" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -26472,7 +26598,7 @@
       <c r="K219" s="373"/>
       <c r="L219" s="373"/>
       <c r="M219" s="377"/>
-      <c r="O219" s="611" t="str">
+      <c r="O219" s="589" t="str">
         <f>$T$139</f>
         <v>Auto 2</v>
       </c>
@@ -26522,7 +26648,7 @@
       <c r="K220" s="373"/>
       <c r="L220" s="373"/>
       <c r="M220" s="377"/>
-      <c r="O220" s="611"/>
+      <c r="O220" s="589"/>
       <c r="P220" s="147" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -26575,7 +26701,7 @@
       <c r="K221" s="373"/>
       <c r="L221" s="373"/>
       <c r="M221" s="377"/>
-      <c r="O221" s="611"/>
+      <c r="O221" s="589"/>
       <c r="P221" s="147" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -26633,7 +26759,7 @@
       <c r="K222" s="373"/>
       <c r="L222" s="373"/>
       <c r="M222" s="377"/>
-      <c r="O222" s="611"/>
+      <c r="O222" s="589"/>
       <c r="P222" s="147" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -26688,7 +26814,7 @@
       <c r="K223" s="373"/>
       <c r="L223" s="373"/>
       <c r="M223" s="377"/>
-      <c r="O223" s="611"/>
+      <c r="O223" s="589"/>
       <c r="P223" s="137" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -26743,7 +26869,7 @@
       <c r="K224" s="373"/>
       <c r="L224" s="373"/>
       <c r="M224" s="377"/>
-      <c r="O224" s="611" t="str">
+      <c r="O224" s="589" t="str">
         <f>$W$139</f>
         <v>High Level</v>
       </c>
@@ -26801,7 +26927,7 @@
       <c r="K225" s="373"/>
       <c r="L225" s="373"/>
       <c r="M225" s="377"/>
-      <c r="O225" s="611"/>
+      <c r="O225" s="589"/>
       <c r="P225" s="147" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -26852,7 +26978,7 @@
       <c r="K226" s="373"/>
       <c r="L226" s="373"/>
       <c r="M226" s="377"/>
-      <c r="O226" s="611"/>
+      <c r="O226" s="589"/>
       <c r="P226" s="147" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -26906,7 +27032,7 @@
       <c r="K227" s="373"/>
       <c r="L227" s="373"/>
       <c r="M227" s="377"/>
-      <c r="O227" s="611"/>
+      <c r="O227" s="589"/>
       <c r="P227" s="147" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -26954,7 +27080,7 @@
       <c r="K228" s="373"/>
       <c r="L228" s="373"/>
       <c r="M228" s="377"/>
-      <c r="O228" s="611"/>
+      <c r="O228" s="589"/>
       <c r="P228" s="137" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -27480,7 +27606,7 @@
       <c r="K240" s="373"/>
       <c r="L240" s="373"/>
       <c r="M240" s="377"/>
-      <c r="O240" s="612" t="s">
+      <c r="O240" s="597" t="s">
         <v>296</v>
       </c>
       <c r="P240" s="172" t="s">
@@ -27542,7 +27668,7 @@
       <c r="K241" s="373"/>
       <c r="L241" s="373"/>
       <c r="M241" s="377"/>
-      <c r="O241" s="612"/>
+      <c r="O241" s="597"/>
       <c r="P241" s="177" t="s">
         <v>299</v>
       </c>
@@ -27593,7 +27719,7 @@
       <c r="K242" s="373"/>
       <c r="L242" s="373"/>
       <c r="M242" s="377"/>
-      <c r="O242" s="612" t="str">
+      <c r="O242" s="597" t="str">
         <f>IF($U$137=1,"Scatter - Pulse", "Scatter – Digital acq")</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -27653,7 +27779,7 @@
       <c r="K243" s="373"/>
       <c r="L243" s="373"/>
       <c r="M243" s="377"/>
-      <c r="O243" s="612"/>
+      <c r="O243" s="597"/>
       <c r="P243" s="177" t="s">
         <v>299</v>
       </c>
@@ -28179,17 +28305,17 @@
       <c r="P257" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="Q257" s="613" t="s">
+      <c r="Q257" s="598" t="s">
         <v>315</v>
       </c>
-      <c r="R257" s="613"/>
+      <c r="R257" s="598"/>
       <c r="S257" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="T257" s="613" t="s">
+      <c r="T257" s="598" t="s">
         <v>317</v>
       </c>
-      <c r="U257" s="613"/>
+      <c r="U257" s="598"/>
       <c r="V257" s="1" t="s">
         <v>318</v>
       </c>
@@ -28654,24 +28780,24 @@
         <f t="shared" si="41"/>
         <v>Attenuator</v>
       </c>
-      <c r="E269" s="605" t="str">
+      <c r="E269" s="599" t="str">
         <f>Q107</f>
         <v>Auto 1</v>
       </c>
-      <c r="F269" s="606"/>
-      <c r="G269" s="606"/>
-      <c r="H269" s="606" t="str">
+      <c r="F269" s="600"/>
+      <c r="G269" s="600"/>
+      <c r="H269" s="600" t="str">
         <f>T107</f>
         <v>Auto 2</v>
       </c>
-      <c r="I269" s="606"/>
-      <c r="J269" s="606"/>
-      <c r="K269" s="607" t="str">
+      <c r="I269" s="600"/>
+      <c r="J269" s="600"/>
+      <c r="K269" s="601" t="str">
         <f>W107</f>
         <v>High Level</v>
       </c>
-      <c r="L269" s="607"/>
-      <c r="M269" s="608"/>
+      <c r="L269" s="601"/>
+      <c r="M269" s="602"/>
       <c r="O269" s="196" t="str">
         <f t="shared" si="42"/>
         <v/>
@@ -28773,7 +28899,7 @@
         <v>7</v>
       </c>
       <c r="B271" s="351"/>
-      <c r="C271" s="595" t="str">
+      <c r="C271" s="603" t="str">
         <f>O110&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -28842,7 +28968,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="351"/>
-      <c r="C272" s="595"/>
+      <c r="C272" s="603"/>
       <c r="D272" s="449">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -28915,7 +29041,7 @@
         <v>9</v>
       </c>
       <c r="B273" s="351"/>
-      <c r="C273" s="595"/>
+      <c r="C273" s="603"/>
       <c r="D273" s="452">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -28981,7 +29107,7 @@
         <v>10</v>
       </c>
       <c r="B274" s="351"/>
-      <c r="C274" s="595" t="str">
+      <c r="C274" s="603" t="str">
         <f>O113&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29057,7 +29183,7 @@
         <v>11</v>
       </c>
       <c r="B275" s="351"/>
-      <c r="C275" s="595"/>
+      <c r="C275" s="603"/>
       <c r="D275" s="449">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -29123,7 +29249,7 @@
         <v>12</v>
       </c>
       <c r="B276" s="351"/>
-      <c r="C276" s="595"/>
+      <c r="C276" s="603"/>
       <c r="D276" s="452">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -29164,17 +29290,17 @@
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="O276" s="609" t="s">
+      <c r="O276" s="604" t="s">
         <v>264</v>
       </c>
-      <c r="P276" s="610" t="s">
+      <c r="P276" s="605" t="s">
         <v>265</v>
       </c>
-      <c r="R276" s="610" t="str">
+      <c r="R276" s="605" t="str">
         <f>"Ind AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="S276" s="610" t="str">
+      <c r="S276" s="605" t="str">
         <f>"Meas AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -29203,7 +29329,7 @@
         <v>13</v>
       </c>
       <c r="B277" s="351"/>
-      <c r="C277" s="595" t="str">
+      <c r="C277" s="603" t="str">
         <f>O116&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29247,13 +29373,13 @@
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="O277" s="609"/>
-      <c r="P277" s="610"/>
+      <c r="O277" s="604"/>
+      <c r="P277" s="605"/>
       <c r="Q277" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="R277" s="610"/>
-      <c r="S277" s="610"/>
+      <c r="R277" s="605"/>
+      <c r="S277" s="605"/>
       <c r="T277" s="1" t="s">
         <v>324</v>
       </c>
@@ -29288,7 +29414,7 @@
         <v>14</v>
       </c>
       <c r="B278" s="351"/>
-      <c r="C278" s="595"/>
+      <c r="C278" s="603"/>
       <c r="D278" s="449">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -29375,7 +29501,7 @@
         <v>15</v>
       </c>
       <c r="B279" s="351"/>
-      <c r="C279" s="595"/>
+      <c r="C279" s="603"/>
       <c r="D279" s="452">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -29469,7 +29595,7 @@
         <v>16</v>
       </c>
       <c r="B280" s="351"/>
-      <c r="C280" s="595" t="str">
+      <c r="C280" s="603" t="str">
         <f>O119&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29559,7 +29685,7 @@
         <v>17</v>
       </c>
       <c r="B281" s="351"/>
-      <c r="C281" s="595"/>
+      <c r="C281" s="603"/>
       <c r="D281" s="449">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -29653,7 +29779,7 @@
         <v>18</v>
       </c>
       <c r="B282" s="351"/>
-      <c r="C282" s="595"/>
+      <c r="C282" s="603"/>
       <c r="D282" s="452">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -29740,7 +29866,7 @@
         <v>19</v>
       </c>
       <c r="B283" s="351"/>
-      <c r="C283" s="595" t="str">
+      <c r="C283" s="603" t="str">
         <f>O122&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29837,7 +29963,7 @@
         <v>20</v>
       </c>
       <c r="B284" s="351"/>
-      <c r="C284" s="595"/>
+      <c r="C284" s="603"/>
       <c r="D284" s="449">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -29924,7 +30050,7 @@
         <v>21</v>
       </c>
       <c r="B285" s="351"/>
-      <c r="C285" s="595"/>
+      <c r="C285" s="603"/>
       <c r="D285" s="449">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -30355,12 +30481,12 @@
       <c r="L293" s="138"/>
       <c r="M293" s="353"/>
       <c r="O293" s="241"/>
-      <c r="P293" s="600" t="s">
+      <c r="P293" s="606" t="s">
         <v>330</v>
       </c>
-      <c r="Q293" s="600"/>
-      <c r="R293" s="600"/>
-      <c r="S293" s="600"/>
+      <c r="Q293" s="606"/>
+      <c r="R293" s="606"/>
+      <c r="S293" s="606"/>
       <c r="T293" s="239"/>
       <c r="U293" s="239"/>
       <c r="V293" s="239"/>
@@ -30744,12 +30870,12 @@
       <c r="L302" s="138"/>
       <c r="M302" s="353"/>
       <c r="O302" s="241"/>
-      <c r="P302" s="600" t="s">
+      <c r="P302" s="606" t="s">
         <v>330</v>
       </c>
-      <c r="Q302" s="600"/>
-      <c r="R302" s="600"/>
-      <c r="S302" s="600"/>
+      <c r="Q302" s="606"/>
+      <c r="R302" s="606"/>
+      <c r="S302" s="606"/>
       <c r="T302" s="239"/>
       <c r="U302" s="239"/>
       <c r="V302" s="239"/>
@@ -30764,7 +30890,7 @@
         <v>39</v>
       </c>
       <c r="B303" s="351"/>
-      <c r="C303" s="578" t="str">
+      <c r="C303" s="607" t="str">
         <f>O190</f>
         <v>Auto 1</v>
       </c>
@@ -30832,7 +30958,7 @@
         <v>40</v>
       </c>
       <c r="B304" s="351"/>
-      <c r="C304" s="579"/>
+      <c r="C304" s="608"/>
       <c r="D304" s="491" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -30895,7 +31021,7 @@
         <v>41</v>
       </c>
       <c r="B305" s="351"/>
-      <c r="C305" s="579"/>
+      <c r="C305" s="608"/>
       <c r="D305" s="491" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -30950,7 +31076,7 @@
         <v>42</v>
       </c>
       <c r="B306" s="351"/>
-      <c r="C306" s="579"/>
+      <c r="C306" s="608"/>
       <c r="D306" s="491" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -30995,7 +31121,7 @@
         <v>43</v>
       </c>
       <c r="B307" s="351"/>
-      <c r="C307" s="601"/>
+      <c r="C307" s="609"/>
       <c r="D307" s="494" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31047,7 +31173,7 @@
         <v>44</v>
       </c>
       <c r="B308" s="351"/>
-      <c r="C308" s="578" t="str">
+      <c r="C308" s="607" t="str">
         <f>O195</f>
         <v>Auto 2</v>
       </c>
@@ -31095,7 +31221,7 @@
         <v>45</v>
       </c>
       <c r="B309" s="351"/>
-      <c r="C309" s="579"/>
+      <c r="C309" s="608"/>
       <c r="D309" s="491" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31152,7 +31278,7 @@
         <v>46</v>
       </c>
       <c r="B310" s="351"/>
-      <c r="C310" s="579"/>
+      <c r="C310" s="608"/>
       <c r="D310" s="491" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31202,7 +31328,7 @@
         <v>47</v>
       </c>
       <c r="B311" s="351"/>
-      <c r="C311" s="579"/>
+      <c r="C311" s="608"/>
       <c r="D311" s="491" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31259,7 +31385,7 @@
         <v>48</v>
       </c>
       <c r="B312" s="351"/>
-      <c r="C312" s="580"/>
+      <c r="C312" s="610"/>
       <c r="D312" s="497" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31309,7 +31435,7 @@
         <v>49</v>
       </c>
       <c r="B313" s="351"/>
-      <c r="C313" s="602" t="str">
+      <c r="C313" s="611" t="str">
         <f>O200</f>
         <v>High Level</v>
       </c>
@@ -31368,7 +31494,7 @@
         <v>50</v>
       </c>
       <c r="B314" s="351"/>
-      <c r="C314" s="579"/>
+      <c r="C314" s="608"/>
       <c r="D314" s="491" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31411,7 +31537,7 @@
         <v>51</v>
       </c>
       <c r="B315" s="351"/>
-      <c r="C315" s="579"/>
+      <c r="C315" s="608"/>
       <c r="D315" s="491" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31454,7 +31580,7 @@
         <v>52</v>
       </c>
       <c r="B316" s="351"/>
-      <c r="C316" s="579"/>
+      <c r="C316" s="608"/>
       <c r="D316" s="491" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31499,7 +31625,7 @@
         <v>53</v>
       </c>
       <c r="B317" s="351"/>
-      <c r="C317" s="580"/>
+      <c r="C317" s="610"/>
       <c r="D317" s="497" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31609,10 +31735,10 @@
       <c r="R319" s="280"/>
       <c r="S319" s="281"/>
       <c r="T319" s="281"/>
-      <c r="V319" s="603" t="s">
+      <c r="V319" s="588" t="s">
         <v>342</v>
       </c>
-      <c r="W319" s="603"/>
+      <c r="W319" s="588"/>
       <c r="X319" s="18" t="s">
         <v>343</v>
       </c>
@@ -31813,7 +31939,7 @@
         <v>60</v>
       </c>
       <c r="B324" s="351"/>
-      <c r="C324" s="584" t="str">
+      <c r="C324" s="612" t="str">
         <f>O240</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -31863,7 +31989,7 @@
         <v>61</v>
       </c>
       <c r="B325" s="351"/>
-      <c r="C325" s="585"/>
+      <c r="C325" s="613"/>
       <c r="D325" s="506" t="str">
         <f>P241</f>
         <v>Waist level</v>
@@ -32021,13 +32147,13 @@
         <v>350</v>
       </c>
       <c r="P329" s="56"/>
-      <c r="Q329" s="604" t="s">
+      <c r="Q329" s="614" t="s">
         <v>351</v>
       </c>
-      <c r="R329" s="604"/>
-      <c r="S329" s="604"/>
-      <c r="T329" s="604"/>
-      <c r="U329" s="604"/>
+      <c r="R329" s="614"/>
+      <c r="S329" s="614"/>
+      <c r="T329" s="614"/>
+      <c r="U329" s="614"/>
       <c r="Y329" s="15"/>
     </row>
     <row r="330" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32216,24 +32342,24 @@
         <f t="shared" si="69"/>
         <v>Attenuator</v>
       </c>
-      <c r="E335" s="605" t="str">
+      <c r="E335" s="599" t="str">
         <f>Q139</f>
         <v>Auto 1</v>
       </c>
-      <c r="F335" s="606"/>
-      <c r="G335" s="606"/>
-      <c r="H335" s="606" t="str">
+      <c r="F335" s="600"/>
+      <c r="G335" s="600"/>
+      <c r="H335" s="600" t="str">
         <f>T139</f>
         <v>Auto 2</v>
       </c>
-      <c r="I335" s="606"/>
-      <c r="J335" s="606"/>
-      <c r="K335" s="607" t="str">
+      <c r="I335" s="600"/>
+      <c r="J335" s="600"/>
+      <c r="K335" s="601" t="str">
         <f>W139</f>
         <v>High Level</v>
       </c>
-      <c r="L335" s="607"/>
-      <c r="M335" s="608"/>
+      <c r="L335" s="601"/>
+      <c r="M335" s="602"/>
       <c r="O335" s="133"/>
       <c r="P335" s="132" t="s">
         <v>357</v>
@@ -32322,7 +32448,7 @@
         <v>7</v>
       </c>
       <c r="B337" s="351"/>
-      <c r="C337" s="595" t="str">
+      <c r="C337" s="603" t="str">
         <f>O142&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -32388,7 +32514,7 @@
         <v>8</v>
       </c>
       <c r="B338" s="351"/>
-      <c r="C338" s="595"/>
+      <c r="C338" s="603"/>
       <c r="D338" s="520">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -32451,7 +32577,7 @@
         <v>9</v>
       </c>
       <c r="B339" s="351"/>
-      <c r="C339" s="595"/>
+      <c r="C339" s="603"/>
       <c r="D339" s="521">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -32514,7 +32640,7 @@
         <v>10</v>
       </c>
       <c r="B340" s="351"/>
-      <c r="C340" s="595" t="str">
+      <c r="C340" s="603" t="str">
         <f>O145&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -32580,7 +32706,7 @@
         <v>11</v>
       </c>
       <c r="B341" s="351"/>
-      <c r="C341" s="595"/>
+      <c r="C341" s="603"/>
       <c r="D341" s="520">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -32643,7 +32769,7 @@
         <v>12</v>
       </c>
       <c r="B342" s="351"/>
-      <c r="C342" s="595"/>
+      <c r="C342" s="603"/>
       <c r="D342" s="522">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -32706,7 +32832,7 @@
         <v>13</v>
       </c>
       <c r="B343" s="351"/>
-      <c r="C343" s="595" t="str">
+      <c r="C343" s="603" t="str">
         <f>O148&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -32758,7 +32884,7 @@
         <v>14</v>
       </c>
       <c r="B344" s="351"/>
-      <c r="C344" s="595"/>
+      <c r="C344" s="603"/>
       <c r="D344" s="520">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -32820,7 +32946,7 @@
         <v>15</v>
       </c>
       <c r="B345" s="351"/>
-      <c r="C345" s="595"/>
+      <c r="C345" s="603"/>
       <c r="D345" s="521">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -32883,7 +33009,7 @@
         <v>16</v>
       </c>
       <c r="B346" s="351"/>
-      <c r="C346" s="595" t="str">
+      <c r="C346" s="603" t="str">
         <f>O151&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -32946,7 +33072,7 @@
         <v>17</v>
       </c>
       <c r="B347" s="351"/>
-      <c r="C347" s="595"/>
+      <c r="C347" s="603"/>
       <c r="D347" s="520">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33004,7 +33130,7 @@
         <v>18</v>
       </c>
       <c r="B348" s="351"/>
-      <c r="C348" s="595"/>
+      <c r="C348" s="603"/>
       <c r="D348" s="522">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -33082,7 +33208,7 @@
         <v>19</v>
       </c>
       <c r="B349" s="351"/>
-      <c r="C349" s="595" t="str">
+      <c r="C349" s="603" t="str">
         <f>O154&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33145,7 +33271,7 @@
         <v>20</v>
       </c>
       <c r="B350" s="351"/>
-      <c r="C350" s="595"/>
+      <c r="C350" s="603"/>
       <c r="D350" s="520">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33204,7 +33330,7 @@
         <v>21</v>
       </c>
       <c r="B351" s="351"/>
-      <c r="C351" s="595"/>
+      <c r="C351" s="603"/>
       <c r="D351" s="522">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -33513,11 +33639,11 @@
         <f>IF(OR(V358="",V359="",V362=""),"",(V358-V359)*V362)</f>
         <v/>
       </c>
-      <c r="Q358" s="596" t="str">
+      <c r="Q358" s="615" t="str">
         <f>IF(OR(P358="",P359=""),"",(ABS(P358)+ABS(P359))/$O$355)</f>
         <v/>
       </c>
-      <c r="R358" s="597" t="str">
+      <c r="R358" s="616" t="str">
         <f>IF(OR(Q358="",Q360=""),"",Q358+Q360)</f>
         <v/>
       </c>
@@ -33556,8 +33682,8 @@
         <f>IF(OR(W358="",W359="",V362=""),"",(W358-W359)*V362)</f>
         <v/>
       </c>
-      <c r="Q359" s="596"/>
-      <c r="R359" s="596"/>
+      <c r="Q359" s="615"/>
+      <c r="R359" s="615"/>
       <c r="S359" s="149" t="str">
         <f>IF(AB168="","",AB168)</f>
         <v/>
@@ -33593,11 +33719,11 @@
         <f>IF(OR(X358="",X359="",V362=""),"",(X358-X359)*V362)</f>
         <v/>
       </c>
-      <c r="Q360" s="597" t="str">
+      <c r="Q360" s="616" t="str">
         <f>IF(OR(P360="",P361=""),"",(ABS(P360)+ABS(P361))/$O$355)</f>
         <v/>
       </c>
-      <c r="R360" s="597"/>
+      <c r="R360" s="616"/>
       <c r="S360" s="149" t="str">
         <f>IF(AB169="","",AB169)</f>
         <v/>
@@ -33639,8 +33765,8 @@
         <f>IF(OR(Y358="",Y359="",V362=""),"",(Y358-Y359)*V362)</f>
         <v/>
       </c>
-      <c r="Q361" s="597"/>
-      <c r="R361" s="597"/>
+      <c r="Q361" s="616"/>
+      <c r="R361" s="616"/>
       <c r="S361" s="151" t="str">
         <f>IF(AB170="","",AB170)</f>
         <v/>
@@ -33812,7 +33938,7 @@
         <v>36</v>
       </c>
       <c r="B366" s="351"/>
-      <c r="C366" s="598" t="str">
+      <c r="C366" s="617" t="str">
         <f>O214</f>
         <v>Auto 1</v>
       </c>
@@ -33863,7 +33989,7 @@
         <v>37</v>
       </c>
       <c r="B367" s="351"/>
-      <c r="C367" s="599"/>
+      <c r="C367" s="618"/>
       <c r="D367" s="491" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -33909,7 +34035,7 @@
         <v>38</v>
       </c>
       <c r="B368" s="351"/>
-      <c r="C368" s="599"/>
+      <c r="C368" s="618"/>
       <c r="D368" s="491" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -33944,7 +34070,7 @@
         <v>39</v>
       </c>
       <c r="B369" s="351"/>
-      <c r="C369" s="599"/>
+      <c r="C369" s="618"/>
       <c r="D369" s="491" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -33979,7 +34105,7 @@
         <v>40</v>
       </c>
       <c r="B370" s="351"/>
-      <c r="C370" s="599"/>
+      <c r="C370" s="618"/>
       <c r="D370" s="497" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34024,7 +34150,7 @@
         <v>41</v>
       </c>
       <c r="B371" s="351"/>
-      <c r="C371" s="578" t="str">
+      <c r="C371" s="607" t="str">
         <f>O219</f>
         <v>Auto 2</v>
       </c>
@@ -34074,7 +34200,7 @@
         <v>42</v>
       </c>
       <c r="B372" s="351"/>
-      <c r="C372" s="579"/>
+      <c r="C372" s="608"/>
       <c r="D372" s="491" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34124,7 +34250,7 @@
         <v>43</v>
       </c>
       <c r="B373" s="351"/>
-      <c r="C373" s="579"/>
+      <c r="C373" s="608"/>
       <c r="D373" s="491" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34171,7 +34297,7 @@
         <v>44</v>
       </c>
       <c r="B374" s="351"/>
-      <c r="C374" s="579"/>
+      <c r="C374" s="608"/>
       <c r="D374" s="491" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34221,7 +34347,7 @@
         <v>45</v>
       </c>
       <c r="B375" s="351"/>
-      <c r="C375" s="580"/>
+      <c r="C375" s="610"/>
       <c r="D375" s="497" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34268,7 +34394,7 @@
         <v>46</v>
       </c>
       <c r="B376" s="351"/>
-      <c r="C376" s="581" t="str">
+      <c r="C376" s="619" t="str">
         <f>O224</f>
         <v>High Level</v>
       </c>
@@ -34321,7 +34447,7 @@
         <v>47</v>
       </c>
       <c r="B377" s="351"/>
-      <c r="C377" s="582"/>
+      <c r="C377" s="620"/>
       <c r="D377" s="491" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34368,7 +34494,7 @@
         <v>48</v>
       </c>
       <c r="B378" s="351"/>
-      <c r="C378" s="582"/>
+      <c r="C378" s="620"/>
       <c r="D378" s="491" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34418,7 +34544,7 @@
         <v>49</v>
       </c>
       <c r="B379" s="351"/>
-      <c r="C379" s="582"/>
+      <c r="C379" s="620"/>
       <c r="D379" s="491" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34465,7 +34591,7 @@
         <v>50</v>
       </c>
       <c r="B380" s="351"/>
-      <c r="C380" s="583"/>
+      <c r="C380" s="621"/>
       <c r="D380" s="497" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34775,7 +34901,7 @@
         <v>58</v>
       </c>
       <c r="B388" s="351"/>
-      <c r="C388" s="584" t="str">
+      <c r="C388" s="612" t="str">
         <f>O242</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -34826,7 +34952,7 @@
         <v>59</v>
       </c>
       <c r="B389" s="351"/>
-      <c r="C389" s="585"/>
+      <c r="C389" s="613"/>
       <c r="D389" s="506" t="str">
         <f>P243</f>
         <v>Waist level</v>
@@ -35177,14 +35303,14 @@
       <c r="E399" s="349"/>
       <c r="F399" s="349"/>
       <c r="G399" s="349"/>
-      <c r="H399" s="586" t="s">
+      <c r="H399" s="622" t="s">
         <v>397</v>
       </c>
-      <c r="I399" s="586"/>
-      <c r="J399" s="586" t="s">
+      <c r="I399" s="622"/>
+      <c r="J399" s="622" t="s">
         <v>398</v>
       </c>
-      <c r="K399" s="586"/>
+      <c r="K399" s="622"/>
       <c r="L399" s="349"/>
       <c r="M399" s="350"/>
       <c r="O399" s="14"/>
@@ -35758,20 +35884,20 @@
       </c>
       <c r="B413" s="351"/>
       <c r="C413" s="45"/>
-      <c r="D413" s="587" t="s">
+      <c r="D413" s="623" t="s">
         <v>404</v>
       </c>
-      <c r="E413" s="587"/>
-      <c r="F413" s="587"/>
-      <c r="G413" s="587"/>
-      <c r="H413" s="587"/>
-      <c r="I413" s="587" t="s">
+      <c r="E413" s="623"/>
+      <c r="F413" s="623"/>
+      <c r="G413" s="623"/>
+      <c r="H413" s="623"/>
+      <c r="I413" s="623" t="s">
         <v>405</v>
       </c>
-      <c r="J413" s="587"/>
-      <c r="K413" s="587"/>
-      <c r="L413" s="587"/>
-      <c r="M413" s="588"/>
+      <c r="J413" s="623"/>
+      <c r="K413" s="623"/>
+      <c r="L413" s="623"/>
+      <c r="M413" s="624"/>
       <c r="O413" s="14"/>
       <c r="P413" s="2" t="s">
         <v>191</v>
@@ -37251,11 +37377,11 @@
         <f t="shared" si="92"/>
         <v/>
       </c>
-      <c r="F442" s="589" t="str">
+      <c r="F442" s="625" t="str">
         <f t="shared" si="92"/>
         <v/>
       </c>
-      <c r="G442" s="591" t="str">
+      <c r="G442" s="627" t="str">
         <f t="shared" si="92"/>
         <v/>
       </c>
@@ -37296,8 +37422,8 @@
         <f>P359</f>
         <v/>
       </c>
-      <c r="F443" s="590"/>
-      <c r="G443" s="592"/>
+      <c r="F443" s="626"/>
+      <c r="G443" s="628"/>
       <c r="H443" s="207"/>
       <c r="I443" s="85" t="str">
         <f>T360</f>
@@ -37337,11 +37463,11 @@
         <f>P360</f>
         <v/>
       </c>
-      <c r="F444" s="590" t="str">
+      <c r="F444" s="626" t="str">
         <f>Q360</f>
         <v/>
       </c>
-      <c r="G444" s="592"/>
+      <c r="G444" s="628"/>
       <c r="H444" s="138"/>
       <c r="I444" s="94" t="str">
         <f>T361</f>
@@ -37382,8 +37508,8 @@
         <f>P361</f>
         <v/>
       </c>
-      <c r="F445" s="594"/>
-      <c r="G445" s="593"/>
+      <c r="F445" s="630"/>
+      <c r="G445" s="629"/>
       <c r="H445" s="138"/>
       <c r="I445" s="138"/>
       <c r="J445" s="138"/>
@@ -43719,43 +43845,66 @@
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="C371:C375"/>
+    <mergeCell ref="C376:C380"/>
+    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="H399:I399"/>
+    <mergeCell ref="J399:K399"/>
+    <mergeCell ref="D413:H413"/>
+    <mergeCell ref="I413:M413"/>
+    <mergeCell ref="F442:F443"/>
+    <mergeCell ref="G442:G445"/>
+    <mergeCell ref="F444:F445"/>
+    <mergeCell ref="C337:C339"/>
+    <mergeCell ref="C340:C342"/>
+    <mergeCell ref="C343:C345"/>
+    <mergeCell ref="C346:C348"/>
+    <mergeCell ref="C349:C351"/>
+    <mergeCell ref="Q358:Q359"/>
+    <mergeCell ref="R358:R361"/>
+    <mergeCell ref="Q360:Q361"/>
+    <mergeCell ref="C366:C370"/>
+    <mergeCell ref="P293:S293"/>
+    <mergeCell ref="P302:S302"/>
+    <mergeCell ref="C303:C307"/>
+    <mergeCell ref="C308:C312"/>
+    <mergeCell ref="C313:C317"/>
+    <mergeCell ref="V319:W319"/>
+    <mergeCell ref="C324:C325"/>
+    <mergeCell ref="Q329:U329"/>
+    <mergeCell ref="E335:G335"/>
+    <mergeCell ref="H335:J335"/>
+    <mergeCell ref="K335:M335"/>
+    <mergeCell ref="C271:C273"/>
+    <mergeCell ref="C274:C276"/>
+    <mergeCell ref="O276:O277"/>
+    <mergeCell ref="P276:P277"/>
+    <mergeCell ref="R276:R277"/>
+    <mergeCell ref="S276:S277"/>
+    <mergeCell ref="C277:C279"/>
+    <mergeCell ref="C280:C282"/>
+    <mergeCell ref="C283:C285"/>
+    <mergeCell ref="O214:O218"/>
+    <mergeCell ref="O219:O223"/>
+    <mergeCell ref="O224:O228"/>
+    <mergeCell ref="O240:O241"/>
+    <mergeCell ref="O242:O243"/>
+    <mergeCell ref="Q257:R257"/>
+    <mergeCell ref="T257:U257"/>
+    <mergeCell ref="E269:G269"/>
+    <mergeCell ref="H269:J269"/>
+    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="T181:U181"/>
+    <mergeCell ref="O190:O194"/>
+    <mergeCell ref="O195:O199"/>
+    <mergeCell ref="O200:O204"/>
+    <mergeCell ref="E202:E203"/>
+    <mergeCell ref="F202:F203"/>
+    <mergeCell ref="G202:G203"/>
+    <mergeCell ref="H202:H203"/>
+    <mergeCell ref="I202:I203"/>
+    <mergeCell ref="J202:J203"/>
+    <mergeCell ref="M202:M203"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="K40:L40"/>
     <mergeCell ref="F41:G41"/>
@@ -43767,66 +43916,43 @@
     <mergeCell ref="Q139:S139"/>
     <mergeCell ref="T139:V139"/>
     <mergeCell ref="W139:Y139"/>
-    <mergeCell ref="T181:U181"/>
-    <mergeCell ref="O190:O194"/>
-    <mergeCell ref="O195:O199"/>
-    <mergeCell ref="O200:O204"/>
-    <mergeCell ref="E202:E203"/>
-    <mergeCell ref="F202:F203"/>
-    <mergeCell ref="G202:G203"/>
-    <mergeCell ref="H202:H203"/>
-    <mergeCell ref="I202:I203"/>
-    <mergeCell ref="J202:J203"/>
-    <mergeCell ref="M202:M203"/>
-    <mergeCell ref="O214:O218"/>
-    <mergeCell ref="O219:O223"/>
-    <mergeCell ref="O224:O228"/>
-    <mergeCell ref="O240:O241"/>
-    <mergeCell ref="O242:O243"/>
-    <mergeCell ref="Q257:R257"/>
-    <mergeCell ref="T257:U257"/>
-    <mergeCell ref="E269:G269"/>
-    <mergeCell ref="H269:J269"/>
-    <mergeCell ref="K269:M269"/>
-    <mergeCell ref="C271:C273"/>
-    <mergeCell ref="C274:C276"/>
-    <mergeCell ref="O276:O277"/>
-    <mergeCell ref="P276:P277"/>
-    <mergeCell ref="R276:R277"/>
-    <mergeCell ref="S276:S277"/>
-    <mergeCell ref="C277:C279"/>
-    <mergeCell ref="C280:C282"/>
-    <mergeCell ref="C283:C285"/>
-    <mergeCell ref="P293:S293"/>
-    <mergeCell ref="P302:S302"/>
-    <mergeCell ref="C303:C307"/>
-    <mergeCell ref="C308:C312"/>
-    <mergeCell ref="C313:C317"/>
-    <mergeCell ref="V319:W319"/>
-    <mergeCell ref="C324:C325"/>
-    <mergeCell ref="Q329:U329"/>
-    <mergeCell ref="E335:G335"/>
-    <mergeCell ref="H335:J335"/>
-    <mergeCell ref="K335:M335"/>
-    <mergeCell ref="C337:C339"/>
-    <mergeCell ref="C340:C342"/>
-    <mergeCell ref="C343:C345"/>
-    <mergeCell ref="C346:C348"/>
-    <mergeCell ref="C349:C351"/>
-    <mergeCell ref="Q358:Q359"/>
-    <mergeCell ref="R358:R361"/>
-    <mergeCell ref="Q360:Q361"/>
-    <mergeCell ref="C366:C370"/>
-    <mergeCell ref="C371:C375"/>
-    <mergeCell ref="C376:C380"/>
-    <mergeCell ref="C388:C389"/>
-    <mergeCell ref="H399:I399"/>
-    <mergeCell ref="J399:K399"/>
-    <mergeCell ref="D413:H413"/>
-    <mergeCell ref="I413:M413"/>
-    <mergeCell ref="F442:F443"/>
-    <mergeCell ref="G442:G445"/>
-    <mergeCell ref="F444:F445"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
   </mergeCells>
   <conditionalFormatting sqref="S126 V126 Y126 S158 V158 Y158">
     <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
@@ -43984,7 +44110,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK1048576"/>
   <sheetViews>
-    <sheetView defaultGridColor="0" colorId="9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -44091,39 +44219,39 @@
         <f>Fluoro!D269</f>
         <v>Attenuator</v>
       </c>
-      <c r="E5" s="606" t="str">
+      <c r="E5" s="600" t="str">
         <f>Fluoro!E269</f>
         <v>Auto 1</v>
       </c>
-      <c r="F5" s="606">
+      <c r="F5" s="600">
         <f>Fluoro!F269</f>
         <v>0</v>
       </c>
-      <c r="G5" s="606">
+      <c r="G5" s="600">
         <f>Fluoro!G269</f>
         <v>0</v>
       </c>
-      <c r="H5" s="606" t="str">
+      <c r="H5" s="600" t="str">
         <f>Fluoro!H269</f>
         <v>Auto 2</v>
       </c>
-      <c r="I5" s="606">
+      <c r="I5" s="600">
         <f>Fluoro!I269</f>
         <v>0</v>
       </c>
-      <c r="J5" s="606">
+      <c r="J5" s="600">
         <f>Fluoro!J269</f>
         <v>0</v>
       </c>
-      <c r="K5" s="607" t="str">
+      <c r="K5" s="601" t="str">
         <f>Fluoro!K269</f>
         <v>High Level</v>
       </c>
-      <c r="L5" s="607">
+      <c r="L5" s="601">
         <f>Fluoro!L269</f>
         <v>0</v>
       </c>
-      <c r="M5" s="607">
+      <c r="M5" s="601">
         <f>Fluoro!M269</f>
         <v>0</v>
       </c>
@@ -44180,7 +44308,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="634" t="str">
+      <c r="C7" s="631" t="str">
         <f>Fluoro!C271</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -44230,7 +44358,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="634">
+      <c r="C8" s="631">
         <f>Fluoro!C272</f>
         <v>0</v>
       </c>
@@ -44280,7 +44408,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="634">
+      <c r="C9" s="631">
         <f>Fluoro!C273</f>
         <v>0</v>
       </c>
@@ -44330,7 +44458,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="634" t="str">
+      <c r="C10" s="631" t="str">
         <f>Fluoro!C274</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -44380,7 +44508,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="634">
+      <c r="C11" s="631">
         <f>Fluoro!C275</f>
         <v>0</v>
       </c>
@@ -44430,7 +44558,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="634">
+      <c r="C12" s="631">
         <f>Fluoro!C276</f>
         <v>0</v>
       </c>
@@ -44480,7 +44608,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="634" t="str">
+      <c r="C13" s="631" t="str">
         <f>Fluoro!C277</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -44530,7 +44658,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="634">
+      <c r="C14" s="631">
         <f>Fluoro!C278</f>
         <v>0</v>
       </c>
@@ -44580,7 +44708,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="634">
+      <c r="C15" s="631">
         <f>Fluoro!C279</f>
         <v>0</v>
       </c>
@@ -44630,7 +44758,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="634" t="str">
+      <c r="C16" s="631" t="str">
         <f>Fluoro!C280</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -44680,7 +44808,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="634">
+      <c r="C17" s="631">
         <f>Fluoro!C281</f>
         <v>0</v>
       </c>
@@ -44730,7 +44858,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="11"/>
-      <c r="C18" s="634">
+      <c r="C18" s="631">
         <f>Fluoro!C282</f>
         <v>0</v>
       </c>
@@ -44780,7 +44908,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="11"/>
-      <c r="C19" s="634" t="str">
+      <c r="C19" s="631" t="str">
         <f>Fluoro!C283</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -44830,7 +44958,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="634">
+      <c r="C20" s="631">
         <f>Fluoro!C284</f>
         <v>0</v>
       </c>
@@ -44880,7 +45008,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="634">
+      <c r="C21" s="631">
         <f>Fluoro!C285</f>
         <v>0</v>
       </c>
@@ -45329,7 +45457,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="631" t="str">
+      <c r="C39" s="632" t="str">
         <f>Fluoro!C303</f>
         <v>Auto 1</v>
       </c>
@@ -45367,7 +45495,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="11"/>
-      <c r="C40" s="631">
+      <c r="C40" s="632">
         <f>Fluoro!C304</f>
         <v>0</v>
       </c>
@@ -45405,7 +45533,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="11"/>
-      <c r="C41" s="631">
+      <c r="C41" s="632">
         <f>Fluoro!C305</f>
         <v>0</v>
       </c>
@@ -45443,7 +45571,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="631">
+      <c r="C42" s="632">
         <f>Fluoro!C306</f>
         <v>0</v>
       </c>
@@ -45478,7 +45606,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="631">
+      <c r="C43" s="632">
         <f>Fluoro!C307</f>
         <v>0</v>
       </c>
@@ -45513,7 +45641,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="11"/>
-      <c r="C44" s="632" t="str">
+      <c r="C44" s="633" t="str">
         <f>Fluoro!C308</f>
         <v>Auto 2</v>
       </c>
@@ -45548,7 +45676,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="11"/>
-      <c r="C45" s="632">
+      <c r="C45" s="633">
         <f>Fluoro!C309</f>
         <v>0</v>
       </c>
@@ -45583,7 +45711,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="11"/>
-      <c r="C46" s="632">
+      <c r="C46" s="633">
         <f>Fluoro!C310</f>
         <v>0</v>
       </c>
@@ -45618,7 +45746,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="632">
+      <c r="C47" s="633">
         <f>Fluoro!C311</f>
         <v>0</v>
       </c>
@@ -45653,7 +45781,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="11"/>
-      <c r="C48" s="632">
+      <c r="C48" s="633">
         <f>Fluoro!C312</f>
         <v>0</v>
       </c>
@@ -45688,7 +45816,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="11"/>
-      <c r="C49" s="632" t="str">
+      <c r="C49" s="633" t="str">
         <f>Fluoro!C313</f>
         <v>High Level</v>
       </c>
@@ -45723,7 +45851,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="11"/>
-      <c r="C50" s="632">
+      <c r="C50" s="633">
         <f>Fluoro!C314</f>
         <v>0</v>
       </c>
@@ -45758,7 +45886,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="11"/>
-      <c r="C51" s="632">
+      <c r="C51" s="633">
         <f>Fluoro!C315</f>
         <v>0</v>
       </c>
@@ -45789,7 +45917,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="11"/>
-      <c r="C52" s="632">
+      <c r="C52" s="633">
         <f>Fluoro!C316</f>
         <v>0</v>
       </c>
@@ -45820,7 +45948,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="11"/>
-      <c r="C53" s="632">
+      <c r="C53" s="633">
         <f>Fluoro!C317</f>
         <v>0</v>
       </c>
@@ -46006,7 +46134,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="11"/>
-      <c r="C60" s="633" t="str">
+      <c r="C60" s="634" t="str">
         <f>Fluoro!C324</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -46041,7 +46169,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="11"/>
-      <c r="C61" s="633">
+      <c r="C61" s="634">
         <f>Fluoro!C325</f>
         <v>0</v>
       </c>
@@ -46287,39 +46415,39 @@
         <f>Fluoro!D335</f>
         <v>Attenuator</v>
       </c>
-      <c r="E71" s="606" t="str">
+      <c r="E71" s="600" t="str">
         <f>Fluoro!E335</f>
         <v>Auto 1</v>
       </c>
-      <c r="F71" s="606">
+      <c r="F71" s="600">
         <f>Fluoro!F335</f>
         <v>0</v>
       </c>
-      <c r="G71" s="606">
+      <c r="G71" s="600">
         <f>Fluoro!G335</f>
         <v>0</v>
       </c>
-      <c r="H71" s="606" t="str">
+      <c r="H71" s="600" t="str">
         <f>Fluoro!H335</f>
         <v>Auto 2</v>
       </c>
-      <c r="I71" s="606">
+      <c r="I71" s="600">
         <f>Fluoro!I335</f>
         <v>0</v>
       </c>
-      <c r="J71" s="606">
+      <c r="J71" s="600">
         <f>Fluoro!J335</f>
         <v>0</v>
       </c>
-      <c r="K71" s="607" t="str">
+      <c r="K71" s="601" t="str">
         <f>Fluoro!K335</f>
         <v>High Level</v>
       </c>
-      <c r="L71" s="607">
+      <c r="L71" s="601">
         <f>Fluoro!L335</f>
         <v>0</v>
       </c>
-      <c r="M71" s="607">
+      <c r="M71" s="601">
         <f>Fluoro!M335</f>
         <v>0</v>
       </c>
@@ -46376,7 +46504,7 @@
         <v>7</v>
       </c>
       <c r="B73" s="11"/>
-      <c r="C73" s="634" t="str">
+      <c r="C73" s="631" t="str">
         <f>Fluoro!C337</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -46426,7 +46554,7 @@
         <v>8</v>
       </c>
       <c r="B74" s="11"/>
-      <c r="C74" s="634">
+      <c r="C74" s="631">
         <f>Fluoro!C338</f>
         <v>0</v>
       </c>
@@ -46476,7 +46604,7 @@
         <v>9</v>
       </c>
       <c r="B75" s="11"/>
-      <c r="C75" s="634">
+      <c r="C75" s="631">
         <f>Fluoro!C339</f>
         <v>0</v>
       </c>
@@ -46526,7 +46654,7 @@
         <v>10</v>
       </c>
       <c r="B76" s="11"/>
-      <c r="C76" s="634" t="str">
+      <c r="C76" s="631" t="str">
         <f>Fluoro!C340</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -46576,7 +46704,7 @@
         <v>11</v>
       </c>
       <c r="B77" s="11"/>
-      <c r="C77" s="634">
+      <c r="C77" s="631">
         <f>Fluoro!C341</f>
         <v>0</v>
       </c>
@@ -46626,7 +46754,7 @@
         <v>12</v>
       </c>
       <c r="B78" s="11"/>
-      <c r="C78" s="634">
+      <c r="C78" s="631">
         <f>Fluoro!C342</f>
         <v>0</v>
       </c>
@@ -46676,7 +46804,7 @@
         <v>13</v>
       </c>
       <c r="B79" s="11"/>
-      <c r="C79" s="634" t="str">
+      <c r="C79" s="631" t="str">
         <f>Fluoro!C343</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -46726,7 +46854,7 @@
         <v>14</v>
       </c>
       <c r="B80" s="11"/>
-      <c r="C80" s="634">
+      <c r="C80" s="631">
         <f>Fluoro!C344</f>
         <v>0</v>
       </c>
@@ -46776,7 +46904,7 @@
         <v>15</v>
       </c>
       <c r="B81" s="11"/>
-      <c r="C81" s="634">
+      <c r="C81" s="631">
         <f>Fluoro!C345</f>
         <v>0</v>
       </c>
@@ -46826,7 +46954,7 @@
         <v>16</v>
       </c>
       <c r="B82" s="11"/>
-      <c r="C82" s="634" t="str">
+      <c r="C82" s="631" t="str">
         <f>Fluoro!C346</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -46876,7 +47004,7 @@
         <v>17</v>
       </c>
       <c r="B83" s="11"/>
-      <c r="C83" s="634">
+      <c r="C83" s="631">
         <f>Fluoro!C347</f>
         <v>0</v>
       </c>
@@ -46926,7 +47054,7 @@
         <v>18</v>
       </c>
       <c r="B84" s="11"/>
-      <c r="C84" s="634">
+      <c r="C84" s="631">
         <f>Fluoro!C348</f>
         <v>0</v>
       </c>
@@ -46976,7 +47104,7 @@
         <v>19</v>
       </c>
       <c r="B85" s="11"/>
-      <c r="C85" s="634" t="str">
+      <c r="C85" s="631" t="str">
         <f>Fluoro!C349</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -47026,7 +47154,7 @@
         <v>20</v>
       </c>
       <c r="B86" s="11"/>
-      <c r="C86" s="634">
+      <c r="C86" s="631">
         <f>Fluoro!C350</f>
         <v>0</v>
       </c>
@@ -47076,7 +47204,7 @@
         <v>21</v>
       </c>
       <c r="B87" s="11"/>
-      <c r="C87" s="634">
+      <c r="C87" s="631">
         <f>Fluoro!C351</f>
         <v>0</v>
       </c>
@@ -47423,7 +47551,7 @@
         <v>36</v>
       </c>
       <c r="B102" s="11"/>
-      <c r="C102" s="631" t="str">
+      <c r="C102" s="632" t="str">
         <f>Fluoro!C366</f>
         <v>Auto 1</v>
       </c>
@@ -47461,7 +47589,7 @@
         <v>37</v>
       </c>
       <c r="B103" s="11"/>
-      <c r="C103" s="631">
+      <c r="C103" s="632">
         <f>Fluoro!C367</f>
         <v>0</v>
       </c>
@@ -47499,7 +47627,7 @@
         <v>38</v>
       </c>
       <c r="B104" s="11"/>
-      <c r="C104" s="631">
+      <c r="C104" s="632">
         <f>Fluoro!C368</f>
         <v>0</v>
       </c>
@@ -47537,7 +47665,7 @@
         <v>39</v>
       </c>
       <c r="B105" s="11"/>
-      <c r="C105" s="631">
+      <c r="C105" s="632">
         <f>Fluoro!C369</f>
         <v>0</v>
       </c>
@@ -47572,7 +47700,7 @@
         <v>40</v>
       </c>
       <c r="B106" s="11"/>
-      <c r="C106" s="631">
+      <c r="C106" s="632">
         <f>Fluoro!C370</f>
         <v>0</v>
       </c>
@@ -47607,7 +47735,7 @@
         <v>41</v>
       </c>
       <c r="B107" s="11"/>
-      <c r="C107" s="632" t="str">
+      <c r="C107" s="633" t="str">
         <f>Fluoro!C371</f>
         <v>Auto 2</v>
       </c>
@@ -47642,7 +47770,7 @@
         <v>42</v>
       </c>
       <c r="B108" s="11"/>
-      <c r="C108" s="632">
+      <c r="C108" s="633">
         <f>Fluoro!C372</f>
         <v>0</v>
       </c>
@@ -47677,7 +47805,7 @@
         <v>43</v>
       </c>
       <c r="B109" s="11"/>
-      <c r="C109" s="632">
+      <c r="C109" s="633">
         <f>Fluoro!C373</f>
         <v>0</v>
       </c>
@@ -47712,7 +47840,7 @@
         <v>44</v>
       </c>
       <c r="B110" s="11"/>
-      <c r="C110" s="632">
+      <c r="C110" s="633">
         <f>Fluoro!C374</f>
         <v>0</v>
       </c>
@@ -47747,7 +47875,7 @@
         <v>45</v>
       </c>
       <c r="B111" s="11"/>
-      <c r="C111" s="632">
+      <c r="C111" s="633">
         <f>Fluoro!C375</f>
         <v>0</v>
       </c>
@@ -47782,7 +47910,7 @@
         <v>46</v>
       </c>
       <c r="B112" s="11"/>
-      <c r="C112" s="632" t="str">
+      <c r="C112" s="633" t="str">
         <f>Fluoro!C376</f>
         <v>High Level</v>
       </c>
@@ -47817,7 +47945,7 @@
         <v>47</v>
       </c>
       <c r="B113" s="11"/>
-      <c r="C113" s="632">
+      <c r="C113" s="633">
         <f>Fluoro!C377</f>
         <v>0</v>
       </c>
@@ -47852,7 +47980,7 @@
         <v>48</v>
       </c>
       <c r="B114" s="11"/>
-      <c r="C114" s="632">
+      <c r="C114" s="633">
         <f>Fluoro!C378</f>
         <v>0</v>
       </c>
@@ -47883,7 +48011,7 @@
         <v>49</v>
       </c>
       <c r="B115" s="11"/>
-      <c r="C115" s="632">
+      <c r="C115" s="633">
         <f>Fluoro!C379</f>
         <v>0</v>
       </c>
@@ -47914,7 +48042,7 @@
         <v>50</v>
       </c>
       <c r="B116" s="11"/>
-      <c r="C116" s="632">
+      <c r="C116" s="633">
         <f>Fluoro!C380</f>
         <v>0</v>
       </c>
@@ -48088,7 +48216,7 @@
         <v>58</v>
       </c>
       <c r="B124" s="11"/>
-      <c r="C124" s="633" t="str">
+      <c r="C124" s="634" t="str">
         <f>Fluoro!C388</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -48123,7 +48251,7 @@
         <v>59</v>
       </c>
       <c r="B125" s="11"/>
-      <c r="C125" s="633">
+      <c r="C125" s="634">
         <f>Fluoro!C389</f>
         <v>0</v>
       </c>
@@ -48432,21 +48560,6 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="H71:J71"/>
-    <mergeCell ref="K71:M71"/>
     <mergeCell ref="C102:C106"/>
     <mergeCell ref="C107:C111"/>
     <mergeCell ref="C112:C116"/>
@@ -48456,9 +48569,24 @@
     <mergeCell ref="C79:C81"/>
     <mergeCell ref="C82:C84"/>
     <mergeCell ref="C85:C87"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="H71:J71"/>
+    <mergeCell ref="K71:M71"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup scale="68" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup scale="68" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
   </headerFooter>
@@ -48472,8 +48600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK143"/>
   <sheetViews>
-    <sheetView defaultGridColor="0" colorId="9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView topLeftCell="A31" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -48487,29 +48615,29 @@
       </c>
       <c r="B1" s="635"/>
       <c r="N1" s="328"/>
-      <c r="O1" s="600" t="str">
+      <c r="O1" s="606" t="str">
         <f>Fluoro!O105</f>
         <v>Patient Entrance Exposure Rate (Fluoroscopy)*</v>
       </c>
-      <c r="P1" s="600"/>
-      <c r="Q1" s="600"/>
-      <c r="R1" s="600" t="s">
+      <c r="P1" s="606"/>
+      <c r="Q1" s="606"/>
+      <c r="R1" s="606" t="s">
         <v>411</v>
       </c>
-      <c r="S1" s="600"/>
-      <c r="T1" s="600"/>
+      <c r="S1" s="606"/>
+      <c r="T1" s="606"/>
       <c r="V1" s="328"/>
-      <c r="W1" s="600" t="str">
+      <c r="W1" s="606" t="str">
         <f>Fluoro!O137</f>
         <v>Patient Entrance Exposure Rate – Digital Acquisition</v>
       </c>
-      <c r="X1" s="600"/>
-      <c r="Y1" s="600"/>
-      <c r="Z1" s="600" t="s">
+      <c r="X1" s="606"/>
+      <c r="Y1" s="606"/>
+      <c r="Z1" s="606" t="s">
         <v>411</v>
       </c>
-      <c r="AA1" s="600"/>
-      <c r="AB1" s="600"/>
+      <c r="AA1" s="606"/>
+      <c r="AB1" s="606"/>
       <c r="AC1" s="239"/>
     </row>
     <row r="2" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -52552,14 +52680,14 @@
       <c r="B75" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="E75" s="600" t="s">
+      <c r="E75" s="606" t="s">
         <v>424</v>
       </c>
-      <c r="F75" s="600"/>
-      <c r="I75" s="600" t="s">
+      <c r="F75" s="606"/>
+      <c r="I75" s="606" t="s">
         <v>425</v>
       </c>
-      <c r="J75" s="600"/>
+      <c r="J75" s="606"/>
     </row>
     <row r="76" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
@@ -54279,7 +54407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView defaultGridColor="0" colorId="9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -55021,7 +55149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView defaultGridColor="0" colorId="9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Fix units lookup in KAP section
</commit_message>
<xml_diff>
--- a/MUSCCArm.xlsx
+++ b/MUSCCArm.xlsx
@@ -1479,8 +1479,8 @@
     <numFmt numFmtId="169" formatCode="0.0%"/>
     <numFmt numFmtId="170" formatCode="0.000"/>
     <numFmt numFmtId="171" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="[$-409]d/mmm/yyyy;@"/>
-    <numFmt numFmtId="174" formatCode="mmm/yyyy"/>
+    <numFmt numFmtId="172" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="173" formatCode="mmm/yyyy"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -6279,190 +6279,190 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="225" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="172" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="161" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="162" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="163" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="195" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="204" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="205" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="137" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="166" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="192" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="120" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="167" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="194" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="187" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="188" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="113" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="129" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="130" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="126" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="133" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="119" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="110" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="118" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="119" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="110" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="129" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="130" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="126" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="133" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="113" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="120" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="161" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="162" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="187" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="163" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="188" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="137" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="167" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="194" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="195" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="204" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="205" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="166" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="192" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7218,7 +7218,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7445,7 +7444,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7517,7 +7515,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7643,7 +7640,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9316,7 +9312,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9388,7 +9383,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9435,7 +9429,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9503,7 +9496,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9730,7 +9722,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9802,7 +9793,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9928,7 +9918,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11601,7 +11590,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11673,7 +11661,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11720,7 +11707,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11804,7 +11790,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12557,7 +12542,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12781,7 +12765,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13534,7 +13517,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16035,6 +16017,150 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -16496,7 +16622,7 @@
       <c r="O7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="634"/>
+      <c r="P7" s="576"/>
       <c r="Q7" s="26"/>
       <c r="W7" s="1" t="s">
         <v>11</v>
@@ -16531,7 +16657,7 @@
       <c r="O8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P8" s="635" t="str">
+      <c r="P8" s="577" t="str">
         <f>IF(AB8="","",AB8)</f>
         <v/>
       </c>
@@ -16613,21 +16739,21 @@
       <c r="E10" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="576" t="str">
+      <c r="F10" s="629" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="576"/>
+      <c r="G10" s="629"/>
       <c r="H10" s="43"/>
       <c r="I10" s="43"/>
       <c r="J10" s="163" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="577" t="str">
+      <c r="K10" s="622" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="577"/>
+      <c r="L10" s="622"/>
       <c r="M10" s="360"/>
       <c r="O10" s="14"/>
       <c r="Q10" s="2" t="s">
@@ -16670,21 +16796,21 @@
       <c r="E11" s="163" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="578" t="str">
+      <c r="F11" s="623" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="578"/>
+      <c r="G11" s="623"/>
       <c r="H11" s="43"/>
       <c r="I11" s="43"/>
       <c r="J11" s="163" t="s">
         <v>22</v>
       </c>
-      <c r="K11" s="578" t="str">
+      <c r="K11" s="623" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="578"/>
+      <c r="L11" s="623"/>
       <c r="M11" s="360"/>
       <c r="O11" s="14"/>
       <c r="Q11" s="2" t="s">
@@ -16727,21 +16853,21 @@
       <c r="E12" s="163" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="578" t="str">
+      <c r="F12" s="623" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="578"/>
+      <c r="G12" s="623"/>
       <c r="H12" s="43"/>
       <c r="I12" s="43"/>
       <c r="J12" s="163" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="636" t="str">
+      <c r="K12" s="631" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="636"/>
+      <c r="L12" s="631"/>
       <c r="M12" s="360"/>
       <c r="O12" s="14"/>
       <c r="Q12" s="2" t="s">
@@ -16784,21 +16910,21 @@
       <c r="E13" s="163" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="580" t="str">
+      <c r="F13" s="624" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="580"/>
+      <c r="G13" s="624"/>
       <c r="H13" s="43"/>
       <c r="I13" s="43"/>
       <c r="J13" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="580" t="str">
+      <c r="K13" s="624" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="580"/>
+      <c r="L13" s="624"/>
       <c r="M13" s="360"/>
       <c r="O13" s="14"/>
       <c r="Q13" s="2" t="s">
@@ -16921,21 +17047,21 @@
       <c r="E16" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="576" t="str">
+      <c r="F16" s="629" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="576"/>
+      <c r="G16" s="629"/>
       <c r="H16" s="43"/>
       <c r="I16" s="43"/>
       <c r="J16" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="581" t="str">
+      <c r="K16" s="632" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="581"/>
+      <c r="L16" s="632"/>
       <c r="M16" s="360"/>
       <c r="O16" s="14"/>
       <c r="P16" s="51" t="s">
@@ -16965,21 +17091,21 @@
       <c r="E17" s="163" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="578" t="str">
+      <c r="F17" s="623" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="578"/>
+      <c r="G17" s="623"/>
       <c r="H17" s="43"/>
       <c r="I17" s="43"/>
       <c r="J17" s="163" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="580" t="str">
+      <c r="K17" s="624" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="580"/>
+      <c r="L17" s="624"/>
       <c r="M17" s="360"/>
       <c r="O17" s="14"/>
       <c r="Q17" s="2" t="s">
@@ -17022,21 +17148,21 @@
       <c r="E18" s="163" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="580" t="str">
+      <c r="F18" s="624" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="580"/>
+      <c r="G18" s="624"/>
       <c r="H18" s="43"/>
       <c r="I18" s="43"/>
       <c r="J18" s="163" t="s">
         <v>35</v>
       </c>
-      <c r="K18" s="580" t="str">
+      <c r="K18" s="624" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="580"/>
+      <c r="L18" s="624"/>
       <c r="M18" s="360"/>
       <c r="O18" s="14"/>
       <c r="Q18" s="2" t="s">
@@ -17084,11 +17210,11 @@
       <c r="J19" s="163" t="s">
         <v>36</v>
       </c>
-      <c r="K19" s="580" t="str">
+      <c r="K19" s="624" t="str">
         <f>IF(V20="","",V20)</f>
         <v/>
       </c>
-      <c r="L19" s="580"/>
+      <c r="L19" s="624"/>
       <c r="M19" s="360"/>
       <c r="O19" s="14"/>
       <c r="Q19" s="2" t="s">
@@ -17163,11 +17289,11 @@
       <c r="E21" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="576" t="str">
+      <c r="F21" s="629" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="576"/>
+      <c r="G21" s="629"/>
       <c r="H21" s="43"/>
       <c r="I21" s="43"/>
       <c r="J21" s="74" t="s">
@@ -17207,21 +17333,21 @@
       <c r="E22" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="579" t="str">
+      <c r="F22" s="630" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="579"/>
+      <c r="G22" s="630"/>
       <c r="H22" s="43"/>
       <c r="I22" s="43"/>
       <c r="J22" s="163" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="576" t="str">
+      <c r="K22" s="629" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="576"/>
+      <c r="L22" s="629"/>
       <c r="M22" s="360"/>
       <c r="O22" s="14"/>
       <c r="Q22" s="2" t="s">
@@ -17266,11 +17392,11 @@
       <c r="J23" s="163" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="578" t="str">
+      <c r="K23" s="623" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="578"/>
+      <c r="L23" s="623"/>
       <c r="M23" s="360"/>
       <c r="O23" s="14"/>
       <c r="Q23" s="2" t="s">
@@ -17313,21 +17439,21 @@
       <c r="E24" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="577" t="str">
+      <c r="F24" s="622" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="577"/>
+      <c r="G24" s="622"/>
       <c r="H24" s="43"/>
       <c r="I24" s="43"/>
       <c r="J24" s="163" t="s">
         <v>44</v>
       </c>
-      <c r="K24" s="578" t="str">
+      <c r="K24" s="623" t="str">
         <f>IF(V25="","",V25)</f>
         <v/>
       </c>
-      <c r="L24" s="578"/>
+      <c r="L24" s="623"/>
       <c r="M24" s="360"/>
       <c r="O24" s="14"/>
       <c r="P24" s="51" t="s">
@@ -17365,11 +17491,11 @@
       <c r="E25" s="163" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="580" t="str">
+      <c r="F25" s="624" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="580"/>
+      <c r="G25" s="624"/>
       <c r="H25" s="43"/>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -17417,11 +17543,11 @@
       <c r="E26" s="163" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="580" t="str">
+      <c r="F26" s="624" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="580"/>
+      <c r="G26" s="624"/>
       <c r="H26" s="43"/>
       <c r="I26" s="43"/>
       <c r="J26" s="361" t="s">
@@ -17470,11 +17596,11 @@
       <c r="J27" s="163" t="s">
         <v>47</v>
       </c>
-      <c r="K27" s="576" t="str">
+      <c r="K27" s="629" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="576"/>
+      <c r="L27" s="629"/>
       <c r="M27" s="360"/>
       <c r="O27" s="14"/>
       <c r="Q27" s="2" t="s">
@@ -17512,21 +17638,21 @@
       <c r="E28" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F28" s="577" t="str">
+      <c r="F28" s="622" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="577"/>
+      <c r="G28" s="622"/>
       <c r="H28" s="43"/>
       <c r="I28" s="43"/>
       <c r="J28" s="163" t="s">
         <v>48</v>
       </c>
-      <c r="K28" s="578" t="str">
+      <c r="K28" s="623" t="str">
         <f>IF(V29="","",V29)</f>
         <v/>
       </c>
-      <c r="L28" s="578"/>
+      <c r="L28" s="623"/>
       <c r="M28" s="360"/>
       <c r="O28" s="14"/>
       <c r="P28" s="51" t="s">
@@ -17555,11 +17681,11 @@
       <c r="E29" s="163" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="580" t="str">
+      <c r="F29" s="624" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="580"/>
+      <c r="G29" s="624"/>
       <c r="H29" s="43"/>
       <c r="I29" s="43"/>
       <c r="J29" s="43"/>
@@ -17607,11 +17733,11 @@
       <c r="E30" s="163" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="580" t="str">
+      <c r="F30" s="624" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="580"/>
+      <c r="G30" s="624"/>
       <c r="H30" s="43"/>
       <c r="I30" s="43"/>
       <c r="J30" s="43"/>
@@ -17726,11 +17852,11 @@
       <c r="E33" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="576" t="str">
+      <c r="F33" s="629" t="str">
         <f>IF(R34="","",R34)</f>
         <v/>
       </c>
-      <c r="G33" s="576"/>
+      <c r="G33" s="629"/>
       <c r="H33" s="43"/>
       <c r="I33" s="43"/>
       <c r="J33" s="74" t="s">
@@ -17767,21 +17893,21 @@
       <c r="E34" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="579" t="str">
+      <c r="F34" s="630" t="str">
         <f>IF(R35="","",R35)</f>
         <v/>
       </c>
-      <c r="G34" s="579"/>
+      <c r="G34" s="630"/>
       <c r="H34" s="43"/>
       <c r="I34" s="43"/>
       <c r="J34" s="163" t="s">
         <v>41</v>
       </c>
-      <c r="K34" s="576" t="str">
+      <c r="K34" s="629" t="str">
         <f>IF(V35="","",V35)</f>
         <v/>
       </c>
-      <c r="L34" s="576"/>
+      <c r="L34" s="629"/>
       <c r="M34" s="360"/>
       <c r="O34" s="14"/>
       <c r="Q34" s="2" t="s">
@@ -17826,11 +17952,11 @@
       <c r="J35" s="163" t="s">
         <v>43</v>
       </c>
-      <c r="K35" s="578" t="str">
+      <c r="K35" s="623" t="str">
         <f>IF(V36="","",V36)</f>
         <v/>
       </c>
-      <c r="L35" s="578"/>
+      <c r="L35" s="623"/>
       <c r="M35" s="360"/>
       <c r="O35" s="14"/>
       <c r="Q35" s="2" t="s">
@@ -17873,21 +17999,21 @@
       <c r="E36" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F36" s="577" t="str">
+      <c r="F36" s="622" t="str">
         <f>IF(R37="","",R37)</f>
         <v/>
       </c>
-      <c r="G36" s="577"/>
+      <c r="G36" s="622"/>
       <c r="H36" s="43"/>
       <c r="I36" s="43"/>
       <c r="J36" s="163" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="578" t="str">
+      <c r="K36" s="623" t="str">
         <f>IF(V37="","",V37)</f>
         <v/>
       </c>
-      <c r="L36" s="578"/>
+      <c r="L36" s="623"/>
       <c r="M36" s="360"/>
       <c r="O36" s="14"/>
       <c r="P36" s="51" t="s">
@@ -17925,11 +18051,11 @@
       <c r="E37" s="163" t="s">
         <v>32</v>
       </c>
-      <c r="F37" s="580" t="str">
+      <c r="F37" s="624" t="str">
         <f>IF(R38="","",R38)</f>
         <v/>
       </c>
-      <c r="G37" s="580"/>
+      <c r="G37" s="624"/>
       <c r="H37" s="43"/>
       <c r="I37" s="43"/>
       <c r="J37" s="43"/>
@@ -17977,11 +18103,11 @@
       <c r="E38" s="163" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="580" t="str">
+      <c r="F38" s="624" t="str">
         <f>IF(R39="","",R39)</f>
         <v/>
       </c>
-      <c r="G38" s="580"/>
+      <c r="G38" s="624"/>
       <c r="H38" s="43"/>
       <c r="I38" s="43"/>
       <c r="J38" s="361" t="s">
@@ -18028,11 +18154,11 @@
       <c r="J39" s="163" t="s">
         <v>47</v>
       </c>
-      <c r="K39" s="576" t="str">
+      <c r="K39" s="629" t="str">
         <f>IF(V40="","",V40)</f>
         <v/>
       </c>
-      <c r="L39" s="576"/>
+      <c r="L39" s="629"/>
       <c r="M39" s="360"/>
       <c r="O39" s="14"/>
       <c r="Q39" s="2" t="s">
@@ -18070,21 +18196,21 @@
       <c r="E40" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F40" s="577" t="str">
+      <c r="F40" s="622" t="str">
         <f>IF(R41="","",R41)</f>
         <v/>
       </c>
-      <c r="G40" s="577"/>
+      <c r="G40" s="622"/>
       <c r="H40" s="43"/>
       <c r="I40" s="43"/>
       <c r="J40" s="163" t="s">
         <v>48</v>
       </c>
-      <c r="K40" s="578" t="str">
+      <c r="K40" s="623" t="str">
         <f>IF(V41="","",V41)</f>
         <v/>
       </c>
-      <c r="L40" s="578"/>
+      <c r="L40" s="623"/>
       <c r="M40" s="360"/>
       <c r="O40" s="14"/>
       <c r="P40" s="51" t="s">
@@ -18122,11 +18248,11 @@
       <c r="E41" s="163" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="580" t="str">
+      <c r="F41" s="624" t="str">
         <f>IF(R42="","",R42)</f>
         <v/>
       </c>
-      <c r="G41" s="580"/>
+      <c r="G41" s="624"/>
       <c r="H41" s="43"/>
       <c r="I41" s="43"/>
       <c r="J41" s="43"/>
@@ -18174,11 +18300,11 @@
       <c r="E42" s="163" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="580" t="str">
+      <c r="F42" s="624" t="str">
         <f>IF(R43="","",R43)</f>
         <v/>
       </c>
-      <c r="G42" s="580"/>
+      <c r="G42" s="624"/>
       <c r="H42" s="43"/>
       <c r="I42" s="43"/>
       <c r="J42" s="43"/>
@@ -18806,7 +18932,7 @@
       <c r="C65" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D65" s="637" t="str">
+      <c r="D65" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -18936,10 +19062,10 @@
       <c r="I69" s="347"/>
       <c r="J69" s="347"/>
       <c r="K69" s="347"/>
-      <c r="L69" s="582" t="s">
+      <c r="L69" s="625" t="s">
         <v>86</v>
       </c>
-      <c r="M69" s="583"/>
+      <c r="M69" s="626"/>
       <c r="O69" s="57"/>
       <c r="P69" s="18" t="s">
         <v>87</v>
@@ -20571,24 +20697,24 @@
       <c r="P107" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="Q107" s="584" t="str">
+      <c r="Q107" s="627" t="str">
         <f>IF(Q106&lt;&gt;"",Q106,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R107" s="584"/>
-      <c r="S107" s="584"/>
-      <c r="T107" s="585" t="str">
+      <c r="R107" s="627"/>
+      <c r="S107" s="627"/>
+      <c r="T107" s="628" t="str">
         <f>IF(T106&lt;&gt;"",T106,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v>Auto 2</v>
       </c>
-      <c r="U107" s="585"/>
-      <c r="V107" s="585"/>
-      <c r="W107" s="585" t="str">
+      <c r="U107" s="628"/>
+      <c r="V107" s="628"/>
+      <c r="W107" s="628" t="str">
         <f>IF(W106&lt;&gt;"",W106,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v>High Level</v>
       </c>
-      <c r="X107" s="585"/>
-      <c r="Y107" s="585"/>
+      <c r="X107" s="628"/>
+      <c r="Y107" s="628"/>
       <c r="AA107" s="2" t="s">
         <v>113</v>
       </c>
@@ -22181,7 +22307,7 @@
       <c r="C131" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D131" s="637" t="str">
+      <c r="D131" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -22582,24 +22708,24 @@
       <c r="P139" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="Q139" s="584" t="str">
+      <c r="Q139" s="627" t="str">
         <f>IF(Q138&lt;&gt;"",Q138,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R139" s="584"/>
-      <c r="S139" s="584"/>
-      <c r="T139" s="585" t="str">
+      <c r="R139" s="627"/>
+      <c r="S139" s="627"/>
+      <c r="T139" s="628" t="str">
         <f>IF(T138&lt;&gt;"",T138,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v>Auto 2</v>
       </c>
-      <c r="U139" s="585"/>
-      <c r="V139" s="585"/>
-      <c r="W139" s="585" t="str">
+      <c r="U139" s="628"/>
+      <c r="V139" s="628"/>
+      <c r="W139" s="628" t="str">
         <f>IF(W138&lt;&gt;"",W138,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v>High Level</v>
       </c>
-      <c r="X139" s="585"/>
-      <c r="Y139" s="585"/>
+      <c r="X139" s="628"/>
+      <c r="Y139" s="628"/>
       <c r="AA139" s="2" t="str">
         <f>$W$139&amp;" Mag 2"</f>
         <v>High Level Mag 2</v>
@@ -24942,10 +25068,10 @@
       <c r="P181" s="136"/>
       <c r="Q181" s="138"/>
       <c r="R181" s="129"/>
-      <c r="T181" s="586" t="s">
+      <c r="T181" s="604" t="s">
         <v>247</v>
       </c>
-      <c r="U181" s="586"/>
+      <c r="U181" s="604"/>
       <c r="W181" s="2" t="s">
         <v>201</v>
       </c>
@@ -25316,7 +25442,7 @@
       <c r="K190" s="371"/>
       <c r="L190" s="371"/>
       <c r="M190" s="375"/>
-      <c r="O190" s="587" t="str">
+      <c r="O190" s="612" t="str">
         <f>$Q$107</f>
         <v>Auto 1</v>
       </c>
@@ -25366,7 +25492,7 @@
       <c r="K191" s="371"/>
       <c r="L191" s="371"/>
       <c r="M191" s="351"/>
-      <c r="O191" s="587"/>
+      <c r="O191" s="612"/>
       <c r="P191" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -25412,7 +25538,7 @@
       <c r="K192" s="136"/>
       <c r="L192" s="136"/>
       <c r="M192" s="351"/>
-      <c r="O192" s="587"/>
+      <c r="O192" s="612"/>
       <c r="P192" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -25458,7 +25584,7 @@
       <c r="K193" s="136"/>
       <c r="L193" s="136"/>
       <c r="M193" s="351"/>
-      <c r="O193" s="587"/>
+      <c r="O193" s="612"/>
       <c r="P193" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -25501,7 +25627,7 @@
       <c r="K194" s="136"/>
       <c r="L194" s="136"/>
       <c r="M194" s="351"/>
-      <c r="O194" s="587"/>
+      <c r="O194" s="612"/>
       <c r="P194" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -25544,7 +25670,7 @@
       <c r="K195" s="136"/>
       <c r="L195" s="136"/>
       <c r="M195" s="351"/>
-      <c r="O195" s="587" t="str">
+      <c r="O195" s="612" t="str">
         <f>$T$107</f>
         <v>Auto 2</v>
       </c>
@@ -25590,7 +25716,7 @@
       <c r="K196" s="353"/>
       <c r="L196" s="353"/>
       <c r="M196" s="354"/>
-      <c r="O196" s="587"/>
+      <c r="O196" s="612"/>
       <c r="P196" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -25624,7 +25750,7 @@
       <c r="C197" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D197" s="637" t="str">
+      <c r="D197" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -25635,7 +25761,7 @@
         <f>IF($X$7="","",$X$7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="O197" s="587"/>
+      <c r="O197" s="612"/>
       <c r="P197" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -25680,7 +25806,7 @@
         <f>IF($R$13="","",$R$13)</f>
         <v/>
       </c>
-      <c r="O198" s="587"/>
+      <c r="O198" s="612"/>
       <c r="P198" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -25726,7 +25852,7 @@
         <f>$H$2</f>
         <v>Medical University of South Carolina</v>
       </c>
-      <c r="O199" s="587"/>
+      <c r="O199" s="612"/>
       <c r="P199" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -25775,7 +25901,7 @@
         <f>$H$5</f>
         <v>Fluoroscopy System Compliance Inspection</v>
       </c>
-      <c r="O200" s="587" t="str">
+      <c r="O200" s="612" t="str">
         <f>$W$107</f>
         <v>High Level</v>
       </c>
@@ -25824,7 +25950,7 @@
       <c r="K201" s="347"/>
       <c r="L201" s="347"/>
       <c r="M201" s="348"/>
-      <c r="O201" s="587"/>
+      <c r="O201" s="612"/>
       <c r="P201" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -25858,24 +25984,24 @@
       <c r="B202" s="349"/>
       <c r="C202" s="399"/>
       <c r="D202" s="371"/>
-      <c r="E202" s="588" t="s">
+      <c r="E202" s="615" t="s">
         <v>264</v>
       </c>
-      <c r="F202" s="589" t="s">
+      <c r="F202" s="616" t="s">
         <v>265</v>
       </c>
-      <c r="G202" s="590" t="s">
+      <c r="G202" s="617" t="s">
         <v>266</v>
       </c>
-      <c r="H202" s="591" t="str">
+      <c r="H202" s="618" t="str">
         <f>R276</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="I202" s="592" t="str">
+      <c r="I202" s="619" t="str">
         <f>S276</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="J202" s="593" t="s">
+      <c r="J202" s="620" t="s">
         <v>267</v>
       </c>
       <c r="K202" s="136" t="s">
@@ -25884,10 +26010,10 @@
       <c r="L202" s="136" t="s">
         <v>269</v>
       </c>
-      <c r="M202" s="594" t="s">
+      <c r="M202" s="621" t="s">
         <v>270</v>
       </c>
-      <c r="O202" s="587"/>
+      <c r="O202" s="612"/>
       <c r="P202" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -25925,12 +26051,12 @@
       <c r="D203" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="E203" s="588"/>
-      <c r="F203" s="589"/>
-      <c r="G203" s="590"/>
-      <c r="H203" s="591"/>
-      <c r="I203" s="592"/>
-      <c r="J203" s="593"/>
+      <c r="E203" s="615"/>
+      <c r="F203" s="616"/>
+      <c r="G203" s="617"/>
+      <c r="H203" s="618"/>
+      <c r="I203" s="619"/>
+      <c r="J203" s="620"/>
       <c r="K203" s="136" t="str">
         <f>U277</f>
         <v>mGy/min</v>
@@ -25939,8 +26065,8 @@
         <f>V277</f>
         <v>mGy/min</v>
       </c>
-      <c r="M203" s="594"/>
-      <c r="O203" s="587"/>
+      <c r="M203" s="621"/>
+      <c r="O203" s="612"/>
       <c r="P203" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -26016,7 +26142,7 @@
         <f t="shared" si="30"/>
         <v/>
       </c>
-      <c r="O204" s="587"/>
+      <c r="O204" s="612"/>
       <c r="P204" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -26675,7 +26801,7 @@
       <c r="K214" s="371"/>
       <c r="L214" s="371"/>
       <c r="M214" s="351"/>
-      <c r="O214" s="587" t="str">
+      <c r="O214" s="612" t="str">
         <f>$Q$139</f>
         <v>Auto 1</v>
       </c>
@@ -26725,7 +26851,7 @@
       <c r="K215" s="420"/>
       <c r="L215" s="420"/>
       <c r="M215" s="421"/>
-      <c r="O215" s="587"/>
+      <c r="O215" s="612"/>
       <c r="P215" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -26775,7 +26901,7 @@
       <c r="K216" s="371"/>
       <c r="L216" s="371"/>
       <c r="M216" s="351"/>
-      <c r="O216" s="587"/>
+      <c r="O216" s="612"/>
       <c r="P216" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -26821,7 +26947,7 @@
       <c r="K217" s="371"/>
       <c r="L217" s="371"/>
       <c r="M217" s="375"/>
-      <c r="O217" s="587"/>
+      <c r="O217" s="612"/>
       <c r="P217" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -26869,7 +26995,7 @@
       <c r="K218" s="371"/>
       <c r="L218" s="371"/>
       <c r="M218" s="375"/>
-      <c r="O218" s="587"/>
+      <c r="O218" s="612"/>
       <c r="P218" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -26912,7 +27038,7 @@
       <c r="K219" s="371"/>
       <c r="L219" s="371"/>
       <c r="M219" s="375"/>
-      <c r="O219" s="587" t="str">
+      <c r="O219" s="612" t="str">
         <f>$T$139</f>
         <v>Auto 2</v>
       </c>
@@ -26962,7 +27088,7 @@
       <c r="K220" s="371"/>
       <c r="L220" s="371"/>
       <c r="M220" s="375"/>
-      <c r="O220" s="587"/>
+      <c r="O220" s="612"/>
       <c r="P220" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -27015,7 +27141,7 @@
       <c r="K221" s="371"/>
       <c r="L221" s="371"/>
       <c r="M221" s="375"/>
-      <c r="O221" s="587"/>
+      <c r="O221" s="612"/>
       <c r="P221" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -27073,7 +27199,7 @@
       <c r="K222" s="371"/>
       <c r="L222" s="371"/>
       <c r="M222" s="375"/>
-      <c r="O222" s="587"/>
+      <c r="O222" s="612"/>
       <c r="P222" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -27128,7 +27254,7 @@
       <c r="K223" s="371"/>
       <c r="L223" s="371"/>
       <c r="M223" s="375"/>
-      <c r="O223" s="587"/>
+      <c r="O223" s="612"/>
       <c r="P223" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -27183,7 +27309,7 @@
       <c r="K224" s="371"/>
       <c r="L224" s="371"/>
       <c r="M224" s="375"/>
-      <c r="O224" s="587" t="str">
+      <c r="O224" s="612" t="str">
         <f>$W$139</f>
         <v>High Level</v>
       </c>
@@ -27241,7 +27367,7 @@
       <c r="K225" s="371"/>
       <c r="L225" s="371"/>
       <c r="M225" s="375"/>
-      <c r="O225" s="587"/>
+      <c r="O225" s="612"/>
       <c r="P225" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -27292,7 +27418,7 @@
       <c r="K226" s="371"/>
       <c r="L226" s="371"/>
       <c r="M226" s="375"/>
-      <c r="O226" s="587"/>
+      <c r="O226" s="612"/>
       <c r="P226" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -27346,7 +27472,7 @@
       <c r="K227" s="371"/>
       <c r="L227" s="371"/>
       <c r="M227" s="375"/>
-      <c r="O227" s="587"/>
+      <c r="O227" s="612"/>
       <c r="P227" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -27394,7 +27520,7 @@
       <c r="K228" s="371"/>
       <c r="L228" s="371"/>
       <c r="M228" s="375"/>
-      <c r="O228" s="587"/>
+      <c r="O228" s="612"/>
       <c r="P228" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -27920,7 +28046,7 @@
       <c r="K240" s="371"/>
       <c r="L240" s="371"/>
       <c r="M240" s="375"/>
-      <c r="O240" s="595" t="s">
+      <c r="O240" s="613" t="s">
         <v>296</v>
       </c>
       <c r="P240" s="170" t="s">
@@ -27982,7 +28108,7 @@
       <c r="K241" s="371"/>
       <c r="L241" s="371"/>
       <c r="M241" s="375"/>
-      <c r="O241" s="595"/>
+      <c r="O241" s="613"/>
       <c r="P241" s="175" t="s">
         <v>299</v>
       </c>
@@ -28033,7 +28159,7 @@
       <c r="K242" s="371"/>
       <c r="L242" s="371"/>
       <c r="M242" s="375"/>
-      <c r="O242" s="595" t="str">
+      <c r="O242" s="613" t="str">
         <f>IF($U$137=1,"Scatter - Pulse", "Scatter – Digital acq")</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -28093,7 +28219,7 @@
       <c r="K243" s="371"/>
       <c r="L243" s="371"/>
       <c r="M243" s="375"/>
-      <c r="O243" s="595"/>
+      <c r="O243" s="613"/>
       <c r="P243" s="175" t="s">
         <v>299</v>
       </c>
@@ -28619,17 +28745,17 @@
       <c r="P257" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="Q257" s="596" t="s">
+      <c r="Q257" s="614" t="s">
         <v>315</v>
       </c>
-      <c r="R257" s="596"/>
+      <c r="R257" s="614"/>
       <c r="S257" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="T257" s="596" t="s">
+      <c r="T257" s="614" t="s">
         <v>317</v>
       </c>
-      <c r="U257" s="596"/>
+      <c r="U257" s="614"/>
       <c r="V257" s="1" t="s">
         <v>318</v>
       </c>
@@ -28852,7 +28978,7 @@
       <c r="C263" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D263" s="637" t="str">
+      <c r="D263" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -29094,24 +29220,24 @@
         <f t="shared" si="41"/>
         <v>Attenuator</v>
       </c>
-      <c r="E269" s="597" t="str">
+      <c r="E269" s="606" t="str">
         <f>Q107</f>
         <v>Auto 1</v>
       </c>
-      <c r="F269" s="598"/>
-      <c r="G269" s="598"/>
-      <c r="H269" s="598" t="str">
+      <c r="F269" s="607"/>
+      <c r="G269" s="607"/>
+      <c r="H269" s="607" t="str">
         <f>T107</f>
         <v>Auto 2</v>
       </c>
-      <c r="I269" s="598"/>
-      <c r="J269" s="598"/>
-      <c r="K269" s="599" t="str">
+      <c r="I269" s="607"/>
+      <c r="J269" s="607"/>
+      <c r="K269" s="608" t="str">
         <f>W107</f>
         <v>High Level</v>
       </c>
-      <c r="L269" s="599"/>
-      <c r="M269" s="600"/>
+      <c r="L269" s="608"/>
+      <c r="M269" s="609"/>
       <c r="O269" s="194" t="str">
         <f t="shared" si="42"/>
         <v/>
@@ -29213,7 +29339,7 @@
         <v>7</v>
       </c>
       <c r="B271" s="349"/>
-      <c r="C271" s="601" t="str">
+      <c r="C271" s="596" t="str">
         <f>O110&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29282,7 +29408,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="349"/>
-      <c r="C272" s="601"/>
+      <c r="C272" s="596"/>
       <c r="D272" s="447">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -29355,7 +29481,7 @@
         <v>9</v>
       </c>
       <c r="B273" s="349"/>
-      <c r="C273" s="601"/>
+      <c r="C273" s="596"/>
       <c r="D273" s="450">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -29421,7 +29547,7 @@
         <v>10</v>
       </c>
       <c r="B274" s="349"/>
-      <c r="C274" s="601" t="str">
+      <c r="C274" s="596" t="str">
         <f>O113&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29497,7 +29623,7 @@
         <v>11</v>
       </c>
       <c r="B275" s="349"/>
-      <c r="C275" s="601"/>
+      <c r="C275" s="596"/>
       <c r="D275" s="447">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -29563,7 +29689,7 @@
         <v>12</v>
       </c>
       <c r="B276" s="349"/>
-      <c r="C276" s="601"/>
+      <c r="C276" s="596"/>
       <c r="D276" s="450">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -29604,17 +29730,17 @@
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="O276" s="602" t="s">
+      <c r="O276" s="610" t="s">
         <v>264</v>
       </c>
-      <c r="P276" s="603" t="s">
+      <c r="P276" s="611" t="s">
         <v>265</v>
       </c>
-      <c r="R276" s="603" t="str">
+      <c r="R276" s="611" t="str">
         <f>"Ind AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="S276" s="603" t="str">
+      <c r="S276" s="611" t="str">
         <f>"Meas AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -29643,7 +29769,7 @@
         <v>13</v>
       </c>
       <c r="B277" s="349"/>
-      <c r="C277" s="601" t="str">
+      <c r="C277" s="596" t="str">
         <f>O116&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29687,13 +29813,13 @@
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="O277" s="602"/>
-      <c r="P277" s="603"/>
+      <c r="O277" s="610"/>
+      <c r="P277" s="611"/>
       <c r="Q277" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="R277" s="603"/>
-      <c r="S277" s="603"/>
+      <c r="R277" s="611"/>
+      <c r="S277" s="611"/>
       <c r="T277" s="1" t="s">
         <v>324</v>
       </c>
@@ -29728,7 +29854,7 @@
         <v>14</v>
       </c>
       <c r="B278" s="349"/>
-      <c r="C278" s="601"/>
+      <c r="C278" s="596"/>
       <c r="D278" s="447">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -29770,7 +29896,7 @@
         <v>0</v>
       </c>
       <c r="O278" s="192" t="str">
-        <f>IF(S258="","",S258*VLOOKUP($Q$257,Tables!$A$112:$B$115,2))</f>
+        <f>IF(S258="","",S258*VLOOKUP($Q$257,Tables!$A$112:$B$116,2,FALSE))</f>
         <v/>
       </c>
       <c r="P278" s="206" t="str">
@@ -29815,7 +29941,7 @@
         <v>15</v>
       </c>
       <c r="B279" s="349"/>
-      <c r="C279" s="601"/>
+      <c r="C279" s="596"/>
       <c r="D279" s="450">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -29857,7 +29983,7 @@
         <v>0</v>
       </c>
       <c r="O279" s="194" t="str">
-        <f>IF(S259="","",S259*VLOOKUP($Q$257,Tables!$A$112:$B$115,2))</f>
+        <f>IF(S259="","",S259*VLOOKUP($Q$257,Tables!$A$112:$B$116,2,FALSE))</f>
         <v/>
       </c>
       <c r="P279" s="211" t="str">
@@ -29909,7 +30035,7 @@
         <v>16</v>
       </c>
       <c r="B280" s="349"/>
-      <c r="C280" s="601" t="str">
+      <c r="C280" s="596" t="str">
         <f>O119&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29954,7 +30080,7 @@
         <v>0</v>
       </c>
       <c r="O280" s="194" t="str">
-        <f>IF(S260="","",S260*VLOOKUP($Q$257,Tables!$A$112:$B$115,2))</f>
+        <f>IF(S260="","",S260*VLOOKUP($Q$257,Tables!$A$112:$B$116,2,FALSE))</f>
         <v/>
       </c>
       <c r="P280" s="211" t="str">
@@ -29999,7 +30125,7 @@
         <v>17</v>
       </c>
       <c r="B281" s="349"/>
-      <c r="C281" s="601"/>
+      <c r="C281" s="596"/>
       <c r="D281" s="447">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -30041,7 +30167,7 @@
         <v>0</v>
       </c>
       <c r="O281" s="194" t="str">
-        <f>IF(S261="","",S261*VLOOKUP($Q$257,Tables!$A$112:$B$115,2))</f>
+        <f>IF(S261="","",S261*VLOOKUP($Q$257,Tables!$A$112:$B$116,2,FALSE))</f>
         <v/>
       </c>
       <c r="P281" s="211" t="str">
@@ -30093,7 +30219,7 @@
         <v>18</v>
       </c>
       <c r="B282" s="349"/>
-      <c r="C282" s="601"/>
+      <c r="C282" s="596"/>
       <c r="D282" s="450">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -30135,7 +30261,7 @@
         <v>0</v>
       </c>
       <c r="O282" s="194" t="str">
-        <f>IF(S262="","",S262*VLOOKUP($Q$257,Tables!$A$112:$B$115,2))</f>
+        <f>IF(S262="","",S262*VLOOKUP($Q$257,Tables!$A$112:$B$116,2,FALSE))</f>
         <v/>
       </c>
       <c r="P282" s="211" t="str">
@@ -30180,7 +30306,7 @@
         <v>19</v>
       </c>
       <c r="B283" s="349"/>
-      <c r="C283" s="601" t="str">
+      <c r="C283" s="596" t="str">
         <f>O122&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -30225,7 +30351,7 @@
         <v>0</v>
       </c>
       <c r="O283" s="194" t="str">
-        <f>IF(S263="","",S263*VLOOKUP($Q$257,Tables!$A$112:$B$115,2))</f>
+        <f>IF(S263="","",S263*VLOOKUP($Q$257,Tables!$A$112:$B$116,2,FALSE))</f>
         <v/>
       </c>
       <c r="P283" s="211" t="str">
@@ -30277,7 +30403,7 @@
         <v>20</v>
       </c>
       <c r="B284" s="349"/>
-      <c r="C284" s="601"/>
+      <c r="C284" s="596"/>
       <c r="D284" s="447">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -30319,7 +30445,7 @@
         <v>0</v>
       </c>
       <c r="O284" s="194" t="str">
-        <f>IF(S264="","",S264*VLOOKUP($Q$257,Tables!$A$112:$B$115,2))</f>
+        <f>IF(S264="","",S264*VLOOKUP($Q$257,Tables!$A$112:$B$116,2,FALSE))</f>
         <v/>
       </c>
       <c r="P284" s="211" t="str">
@@ -30364,7 +30490,7 @@
         <v>21</v>
       </c>
       <c r="B285" s="349"/>
-      <c r="C285" s="601"/>
+      <c r="C285" s="596"/>
       <c r="D285" s="447">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -30406,7 +30532,7 @@
         <v>0</v>
       </c>
       <c r="O285" s="203" t="str">
-        <f>IF(S265="","",S265*VLOOKUP($Q$257,Tables!$A$112:$B$115,2))</f>
+        <f>IF(S265="","",S265*VLOOKUP($Q$257,Tables!$A$112:$B$116,2,FALSE))</f>
         <v/>
       </c>
       <c r="P285" s="217" t="str">
@@ -30795,12 +30921,12 @@
       <c r="L293" s="136"/>
       <c r="M293" s="351"/>
       <c r="O293" s="239"/>
-      <c r="P293" s="604" t="s">
+      <c r="P293" s="601" t="s">
         <v>330</v>
       </c>
-      <c r="Q293" s="604"/>
-      <c r="R293" s="604"/>
-      <c r="S293" s="604"/>
+      <c r="Q293" s="601"/>
+      <c r="R293" s="601"/>
+      <c r="S293" s="601"/>
       <c r="T293" s="237"/>
       <c r="U293" s="237"/>
       <c r="V293" s="237"/>
@@ -31184,12 +31310,12 @@
       <c r="L302" s="136"/>
       <c r="M302" s="351"/>
       <c r="O302" s="239"/>
-      <c r="P302" s="604" t="s">
+      <c r="P302" s="601" t="s">
         <v>330</v>
       </c>
-      <c r="Q302" s="604"/>
-      <c r="R302" s="604"/>
-      <c r="S302" s="604"/>
+      <c r="Q302" s="601"/>
+      <c r="R302" s="601"/>
+      <c r="S302" s="601"/>
       <c r="T302" s="237"/>
       <c r="U302" s="237"/>
       <c r="V302" s="237"/>
@@ -31204,7 +31330,7 @@
         <v>39</v>
       </c>
       <c r="B303" s="349"/>
-      <c r="C303" s="605" t="str">
+      <c r="C303" s="579" t="str">
         <f>O190</f>
         <v>Auto 1</v>
       </c>
@@ -31272,7 +31398,7 @@
         <v>40</v>
       </c>
       <c r="B304" s="349"/>
-      <c r="C304" s="606"/>
+      <c r="C304" s="580"/>
       <c r="D304" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31335,7 +31461,7 @@
         <v>41</v>
       </c>
       <c r="B305" s="349"/>
-      <c r="C305" s="606"/>
+      <c r="C305" s="580"/>
       <c r="D305" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31390,7 +31516,7 @@
         <v>42</v>
       </c>
       <c r="B306" s="349"/>
-      <c r="C306" s="606"/>
+      <c r="C306" s="580"/>
       <c r="D306" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31435,7 +31561,7 @@
         <v>43</v>
       </c>
       <c r="B307" s="349"/>
-      <c r="C307" s="607"/>
+      <c r="C307" s="602"/>
       <c r="D307" s="492" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31487,7 +31613,7 @@
         <v>44</v>
       </c>
       <c r="B308" s="349"/>
-      <c r="C308" s="605" t="str">
+      <c r="C308" s="579" t="str">
         <f>O195</f>
         <v>Auto 2</v>
       </c>
@@ -31535,7 +31661,7 @@
         <v>45</v>
       </c>
       <c r="B309" s="349"/>
-      <c r="C309" s="606"/>
+      <c r="C309" s="580"/>
       <c r="D309" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31592,7 +31718,7 @@
         <v>46</v>
       </c>
       <c r="B310" s="349"/>
-      <c r="C310" s="606"/>
+      <c r="C310" s="580"/>
       <c r="D310" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31642,7 +31768,7 @@
         <v>47</v>
       </c>
       <c r="B311" s="349"/>
-      <c r="C311" s="606"/>
+      <c r="C311" s="580"/>
       <c r="D311" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31699,7 +31825,7 @@
         <v>48</v>
       </c>
       <c r="B312" s="349"/>
-      <c r="C312" s="608"/>
+      <c r="C312" s="581"/>
       <c r="D312" s="495" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31749,7 +31875,7 @@
         <v>49</v>
       </c>
       <c r="B313" s="349"/>
-      <c r="C313" s="609" t="str">
+      <c r="C313" s="603" t="str">
         <f>O200</f>
         <v>High Level</v>
       </c>
@@ -31808,7 +31934,7 @@
         <v>50</v>
       </c>
       <c r="B314" s="349"/>
-      <c r="C314" s="606"/>
+      <c r="C314" s="580"/>
       <c r="D314" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31851,7 +31977,7 @@
         <v>51</v>
       </c>
       <c r="B315" s="349"/>
-      <c r="C315" s="606"/>
+      <c r="C315" s="580"/>
       <c r="D315" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31894,7 +32020,7 @@
         <v>52</v>
       </c>
       <c r="B316" s="349"/>
-      <c r="C316" s="606"/>
+      <c r="C316" s="580"/>
       <c r="D316" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31939,7 +32065,7 @@
         <v>53</v>
       </c>
       <c r="B317" s="349"/>
-      <c r="C317" s="608"/>
+      <c r="C317" s="581"/>
       <c r="D317" s="495" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -32049,10 +32175,10 @@
       <c r="R319" s="278"/>
       <c r="S319" s="279"/>
       <c r="T319" s="279"/>
-      <c r="V319" s="586" t="s">
+      <c r="V319" s="604" t="s">
         <v>342</v>
       </c>
-      <c r="W319" s="586"/>
+      <c r="W319" s="604"/>
       <c r="X319" s="18" t="s">
         <v>343</v>
       </c>
@@ -32253,7 +32379,7 @@
         <v>60</v>
       </c>
       <c r="B324" s="349"/>
-      <c r="C324" s="610" t="str">
+      <c r="C324" s="585" t="str">
         <f>O240</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -32303,7 +32429,7 @@
         <v>61</v>
       </c>
       <c r="B325" s="349"/>
-      <c r="C325" s="611"/>
+      <c r="C325" s="586"/>
       <c r="D325" s="504" t="str">
         <f>P241</f>
         <v>Waist level</v>
@@ -32446,7 +32572,7 @@
       <c r="C329" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D329" s="637" t="str">
+      <c r="D329" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -32461,13 +32587,13 @@
         <v>350</v>
       </c>
       <c r="P329" s="54"/>
-      <c r="Q329" s="612" t="s">
+      <c r="Q329" s="605" t="s">
         <v>351</v>
       </c>
-      <c r="R329" s="612"/>
-      <c r="S329" s="612"/>
-      <c r="T329" s="612"/>
-      <c r="U329" s="612"/>
+      <c r="R329" s="605"/>
+      <c r="S329" s="605"/>
+      <c r="T329" s="605"/>
+      <c r="U329" s="605"/>
       <c r="Y329" s="15"/>
     </row>
     <row r="330" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32632,24 +32758,24 @@
         <f t="shared" si="69"/>
         <v>Attenuator</v>
       </c>
-      <c r="E335" s="597" t="str">
+      <c r="E335" s="606" t="str">
         <f>Q139</f>
         <v>Auto 1</v>
       </c>
-      <c r="F335" s="598"/>
-      <c r="G335" s="598"/>
-      <c r="H335" s="598" t="str">
+      <c r="F335" s="607"/>
+      <c r="G335" s="607"/>
+      <c r="H335" s="607" t="str">
         <f>T139</f>
         <v>Auto 2</v>
       </c>
-      <c r="I335" s="598"/>
-      <c r="J335" s="598"/>
-      <c r="K335" s="599" t="str">
+      <c r="I335" s="607"/>
+      <c r="J335" s="607"/>
+      <c r="K335" s="608" t="str">
         <f>W139</f>
         <v>High Level</v>
       </c>
-      <c r="L335" s="599"/>
-      <c r="M335" s="600"/>
+      <c r="L335" s="608"/>
+      <c r="M335" s="609"/>
       <c r="O335" s="131"/>
       <c r="P335" s="130" t="s">
         <v>357</v>
@@ -32726,7 +32852,7 @@
         <v>7</v>
       </c>
       <c r="B337" s="349"/>
-      <c r="C337" s="601" t="str">
+      <c r="C337" s="596" t="str">
         <f>O142&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -32786,7 +32912,7 @@
         <v>8</v>
       </c>
       <c r="B338" s="349"/>
-      <c r="C338" s="601"/>
+      <c r="C338" s="596"/>
       <c r="D338" s="518">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -32843,7 +32969,7 @@
         <v>9</v>
       </c>
       <c r="B339" s="349"/>
-      <c r="C339" s="601"/>
+      <c r="C339" s="596"/>
       <c r="D339" s="519">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -32900,7 +33026,7 @@
         <v>10</v>
       </c>
       <c r="B340" s="349"/>
-      <c r="C340" s="601" t="str">
+      <c r="C340" s="596" t="str">
         <f>O145&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -32960,7 +33086,7 @@
         <v>11</v>
       </c>
       <c r="B341" s="349"/>
-      <c r="C341" s="601"/>
+      <c r="C341" s="596"/>
       <c r="D341" s="518">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33017,7 +33143,7 @@
         <v>12</v>
       </c>
       <c r="B342" s="349"/>
-      <c r="C342" s="601"/>
+      <c r="C342" s="596"/>
       <c r="D342" s="520">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -33074,7 +33200,7 @@
         <v>13</v>
       </c>
       <c r="B343" s="349"/>
-      <c r="C343" s="601" t="str">
+      <c r="C343" s="596" t="str">
         <f>O148&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33126,7 +33252,7 @@
         <v>14</v>
       </c>
       <c r="B344" s="349"/>
-      <c r="C344" s="601"/>
+      <c r="C344" s="596"/>
       <c r="D344" s="518">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33188,7 +33314,7 @@
         <v>15</v>
       </c>
       <c r="B345" s="349"/>
-      <c r="C345" s="601"/>
+      <c r="C345" s="596"/>
       <c r="D345" s="519">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -33251,7 +33377,7 @@
         <v>16</v>
       </c>
       <c r="B346" s="349"/>
-      <c r="C346" s="601" t="str">
+      <c r="C346" s="596" t="str">
         <f>O151&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33314,7 +33440,7 @@
         <v>17</v>
       </c>
       <c r="B347" s="349"/>
-      <c r="C347" s="601"/>
+      <c r="C347" s="596"/>
       <c r="D347" s="518">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33372,7 +33498,7 @@
         <v>18</v>
       </c>
       <c r="B348" s="349"/>
-      <c r="C348" s="601"/>
+      <c r="C348" s="596"/>
       <c r="D348" s="520">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -33450,7 +33576,7 @@
         <v>19</v>
       </c>
       <c r="B349" s="349"/>
-      <c r="C349" s="601" t="str">
+      <c r="C349" s="596" t="str">
         <f>O154&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33513,7 +33639,7 @@
         <v>20</v>
       </c>
       <c r="B350" s="349"/>
-      <c r="C350" s="601"/>
+      <c r="C350" s="596"/>
       <c r="D350" s="518">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33572,7 +33698,7 @@
         <v>21</v>
       </c>
       <c r="B351" s="349"/>
-      <c r="C351" s="601"/>
+      <c r="C351" s="596"/>
       <c r="D351" s="520">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -33881,11 +34007,11 @@
         <f>IF(OR(V358="",V359="",V362=""),"",(V358-V359)*V362)</f>
         <v/>
       </c>
-      <c r="Q358" s="613" t="str">
+      <c r="Q358" s="597" t="str">
         <f>IF(OR(P358="",P359=""),"",(ABS(P358)+ABS(P359))/$O$355)</f>
         <v/>
       </c>
-      <c r="R358" s="614" t="str">
+      <c r="R358" s="598" t="str">
         <f>IF(OR(Q358="",Q360=""),"",Q358+Q360)</f>
         <v/>
       </c>
@@ -33924,8 +34050,8 @@
         <f>IF(OR(W358="",W359="",V362=""),"",(W358-W359)*V362)</f>
         <v/>
       </c>
-      <c r="Q359" s="613"/>
-      <c r="R359" s="613"/>
+      <c r="Q359" s="597"/>
+      <c r="R359" s="597"/>
       <c r="S359" s="147" t="str">
         <f>IF(AB168="","",AB168)</f>
         <v/>
@@ -33961,11 +34087,11 @@
         <f>IF(OR(X358="",X359="",V362=""),"",(X358-X359)*V362)</f>
         <v/>
       </c>
-      <c r="Q360" s="614" t="str">
+      <c r="Q360" s="598" t="str">
         <f>IF(OR(P360="",P361=""),"",(ABS(P360)+ABS(P361))/$O$355)</f>
         <v/>
       </c>
-      <c r="R360" s="614"/>
+      <c r="R360" s="598"/>
       <c r="S360" s="147" t="str">
         <f>IF(AB169="","",AB169)</f>
         <v/>
@@ -34007,8 +34133,8 @@
         <f>IF(OR(Y358="",Y359="",V362=""),"",(Y358-Y359)*V362)</f>
         <v/>
       </c>
-      <c r="Q361" s="614"/>
-      <c r="R361" s="614"/>
+      <c r="Q361" s="598"/>
+      <c r="R361" s="598"/>
       <c r="S361" s="149" t="str">
         <f>IF(AB170="","",AB170)</f>
         <v/>
@@ -34180,7 +34306,7 @@
         <v>36</v>
       </c>
       <c r="B366" s="349"/>
-      <c r="C366" s="615" t="str">
+      <c r="C366" s="599" t="str">
         <f>O214</f>
         <v>Auto 1</v>
       </c>
@@ -34231,7 +34357,7 @@
         <v>37</v>
       </c>
       <c r="B367" s="349"/>
-      <c r="C367" s="616"/>
+      <c r="C367" s="600"/>
       <c r="D367" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34277,7 +34403,7 @@
         <v>38</v>
       </c>
       <c r="B368" s="349"/>
-      <c r="C368" s="616"/>
+      <c r="C368" s="600"/>
       <c r="D368" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34312,7 +34438,7 @@
         <v>39</v>
       </c>
       <c r="B369" s="349"/>
-      <c r="C369" s="616"/>
+      <c r="C369" s="600"/>
       <c r="D369" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34347,7 +34473,7 @@
         <v>40</v>
       </c>
       <c r="B370" s="349"/>
-      <c r="C370" s="616"/>
+      <c r="C370" s="600"/>
       <c r="D370" s="495" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34392,7 +34518,7 @@
         <v>41</v>
       </c>
       <c r="B371" s="349"/>
-      <c r="C371" s="605" t="str">
+      <c r="C371" s="579" t="str">
         <f>O219</f>
         <v>Auto 2</v>
       </c>
@@ -34442,7 +34568,7 @@
         <v>42</v>
       </c>
       <c r="B372" s="349"/>
-      <c r="C372" s="606"/>
+      <c r="C372" s="580"/>
       <c r="D372" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34492,7 +34618,7 @@
         <v>43</v>
       </c>
       <c r="B373" s="349"/>
-      <c r="C373" s="606"/>
+      <c r="C373" s="580"/>
       <c r="D373" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34539,7 +34665,7 @@
         <v>44</v>
       </c>
       <c r="B374" s="349"/>
-      <c r="C374" s="606"/>
+      <c r="C374" s="580"/>
       <c r="D374" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34589,7 +34715,7 @@
         <v>45</v>
       </c>
       <c r="B375" s="349"/>
-      <c r="C375" s="608"/>
+      <c r="C375" s="581"/>
       <c r="D375" s="495" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34636,7 +34762,7 @@
         <v>46</v>
       </c>
       <c r="B376" s="349"/>
-      <c r="C376" s="617" t="str">
+      <c r="C376" s="582" t="str">
         <f>O224</f>
         <v>High Level</v>
       </c>
@@ -34689,7 +34815,7 @@
         <v>47</v>
       </c>
       <c r="B377" s="349"/>
-      <c r="C377" s="618"/>
+      <c r="C377" s="583"/>
       <c r="D377" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34736,7 +34862,7 @@
         <v>48</v>
       </c>
       <c r="B378" s="349"/>
-      <c r="C378" s="618"/>
+      <c r="C378" s="583"/>
       <c r="D378" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34786,7 +34912,7 @@
         <v>49</v>
       </c>
       <c r="B379" s="349"/>
-      <c r="C379" s="618"/>
+      <c r="C379" s="583"/>
       <c r="D379" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34833,7 +34959,7 @@
         <v>50</v>
       </c>
       <c r="B380" s="349"/>
-      <c r="C380" s="619"/>
+      <c r="C380" s="584"/>
       <c r="D380" s="495" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -35143,7 +35269,7 @@
         <v>58</v>
       </c>
       <c r="B388" s="349"/>
-      <c r="C388" s="610" t="str">
+      <c r="C388" s="585" t="str">
         <f>O242</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -35194,7 +35320,7 @@
         <v>59</v>
       </c>
       <c r="B389" s="349"/>
-      <c r="C389" s="611"/>
+      <c r="C389" s="586"/>
       <c r="D389" s="504" t="str">
         <f>P243</f>
         <v>Waist level</v>
@@ -35418,7 +35544,7 @@
       <c r="C395" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D395" s="637" t="str">
+      <c r="D395" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -35545,14 +35671,14 @@
       <c r="E399" s="347"/>
       <c r="F399" s="347"/>
       <c r="G399" s="347"/>
-      <c r="H399" s="620" t="s">
+      <c r="H399" s="587" t="s">
         <v>397</v>
       </c>
-      <c r="I399" s="620"/>
-      <c r="J399" s="620" t="s">
+      <c r="I399" s="587"/>
+      <c r="J399" s="587" t="s">
         <v>398</v>
       </c>
-      <c r="K399" s="620"/>
+      <c r="K399" s="587"/>
       <c r="L399" s="347"/>
       <c r="M399" s="348"/>
       <c r="O399" s="14"/>
@@ -36126,20 +36252,20 @@
       </c>
       <c r="B413" s="349"/>
       <c r="C413" s="43"/>
-      <c r="D413" s="621" t="s">
+      <c r="D413" s="588" t="s">
         <v>404</v>
       </c>
-      <c r="E413" s="621"/>
-      <c r="F413" s="621"/>
-      <c r="G413" s="621"/>
-      <c r="H413" s="621"/>
-      <c r="I413" s="621" t="s">
+      <c r="E413" s="588"/>
+      <c r="F413" s="588"/>
+      <c r="G413" s="588"/>
+      <c r="H413" s="588"/>
+      <c r="I413" s="588" t="s">
         <v>405</v>
       </c>
-      <c r="J413" s="621"/>
-      <c r="K413" s="621"/>
-      <c r="L413" s="621"/>
-      <c r="M413" s="622"/>
+      <c r="J413" s="588"/>
+      <c r="K413" s="588"/>
+      <c r="L413" s="588"/>
+      <c r="M413" s="589"/>
       <c r="O413" s="14"/>
       <c r="P413" s="2" t="s">
         <v>191</v>
@@ -37619,11 +37745,11 @@
         <f t="shared" si="92"/>
         <v/>
       </c>
-      <c r="F442" s="623" t="str">
+      <c r="F442" s="590" t="str">
         <f t="shared" si="92"/>
         <v/>
       </c>
-      <c r="G442" s="625" t="str">
+      <c r="G442" s="592" t="str">
         <f t="shared" si="92"/>
         <v/>
       </c>
@@ -37664,8 +37790,8 @@
         <f>P359</f>
         <v/>
       </c>
-      <c r="F443" s="624"/>
-      <c r="G443" s="626"/>
+      <c r="F443" s="591"/>
+      <c r="G443" s="593"/>
       <c r="H443" s="205"/>
       <c r="I443" s="83" t="str">
         <f>T360</f>
@@ -37705,11 +37831,11 @@
         <f>P360</f>
         <v/>
       </c>
-      <c r="F444" s="624" t="str">
+      <c r="F444" s="591" t="str">
         <f>Q360</f>
         <v/>
       </c>
-      <c r="G444" s="626"/>
+      <c r="G444" s="593"/>
       <c r="H444" s="136"/>
       <c r="I444" s="92" t="str">
         <f>T361</f>
@@ -37750,8 +37876,8 @@
         <f>P361</f>
         <v/>
       </c>
-      <c r="F445" s="628"/>
-      <c r="G445" s="627"/>
+      <c r="F445" s="595"/>
+      <c r="G445" s="594"/>
       <c r="H445" s="136"/>
       <c r="I445" s="136"/>
       <c r="J445" s="136"/>
@@ -38146,7 +38272,7 @@
       <c r="C461" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D461" s="637" t="str">
+      <c r="D461" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -39430,7 +39556,7 @@
       <c r="C527" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D527" s="637" t="str">
+      <c r="D527" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -40714,7 +40840,7 @@
       <c r="C593" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D593" s="637" t="str">
+      <c r="D593" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -41827,7 +41953,7 @@
       <c r="C659" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D659" s="637" t="str">
+      <c r="D659" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -42941,7 +43067,7 @@
       <c r="C725" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D725" s="637" t="str">
+      <c r="D725" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -44054,7 +44180,7 @@
       <c r="C791" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D791" s="637" t="str">
+      <c r="D791" s="578" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -44087,25 +44213,84 @@
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="C371:C375"/>
-    <mergeCell ref="C376:C380"/>
-    <mergeCell ref="C388:C389"/>
-    <mergeCell ref="H399:I399"/>
-    <mergeCell ref="J399:K399"/>
-    <mergeCell ref="D413:H413"/>
-    <mergeCell ref="I413:M413"/>
-    <mergeCell ref="F442:F443"/>
-    <mergeCell ref="G442:G445"/>
-    <mergeCell ref="F444:F445"/>
-    <mergeCell ref="C337:C339"/>
-    <mergeCell ref="C340:C342"/>
-    <mergeCell ref="C343:C345"/>
-    <mergeCell ref="C346:C348"/>
-    <mergeCell ref="C349:C351"/>
-    <mergeCell ref="Q358:Q359"/>
-    <mergeCell ref="R358:R361"/>
-    <mergeCell ref="Q360:Q361"/>
-    <mergeCell ref="C366:C370"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="Q107:S107"/>
+    <mergeCell ref="T107:V107"/>
+    <mergeCell ref="W107:Y107"/>
+    <mergeCell ref="Q139:S139"/>
+    <mergeCell ref="T139:V139"/>
+    <mergeCell ref="W139:Y139"/>
+    <mergeCell ref="T181:U181"/>
+    <mergeCell ref="O190:O194"/>
+    <mergeCell ref="O195:O199"/>
+    <mergeCell ref="O200:O204"/>
+    <mergeCell ref="E202:E203"/>
+    <mergeCell ref="F202:F203"/>
+    <mergeCell ref="G202:G203"/>
+    <mergeCell ref="H202:H203"/>
+    <mergeCell ref="I202:I203"/>
+    <mergeCell ref="J202:J203"/>
+    <mergeCell ref="M202:M203"/>
+    <mergeCell ref="O214:O218"/>
+    <mergeCell ref="O219:O223"/>
+    <mergeCell ref="O224:O228"/>
+    <mergeCell ref="O240:O241"/>
+    <mergeCell ref="O242:O243"/>
+    <mergeCell ref="Q257:R257"/>
+    <mergeCell ref="T257:U257"/>
+    <mergeCell ref="E269:G269"/>
+    <mergeCell ref="H269:J269"/>
+    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="C271:C273"/>
+    <mergeCell ref="C274:C276"/>
+    <mergeCell ref="O276:O277"/>
+    <mergeCell ref="P276:P277"/>
+    <mergeCell ref="R276:R277"/>
+    <mergeCell ref="S276:S277"/>
+    <mergeCell ref="C277:C279"/>
+    <mergeCell ref="C280:C282"/>
+    <mergeCell ref="C283:C285"/>
     <mergeCell ref="P293:S293"/>
     <mergeCell ref="P302:S302"/>
     <mergeCell ref="C303:C307"/>
@@ -44117,84 +44302,25 @@
     <mergeCell ref="E335:G335"/>
     <mergeCell ref="H335:J335"/>
     <mergeCell ref="K335:M335"/>
-    <mergeCell ref="C271:C273"/>
-    <mergeCell ref="C274:C276"/>
-    <mergeCell ref="O276:O277"/>
-    <mergeCell ref="P276:P277"/>
-    <mergeCell ref="R276:R277"/>
-    <mergeCell ref="S276:S277"/>
-    <mergeCell ref="C277:C279"/>
-    <mergeCell ref="C280:C282"/>
-    <mergeCell ref="C283:C285"/>
-    <mergeCell ref="O214:O218"/>
-    <mergeCell ref="O219:O223"/>
-    <mergeCell ref="O224:O228"/>
-    <mergeCell ref="O240:O241"/>
-    <mergeCell ref="O242:O243"/>
-    <mergeCell ref="Q257:R257"/>
-    <mergeCell ref="T257:U257"/>
-    <mergeCell ref="E269:G269"/>
-    <mergeCell ref="H269:J269"/>
-    <mergeCell ref="K269:M269"/>
-    <mergeCell ref="T181:U181"/>
-    <mergeCell ref="O190:O194"/>
-    <mergeCell ref="O195:O199"/>
-    <mergeCell ref="O200:O204"/>
-    <mergeCell ref="E202:E203"/>
-    <mergeCell ref="F202:F203"/>
-    <mergeCell ref="G202:G203"/>
-    <mergeCell ref="H202:H203"/>
-    <mergeCell ref="I202:I203"/>
-    <mergeCell ref="J202:J203"/>
-    <mergeCell ref="M202:M203"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="Q107:S107"/>
-    <mergeCell ref="T107:V107"/>
-    <mergeCell ref="W107:Y107"/>
-    <mergeCell ref="Q139:S139"/>
-    <mergeCell ref="T139:V139"/>
-    <mergeCell ref="W139:Y139"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C337:C339"/>
+    <mergeCell ref="C340:C342"/>
+    <mergeCell ref="C343:C345"/>
+    <mergeCell ref="C346:C348"/>
+    <mergeCell ref="C349:C351"/>
+    <mergeCell ref="Q358:Q359"/>
+    <mergeCell ref="R358:R361"/>
+    <mergeCell ref="Q360:Q361"/>
+    <mergeCell ref="C366:C370"/>
+    <mergeCell ref="C371:C375"/>
+    <mergeCell ref="C376:C380"/>
+    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="H399:I399"/>
+    <mergeCell ref="J399:K399"/>
+    <mergeCell ref="D413:H413"/>
+    <mergeCell ref="I413:M413"/>
+    <mergeCell ref="F442:F443"/>
+    <mergeCell ref="G442:G445"/>
+    <mergeCell ref="F444:F445"/>
   </mergeCells>
   <conditionalFormatting sqref="S126 V126 Y126 S158 V158 Y158">
     <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
@@ -44459,39 +44585,39 @@
         <f>Fluoro!D269</f>
         <v>Attenuator</v>
       </c>
-      <c r="E5" s="598" t="str">
+      <c r="E5" s="607" t="str">
         <f>Fluoro!E269</f>
         <v>Auto 1</v>
       </c>
-      <c r="F5" s="598">
+      <c r="F5" s="607">
         <f>Fluoro!F269</f>
         <v>0</v>
       </c>
-      <c r="G5" s="598">
+      <c r="G5" s="607">
         <f>Fluoro!G269</f>
         <v>0</v>
       </c>
-      <c r="H5" s="598" t="str">
+      <c r="H5" s="607" t="str">
         <f>Fluoro!H269</f>
         <v>Auto 2</v>
       </c>
-      <c r="I5" s="598">
+      <c r="I5" s="607">
         <f>Fluoro!I269</f>
         <v>0</v>
       </c>
-      <c r="J5" s="598">
+      <c r="J5" s="607">
         <f>Fluoro!J269</f>
         <v>0</v>
       </c>
-      <c r="K5" s="599" t="str">
+      <c r="K5" s="608" t="str">
         <f>Fluoro!K269</f>
         <v>High Level</v>
       </c>
-      <c r="L5" s="599">
+      <c r="L5" s="608">
         <f>Fluoro!L269</f>
         <v>0</v>
       </c>
-      <c r="M5" s="599">
+      <c r="M5" s="608">
         <f>Fluoro!M269</f>
         <v>0</v>
       </c>
@@ -44548,7 +44674,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="629" t="str">
+      <c r="C7" s="636" t="str">
         <f>Fluoro!C271</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -44598,7 +44724,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="629">
+      <c r="C8" s="636">
         <f>Fluoro!C272</f>
         <v>0</v>
       </c>
@@ -44648,7 +44774,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="629">
+      <c r="C9" s="636">
         <f>Fluoro!C273</f>
         <v>0</v>
       </c>
@@ -44698,7 +44824,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="629" t="str">
+      <c r="C10" s="636" t="str">
         <f>Fluoro!C274</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -44748,7 +44874,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="629">
+      <c r="C11" s="636">
         <f>Fluoro!C275</f>
         <v>0</v>
       </c>
@@ -44798,7 +44924,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="629">
+      <c r="C12" s="636">
         <f>Fluoro!C276</f>
         <v>0</v>
       </c>
@@ -44848,7 +44974,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="629" t="str">
+      <c r="C13" s="636" t="str">
         <f>Fluoro!C277</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -44898,7 +45024,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="629">
+      <c r="C14" s="636">
         <f>Fluoro!C278</f>
         <v>0</v>
       </c>
@@ -44948,7 +45074,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="629">
+      <c r="C15" s="636">
         <f>Fluoro!C279</f>
         <v>0</v>
       </c>
@@ -44998,7 +45124,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="629" t="str">
+      <c r="C16" s="636" t="str">
         <f>Fluoro!C280</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -45048,7 +45174,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="629">
+      <c r="C17" s="636">
         <f>Fluoro!C281</f>
         <v>0</v>
       </c>
@@ -45098,7 +45224,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="11"/>
-      <c r="C18" s="629">
+      <c r="C18" s="636">
         <f>Fluoro!C282</f>
         <v>0</v>
       </c>
@@ -45148,7 +45274,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="11"/>
-      <c r="C19" s="629" t="str">
+      <c r="C19" s="636" t="str">
         <f>Fluoro!C283</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -45198,7 +45324,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="629">
+      <c r="C20" s="636">
         <f>Fluoro!C284</f>
         <v>0</v>
       </c>
@@ -45248,7 +45374,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="629">
+      <c r="C21" s="636">
         <f>Fluoro!C285</f>
         <v>0</v>
       </c>
@@ -45697,7 +45823,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="630" t="str">
+      <c r="C39" s="633" t="str">
         <f>Fluoro!C303</f>
         <v>Auto 1</v>
       </c>
@@ -45735,7 +45861,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="11"/>
-      <c r="C40" s="630">
+      <c r="C40" s="633">
         <f>Fluoro!C304</f>
         <v>0</v>
       </c>
@@ -45773,7 +45899,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="11"/>
-      <c r="C41" s="630">
+      <c r="C41" s="633">
         <f>Fluoro!C305</f>
         <v>0</v>
       </c>
@@ -45811,7 +45937,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="630">
+      <c r="C42" s="633">
         <f>Fluoro!C306</f>
         <v>0</v>
       </c>
@@ -45846,7 +45972,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="630">
+      <c r="C43" s="633">
         <f>Fluoro!C307</f>
         <v>0</v>
       </c>
@@ -45881,7 +46007,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="11"/>
-      <c r="C44" s="631" t="str">
+      <c r="C44" s="634" t="str">
         <f>Fluoro!C308</f>
         <v>Auto 2</v>
       </c>
@@ -45916,7 +46042,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="11"/>
-      <c r="C45" s="631">
+      <c r="C45" s="634">
         <f>Fluoro!C309</f>
         <v>0</v>
       </c>
@@ -45951,7 +46077,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="11"/>
-      <c r="C46" s="631">
+      <c r="C46" s="634">
         <f>Fluoro!C310</f>
         <v>0</v>
       </c>
@@ -45986,7 +46112,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="631">
+      <c r="C47" s="634">
         <f>Fluoro!C311</f>
         <v>0</v>
       </c>
@@ -46021,7 +46147,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="11"/>
-      <c r="C48" s="631">
+      <c r="C48" s="634">
         <f>Fluoro!C312</f>
         <v>0</v>
       </c>
@@ -46056,7 +46182,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="11"/>
-      <c r="C49" s="631" t="str">
+      <c r="C49" s="634" t="str">
         <f>Fluoro!C313</f>
         <v>High Level</v>
       </c>
@@ -46091,7 +46217,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="11"/>
-      <c r="C50" s="631">
+      <c r="C50" s="634">
         <f>Fluoro!C314</f>
         <v>0</v>
       </c>
@@ -46126,7 +46252,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="11"/>
-      <c r="C51" s="631">
+      <c r="C51" s="634">
         <f>Fluoro!C315</f>
         <v>0</v>
       </c>
@@ -46157,7 +46283,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="11"/>
-      <c r="C52" s="631">
+      <c r="C52" s="634">
         <f>Fluoro!C316</f>
         <v>0</v>
       </c>
@@ -46188,7 +46314,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="11"/>
-      <c r="C53" s="631">
+      <c r="C53" s="634">
         <f>Fluoro!C317</f>
         <v>0</v>
       </c>
@@ -46374,7 +46500,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="11"/>
-      <c r="C60" s="632" t="str">
+      <c r="C60" s="635" t="str">
         <f>Fluoro!C324</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -46409,7 +46535,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="11"/>
-      <c r="C61" s="632">
+      <c r="C61" s="635">
         <f>Fluoro!C325</f>
         <v>0</v>
       </c>
@@ -46655,39 +46781,39 @@
         <f>Fluoro!D335</f>
         <v>Attenuator</v>
       </c>
-      <c r="E71" s="598" t="str">
+      <c r="E71" s="607" t="str">
         <f>Fluoro!E335</f>
         <v>Auto 1</v>
       </c>
-      <c r="F71" s="598">
+      <c r="F71" s="607">
         <f>Fluoro!F335</f>
         <v>0</v>
       </c>
-      <c r="G71" s="598">
+      <c r="G71" s="607">
         <f>Fluoro!G335</f>
         <v>0</v>
       </c>
-      <c r="H71" s="598" t="str">
+      <c r="H71" s="607" t="str">
         <f>Fluoro!H335</f>
         <v>Auto 2</v>
       </c>
-      <c r="I71" s="598">
+      <c r="I71" s="607">
         <f>Fluoro!I335</f>
         <v>0</v>
       </c>
-      <c r="J71" s="598">
+      <c r="J71" s="607">
         <f>Fluoro!J335</f>
         <v>0</v>
       </c>
-      <c r="K71" s="599" t="str">
+      <c r="K71" s="608" t="str">
         <f>Fluoro!K335</f>
         <v>High Level</v>
       </c>
-      <c r="L71" s="599">
+      <c r="L71" s="608">
         <f>Fluoro!L335</f>
         <v>0</v>
       </c>
-      <c r="M71" s="599">
+      <c r="M71" s="608">
         <f>Fluoro!M335</f>
         <v>0</v>
       </c>
@@ -46744,7 +46870,7 @@
         <v>7</v>
       </c>
       <c r="B73" s="11"/>
-      <c r="C73" s="629" t="str">
+      <c r="C73" s="636" t="str">
         <f>Fluoro!C337</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -46794,7 +46920,7 @@
         <v>8</v>
       </c>
       <c r="B74" s="11"/>
-      <c r="C74" s="629">
+      <c r="C74" s="636">
         <f>Fluoro!C338</f>
         <v>0</v>
       </c>
@@ -46844,7 +46970,7 @@
         <v>9</v>
       </c>
       <c r="B75" s="11"/>
-      <c r="C75" s="629">
+      <c r="C75" s="636">
         <f>Fluoro!C339</f>
         <v>0</v>
       </c>
@@ -46894,7 +47020,7 @@
         <v>10</v>
       </c>
       <c r="B76" s="11"/>
-      <c r="C76" s="629" t="str">
+      <c r="C76" s="636" t="str">
         <f>Fluoro!C340</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -46944,7 +47070,7 @@
         <v>11</v>
       </c>
       <c r="B77" s="11"/>
-      <c r="C77" s="629">
+      <c r="C77" s="636">
         <f>Fluoro!C341</f>
         <v>0</v>
       </c>
@@ -46994,7 +47120,7 @@
         <v>12</v>
       </c>
       <c r="B78" s="11"/>
-      <c r="C78" s="629">
+      <c r="C78" s="636">
         <f>Fluoro!C342</f>
         <v>0</v>
       </c>
@@ -47044,7 +47170,7 @@
         <v>13</v>
       </c>
       <c r="B79" s="11"/>
-      <c r="C79" s="629" t="str">
+      <c r="C79" s="636" t="str">
         <f>Fluoro!C343</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -47094,7 +47220,7 @@
         <v>14</v>
       </c>
       <c r="B80" s="11"/>
-      <c r="C80" s="629">
+      <c r="C80" s="636">
         <f>Fluoro!C344</f>
         <v>0</v>
       </c>
@@ -47144,7 +47270,7 @@
         <v>15</v>
       </c>
       <c r="B81" s="11"/>
-      <c r="C81" s="629">
+      <c r="C81" s="636">
         <f>Fluoro!C345</f>
         <v>0</v>
       </c>
@@ -47194,7 +47320,7 @@
         <v>16</v>
       </c>
       <c r="B82" s="11"/>
-      <c r="C82" s="629" t="str">
+      <c r="C82" s="636" t="str">
         <f>Fluoro!C346</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -47244,7 +47370,7 @@
         <v>17</v>
       </c>
       <c r="B83" s="11"/>
-      <c r="C83" s="629">
+      <c r="C83" s="636">
         <f>Fluoro!C347</f>
         <v>0</v>
       </c>
@@ -47294,7 +47420,7 @@
         <v>18</v>
       </c>
       <c r="B84" s="11"/>
-      <c r="C84" s="629">
+      <c r="C84" s="636">
         <f>Fluoro!C348</f>
         <v>0</v>
       </c>
@@ -47344,7 +47470,7 @@
         <v>19</v>
       </c>
       <c r="B85" s="11"/>
-      <c r="C85" s="629" t="str">
+      <c r="C85" s="636" t="str">
         <f>Fluoro!C349</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -47394,7 +47520,7 @@
         <v>20</v>
       </c>
       <c r="B86" s="11"/>
-      <c r="C86" s="629">
+      <c r="C86" s="636">
         <f>Fluoro!C350</f>
         <v>0</v>
       </c>
@@ -47444,7 +47570,7 @@
         <v>21</v>
       </c>
       <c r="B87" s="11"/>
-      <c r="C87" s="629">
+      <c r="C87" s="636">
         <f>Fluoro!C351</f>
         <v>0</v>
       </c>
@@ -47791,7 +47917,7 @@
         <v>36</v>
       </c>
       <c r="B102" s="11"/>
-      <c r="C102" s="630" t="str">
+      <c r="C102" s="633" t="str">
         <f>Fluoro!C366</f>
         <v>Auto 1</v>
       </c>
@@ -47829,7 +47955,7 @@
         <v>37</v>
       </c>
       <c r="B103" s="11"/>
-      <c r="C103" s="630">
+      <c r="C103" s="633">
         <f>Fluoro!C367</f>
         <v>0</v>
       </c>
@@ -47867,7 +47993,7 @@
         <v>38</v>
       </c>
       <c r="B104" s="11"/>
-      <c r="C104" s="630">
+      <c r="C104" s="633">
         <f>Fluoro!C368</f>
         <v>0</v>
       </c>
@@ -47905,7 +48031,7 @@
         <v>39</v>
       </c>
       <c r="B105" s="11"/>
-      <c r="C105" s="630">
+      <c r="C105" s="633">
         <f>Fluoro!C369</f>
         <v>0</v>
       </c>
@@ -47940,7 +48066,7 @@
         <v>40</v>
       </c>
       <c r="B106" s="11"/>
-      <c r="C106" s="630">
+      <c r="C106" s="633">
         <f>Fluoro!C370</f>
         <v>0</v>
       </c>
@@ -47975,7 +48101,7 @@
         <v>41</v>
       </c>
       <c r="B107" s="11"/>
-      <c r="C107" s="631" t="str">
+      <c r="C107" s="634" t="str">
         <f>Fluoro!C371</f>
         <v>Auto 2</v>
       </c>
@@ -48010,7 +48136,7 @@
         <v>42</v>
       </c>
       <c r="B108" s="11"/>
-      <c r="C108" s="631">
+      <c r="C108" s="634">
         <f>Fluoro!C372</f>
         <v>0</v>
       </c>
@@ -48045,7 +48171,7 @@
         <v>43</v>
       </c>
       <c r="B109" s="11"/>
-      <c r="C109" s="631">
+      <c r="C109" s="634">
         <f>Fluoro!C373</f>
         <v>0</v>
       </c>
@@ -48080,7 +48206,7 @@
         <v>44</v>
       </c>
       <c r="B110" s="11"/>
-      <c r="C110" s="631">
+      <c r="C110" s="634">
         <f>Fluoro!C374</f>
         <v>0</v>
       </c>
@@ -48115,7 +48241,7 @@
         <v>45</v>
       </c>
       <c r="B111" s="11"/>
-      <c r="C111" s="631">
+      <c r="C111" s="634">
         <f>Fluoro!C375</f>
         <v>0</v>
       </c>
@@ -48150,7 +48276,7 @@
         <v>46</v>
       </c>
       <c r="B112" s="11"/>
-      <c r="C112" s="631" t="str">
+      <c r="C112" s="634" t="str">
         <f>Fluoro!C376</f>
         <v>High Level</v>
       </c>
@@ -48185,7 +48311,7 @@
         <v>47</v>
       </c>
       <c r="B113" s="11"/>
-      <c r="C113" s="631">
+      <c r="C113" s="634">
         <f>Fluoro!C377</f>
         <v>0</v>
       </c>
@@ -48220,7 +48346,7 @@
         <v>48</v>
       </c>
       <c r="B114" s="11"/>
-      <c r="C114" s="631">
+      <c r="C114" s="634">
         <f>Fluoro!C378</f>
         <v>0</v>
       </c>
@@ -48251,7 +48377,7 @@
         <v>49</v>
       </c>
       <c r="B115" s="11"/>
-      <c r="C115" s="631">
+      <c r="C115" s="634">
         <f>Fluoro!C379</f>
         <v>0</v>
       </c>
@@ -48282,7 +48408,7 @@
         <v>50</v>
       </c>
       <c r="B116" s="11"/>
-      <c r="C116" s="631">
+      <c r="C116" s="634">
         <f>Fluoro!C380</f>
         <v>0</v>
       </c>
@@ -48456,7 +48582,7 @@
         <v>58</v>
       </c>
       <c r="B124" s="11"/>
-      <c r="C124" s="632" t="str">
+      <c r="C124" s="635" t="str">
         <f>Fluoro!C388</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -48491,7 +48617,7 @@
         <v>59</v>
       </c>
       <c r="B125" s="11"/>
-      <c r="C125" s="632">
+      <c r="C125" s="635">
         <f>Fluoro!C389</f>
         <v>0</v>
       </c>
@@ -48668,6 +48794,21 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="H71:J71"/>
+    <mergeCell ref="K71:M71"/>
     <mergeCell ref="C102:C106"/>
     <mergeCell ref="C107:C111"/>
     <mergeCell ref="C112:C116"/>
@@ -48677,21 +48818,6 @@
     <mergeCell ref="C79:C81"/>
     <mergeCell ref="C82:C84"/>
     <mergeCell ref="C85:C87"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="H71:J71"/>
-    <mergeCell ref="K71:M71"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="68" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -48718,34 +48844,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="633" t="s">
+      <c r="A1" s="637" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="633"/>
+      <c r="B1" s="637"/>
       <c r="N1" s="326"/>
-      <c r="O1" s="604" t="str">
+      <c r="O1" s="601" t="str">
         <f>Fluoro!O105</f>
         <v>Patient Entrance Exposure Rate (Fluoroscopy)*</v>
       </c>
-      <c r="P1" s="604"/>
-      <c r="Q1" s="604"/>
-      <c r="R1" s="604" t="s">
+      <c r="P1" s="601"/>
+      <c r="Q1" s="601"/>
+      <c r="R1" s="601" t="s">
         <v>411</v>
       </c>
-      <c r="S1" s="604"/>
-      <c r="T1" s="604"/>
+      <c r="S1" s="601"/>
+      <c r="T1" s="601"/>
       <c r="V1" s="326"/>
-      <c r="W1" s="604" t="str">
+      <c r="W1" s="601" t="str">
         <f>Fluoro!O137</f>
         <v>Patient Entrance Exposure Rate – Digital Acquisition</v>
       </c>
-      <c r="X1" s="604"/>
-      <c r="Y1" s="604"/>
-      <c r="Z1" s="604" t="s">
+      <c r="X1" s="601"/>
+      <c r="Y1" s="601"/>
+      <c r="Z1" s="601" t="s">
         <v>411</v>
       </c>
-      <c r="AA1" s="604"/>
-      <c r="AB1" s="604"/>
+      <c r="AA1" s="601"/>
+      <c r="AB1" s="601"/>
     </row>
     <row r="2" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="327">
@@ -48948,10 +49074,10 @@
       <c r="AB6" s="326"/>
     </row>
     <row r="7" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="633" t="s">
+      <c r="A7" s="637" t="s">
         <v>414</v>
       </c>
-      <c r="B7" s="633"/>
+      <c r="B7" s="637"/>
       <c r="D7" s="211" t="s">
         <v>415</v>
       </c>
@@ -52738,14 +52864,14 @@
       <c r="B75" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="E75" s="604" t="s">
+      <c r="E75" s="601" t="s">
         <v>424</v>
       </c>
-      <c r="F75" s="604"/>
-      <c r="I75" s="604" t="s">
+      <c r="F75" s="601"/>
+      <c r="I75" s="601" t="s">
         <v>425</v>
       </c>
-      <c r="J75" s="604"/>
+      <c r="J75" s="601"/>
     </row>
     <row r="76" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">

</xml_diff>

<commit_message>
Update cell with list of named print ranges
</commit_message>
<xml_diff>
--- a/MUSCCArm.xlsx
+++ b/MUSCCArm.xlsx
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="449">
   <si>
     <t>Print Area</t>
   </si>
@@ -1463,6 +1463,9 @@
   </si>
   <si>
     <t>Page1,Page2,HVLPage,ExpChartFluoroPage,ExpChartDAPage,ImgQualityPage,Com1Page,Com2Page,OutputGraphFluoroPage,OutputGraphDAPage,LeedsTO10Page,ExpChartRFluoro,ExpChartRDA</t>
+  </si>
+  <si>
+    <t>Page1,Page2,HVLPage,ExpChartFluoroPage,ExpChartDAPage,ImgQualityPage,Com1Page,Com2Page,OutputGraphFluoroPage,OutputGraphDAPage,LeedsTO10Page</t>
   </si>
 </sst>
 </file>
@@ -6287,179 +6290,179 @@
     <xf numFmtId="172" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="161" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="162" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="163" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="195" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="204" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="205" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="137" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="166" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="192" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="120" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="167" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="194" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="187" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="188" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="113" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="129" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="130" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="126" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="133" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="119" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="110" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="118" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="119" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="110" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="129" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="130" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="126" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="133" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="113" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="120" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="161" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="162" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="187" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="163" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="188" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="137" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="167" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="194" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="195" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="204" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="205" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="166" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="192" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6875,7 +6878,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7053,7 +7055,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7125,7 +7126,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7217,7 +7217,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7444,7 +7443,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7516,7 +7514,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7642,7 +7639,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9315,7 +9311,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9387,7 +9382,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9434,7 +9428,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9502,7 +9495,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9729,7 +9721,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9801,7 +9792,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9927,7 +9917,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11600,7 +11589,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11672,7 +11660,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11719,7 +11706,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11803,7 +11789,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12556,7 +12541,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12780,7 +12764,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13533,7 +13516,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -16322,6 +16304,150 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -16590,9 +16716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD792"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16661,7 +16785,7 @@
       </c>
       <c r="Y2" s="15"/>
       <c r="AA2" s="16" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16807,7 +16931,7 @@
       </c>
       <c r="AD7" s="31" t="str">
         <f>IF(OR(AA2="",AA2=0),"",AA2)</f>
-        <v>Page1,Page2,HVLPage,ExpChartFluoroPage,ExpChartDAPage,ImgQualityPage,Com1Page,Com2Page,OutputGraphFluoroPage,OutputGraphDAPage,LeedsTO10Page,ExpChartRFluoro,ExpChartRDA</v>
+        <v>Page1,Page2,HVLPage,ExpChartFluoroPage,ExpChartDAPage,ImgQualityPage,Com1Page,Com2Page,OutputGraphFluoroPage,OutputGraphDAPage,LeedsTO10Page</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16902,21 +17026,21 @@
       <c r="E10" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="579" t="str">
+      <c r="F10" s="629" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="579"/>
+      <c r="G10" s="629"/>
       <c r="H10" s="43"/>
       <c r="I10" s="43"/>
       <c r="J10" s="163" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="580" t="str">
+      <c r="K10" s="622" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="580"/>
+      <c r="L10" s="622"/>
       <c r="M10" s="360"/>
       <c r="O10" s="14"/>
       <c r="Q10" s="2" t="s">
@@ -16959,21 +17083,21 @@
       <c r="E11" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="581" t="str">
+      <c r="F11" s="623" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="581"/>
+      <c r="G11" s="623"/>
       <c r="H11" s="43"/>
       <c r="I11" s="43"/>
       <c r="J11" s="163" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="581" t="str">
+      <c r="K11" s="623" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="581"/>
+      <c r="L11" s="623"/>
       <c r="M11" s="360"/>
       <c r="O11" s="14"/>
       <c r="Q11" s="2" t="s">
@@ -17016,21 +17140,21 @@
       <c r="E12" s="163" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="581" t="str">
+      <c r="F12" s="623" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="581"/>
+      <c r="G12" s="623"/>
       <c r="H12" s="43"/>
       <c r="I12" s="43"/>
       <c r="J12" s="163" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="582" t="str">
+      <c r="K12" s="631" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="582"/>
+      <c r="L12" s="631"/>
       <c r="M12" s="360"/>
       <c r="O12" s="14"/>
       <c r="Q12" s="2" t="s">
@@ -17073,21 +17197,21 @@
       <c r="E13" s="163" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="583" t="str">
+      <c r="F13" s="624" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="583"/>
+      <c r="G13" s="624"/>
       <c r="H13" s="43"/>
       <c r="I13" s="43"/>
       <c r="J13" s="163" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="583" t="str">
+      <c r="K13" s="624" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="583"/>
+      <c r="L13" s="624"/>
       <c r="M13" s="360"/>
       <c r="O13" s="14"/>
       <c r="Q13" s="2" t="s">
@@ -17210,21 +17334,21 @@
       <c r="E16" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="579" t="str">
+      <c r="F16" s="629" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="579"/>
+      <c r="G16" s="629"/>
       <c r="H16" s="43"/>
       <c r="I16" s="43"/>
       <c r="J16" s="163" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="584" t="str">
+      <c r="K16" s="632" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="584"/>
+      <c r="L16" s="632"/>
       <c r="M16" s="360"/>
       <c r="O16" s="14"/>
       <c r="P16" s="51" t="s">
@@ -17254,21 +17378,21 @@
       <c r="E17" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="581" t="str">
+      <c r="F17" s="623" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="581"/>
+      <c r="G17" s="623"/>
       <c r="H17" s="43"/>
       <c r="I17" s="43"/>
       <c r="J17" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="583" t="str">
+      <c r="K17" s="624" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="583"/>
+      <c r="L17" s="624"/>
       <c r="M17" s="360"/>
       <c r="O17" s="14"/>
       <c r="Q17" s="2" t="s">
@@ -17311,21 +17435,21 @@
       <c r="E18" s="163" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="583" t="str">
+      <c r="F18" s="624" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="583"/>
+      <c r="G18" s="624"/>
       <c r="H18" s="43"/>
       <c r="I18" s="43"/>
       <c r="J18" s="163" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="583" t="str">
+      <c r="K18" s="624" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="583"/>
+      <c r="L18" s="624"/>
       <c r="M18" s="360"/>
       <c r="O18" s="14"/>
       <c r="Q18" s="2" t="s">
@@ -17373,11 +17497,11 @@
       <c r="J19" s="163" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="583" t="str">
+      <c r="K19" s="624" t="str">
         <f>IF(V20="","",V20)</f>
         <v/>
       </c>
-      <c r="L19" s="583"/>
+      <c r="L19" s="624"/>
       <c r="M19" s="360"/>
       <c r="O19" s="14"/>
       <c r="Q19" s="2" t="s">
@@ -17452,11 +17576,11 @@
       <c r="E21" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="579" t="str">
+      <c r="F21" s="629" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="579"/>
+      <c r="G21" s="629"/>
       <c r="H21" s="43"/>
       <c r="I21" s="43"/>
       <c r="J21" s="74" t="s">
@@ -17496,21 +17620,21 @@
       <c r="E22" s="163" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="585" t="str">
+      <c r="F22" s="630" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="585"/>
+      <c r="G22" s="630"/>
       <c r="H22" s="43"/>
       <c r="I22" s="43"/>
       <c r="J22" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="579" t="str">
+      <c r="K22" s="629" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="579"/>
+      <c r="L22" s="629"/>
       <c r="M22" s="360"/>
       <c r="O22" s="14"/>
       <c r="Q22" s="2" t="s">
@@ -17555,11 +17679,11 @@
       <c r="J23" s="163" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="581" t="str">
+      <c r="K23" s="623" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="581"/>
+      <c r="L23" s="623"/>
       <c r="M23" s="360"/>
       <c r="O23" s="14"/>
       <c r="Q23" s="2" t="s">
@@ -17602,21 +17726,21 @@
       <c r="E24" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="580" t="str">
+      <c r="F24" s="622" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="580"/>
+      <c r="G24" s="622"/>
       <c r="H24" s="43"/>
       <c r="I24" s="43"/>
       <c r="J24" s="163" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="581" t="str">
+      <c r="K24" s="623" t="str">
         <f>IF(V25="","",V25)</f>
         <v/>
       </c>
-      <c r="L24" s="581"/>
+      <c r="L24" s="623"/>
       <c r="M24" s="360"/>
       <c r="O24" s="14"/>
       <c r="P24" s="51" t="s">
@@ -17654,11 +17778,11 @@
       <c r="E25" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="583" t="str">
+      <c r="F25" s="624" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="583"/>
+      <c r="G25" s="624"/>
       <c r="H25" s="43"/>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -17706,11 +17830,11 @@
       <c r="E26" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="583" t="str">
+      <c r="F26" s="624" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="583"/>
+      <c r="G26" s="624"/>
       <c r="H26" s="43"/>
       <c r="I26" s="43"/>
       <c r="J26" s="361" t="s">
@@ -17759,11 +17883,11 @@
       <c r="J27" s="163" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="579" t="str">
+      <c r="K27" s="629" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="579"/>
+      <c r="L27" s="629"/>
       <c r="M27" s="360"/>
       <c r="O27" s="14"/>
       <c r="Q27" s="2" t="s">
@@ -17801,21 +17925,21 @@
       <c r="E28" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="580" t="str">
+      <c r="F28" s="622" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="580"/>
+      <c r="G28" s="622"/>
       <c r="H28" s="43"/>
       <c r="I28" s="43"/>
       <c r="J28" s="163" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="581" t="str">
+      <c r="K28" s="623" t="str">
         <f>IF(V29="","",V29)</f>
         <v/>
       </c>
-      <c r="L28" s="581"/>
+      <c r="L28" s="623"/>
       <c r="M28" s="360"/>
       <c r="O28" s="14"/>
       <c r="P28" s="51" t="s">
@@ -17844,11 +17968,11 @@
       <c r="E29" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="583" t="str">
+      <c r="F29" s="624" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="583"/>
+      <c r="G29" s="624"/>
       <c r="H29" s="43"/>
       <c r="I29" s="43"/>
       <c r="J29" s="43"/>
@@ -17896,11 +18020,11 @@
       <c r="E30" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="583" t="str">
+      <c r="F30" s="624" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="583"/>
+      <c r="G30" s="624"/>
       <c r="H30" s="43"/>
       <c r="I30" s="43"/>
       <c r="J30" s="43"/>
@@ -18015,11 +18139,11 @@
       <c r="E33" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="579" t="str">
+      <c r="F33" s="629" t="str">
         <f>IF(R34="","",R34)</f>
         <v/>
       </c>
-      <c r="G33" s="579"/>
+      <c r="G33" s="629"/>
       <c r="H33" s="43"/>
       <c r="I33" s="43"/>
       <c r="J33" s="74" t="s">
@@ -18056,21 +18180,21 @@
       <c r="E34" s="163" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="585" t="str">
+      <c r="F34" s="630" t="str">
         <f>IF(R35="","",R35)</f>
         <v/>
       </c>
-      <c r="G34" s="585"/>
+      <c r="G34" s="630"/>
       <c r="H34" s="43"/>
       <c r="I34" s="43"/>
       <c r="J34" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="579" t="str">
+      <c r="K34" s="629" t="str">
         <f>IF(V35="","",V35)</f>
         <v/>
       </c>
-      <c r="L34" s="579"/>
+      <c r="L34" s="629"/>
       <c r="M34" s="360"/>
       <c r="O34" s="14"/>
       <c r="Q34" s="2" t="s">
@@ -18115,11 +18239,11 @@
       <c r="J35" s="163" t="s">
         <v>41</v>
       </c>
-      <c r="K35" s="581" t="str">
+      <c r="K35" s="623" t="str">
         <f>IF(V36="","",V36)</f>
         <v/>
       </c>
-      <c r="L35" s="581"/>
+      <c r="L35" s="623"/>
       <c r="M35" s="360"/>
       <c r="O35" s="14"/>
       <c r="Q35" s="2" t="s">
@@ -18162,21 +18286,21 @@
       <c r="E36" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="580" t="str">
+      <c r="F36" s="622" t="str">
         <f>IF(R37="","",R37)</f>
         <v/>
       </c>
-      <c r="G36" s="580"/>
+      <c r="G36" s="622"/>
       <c r="H36" s="43"/>
       <c r="I36" s="43"/>
       <c r="J36" s="163" t="s">
         <v>42</v>
       </c>
-      <c r="K36" s="581" t="str">
+      <c r="K36" s="623" t="str">
         <f>IF(V37="","",V37)</f>
         <v/>
       </c>
-      <c r="L36" s="581"/>
+      <c r="L36" s="623"/>
       <c r="M36" s="360"/>
       <c r="O36" s="14"/>
       <c r="P36" s="51" t="s">
@@ -18214,11 +18338,11 @@
       <c r="E37" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="583" t="str">
+      <c r="F37" s="624" t="str">
         <f>IF(R38="","",R38)</f>
         <v/>
       </c>
-      <c r="G37" s="583"/>
+      <c r="G37" s="624"/>
       <c r="H37" s="43"/>
       <c r="I37" s="43"/>
       <c r="J37" s="43"/>
@@ -18266,11 +18390,11 @@
       <c r="E38" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="583" t="str">
+      <c r="F38" s="624" t="str">
         <f>IF(R39="","",R39)</f>
         <v/>
       </c>
-      <c r="G38" s="583"/>
+      <c r="G38" s="624"/>
       <c r="H38" s="43"/>
       <c r="I38" s="43"/>
       <c r="J38" s="361" t="s">
@@ -18317,11 +18441,11 @@
       <c r="J39" s="163" t="s">
         <v>45</v>
       </c>
-      <c r="K39" s="579" t="str">
+      <c r="K39" s="629" t="str">
         <f>IF(V40="","",V40)</f>
         <v/>
       </c>
-      <c r="L39" s="579"/>
+      <c r="L39" s="629"/>
       <c r="M39" s="360"/>
       <c r="O39" s="14"/>
       <c r="Q39" s="2" t="s">
@@ -18359,21 +18483,21 @@
       <c r="E40" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="580" t="str">
+      <c r="F40" s="622" t="str">
         <f>IF(R41="","",R41)</f>
         <v/>
       </c>
-      <c r="G40" s="580"/>
+      <c r="G40" s="622"/>
       <c r="H40" s="43"/>
       <c r="I40" s="43"/>
       <c r="J40" s="163" t="s">
         <v>46</v>
       </c>
-      <c r="K40" s="581" t="str">
+      <c r="K40" s="623" t="str">
         <f>IF(V41="","",V41)</f>
         <v/>
       </c>
-      <c r="L40" s="581"/>
+      <c r="L40" s="623"/>
       <c r="M40" s="360"/>
       <c r="O40" s="14"/>
       <c r="P40" s="51" t="s">
@@ -18411,11 +18535,11 @@
       <c r="E41" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="583" t="str">
+      <c r="F41" s="624" t="str">
         <f>IF(R42="","",R42)</f>
         <v/>
       </c>
-      <c r="G41" s="583"/>
+      <c r="G41" s="624"/>
       <c r="H41" s="43"/>
       <c r="I41" s="43"/>
       <c r="J41" s="43"/>
@@ -18463,11 +18587,11 @@
       <c r="E42" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="583" t="str">
+      <c r="F42" s="624" t="str">
         <f>IF(R43="","",R43)</f>
         <v/>
       </c>
-      <c r="G42" s="583"/>
+      <c r="G42" s="624"/>
       <c r="H42" s="43"/>
       <c r="I42" s="43"/>
       <c r="J42" s="43"/>
@@ -19225,10 +19349,10 @@
       <c r="I69" s="347"/>
       <c r="J69" s="347"/>
       <c r="K69" s="347"/>
-      <c r="L69" s="586" t="s">
+      <c r="L69" s="625" t="s">
         <v>84</v>
       </c>
-      <c r="M69" s="587"/>
+      <c r="M69" s="626"/>
       <c r="O69" s="57"/>
       <c r="P69" s="18" t="s">
         <v>85</v>
@@ -20860,24 +20984,24 @@
       <c r="P107" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="Q107" s="588" t="str">
+      <c r="Q107" s="627" t="str">
         <f>IF(Q106&lt;&gt;"",Q106,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R107" s="588"/>
-      <c r="S107" s="588"/>
-      <c r="T107" s="589" t="str">
+      <c r="R107" s="627"/>
+      <c r="S107" s="627"/>
+      <c r="T107" s="628" t="str">
         <f>IF(T106&lt;&gt;"",T106,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v>Auto 2</v>
       </c>
-      <c r="U107" s="589"/>
-      <c r="V107" s="589"/>
-      <c r="W107" s="589" t="str">
+      <c r="U107" s="628"/>
+      <c r="V107" s="628"/>
+      <c r="W107" s="628" t="str">
         <f>IF(W106&lt;&gt;"",W106,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v>High Level</v>
       </c>
-      <c r="X107" s="589"/>
-      <c r="Y107" s="589"/>
+      <c r="X107" s="628"/>
+      <c r="Y107" s="628"/>
       <c r="AA107" s="2" t="s">
         <v>111</v>
       </c>
@@ -22871,24 +22995,24 @@
       <c r="P139" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="Q139" s="588" t="str">
+      <c r="Q139" s="627" t="str">
         <f>IF(Q138&lt;&gt;"",Q138,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R139" s="588"/>
-      <c r="S139" s="588"/>
-      <c r="T139" s="589" t="str">
+      <c r="R139" s="627"/>
+      <c r="S139" s="627"/>
+      <c r="T139" s="628" t="str">
         <f>IF(T138&lt;&gt;"",T138,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v>Auto 2</v>
       </c>
-      <c r="U139" s="589"/>
-      <c r="V139" s="589"/>
-      <c r="W139" s="589" t="str">
+      <c r="U139" s="628"/>
+      <c r="V139" s="628"/>
+      <c r="W139" s="628" t="str">
         <f>IF(W138&lt;&gt;"",W138,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v>High Level</v>
       </c>
-      <c r="X139" s="589"/>
-      <c r="Y139" s="589"/>
+      <c r="X139" s="628"/>
+      <c r="Y139" s="628"/>
       <c r="AA139" s="2" t="str">
         <f>$W$139&amp;" Mag 2"</f>
         <v>High Level Mag 2</v>
@@ -25231,10 +25355,10 @@
       <c r="P181" s="136"/>
       <c r="Q181" s="138"/>
       <c r="R181" s="129"/>
-      <c r="T181" s="590" t="s">
+      <c r="T181" s="604" t="s">
         <v>245</v>
       </c>
-      <c r="U181" s="590"/>
+      <c r="U181" s="604"/>
       <c r="W181" s="2" t="s">
         <v>199</v>
       </c>
@@ -25605,7 +25729,7 @@
       <c r="K190" s="371"/>
       <c r="L190" s="371"/>
       <c r="M190" s="375"/>
-      <c r="O190" s="591" t="str">
+      <c r="O190" s="612" t="str">
         <f>$Q$107</f>
         <v>Auto 1</v>
       </c>
@@ -25655,7 +25779,7 @@
       <c r="K191" s="371"/>
       <c r="L191" s="371"/>
       <c r="M191" s="351"/>
-      <c r="O191" s="591"/>
+      <c r="O191" s="612"/>
       <c r="P191" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -25701,7 +25825,7 @@
       <c r="K192" s="136"/>
       <c r="L192" s="136"/>
       <c r="M192" s="351"/>
-      <c r="O192" s="591"/>
+      <c r="O192" s="612"/>
       <c r="P192" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -25747,7 +25871,7 @@
       <c r="K193" s="136"/>
       <c r="L193" s="136"/>
       <c r="M193" s="351"/>
-      <c r="O193" s="591"/>
+      <c r="O193" s="612"/>
       <c r="P193" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -25790,7 +25914,7 @@
       <c r="K194" s="136"/>
       <c r="L194" s="136"/>
       <c r="M194" s="351"/>
-      <c r="O194" s="591"/>
+      <c r="O194" s="612"/>
       <c r="P194" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -25833,7 +25957,7 @@
       <c r="K195" s="136"/>
       <c r="L195" s="136"/>
       <c r="M195" s="351"/>
-      <c r="O195" s="591" t="str">
+      <c r="O195" s="612" t="str">
         <f>$T$107</f>
         <v>Auto 2</v>
       </c>
@@ -25879,7 +26003,7 @@
       <c r="K196" s="353"/>
       <c r="L196" s="353"/>
       <c r="M196" s="354"/>
-      <c r="O196" s="591"/>
+      <c r="O196" s="612"/>
       <c r="P196" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -25924,7 +26048,7 @@
         <f>IF($X$7="","",$X$7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="O197" s="591"/>
+      <c r="O197" s="612"/>
       <c r="P197" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -25969,7 +26093,7 @@
         <f>IF($R$13="","",$R$13)</f>
         <v/>
       </c>
-      <c r="O198" s="591"/>
+      <c r="O198" s="612"/>
       <c r="P198" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -26015,7 +26139,7 @@
         <f>$H$2</f>
         <v>Medical University of South Carolina</v>
       </c>
-      <c r="O199" s="591"/>
+      <c r="O199" s="612"/>
       <c r="P199" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -26064,7 +26188,7 @@
         <f>$H$5</f>
         <v>Fluoroscopy System Compliance Inspection</v>
       </c>
-      <c r="O200" s="591" t="str">
+      <c r="O200" s="612" t="str">
         <f>$W$107</f>
         <v>High Level</v>
       </c>
@@ -26113,7 +26237,7 @@
       <c r="K201" s="347"/>
       <c r="L201" s="347"/>
       <c r="M201" s="348"/>
-      <c r="O201" s="591"/>
+      <c r="O201" s="612"/>
       <c r="P201" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -26147,24 +26271,24 @@
       <c r="B202" s="349"/>
       <c r="C202" s="399"/>
       <c r="D202" s="371"/>
-      <c r="E202" s="592" t="s">
+      <c r="E202" s="615" t="s">
         <v>262</v>
       </c>
-      <c r="F202" s="593" t="s">
+      <c r="F202" s="616" t="s">
         <v>263</v>
       </c>
-      <c r="G202" s="594" t="s">
+      <c r="G202" s="617" t="s">
         <v>264</v>
       </c>
-      <c r="H202" s="595" t="str">
+      <c r="H202" s="618" t="str">
         <f>R276</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="I202" s="596" t="str">
+      <c r="I202" s="619" t="str">
         <f>S276</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="J202" s="597" t="s">
+      <c r="J202" s="620" t="s">
         <v>265</v>
       </c>
       <c r="K202" s="136" t="s">
@@ -26173,10 +26297,10 @@
       <c r="L202" s="136" t="s">
         <v>267</v>
       </c>
-      <c r="M202" s="598" t="s">
+      <c r="M202" s="621" t="s">
         <v>268</v>
       </c>
-      <c r="O202" s="591"/>
+      <c r="O202" s="612"/>
       <c r="P202" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -26214,12 +26338,12 @@
       <c r="D203" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="E203" s="592"/>
-      <c r="F203" s="593"/>
-      <c r="G203" s="594"/>
-      <c r="H203" s="595"/>
-      <c r="I203" s="596"/>
-      <c r="J203" s="597"/>
+      <c r="E203" s="615"/>
+      <c r="F203" s="616"/>
+      <c r="G203" s="617"/>
+      <c r="H203" s="618"/>
+      <c r="I203" s="619"/>
+      <c r="J203" s="620"/>
       <c r="K203" s="136" t="str">
         <f>U277</f>
         <v>mGy/min</v>
@@ -26228,8 +26352,8 @@
         <f>V277</f>
         <v>mGy/min</v>
       </c>
-      <c r="M203" s="598"/>
-      <c r="O203" s="591"/>
+      <c r="M203" s="621"/>
+      <c r="O203" s="612"/>
       <c r="P203" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -26305,7 +26429,7 @@
         <f t="shared" si="30"/>
         <v/>
       </c>
-      <c r="O204" s="591"/>
+      <c r="O204" s="612"/>
       <c r="P204" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -26964,7 +27088,7 @@
       <c r="K214" s="371"/>
       <c r="L214" s="371"/>
       <c r="M214" s="351"/>
-      <c r="O214" s="591" t="str">
+      <c r="O214" s="612" t="str">
         <f>$Q$139</f>
         <v>Auto 1</v>
       </c>
@@ -27014,7 +27138,7 @@
       <c r="K215" s="420"/>
       <c r="L215" s="420"/>
       <c r="M215" s="421"/>
-      <c r="O215" s="591"/>
+      <c r="O215" s="612"/>
       <c r="P215" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -27064,7 +27188,7 @@
       <c r="K216" s="371"/>
       <c r="L216" s="371"/>
       <c r="M216" s="351"/>
-      <c r="O216" s="591"/>
+      <c r="O216" s="612"/>
       <c r="P216" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -27110,7 +27234,7 @@
       <c r="K217" s="371"/>
       <c r="L217" s="371"/>
       <c r="M217" s="375"/>
-      <c r="O217" s="591"/>
+      <c r="O217" s="612"/>
       <c r="P217" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -27158,7 +27282,7 @@
       <c r="K218" s="371"/>
       <c r="L218" s="371"/>
       <c r="M218" s="375"/>
-      <c r="O218" s="591"/>
+      <c r="O218" s="612"/>
       <c r="P218" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -27201,7 +27325,7 @@
       <c r="K219" s="371"/>
       <c r="L219" s="371"/>
       <c r="M219" s="375"/>
-      <c r="O219" s="591" t="str">
+      <c r="O219" s="612" t="str">
         <f>$T$139</f>
         <v>Auto 2</v>
       </c>
@@ -27251,7 +27375,7 @@
       <c r="K220" s="371"/>
       <c r="L220" s="371"/>
       <c r="M220" s="375"/>
-      <c r="O220" s="591"/>
+      <c r="O220" s="612"/>
       <c r="P220" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -27304,7 +27428,7 @@
       <c r="K221" s="371"/>
       <c r="L221" s="371"/>
       <c r="M221" s="375"/>
-      <c r="O221" s="591"/>
+      <c r="O221" s="612"/>
       <c r="P221" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -27362,7 +27486,7 @@
       <c r="K222" s="371"/>
       <c r="L222" s="371"/>
       <c r="M222" s="375"/>
-      <c r="O222" s="591"/>
+      <c r="O222" s="612"/>
       <c r="P222" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -27417,7 +27541,7 @@
       <c r="K223" s="371"/>
       <c r="L223" s="371"/>
       <c r="M223" s="375"/>
-      <c r="O223" s="591"/>
+      <c r="O223" s="612"/>
       <c r="P223" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -27472,7 +27596,7 @@
       <c r="K224" s="371"/>
       <c r="L224" s="371"/>
       <c r="M224" s="375"/>
-      <c r="O224" s="591" t="str">
+      <c r="O224" s="612" t="str">
         <f>$W$139</f>
         <v>High Level</v>
       </c>
@@ -27530,7 +27654,7 @@
       <c r="K225" s="371"/>
       <c r="L225" s="371"/>
       <c r="M225" s="375"/>
-      <c r="O225" s="591"/>
+      <c r="O225" s="612"/>
       <c r="P225" s="145" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -27581,7 +27705,7 @@
       <c r="K226" s="371"/>
       <c r="L226" s="371"/>
       <c r="M226" s="375"/>
-      <c r="O226" s="591"/>
+      <c r="O226" s="612"/>
       <c r="P226" s="145" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -27635,7 +27759,7 @@
       <c r="K227" s="371"/>
       <c r="L227" s="371"/>
       <c r="M227" s="375"/>
-      <c r="O227" s="591"/>
+      <c r="O227" s="612"/>
       <c r="P227" s="145" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -27683,7 +27807,7 @@
       <c r="K228" s="371"/>
       <c r="L228" s="371"/>
       <c r="M228" s="375"/>
-      <c r="O228" s="591"/>
+      <c r="O228" s="612"/>
       <c r="P228" s="135" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -28209,7 +28333,7 @@
       <c r="K240" s="371"/>
       <c r="L240" s="371"/>
       <c r="M240" s="375"/>
-      <c r="O240" s="599" t="s">
+      <c r="O240" s="613" t="s">
         <v>294</v>
       </c>
       <c r="P240" s="170" t="s">
@@ -28271,7 +28395,7 @@
       <c r="K241" s="371"/>
       <c r="L241" s="371"/>
       <c r="M241" s="375"/>
-      <c r="O241" s="599"/>
+      <c r="O241" s="613"/>
       <c r="P241" s="175" t="s">
         <v>297</v>
       </c>
@@ -28322,7 +28446,7 @@
       <c r="K242" s="371"/>
       <c r="L242" s="371"/>
       <c r="M242" s="375"/>
-      <c r="O242" s="599" t="str">
+      <c r="O242" s="613" t="str">
         <f>IF($U$137=1,"Scatter - Pulse", "Scatter – Digital acq")</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -28382,7 +28506,7 @@
       <c r="K243" s="371"/>
       <c r="L243" s="371"/>
       <c r="M243" s="375"/>
-      <c r="O243" s="599"/>
+      <c r="O243" s="613"/>
       <c r="P243" s="175" t="s">
         <v>297</v>
       </c>
@@ -28908,17 +29032,17 @@
       <c r="P257" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="Q257" s="600" t="s">
+      <c r="Q257" s="614" t="s">
         <v>313</v>
       </c>
-      <c r="R257" s="600"/>
+      <c r="R257" s="614"/>
       <c r="S257" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="T257" s="600" t="s">
+      <c r="T257" s="614" t="s">
         <v>315</v>
       </c>
-      <c r="U257" s="600"/>
+      <c r="U257" s="614"/>
       <c r="V257" s="1" t="s">
         <v>316</v>
       </c>
@@ -29383,24 +29507,24 @@
         <f t="shared" si="41"/>
         <v>Attenuator</v>
       </c>
-      <c r="E269" s="601" t="str">
+      <c r="E269" s="606" t="str">
         <f>Q107</f>
         <v>Auto 1</v>
       </c>
-      <c r="F269" s="602"/>
-      <c r="G269" s="602"/>
-      <c r="H269" s="602" t="str">
+      <c r="F269" s="607"/>
+      <c r="G269" s="607"/>
+      <c r="H269" s="607" t="str">
         <f>T107</f>
         <v>Auto 2</v>
       </c>
-      <c r="I269" s="602"/>
-      <c r="J269" s="602"/>
-      <c r="K269" s="603" t="str">
+      <c r="I269" s="607"/>
+      <c r="J269" s="607"/>
+      <c r="K269" s="608" t="str">
         <f>W107</f>
         <v>High Level</v>
       </c>
-      <c r="L269" s="603"/>
-      <c r="M269" s="604"/>
+      <c r="L269" s="608"/>
+      <c r="M269" s="609"/>
       <c r="O269" s="194" t="str">
         <f t="shared" si="42"/>
         <v/>
@@ -29502,7 +29626,7 @@
         <v>7</v>
       </c>
       <c r="B271" s="349"/>
-      <c r="C271" s="605" t="str">
+      <c r="C271" s="596" t="str">
         <f>O110&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29571,7 +29695,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="349"/>
-      <c r="C272" s="605"/>
+      <c r="C272" s="596"/>
       <c r="D272" s="447">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -29644,7 +29768,7 @@
         <v>9</v>
       </c>
       <c r="B273" s="349"/>
-      <c r="C273" s="605"/>
+      <c r="C273" s="596"/>
       <c r="D273" s="450">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -29710,7 +29834,7 @@
         <v>10</v>
       </c>
       <c r="B274" s="349"/>
-      <c r="C274" s="605" t="str">
+      <c r="C274" s="596" t="str">
         <f>O113&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29786,7 +29910,7 @@
         <v>11</v>
       </c>
       <c r="B275" s="349"/>
-      <c r="C275" s="605"/>
+      <c r="C275" s="596"/>
       <c r="D275" s="447">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -29852,7 +29976,7 @@
         <v>12</v>
       </c>
       <c r="B276" s="349"/>
-      <c r="C276" s="605"/>
+      <c r="C276" s="596"/>
       <c r="D276" s="450">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -29893,17 +30017,17 @@
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="O276" s="606" t="s">
+      <c r="O276" s="610" t="s">
         <v>262</v>
       </c>
-      <c r="P276" s="607" t="s">
+      <c r="P276" s="611" t="s">
         <v>263</v>
       </c>
-      <c r="R276" s="607" t="str">
+      <c r="R276" s="611" t="str">
         <f>"Ind AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="S276" s="607" t="str">
+      <c r="S276" s="611" t="str">
         <f>"Meas AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -29932,7 +30056,7 @@
         <v>13</v>
       </c>
       <c r="B277" s="349"/>
-      <c r="C277" s="605" t="str">
+      <c r="C277" s="596" t="str">
         <f>O116&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -29976,13 +30100,13 @@
         <f t="shared" si="52"/>
         <v>0</v>
       </c>
-      <c r="O277" s="606"/>
-      <c r="P277" s="607"/>
+      <c r="O277" s="610"/>
+      <c r="P277" s="611"/>
       <c r="Q277" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="R277" s="607"/>
-      <c r="S277" s="607"/>
+      <c r="R277" s="611"/>
+      <c r="S277" s="611"/>
       <c r="T277" s="1" t="s">
         <v>322</v>
       </c>
@@ -30017,7 +30141,7 @@
         <v>14</v>
       </c>
       <c r="B278" s="349"/>
-      <c r="C278" s="605"/>
+      <c r="C278" s="596"/>
       <c r="D278" s="447">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -30104,7 +30228,7 @@
         <v>15</v>
       </c>
       <c r="B279" s="349"/>
-      <c r="C279" s="605"/>
+      <c r="C279" s="596"/>
       <c r="D279" s="450">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -30198,7 +30322,7 @@
         <v>16</v>
       </c>
       <c r="B280" s="349"/>
-      <c r="C280" s="605" t="str">
+      <c r="C280" s="596" t="str">
         <f>O119&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -30288,7 +30412,7 @@
         <v>17</v>
       </c>
       <c r="B281" s="349"/>
-      <c r="C281" s="605"/>
+      <c r="C281" s="596"/>
       <c r="D281" s="447">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -30382,7 +30506,7 @@
         <v>18</v>
       </c>
       <c r="B282" s="349"/>
-      <c r="C282" s="605"/>
+      <c r="C282" s="596"/>
       <c r="D282" s="450">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -30469,7 +30593,7 @@
         <v>19</v>
       </c>
       <c r="B283" s="349"/>
-      <c r="C283" s="605" t="str">
+      <c r="C283" s="596" t="str">
         <f>O122&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -30566,7 +30690,7 @@
         <v>20</v>
       </c>
       <c r="B284" s="349"/>
-      <c r="C284" s="605"/>
+      <c r="C284" s="596"/>
       <c r="D284" s="447">
         <f t="shared" si="43"/>
         <v>20</v>
@@ -30653,7 +30777,7 @@
         <v>21</v>
       </c>
       <c r="B285" s="349"/>
-      <c r="C285" s="605"/>
+      <c r="C285" s="596"/>
       <c r="D285" s="447">
         <f t="shared" si="43"/>
         <v>30</v>
@@ -31084,12 +31208,12 @@
       <c r="L293" s="136"/>
       <c r="M293" s="351"/>
       <c r="O293" s="239"/>
-      <c r="P293" s="608" t="s">
+      <c r="P293" s="601" t="s">
         <v>328</v>
       </c>
-      <c r="Q293" s="608"/>
-      <c r="R293" s="608"/>
-      <c r="S293" s="608"/>
+      <c r="Q293" s="601"/>
+      <c r="R293" s="601"/>
+      <c r="S293" s="601"/>
       <c r="T293" s="237"/>
       <c r="U293" s="237"/>
       <c r="V293" s="237"/>
@@ -31473,12 +31597,12 @@
       <c r="L302" s="136"/>
       <c r="M302" s="351"/>
       <c r="O302" s="239"/>
-      <c r="P302" s="608" t="s">
+      <c r="P302" s="601" t="s">
         <v>328</v>
       </c>
-      <c r="Q302" s="608"/>
-      <c r="R302" s="608"/>
-      <c r="S302" s="608"/>
+      <c r="Q302" s="601"/>
+      <c r="R302" s="601"/>
+      <c r="S302" s="601"/>
       <c r="T302" s="237"/>
       <c r="U302" s="237"/>
       <c r="V302" s="237"/>
@@ -31493,7 +31617,7 @@
         <v>39</v>
       </c>
       <c r="B303" s="349"/>
-      <c r="C303" s="609" t="str">
+      <c r="C303" s="579" t="str">
         <f>O190</f>
         <v>Auto 1</v>
       </c>
@@ -31561,7 +31685,7 @@
         <v>40</v>
       </c>
       <c r="B304" s="349"/>
-      <c r="C304" s="610"/>
+      <c r="C304" s="580"/>
       <c r="D304" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31624,7 +31748,7 @@
         <v>41</v>
       </c>
       <c r="B305" s="349"/>
-      <c r="C305" s="610"/>
+      <c r="C305" s="580"/>
       <c r="D305" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31679,7 +31803,7 @@
         <v>42</v>
       </c>
       <c r="B306" s="349"/>
-      <c r="C306" s="610"/>
+      <c r="C306" s="580"/>
       <c r="D306" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31724,7 +31848,7 @@
         <v>43</v>
       </c>
       <c r="B307" s="349"/>
-      <c r="C307" s="611"/>
+      <c r="C307" s="602"/>
       <c r="D307" s="492" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31776,7 +31900,7 @@
         <v>44</v>
       </c>
       <c r="B308" s="349"/>
-      <c r="C308" s="609" t="str">
+      <c r="C308" s="579" t="str">
         <f>O195</f>
         <v>Auto 2</v>
       </c>
@@ -31824,7 +31948,7 @@
         <v>45</v>
       </c>
       <c r="B309" s="349"/>
-      <c r="C309" s="610"/>
+      <c r="C309" s="580"/>
       <c r="D309" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31881,7 +32005,7 @@
         <v>46</v>
       </c>
       <c r="B310" s="349"/>
-      <c r="C310" s="610"/>
+      <c r="C310" s="580"/>
       <c r="D310" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31931,7 +32055,7 @@
         <v>47</v>
       </c>
       <c r="B311" s="349"/>
-      <c r="C311" s="610"/>
+      <c r="C311" s="580"/>
       <c r="D311" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -31988,7 +32112,7 @@
         <v>48</v>
       </c>
       <c r="B312" s="349"/>
-      <c r="C312" s="612"/>
+      <c r="C312" s="581"/>
       <c r="D312" s="495" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -32038,7 +32162,7 @@
         <v>49</v>
       </c>
       <c r="B313" s="349"/>
-      <c r="C313" s="613" t="str">
+      <c r="C313" s="603" t="str">
         <f>O200</f>
         <v>High Level</v>
       </c>
@@ -32097,7 +32221,7 @@
         <v>50</v>
       </c>
       <c r="B314" s="349"/>
-      <c r="C314" s="610"/>
+      <c r="C314" s="580"/>
       <c r="D314" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -32140,7 +32264,7 @@
         <v>51</v>
       </c>
       <c r="B315" s="349"/>
-      <c r="C315" s="610"/>
+      <c r="C315" s="580"/>
       <c r="D315" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -32183,7 +32307,7 @@
         <v>52</v>
       </c>
       <c r="B316" s="349"/>
-      <c r="C316" s="610"/>
+      <c r="C316" s="580"/>
       <c r="D316" s="489" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -32228,7 +32352,7 @@
         <v>53</v>
       </c>
       <c r="B317" s="349"/>
-      <c r="C317" s="612"/>
+      <c r="C317" s="581"/>
       <c r="D317" s="495" t="str">
         <f t="shared" si="62"/>
         <v/>
@@ -32338,10 +32462,10 @@
       <c r="R319" s="278"/>
       <c r="S319" s="279"/>
       <c r="T319" s="279"/>
-      <c r="V319" s="590" t="s">
+      <c r="V319" s="604" t="s">
         <v>340</v>
       </c>
-      <c r="W319" s="590"/>
+      <c r="W319" s="604"/>
       <c r="X319" s="18" t="s">
         <v>341</v>
       </c>
@@ -32542,7 +32666,7 @@
         <v>60</v>
       </c>
       <c r="B324" s="349"/>
-      <c r="C324" s="614" t="str">
+      <c r="C324" s="585" t="str">
         <f>O240</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -32592,7 +32716,7 @@
         <v>61</v>
       </c>
       <c r="B325" s="349"/>
-      <c r="C325" s="615"/>
+      <c r="C325" s="586"/>
       <c r="D325" s="504" t="str">
         <f>P241</f>
         <v>Waist level</v>
@@ -32750,13 +32874,13 @@
         <v>348</v>
       </c>
       <c r="P329" s="54"/>
-      <c r="Q329" s="616" t="s">
+      <c r="Q329" s="605" t="s">
         <v>349</v>
       </c>
-      <c r="R329" s="616"/>
-      <c r="S329" s="616"/>
-      <c r="T329" s="616"/>
-      <c r="U329" s="616"/>
+      <c r="R329" s="605"/>
+      <c r="S329" s="605"/>
+      <c r="T329" s="605"/>
+      <c r="U329" s="605"/>
       <c r="Y329" s="15"/>
     </row>
     <row r="330" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -32921,24 +33045,24 @@
         <f t="shared" si="69"/>
         <v>Attenuator</v>
       </c>
-      <c r="E335" s="601" t="str">
+      <c r="E335" s="606" t="str">
         <f>Q139</f>
         <v>Auto 1</v>
       </c>
-      <c r="F335" s="602"/>
-      <c r="G335" s="602"/>
-      <c r="H335" s="602" t="str">
+      <c r="F335" s="607"/>
+      <c r="G335" s="607"/>
+      <c r="H335" s="607" t="str">
         <f>T139</f>
         <v>Auto 2</v>
       </c>
-      <c r="I335" s="602"/>
-      <c r="J335" s="602"/>
-      <c r="K335" s="603" t="str">
+      <c r="I335" s="607"/>
+      <c r="J335" s="607"/>
+      <c r="K335" s="608" t="str">
         <f>W139</f>
         <v>High Level</v>
       </c>
-      <c r="L335" s="603"/>
-      <c r="M335" s="604"/>
+      <c r="L335" s="608"/>
+      <c r="M335" s="609"/>
       <c r="O335" s="131"/>
       <c r="P335" s="130" t="s">
         <v>355</v>
@@ -33015,7 +33139,7 @@
         <v>7</v>
       </c>
       <c r="B337" s="349"/>
-      <c r="C337" s="605" t="str">
+      <c r="C337" s="596" t="str">
         <f>O142&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33075,7 +33199,7 @@
         <v>8</v>
       </c>
       <c r="B338" s="349"/>
-      <c r="C338" s="605"/>
+      <c r="C338" s="596"/>
       <c r="D338" s="518">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33132,7 +33256,7 @@
         <v>9</v>
       </c>
       <c r="B339" s="349"/>
-      <c r="C339" s="605"/>
+      <c r="C339" s="596"/>
       <c r="D339" s="519">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -33189,7 +33313,7 @@
         <v>10</v>
       </c>
       <c r="B340" s="349"/>
-      <c r="C340" s="605" t="str">
+      <c r="C340" s="596" t="str">
         <f>O145&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33249,7 +33373,7 @@
         <v>11</v>
       </c>
       <c r="B341" s="349"/>
-      <c r="C341" s="605"/>
+      <c r="C341" s="596"/>
       <c r="D341" s="518">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33306,7 +33430,7 @@
         <v>12</v>
       </c>
       <c r="B342" s="349"/>
-      <c r="C342" s="605"/>
+      <c r="C342" s="596"/>
       <c r="D342" s="520">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -33363,7 +33487,7 @@
         <v>13</v>
       </c>
       <c r="B343" s="349"/>
-      <c r="C343" s="605" t="str">
+      <c r="C343" s="596" t="str">
         <f>O148&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33415,7 +33539,7 @@
         <v>14</v>
       </c>
       <c r="B344" s="349"/>
-      <c r="C344" s="605"/>
+      <c r="C344" s="596"/>
       <c r="D344" s="518">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33477,7 +33601,7 @@
         <v>15</v>
       </c>
       <c r="B345" s="349"/>
-      <c r="C345" s="605"/>
+      <c r="C345" s="596"/>
       <c r="D345" s="519">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -33540,7 +33664,7 @@
         <v>16</v>
       </c>
       <c r="B346" s="349"/>
-      <c r="C346" s="605" t="str">
+      <c r="C346" s="596" t="str">
         <f>O151&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33603,7 +33727,7 @@
         <v>17</v>
       </c>
       <c r="B347" s="349"/>
-      <c r="C347" s="605"/>
+      <c r="C347" s="596"/>
       <c r="D347" s="518">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33661,7 +33785,7 @@
         <v>18</v>
       </c>
       <c r="B348" s="349"/>
-      <c r="C348" s="605"/>
+      <c r="C348" s="596"/>
       <c r="D348" s="520">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -33739,7 +33863,7 @@
         <v>19</v>
       </c>
       <c r="B349" s="349"/>
-      <c r="C349" s="605" t="str">
+      <c r="C349" s="596" t="str">
         <f>O154&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33802,7 +33926,7 @@
         <v>20</v>
       </c>
       <c r="B350" s="349"/>
-      <c r="C350" s="605"/>
+      <c r="C350" s="596"/>
       <c r="D350" s="518">
         <f t="shared" si="70"/>
         <v>20</v>
@@ -33861,7 +33985,7 @@
         <v>21</v>
       </c>
       <c r="B351" s="349"/>
-      <c r="C351" s="605"/>
+      <c r="C351" s="596"/>
       <c r="D351" s="520">
         <f t="shared" si="70"/>
         <v>30</v>
@@ -34170,11 +34294,11 @@
         <f>IF(OR(V358="",V359="",V362=""),"",(V358-V359)*V362)</f>
         <v/>
       </c>
-      <c r="Q358" s="617" t="str">
+      <c r="Q358" s="597" t="str">
         <f>IF(OR(P358="",P359=""),"",(ABS(P358)+ABS(P359))/$O$355)</f>
         <v/>
       </c>
-      <c r="R358" s="618" t="str">
+      <c r="R358" s="598" t="str">
         <f>IF(OR(Q358="",Q360=""),"",Q358+Q360)</f>
         <v/>
       </c>
@@ -34213,8 +34337,8 @@
         <f>IF(OR(W358="",W359="",V362=""),"",(W358-W359)*V362)</f>
         <v/>
       </c>
-      <c r="Q359" s="617"/>
-      <c r="R359" s="617"/>
+      <c r="Q359" s="597"/>
+      <c r="R359" s="597"/>
       <c r="S359" s="147" t="str">
         <f>IF(AB168="","",AB168)</f>
         <v/>
@@ -34250,11 +34374,11 @@
         <f>IF(OR(X358="",X359="",V362=""),"",(X358-X359)*V362)</f>
         <v/>
       </c>
-      <c r="Q360" s="618" t="str">
+      <c r="Q360" s="598" t="str">
         <f>IF(OR(P360="",P361=""),"",(ABS(P360)+ABS(P361))/$O$355)</f>
         <v/>
       </c>
-      <c r="R360" s="618"/>
+      <c r="R360" s="598"/>
       <c r="S360" s="147" t="str">
         <f>IF(AB169="","",AB169)</f>
         <v/>
@@ -34296,8 +34420,8 @@
         <f>IF(OR(Y358="",Y359="",V362=""),"",(Y358-Y359)*V362)</f>
         <v/>
       </c>
-      <c r="Q361" s="618"/>
-      <c r="R361" s="618"/>
+      <c r="Q361" s="598"/>
+      <c r="R361" s="598"/>
       <c r="S361" s="149" t="str">
         <f>IF(AB170="","",AB170)</f>
         <v/>
@@ -34469,7 +34593,7 @@
         <v>36</v>
       </c>
       <c r="B366" s="349"/>
-      <c r="C366" s="619" t="str">
+      <c r="C366" s="599" t="str">
         <f>O214</f>
         <v>Auto 1</v>
       </c>
@@ -34520,7 +34644,7 @@
         <v>37</v>
       </c>
       <c r="B367" s="349"/>
-      <c r="C367" s="620"/>
+      <c r="C367" s="600"/>
       <c r="D367" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34566,7 +34690,7 @@
         <v>38</v>
       </c>
       <c r="B368" s="349"/>
-      <c r="C368" s="620"/>
+      <c r="C368" s="600"/>
       <c r="D368" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34601,7 +34725,7 @@
         <v>39</v>
       </c>
       <c r="B369" s="349"/>
-      <c r="C369" s="620"/>
+      <c r="C369" s="600"/>
       <c r="D369" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34636,7 +34760,7 @@
         <v>40</v>
       </c>
       <c r="B370" s="349"/>
-      <c r="C370" s="620"/>
+      <c r="C370" s="600"/>
       <c r="D370" s="495" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34681,7 +34805,7 @@
         <v>41</v>
       </c>
       <c r="B371" s="349"/>
-      <c r="C371" s="609" t="str">
+      <c r="C371" s="579" t="str">
         <f>O219</f>
         <v>Auto 2</v>
       </c>
@@ -34731,7 +34855,7 @@
         <v>42</v>
       </c>
       <c r="B372" s="349"/>
-      <c r="C372" s="610"/>
+      <c r="C372" s="580"/>
       <c r="D372" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34781,7 +34905,7 @@
         <v>43</v>
       </c>
       <c r="B373" s="349"/>
-      <c r="C373" s="610"/>
+      <c r="C373" s="580"/>
       <c r="D373" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34828,7 +34952,7 @@
         <v>44</v>
       </c>
       <c r="B374" s="349"/>
-      <c r="C374" s="610"/>
+      <c r="C374" s="580"/>
       <c r="D374" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34878,7 +35002,7 @@
         <v>45</v>
       </c>
       <c r="B375" s="349"/>
-      <c r="C375" s="612"/>
+      <c r="C375" s="581"/>
       <c r="D375" s="495" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -34925,7 +35049,7 @@
         <v>46</v>
       </c>
       <c r="B376" s="349"/>
-      <c r="C376" s="621" t="str">
+      <c r="C376" s="582" t="str">
         <f>O224</f>
         <v>High Level</v>
       </c>
@@ -34978,7 +35102,7 @@
         <v>47</v>
       </c>
       <c r="B377" s="349"/>
-      <c r="C377" s="622"/>
+      <c r="C377" s="583"/>
       <c r="D377" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -35025,7 +35149,7 @@
         <v>48</v>
       </c>
       <c r="B378" s="349"/>
-      <c r="C378" s="622"/>
+      <c r="C378" s="583"/>
       <c r="D378" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -35075,7 +35199,7 @@
         <v>49</v>
       </c>
       <c r="B379" s="349"/>
-      <c r="C379" s="622"/>
+      <c r="C379" s="583"/>
       <c r="D379" s="489" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -35122,7 +35246,7 @@
         <v>50</v>
       </c>
       <c r="B380" s="349"/>
-      <c r="C380" s="623"/>
+      <c r="C380" s="584"/>
       <c r="D380" s="495" t="str">
         <f t="shared" si="80"/>
         <v/>
@@ -35432,7 +35556,7 @@
         <v>58</v>
       </c>
       <c r="B388" s="349"/>
-      <c r="C388" s="614" t="str">
+      <c r="C388" s="585" t="str">
         <f>O242</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -35483,7 +35607,7 @@
         <v>59</v>
       </c>
       <c r="B389" s="349"/>
-      <c r="C389" s="615"/>
+      <c r="C389" s="586"/>
       <c r="D389" s="504" t="str">
         <f>P243</f>
         <v>Waist level</v>
@@ -35834,14 +35958,14 @@
       <c r="E399" s="347"/>
       <c r="F399" s="347"/>
       <c r="G399" s="347"/>
-      <c r="H399" s="624" t="s">
+      <c r="H399" s="587" t="s">
         <v>395</v>
       </c>
-      <c r="I399" s="624"/>
-      <c r="J399" s="624" t="s">
+      <c r="I399" s="587"/>
+      <c r="J399" s="587" t="s">
         <v>396</v>
       </c>
-      <c r="K399" s="624"/>
+      <c r="K399" s="587"/>
       <c r="L399" s="347"/>
       <c r="M399" s="348"/>
       <c r="O399" s="14"/>
@@ -36415,20 +36539,20 @@
       </c>
       <c r="B413" s="349"/>
       <c r="C413" s="43"/>
-      <c r="D413" s="625" t="s">
+      <c r="D413" s="588" t="s">
         <v>402</v>
       </c>
-      <c r="E413" s="625"/>
-      <c r="F413" s="625"/>
-      <c r="G413" s="625"/>
-      <c r="H413" s="625"/>
-      <c r="I413" s="625" t="s">
+      <c r="E413" s="588"/>
+      <c r="F413" s="588"/>
+      <c r="G413" s="588"/>
+      <c r="H413" s="588"/>
+      <c r="I413" s="588" t="s">
         <v>403</v>
       </c>
-      <c r="J413" s="625"/>
-      <c r="K413" s="625"/>
-      <c r="L413" s="625"/>
-      <c r="M413" s="626"/>
+      <c r="J413" s="588"/>
+      <c r="K413" s="588"/>
+      <c r="L413" s="588"/>
+      <c r="M413" s="589"/>
       <c r="O413" s="14"/>
       <c r="P413" s="2" t="s">
         <v>189</v>
@@ -37908,11 +38032,11 @@
         <f t="shared" si="92"/>
         <v/>
       </c>
-      <c r="F442" s="627" t="str">
+      <c r="F442" s="590" t="str">
         <f t="shared" si="92"/>
         <v/>
       </c>
-      <c r="G442" s="629" t="str">
+      <c r="G442" s="592" t="str">
         <f t="shared" si="92"/>
         <v/>
       </c>
@@ -37953,8 +38077,8 @@
         <f>P359</f>
         <v/>
       </c>
-      <c r="F443" s="628"/>
-      <c r="G443" s="630"/>
+      <c r="F443" s="591"/>
+      <c r="G443" s="593"/>
       <c r="H443" s="205"/>
       <c r="I443" s="83" t="str">
         <f>T360</f>
@@ -37994,11 +38118,11 @@
         <f>P360</f>
         <v/>
       </c>
-      <c r="F444" s="628" t="str">
+      <c r="F444" s="591" t="str">
         <f>Q360</f>
         <v/>
       </c>
-      <c r="G444" s="630"/>
+      <c r="G444" s="593"/>
       <c r="H444" s="136"/>
       <c r="I444" s="92" t="str">
         <f>T361</f>
@@ -38039,8 +38163,8 @@
         <f>P361</f>
         <v/>
       </c>
-      <c r="F445" s="632"/>
-      <c r="G445" s="631"/>
+      <c r="F445" s="595"/>
+      <c r="G445" s="594"/>
       <c r="H445" s="136"/>
       <c r="I445" s="136"/>
       <c r="J445" s="136"/>
@@ -44376,25 +44500,84 @@
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="C371:C375"/>
-    <mergeCell ref="C376:C380"/>
-    <mergeCell ref="C388:C389"/>
-    <mergeCell ref="H399:I399"/>
-    <mergeCell ref="J399:K399"/>
-    <mergeCell ref="D413:H413"/>
-    <mergeCell ref="I413:M413"/>
-    <mergeCell ref="F442:F443"/>
-    <mergeCell ref="G442:G445"/>
-    <mergeCell ref="F444:F445"/>
-    <mergeCell ref="C337:C339"/>
-    <mergeCell ref="C340:C342"/>
-    <mergeCell ref="C343:C345"/>
-    <mergeCell ref="C346:C348"/>
-    <mergeCell ref="C349:C351"/>
-    <mergeCell ref="Q358:Q359"/>
-    <mergeCell ref="R358:R361"/>
-    <mergeCell ref="Q360:Q361"/>
-    <mergeCell ref="C366:C370"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="Q107:S107"/>
+    <mergeCell ref="T107:V107"/>
+    <mergeCell ref="W107:Y107"/>
+    <mergeCell ref="Q139:S139"/>
+    <mergeCell ref="T139:V139"/>
+    <mergeCell ref="W139:Y139"/>
+    <mergeCell ref="T181:U181"/>
+    <mergeCell ref="O190:O194"/>
+    <mergeCell ref="O195:O199"/>
+    <mergeCell ref="O200:O204"/>
+    <mergeCell ref="E202:E203"/>
+    <mergeCell ref="F202:F203"/>
+    <mergeCell ref="G202:G203"/>
+    <mergeCell ref="H202:H203"/>
+    <mergeCell ref="I202:I203"/>
+    <mergeCell ref="J202:J203"/>
+    <mergeCell ref="M202:M203"/>
+    <mergeCell ref="O214:O218"/>
+    <mergeCell ref="O219:O223"/>
+    <mergeCell ref="O224:O228"/>
+    <mergeCell ref="O240:O241"/>
+    <mergeCell ref="O242:O243"/>
+    <mergeCell ref="Q257:R257"/>
+    <mergeCell ref="T257:U257"/>
+    <mergeCell ref="E269:G269"/>
+    <mergeCell ref="H269:J269"/>
+    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="C271:C273"/>
+    <mergeCell ref="C274:C276"/>
+    <mergeCell ref="O276:O277"/>
+    <mergeCell ref="P276:P277"/>
+    <mergeCell ref="R276:R277"/>
+    <mergeCell ref="S276:S277"/>
+    <mergeCell ref="C277:C279"/>
+    <mergeCell ref="C280:C282"/>
+    <mergeCell ref="C283:C285"/>
     <mergeCell ref="P293:S293"/>
     <mergeCell ref="P302:S302"/>
     <mergeCell ref="C303:C307"/>
@@ -44406,84 +44589,25 @@
     <mergeCell ref="E335:G335"/>
     <mergeCell ref="H335:J335"/>
     <mergeCell ref="K335:M335"/>
-    <mergeCell ref="C271:C273"/>
-    <mergeCell ref="C274:C276"/>
-    <mergeCell ref="O276:O277"/>
-    <mergeCell ref="P276:P277"/>
-    <mergeCell ref="R276:R277"/>
-    <mergeCell ref="S276:S277"/>
-    <mergeCell ref="C277:C279"/>
-    <mergeCell ref="C280:C282"/>
-    <mergeCell ref="C283:C285"/>
-    <mergeCell ref="O214:O218"/>
-    <mergeCell ref="O219:O223"/>
-    <mergeCell ref="O224:O228"/>
-    <mergeCell ref="O240:O241"/>
-    <mergeCell ref="O242:O243"/>
-    <mergeCell ref="Q257:R257"/>
-    <mergeCell ref="T257:U257"/>
-    <mergeCell ref="E269:G269"/>
-    <mergeCell ref="H269:J269"/>
-    <mergeCell ref="K269:M269"/>
-    <mergeCell ref="T181:U181"/>
-    <mergeCell ref="O190:O194"/>
-    <mergeCell ref="O195:O199"/>
-    <mergeCell ref="O200:O204"/>
-    <mergeCell ref="E202:E203"/>
-    <mergeCell ref="F202:F203"/>
-    <mergeCell ref="G202:G203"/>
-    <mergeCell ref="H202:H203"/>
-    <mergeCell ref="I202:I203"/>
-    <mergeCell ref="J202:J203"/>
-    <mergeCell ref="M202:M203"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="Q107:S107"/>
-    <mergeCell ref="T107:V107"/>
-    <mergeCell ref="W107:Y107"/>
-    <mergeCell ref="Q139:S139"/>
-    <mergeCell ref="T139:V139"/>
-    <mergeCell ref="W139:Y139"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C337:C339"/>
+    <mergeCell ref="C340:C342"/>
+    <mergeCell ref="C343:C345"/>
+    <mergeCell ref="C346:C348"/>
+    <mergeCell ref="C349:C351"/>
+    <mergeCell ref="Q358:Q359"/>
+    <mergeCell ref="R358:R361"/>
+    <mergeCell ref="Q360:Q361"/>
+    <mergeCell ref="C366:C370"/>
+    <mergeCell ref="C371:C375"/>
+    <mergeCell ref="C376:C380"/>
+    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="H399:I399"/>
+    <mergeCell ref="J399:K399"/>
+    <mergeCell ref="D413:H413"/>
+    <mergeCell ref="I413:M413"/>
+    <mergeCell ref="F442:F443"/>
+    <mergeCell ref="G442:G445"/>
+    <mergeCell ref="F444:F445"/>
   </mergeCells>
   <conditionalFormatting sqref="S126 V126 Y126 S158 V158 Y158">
     <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
@@ -44750,39 +44874,39 @@
         <f>Fluoro!D269</f>
         <v>Attenuator</v>
       </c>
-      <c r="E5" s="602" t="str">
+      <c r="E5" s="607" t="str">
         <f>Fluoro!E269</f>
         <v>Auto 1</v>
       </c>
-      <c r="F5" s="602">
+      <c r="F5" s="607">
         <f>Fluoro!F269</f>
         <v>0</v>
       </c>
-      <c r="G5" s="602">
+      <c r="G5" s="607">
         <f>Fluoro!G269</f>
         <v>0</v>
       </c>
-      <c r="H5" s="602" t="str">
+      <c r="H5" s="607" t="str">
         <f>Fluoro!H269</f>
         <v>Auto 2</v>
       </c>
-      <c r="I5" s="602">
+      <c r="I5" s="607">
         <f>Fluoro!I269</f>
         <v>0</v>
       </c>
-      <c r="J5" s="602">
+      <c r="J5" s="607">
         <f>Fluoro!J269</f>
         <v>0</v>
       </c>
-      <c r="K5" s="603" t="str">
+      <c r="K5" s="608" t="str">
         <f>Fluoro!K269</f>
         <v>High Level</v>
       </c>
-      <c r="L5" s="603">
+      <c r="L5" s="608">
         <f>Fluoro!L269</f>
         <v>0</v>
       </c>
-      <c r="M5" s="603">
+      <c r="M5" s="608">
         <f>Fluoro!M269</f>
         <v>0</v>
       </c>
@@ -44839,7 +44963,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="633" t="str">
+      <c r="C7" s="636" t="str">
         <f>Fluoro!C271</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -44889,7 +45013,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="633">
+      <c r="C8" s="636">
         <f>Fluoro!C272</f>
         <v>0</v>
       </c>
@@ -44939,7 +45063,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="633">
+      <c r="C9" s="636">
         <f>Fluoro!C273</f>
         <v>0</v>
       </c>
@@ -44989,7 +45113,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="633" t="str">
+      <c r="C10" s="636" t="str">
         <f>Fluoro!C274</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -45039,7 +45163,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="633">
+      <c r="C11" s="636">
         <f>Fluoro!C275</f>
         <v>0</v>
       </c>
@@ -45089,7 +45213,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="633">
+      <c r="C12" s="636">
         <f>Fluoro!C276</f>
         <v>0</v>
       </c>
@@ -45139,7 +45263,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="633" t="str">
+      <c r="C13" s="636" t="str">
         <f>Fluoro!C277</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -45189,7 +45313,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="633">
+      <c r="C14" s="636">
         <f>Fluoro!C278</f>
         <v>0</v>
       </c>
@@ -45239,7 +45363,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="633">
+      <c r="C15" s="636">
         <f>Fluoro!C279</f>
         <v>0</v>
       </c>
@@ -45289,7 +45413,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="633" t="str">
+      <c r="C16" s="636" t="str">
         <f>Fluoro!C280</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -45339,7 +45463,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="633">
+      <c r="C17" s="636">
         <f>Fluoro!C281</f>
         <v>0</v>
       </c>
@@ -45389,7 +45513,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="11"/>
-      <c r="C18" s="633">
+      <c r="C18" s="636">
         <f>Fluoro!C282</f>
         <v>0</v>
       </c>
@@ -45439,7 +45563,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="11"/>
-      <c r="C19" s="633" t="str">
+      <c r="C19" s="636" t="str">
         <f>Fluoro!C283</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -45489,7 +45613,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="633">
+      <c r="C20" s="636">
         <f>Fluoro!C284</f>
         <v>0</v>
       </c>
@@ -45539,7 +45663,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="633">
+      <c r="C21" s="636">
         <f>Fluoro!C285</f>
         <v>0</v>
       </c>
@@ -45988,7 +46112,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="634" t="str">
+      <c r="C39" s="633" t="str">
         <f>Fluoro!C303</f>
         <v>Auto 1</v>
       </c>
@@ -46026,7 +46150,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="11"/>
-      <c r="C40" s="634">
+      <c r="C40" s="633">
         <f>Fluoro!C304</f>
         <v>0</v>
       </c>
@@ -46064,7 +46188,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="11"/>
-      <c r="C41" s="634">
+      <c r="C41" s="633">
         <f>Fluoro!C305</f>
         <v>0</v>
       </c>
@@ -46102,7 +46226,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="634">
+      <c r="C42" s="633">
         <f>Fluoro!C306</f>
         <v>0</v>
       </c>
@@ -46137,7 +46261,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="634">
+      <c r="C43" s="633">
         <f>Fluoro!C307</f>
         <v>0</v>
       </c>
@@ -46172,7 +46296,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="11"/>
-      <c r="C44" s="635" t="str">
+      <c r="C44" s="634" t="str">
         <f>Fluoro!C308</f>
         <v>Auto 2</v>
       </c>
@@ -46207,7 +46331,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="11"/>
-      <c r="C45" s="635">
+      <c r="C45" s="634">
         <f>Fluoro!C309</f>
         <v>0</v>
       </c>
@@ -46242,7 +46366,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="11"/>
-      <c r="C46" s="635">
+      <c r="C46" s="634">
         <f>Fluoro!C310</f>
         <v>0</v>
       </c>
@@ -46277,7 +46401,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="635">
+      <c r="C47" s="634">
         <f>Fluoro!C311</f>
         <v>0</v>
       </c>
@@ -46312,7 +46436,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="11"/>
-      <c r="C48" s="635">
+      <c r="C48" s="634">
         <f>Fluoro!C312</f>
         <v>0</v>
       </c>
@@ -46347,7 +46471,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="11"/>
-      <c r="C49" s="635" t="str">
+      <c r="C49" s="634" t="str">
         <f>Fluoro!C313</f>
         <v>High Level</v>
       </c>
@@ -46382,7 +46506,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="11"/>
-      <c r="C50" s="635">
+      <c r="C50" s="634">
         <f>Fluoro!C314</f>
         <v>0</v>
       </c>
@@ -46417,7 +46541,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="11"/>
-      <c r="C51" s="635">
+      <c r="C51" s="634">
         <f>Fluoro!C315</f>
         <v>0</v>
       </c>
@@ -46448,7 +46572,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="11"/>
-      <c r="C52" s="635">
+      <c r="C52" s="634">
         <f>Fluoro!C316</f>
         <v>0</v>
       </c>
@@ -46479,7 +46603,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="11"/>
-      <c r="C53" s="635">
+      <c r="C53" s="634">
         <f>Fluoro!C317</f>
         <v>0</v>
       </c>
@@ -46665,7 +46789,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="11"/>
-      <c r="C60" s="636" t="str">
+      <c r="C60" s="635" t="str">
         <f>Fluoro!C324</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -46700,7 +46824,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="11"/>
-      <c r="C61" s="636">
+      <c r="C61" s="635">
         <f>Fluoro!C325</f>
         <v>0</v>
       </c>
@@ -46946,39 +47070,39 @@
         <f>Fluoro!D335</f>
         <v>Attenuator</v>
       </c>
-      <c r="E71" s="602" t="str">
+      <c r="E71" s="607" t="str">
         <f>Fluoro!E335</f>
         <v>Auto 1</v>
       </c>
-      <c r="F71" s="602">
+      <c r="F71" s="607">
         <f>Fluoro!F335</f>
         <v>0</v>
       </c>
-      <c r="G71" s="602">
+      <c r="G71" s="607">
         <f>Fluoro!G335</f>
         <v>0</v>
       </c>
-      <c r="H71" s="602" t="str">
+      <c r="H71" s="607" t="str">
         <f>Fluoro!H335</f>
         <v>Auto 2</v>
       </c>
-      <c r="I71" s="602">
+      <c r="I71" s="607">
         <f>Fluoro!I335</f>
         <v>0</v>
       </c>
-      <c r="J71" s="602">
+      <c r="J71" s="607">
         <f>Fluoro!J335</f>
         <v>0</v>
       </c>
-      <c r="K71" s="603" t="str">
+      <c r="K71" s="608" t="str">
         <f>Fluoro!K335</f>
         <v>High Level</v>
       </c>
-      <c r="L71" s="603">
+      <c r="L71" s="608">
         <f>Fluoro!L335</f>
         <v>0</v>
       </c>
-      <c r="M71" s="603">
+      <c r="M71" s="608">
         <f>Fluoro!M335</f>
         <v>0</v>
       </c>
@@ -47035,7 +47159,7 @@
         <v>7</v>
       </c>
       <c r="B73" s="11"/>
-      <c r="C73" s="633" t="str">
+      <c r="C73" s="636" t="str">
         <f>Fluoro!C337</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -47085,7 +47209,7 @@
         <v>8</v>
       </c>
       <c r="B74" s="11"/>
-      <c r="C74" s="633">
+      <c r="C74" s="636">
         <f>Fluoro!C338</f>
         <v>0</v>
       </c>
@@ -47135,7 +47259,7 @@
         <v>9</v>
       </c>
       <c r="B75" s="11"/>
-      <c r="C75" s="633">
+      <c r="C75" s="636">
         <f>Fluoro!C339</f>
         <v>0</v>
       </c>
@@ -47185,7 +47309,7 @@
         <v>10</v>
       </c>
       <c r="B76" s="11"/>
-      <c r="C76" s="633" t="str">
+      <c r="C76" s="636" t="str">
         <f>Fluoro!C340</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -47235,7 +47359,7 @@
         <v>11</v>
       </c>
       <c r="B77" s="11"/>
-      <c r="C77" s="633">
+      <c r="C77" s="636">
         <f>Fluoro!C341</f>
         <v>0</v>
       </c>
@@ -47285,7 +47409,7 @@
         <v>12</v>
       </c>
       <c r="B78" s="11"/>
-      <c r="C78" s="633">
+      <c r="C78" s="636">
         <f>Fluoro!C342</f>
         <v>0</v>
       </c>
@@ -47335,7 +47459,7 @@
         <v>13</v>
       </c>
       <c r="B79" s="11"/>
-      <c r="C79" s="633" t="str">
+      <c r="C79" s="636" t="str">
         <f>Fluoro!C343</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -47385,7 +47509,7 @@
         <v>14</v>
       </c>
       <c r="B80" s="11"/>
-      <c r="C80" s="633">
+      <c r="C80" s="636">
         <f>Fluoro!C344</f>
         <v>0</v>
       </c>
@@ -47435,7 +47559,7 @@
         <v>15</v>
       </c>
       <c r="B81" s="11"/>
-      <c r="C81" s="633">
+      <c r="C81" s="636">
         <f>Fluoro!C345</f>
         <v>0</v>
       </c>
@@ -47485,7 +47609,7 @@
         <v>16</v>
       </c>
       <c r="B82" s="11"/>
-      <c r="C82" s="633" t="str">
+      <c r="C82" s="636" t="str">
         <f>Fluoro!C346</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -47535,7 +47659,7 @@
         <v>17</v>
       </c>
       <c r="B83" s="11"/>
-      <c r="C83" s="633">
+      <c r="C83" s="636">
         <f>Fluoro!C347</f>
         <v>0</v>
       </c>
@@ -47585,7 +47709,7 @@
         <v>18</v>
       </c>
       <c r="B84" s="11"/>
-      <c r="C84" s="633">
+      <c r="C84" s="636">
         <f>Fluoro!C348</f>
         <v>0</v>
       </c>
@@ -47635,7 +47759,7 @@
         <v>19</v>
       </c>
       <c r="B85" s="11"/>
-      <c r="C85" s="633" t="str">
+      <c r="C85" s="636" t="str">
         <f>Fluoro!C349</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -47685,7 +47809,7 @@
         <v>20</v>
       </c>
       <c r="B86" s="11"/>
-      <c r="C86" s="633">
+      <c r="C86" s="636">
         <f>Fluoro!C350</f>
         <v>0</v>
       </c>
@@ -47735,7 +47859,7 @@
         <v>21</v>
       </c>
       <c r="B87" s="11"/>
-      <c r="C87" s="633">
+      <c r="C87" s="636">
         <f>Fluoro!C351</f>
         <v>0</v>
       </c>
@@ -48082,7 +48206,7 @@
         <v>36</v>
       </c>
       <c r="B102" s="11"/>
-      <c r="C102" s="634" t="str">
+      <c r="C102" s="633" t="str">
         <f>Fluoro!C366</f>
         <v>Auto 1</v>
       </c>
@@ -48120,7 +48244,7 @@
         <v>37</v>
       </c>
       <c r="B103" s="11"/>
-      <c r="C103" s="634">
+      <c r="C103" s="633">
         <f>Fluoro!C367</f>
         <v>0</v>
       </c>
@@ -48158,7 +48282,7 @@
         <v>38</v>
       </c>
       <c r="B104" s="11"/>
-      <c r="C104" s="634">
+      <c r="C104" s="633">
         <f>Fluoro!C368</f>
         <v>0</v>
       </c>
@@ -48196,7 +48320,7 @@
         <v>39</v>
       </c>
       <c r="B105" s="11"/>
-      <c r="C105" s="634">
+      <c r="C105" s="633">
         <f>Fluoro!C369</f>
         <v>0</v>
       </c>
@@ -48231,7 +48355,7 @@
         <v>40</v>
       </c>
       <c r="B106" s="11"/>
-      <c r="C106" s="634">
+      <c r="C106" s="633">
         <f>Fluoro!C370</f>
         <v>0</v>
       </c>
@@ -48266,7 +48390,7 @@
         <v>41</v>
       </c>
       <c r="B107" s="11"/>
-      <c r="C107" s="635" t="str">
+      <c r="C107" s="634" t="str">
         <f>Fluoro!C371</f>
         <v>Auto 2</v>
       </c>
@@ -48301,7 +48425,7 @@
         <v>42</v>
       </c>
       <c r="B108" s="11"/>
-      <c r="C108" s="635">
+      <c r="C108" s="634">
         <f>Fluoro!C372</f>
         <v>0</v>
       </c>
@@ -48336,7 +48460,7 @@
         <v>43</v>
       </c>
       <c r="B109" s="11"/>
-      <c r="C109" s="635">
+      <c r="C109" s="634">
         <f>Fluoro!C373</f>
         <v>0</v>
       </c>
@@ -48371,7 +48495,7 @@
         <v>44</v>
       </c>
       <c r="B110" s="11"/>
-      <c r="C110" s="635">
+      <c r="C110" s="634">
         <f>Fluoro!C374</f>
         <v>0</v>
       </c>
@@ -48406,7 +48530,7 @@
         <v>45</v>
       </c>
       <c r="B111" s="11"/>
-      <c r="C111" s="635">
+      <c r="C111" s="634">
         <f>Fluoro!C375</f>
         <v>0</v>
       </c>
@@ -48441,7 +48565,7 @@
         <v>46</v>
       </c>
       <c r="B112" s="11"/>
-      <c r="C112" s="635" t="str">
+      <c r="C112" s="634" t="str">
         <f>Fluoro!C376</f>
         <v>High Level</v>
       </c>
@@ -48476,7 +48600,7 @@
         <v>47</v>
       </c>
       <c r="B113" s="11"/>
-      <c r="C113" s="635">
+      <c r="C113" s="634">
         <f>Fluoro!C377</f>
         <v>0</v>
       </c>
@@ -48511,7 +48635,7 @@
         <v>48</v>
       </c>
       <c r="B114" s="11"/>
-      <c r="C114" s="635">
+      <c r="C114" s="634">
         <f>Fluoro!C378</f>
         <v>0</v>
       </c>
@@ -48542,7 +48666,7 @@
         <v>49</v>
       </c>
       <c r="B115" s="11"/>
-      <c r="C115" s="635">
+      <c r="C115" s="634">
         <f>Fluoro!C379</f>
         <v>0</v>
       </c>
@@ -48573,7 +48697,7 @@
         <v>50</v>
       </c>
       <c r="B116" s="11"/>
-      <c r="C116" s="635">
+      <c r="C116" s="634">
         <f>Fluoro!C380</f>
         <v>0</v>
       </c>
@@ -48747,7 +48871,7 @@
         <v>58</v>
       </c>
       <c r="B124" s="11"/>
-      <c r="C124" s="636" t="str">
+      <c r="C124" s="635" t="str">
         <f>Fluoro!C388</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -48782,7 +48906,7 @@
         <v>59</v>
       </c>
       <c r="B125" s="11"/>
-      <c r="C125" s="636">
+      <c r="C125" s="635">
         <f>Fluoro!C389</f>
         <v>0</v>
       </c>
@@ -48959,6 +49083,21 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="H71:J71"/>
+    <mergeCell ref="K71:M71"/>
     <mergeCell ref="C102:C106"/>
     <mergeCell ref="C107:C111"/>
     <mergeCell ref="C112:C116"/>
@@ -48968,21 +49107,6 @@
     <mergeCell ref="C79:C81"/>
     <mergeCell ref="C82:C84"/>
     <mergeCell ref="C85:C87"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="H71:J71"/>
-    <mergeCell ref="K71:M71"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="68" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -49014,29 +49138,29 @@
       </c>
       <c r="B1" s="637"/>
       <c r="N1" s="326"/>
-      <c r="O1" s="608" t="str">
+      <c r="O1" s="601" t="str">
         <f>Fluoro!O105</f>
         <v>Patient Entrance Exposure Rate (Fluoroscopy)*</v>
       </c>
-      <c r="P1" s="608"/>
-      <c r="Q1" s="608"/>
-      <c r="R1" s="608" t="s">
+      <c r="P1" s="601"/>
+      <c r="Q1" s="601"/>
+      <c r="R1" s="601" t="s">
         <v>409</v>
       </c>
-      <c r="S1" s="608"/>
-      <c r="T1" s="608"/>
+      <c r="S1" s="601"/>
+      <c r="T1" s="601"/>
       <c r="V1" s="326"/>
-      <c r="W1" s="608" t="str">
+      <c r="W1" s="601" t="str">
         <f>Fluoro!O137</f>
         <v>Patient Entrance Exposure Rate – Digital Acquisition</v>
       </c>
-      <c r="X1" s="608"/>
-      <c r="Y1" s="608"/>
-      <c r="Z1" s="608" t="s">
+      <c r="X1" s="601"/>
+      <c r="Y1" s="601"/>
+      <c r="Z1" s="601" t="s">
         <v>409</v>
       </c>
-      <c r="AA1" s="608"/>
-      <c r="AB1" s="608"/>
+      <c r="AA1" s="601"/>
+      <c r="AB1" s="601"/>
     </row>
     <row r="2" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="327">
@@ -53029,14 +53153,14 @@
       <c r="B75" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="E75" s="608" t="s">
+      <c r="E75" s="601" t="s">
         <v>422</v>
       </c>
-      <c r="F75" s="608"/>
-      <c r="I75" s="608" t="s">
+      <c r="F75" s="601"/>
+      <c r="I75" s="601" t="s">
         <v>423</v>
       </c>
-      <c r="J75" s="608"/>
+      <c r="J75" s="601"/>
     </row>
     <row r="76" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
@@ -54756,7 +54880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix CAK ref point correction factor
</commit_message>
<xml_diff>
--- a/MUSCCArm.xlsx
+++ b/MUSCCArm.xlsx
@@ -6359,6 +6359,135 @@
     <xf numFmtId="172" fontId="4" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="127" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="155" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="182" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="149" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="150" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="175" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="151" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="176" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="154" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="180" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="122" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="123" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="124" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6383,15 +6512,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="149" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="150" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="151" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="183" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6401,133 +6521,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="193" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="127" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="154" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="180" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="122" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="123" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="124" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="155" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="182" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="175" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="176" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7028,7 +7028,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7206,7 +7205,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7278,7 +7276,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -19329,6 +19326,150 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2064" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2065" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2066" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -19597,8 +19738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD792"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" topLeftCell="N239" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O255" sqref="O255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -19909,21 +20050,21 @@
       <c r="E10" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="628" t="str">
+      <c r="F10" s="577" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="628"/>
+      <c r="G10" s="577"/>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
       <c r="J10" s="160" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="621" t="str">
+      <c r="K10" s="578" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="621"/>
+      <c r="L10" s="578"/>
       <c r="M10" s="312"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="2" t="s">
@@ -19966,21 +20107,21 @@
       <c r="E11" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="622" t="str">
+      <c r="F11" s="579" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="622"/>
+      <c r="G11" s="579"/>
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
       <c r="J11" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="622" t="str">
+      <c r="K11" s="579" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="622"/>
+      <c r="L11" s="579"/>
       <c r="M11" s="312"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="2" t="s">
@@ -20023,21 +20164,21 @@
       <c r="E12" s="160" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="622" t="str">
+      <c r="F12" s="579" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="622"/>
+      <c r="G12" s="579"/>
       <c r="H12" s="42"/>
       <c r="I12" s="42"/>
       <c r="J12" s="160" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="630" t="str">
+      <c r="K12" s="580" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="630"/>
+      <c r="L12" s="580"/>
       <c r="M12" s="312"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="2" t="s">
@@ -20080,21 +20221,21 @@
       <c r="E13" s="160" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="623" t="str">
+      <c r="F13" s="581" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="623"/>
+      <c r="G13" s="581"/>
       <c r="H13" s="42"/>
       <c r="I13" s="42"/>
       <c r="J13" s="160" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="623" t="str">
+      <c r="K13" s="581" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="623"/>
+      <c r="L13" s="581"/>
       <c r="M13" s="312"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="2" t="s">
@@ -20217,21 +20358,21 @@
       <c r="E16" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="628" t="str">
+      <c r="F16" s="577" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="628"/>
+      <c r="G16" s="577"/>
       <c r="H16" s="42"/>
       <c r="I16" s="42"/>
       <c r="J16" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="631" t="str">
+      <c r="K16" s="582" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="631"/>
+      <c r="L16" s="582"/>
       <c r="M16" s="312"/>
       <c r="O16" s="13"/>
       <c r="P16" s="50" t="s">
@@ -20261,21 +20402,21 @@
       <c r="E17" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="622" t="str">
+      <c r="F17" s="579" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="622"/>
+      <c r="G17" s="579"/>
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
       <c r="J17" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="623" t="str">
+      <c r="K17" s="581" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="623"/>
+      <c r="L17" s="581"/>
       <c r="M17" s="312"/>
       <c r="O17" s="13"/>
       <c r="Q17" s="2" t="s">
@@ -20318,21 +20459,21 @@
       <c r="E18" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="623" t="str">
+      <c r="F18" s="581" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="623"/>
+      <c r="G18" s="581"/>
       <c r="H18" s="42"/>
       <c r="I18" s="42"/>
       <c r="J18" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="623" t="str">
+      <c r="K18" s="581" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="623"/>
+      <c r="L18" s="581"/>
       <c r="M18" s="312"/>
       <c r="O18" s="13"/>
       <c r="Q18" s="2" t="s">
@@ -20380,11 +20521,11 @@
       <c r="J19" s="160" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="623" t="str">
+      <c r="K19" s="581" t="str">
         <f>IF(V20="","",V20)</f>
         <v/>
       </c>
-      <c r="L19" s="623"/>
+      <c r="L19" s="581"/>
       <c r="M19" s="312"/>
       <c r="O19" s="13"/>
       <c r="Q19" s="2" t="s">
@@ -20459,11 +20600,11 @@
       <c r="E21" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="628" t="str">
+      <c r="F21" s="577" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="628"/>
+      <c r="G21" s="577"/>
       <c r="H21" s="42"/>
       <c r="I21" s="42"/>
       <c r="J21" s="73" t="s">
@@ -20503,21 +20644,21 @@
       <c r="E22" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="629" t="str">
+      <c r="F22" s="583" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="629"/>
+      <c r="G22" s="583"/>
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
       <c r="J22" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="628" t="str">
+      <c r="K22" s="577" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="628"/>
+      <c r="L22" s="577"/>
       <c r="M22" s="312"/>
       <c r="O22" s="13"/>
       <c r="Q22" s="2" t="s">
@@ -20562,11 +20703,11 @@
       <c r="J23" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="622" t="str">
+      <c r="K23" s="579" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="622"/>
+      <c r="L23" s="579"/>
       <c r="M23" s="312"/>
       <c r="O23" s="13"/>
       <c r="Q23" s="2" t="s">
@@ -20609,21 +20750,21 @@
       <c r="E24" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="621" t="str">
+      <c r="F24" s="578" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="621"/>
+      <c r="G24" s="578"/>
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
       <c r="J24" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="622" t="str">
+      <c r="K24" s="579" t="str">
         <f>IF(V25="","",V25)</f>
         <v/>
       </c>
-      <c r="L24" s="622"/>
+      <c r="L24" s="579"/>
       <c r="M24" s="312"/>
       <c r="O24" s="13"/>
       <c r="P24" s="50" t="s">
@@ -20661,11 +20802,11 @@
       <c r="E25" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="623" t="str">
+      <c r="F25" s="581" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="623"/>
+      <c r="G25" s="581"/>
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
@@ -20713,11 +20854,11 @@
       <c r="E26" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="623" t="str">
+      <c r="F26" s="581" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="623"/>
+      <c r="G26" s="581"/>
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
       <c r="J26" s="313" t="s">
@@ -20766,11 +20907,11 @@
       <c r="J27" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="628" t="str">
+      <c r="K27" s="577" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="628"/>
+      <c r="L27" s="577"/>
       <c r="M27" s="312"/>
       <c r="O27" s="13"/>
       <c r="Q27" s="2" t="s">
@@ -20808,21 +20949,21 @@
       <c r="E28" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="621" t="str">
+      <c r="F28" s="578" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="621"/>
+      <c r="G28" s="578"/>
       <c r="H28" s="42"/>
       <c r="I28" s="42"/>
       <c r="J28" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="622" t="str">
+      <c r="K28" s="579" t="str">
         <f>IF(V29="","",V29)</f>
         <v/>
       </c>
-      <c r="L28" s="622"/>
+      <c r="L28" s="579"/>
       <c r="M28" s="312"/>
       <c r="O28" s="13"/>
       <c r="P28" s="50" t="s">
@@ -20851,11 +20992,11 @@
       <c r="E29" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="623" t="str">
+      <c r="F29" s="581" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="623"/>
+      <c r="G29" s="581"/>
       <c r="H29" s="42"/>
       <c r="I29" s="42"/>
       <c r="J29" s="42"/>
@@ -20903,11 +21044,11 @@
       <c r="E30" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="623" t="str">
+      <c r="F30" s="581" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="623"/>
+      <c r="G30" s="581"/>
       <c r="H30" s="42"/>
       <c r="I30" s="42"/>
       <c r="J30" s="42"/>
@@ -21022,11 +21163,11 @@
       <c r="E33" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="628" t="str">
+      <c r="F33" s="577" t="str">
         <f>IF(R34="","",R34)</f>
         <v/>
       </c>
-      <c r="G33" s="628"/>
+      <c r="G33" s="577"/>
       <c r="H33" s="42"/>
       <c r="I33" s="42"/>
       <c r="J33" s="73" t="s">
@@ -21063,21 +21204,21 @@
       <c r="E34" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="629" t="str">
+      <c r="F34" s="583" t="str">
         <f>IF(R35="","",R35)</f>
         <v/>
       </c>
-      <c r="G34" s="629"/>
+      <c r="G34" s="583"/>
       <c r="H34" s="42"/>
       <c r="I34" s="42"/>
       <c r="J34" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="628" t="str">
+      <c r="K34" s="577" t="str">
         <f>IF(V35="","",V35)</f>
         <v/>
       </c>
-      <c r="L34" s="628"/>
+      <c r="L34" s="577"/>
       <c r="M34" s="312"/>
       <c r="O34" s="13"/>
       <c r="Q34" s="2" t="s">
@@ -21122,11 +21263,11 @@
       <c r="J35" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="K35" s="622" t="str">
+      <c r="K35" s="579" t="str">
         <f>IF(V36="","",V36)</f>
         <v/>
       </c>
-      <c r="L35" s="622"/>
+      <c r="L35" s="579"/>
       <c r="M35" s="312"/>
       <c r="O35" s="13"/>
       <c r="Q35" s="2" t="s">
@@ -21169,21 +21310,21 @@
       <c r="E36" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="621" t="str">
+      <c r="F36" s="578" t="str">
         <f>IF(R37="","",R37)</f>
         <v/>
       </c>
-      <c r="G36" s="621"/>
+      <c r="G36" s="578"/>
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
       <c r="J36" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="K36" s="622" t="str">
+      <c r="K36" s="579" t="str">
         <f>IF(V37="","",V37)</f>
         <v/>
       </c>
-      <c r="L36" s="622"/>
+      <c r="L36" s="579"/>
       <c r="M36" s="312"/>
       <c r="O36" s="13"/>
       <c r="P36" s="50" t="s">
@@ -21221,11 +21362,11 @@
       <c r="E37" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="623" t="str">
+      <c r="F37" s="581" t="str">
         <f>IF(R38="","",R38)</f>
         <v/>
       </c>
-      <c r="G37" s="623"/>
+      <c r="G37" s="581"/>
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
       <c r="J37" s="42"/>
@@ -21273,11 +21414,11 @@
       <c r="E38" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="623" t="str">
+      <c r="F38" s="581" t="str">
         <f>IF(R39="","",R39)</f>
         <v/>
       </c>
-      <c r="G38" s="623"/>
+      <c r="G38" s="581"/>
       <c r="H38" s="42"/>
       <c r="I38" s="42"/>
       <c r="J38" s="313" t="s">
@@ -21324,11 +21465,11 @@
       <c r="J39" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="K39" s="628" t="str">
+      <c r="K39" s="577" t="str">
         <f>IF(V40="","",V40)</f>
         <v/>
       </c>
-      <c r="L39" s="628"/>
+      <c r="L39" s="577"/>
       <c r="M39" s="312"/>
       <c r="O39" s="13"/>
       <c r="Q39" s="2" t="s">
@@ -21366,21 +21507,21 @@
       <c r="E40" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="621" t="str">
+      <c r="F40" s="578" t="str">
         <f>IF(R41="","",R41)</f>
         <v/>
       </c>
-      <c r="G40" s="621"/>
+      <c r="G40" s="578"/>
       <c r="H40" s="42"/>
       <c r="I40" s="42"/>
       <c r="J40" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K40" s="622" t="str">
+      <c r="K40" s="579" t="str">
         <f>IF(V41="","",V41)</f>
         <v/>
       </c>
-      <c r="L40" s="622"/>
+      <c r="L40" s="579"/>
       <c r="M40" s="312"/>
       <c r="O40" s="13"/>
       <c r="P40" s="50" t="s">
@@ -21418,11 +21559,11 @@
       <c r="E41" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="623" t="str">
+      <c r="F41" s="581" t="str">
         <f>IF(R42="","",R42)</f>
         <v/>
       </c>
-      <c r="G41" s="623"/>
+      <c r="G41" s="581"/>
       <c r="H41" s="42"/>
       <c r="I41" s="42"/>
       <c r="J41" s="42"/>
@@ -21470,11 +21611,11 @@
       <c r="E42" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="623" t="str">
+      <c r="F42" s="581" t="str">
         <f>IF(R43="","",R43)</f>
         <v/>
       </c>
-      <c r="G42" s="623"/>
+      <c r="G42" s="581"/>
       <c r="H42" s="42"/>
       <c r="I42" s="42"/>
       <c r="J42" s="42"/>
@@ -22239,10 +22380,10 @@
       <c r="I69" s="299"/>
       <c r="J69" s="299"/>
       <c r="K69" s="299"/>
-      <c r="L69" s="624" t="s">
+      <c r="L69" s="588" t="s">
         <v>84</v>
       </c>
-      <c r="M69" s="625"/>
+      <c r="M69" s="589"/>
       <c r="O69" s="56"/>
       <c r="P69" s="17" t="s">
         <v>85</v>
@@ -23911,24 +24052,24 @@
       <c r="P107" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="Q107" s="626" t="str">
+      <c r="Q107" s="585" t="str">
         <f>IF(Q106&lt;&gt;"",Q106,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R107" s="626"/>
-      <c r="S107" s="626"/>
-      <c r="T107" s="627" t="str">
+      <c r="R107" s="585"/>
+      <c r="S107" s="585"/>
+      <c r="T107" s="584" t="str">
         <f>IF(T106&lt;&gt;"",T106,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v/>
       </c>
-      <c r="U107" s="627"/>
-      <c r="V107" s="627"/>
-      <c r="W107" s="627" t="str">
+      <c r="U107" s="584"/>
+      <c r="V107" s="584"/>
+      <c r="W107" s="584" t="str">
         <f>IF(W106&lt;&gt;"",W106,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="X107" s="627"/>
-      <c r="Y107" s="627"/>
+      <c r="X107" s="584"/>
+      <c r="Y107" s="584"/>
       <c r="AA107" s="2" t="s">
         <v>153</v>
       </c>
@@ -25918,24 +26059,24 @@
       <c r="P139" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="Q139" s="626" t="str">
+      <c r="Q139" s="585" t="str">
         <f>IF(Q138&lt;&gt;"",Q138,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R139" s="626"/>
-      <c r="S139" s="626"/>
-      <c r="T139" s="627" t="str">
+      <c r="R139" s="585"/>
+      <c r="S139" s="585"/>
+      <c r="T139" s="584" t="str">
         <f>IF(T138&lt;&gt;"",T138,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v/>
       </c>
-      <c r="U139" s="627"/>
-      <c r="V139" s="627"/>
-      <c r="W139" s="627" t="str">
+      <c r="U139" s="584"/>
+      <c r="V139" s="584"/>
+      <c r="W139" s="584" t="str">
         <f>IF(W138&lt;&gt;"",W138,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="X139" s="627"/>
-      <c r="Y139" s="627"/>
+      <c r="X139" s="584"/>
+      <c r="Y139" s="584"/>
       <c r="AA139" s="2" t="str">
         <f>$T$139&amp;" Mag 4"</f>
         <v xml:space="preserve"> Mag 4</v>
@@ -28279,10 +28420,10 @@
       <c r="P181" s="135"/>
       <c r="Q181" s="137"/>
       <c r="R181" s="128"/>
-      <c r="T181" s="610" t="s">
+      <c r="T181" s="586" t="s">
         <v>245</v>
       </c>
-      <c r="U181" s="610"/>
+      <c r="U181" s="586"/>
       <c r="W181" s="2" t="s">
         <v>199</v>
       </c>
@@ -28653,7 +28794,7 @@
       <c r="K190" s="323"/>
       <c r="L190" s="323"/>
       <c r="M190" s="327"/>
-      <c r="O190" s="618" t="str">
+      <c r="O190" s="587" t="str">
         <f>$Q$107</f>
         <v>Auto 1</v>
       </c>
@@ -28703,7 +28844,7 @@
       <c r="K191" s="323"/>
       <c r="L191" s="323"/>
       <c r="M191" s="303"/>
-      <c r="O191" s="618"/>
+      <c r="O191" s="587"/>
       <c r="P191" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -28749,7 +28890,7 @@
       <c r="K192" s="135"/>
       <c r="L192" s="135"/>
       <c r="M192" s="303"/>
-      <c r="O192" s="618"/>
+      <c r="O192" s="587"/>
       <c r="P192" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -28795,7 +28936,7 @@
       <c r="K193" s="135"/>
       <c r="L193" s="135"/>
       <c r="M193" s="303"/>
-      <c r="O193" s="618"/>
+      <c r="O193" s="587"/>
       <c r="P193" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -28838,7 +28979,7 @@
       <c r="K194" s="135"/>
       <c r="L194" s="135"/>
       <c r="M194" s="303"/>
-      <c r="O194" s="618"/>
+      <c r="O194" s="587"/>
       <c r="P194" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -28881,7 +29022,7 @@
       <c r="K195" s="135"/>
       <c r="L195" s="135"/>
       <c r="M195" s="303"/>
-      <c r="O195" s="618" t="str">
+      <c r="O195" s="587" t="str">
         <f>$T$107</f>
         <v/>
       </c>
@@ -28927,7 +29068,7 @@
       <c r="K196" s="305"/>
       <c r="L196" s="305"/>
       <c r="M196" s="306"/>
-      <c r="O196" s="618"/>
+      <c r="O196" s="587"/>
       <c r="P196" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -28972,7 +29113,7 @@
         <f>IF($X$7="","",$X$7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="O197" s="618"/>
+      <c r="O197" s="587"/>
       <c r="P197" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -29017,7 +29158,7 @@
         <f>IF($R$13="","",$R$13)</f>
         <v/>
       </c>
-      <c r="O198" s="618"/>
+      <c r="O198" s="587"/>
       <c r="P198" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -29063,7 +29204,7 @@
         <f>$H$2</f>
         <v>Medical University of South Carolina</v>
       </c>
-      <c r="O199" s="618"/>
+      <c r="O199" s="587"/>
       <c r="P199" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -29112,7 +29253,7 @@
         <f>$H$5</f>
         <v>Fluoroscopy System Compliance Inspection</v>
       </c>
-      <c r="O200" s="618" t="str">
+      <c r="O200" s="587" t="str">
         <f>$W$107</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -29161,7 +29302,7 @@
       <c r="K201" s="299"/>
       <c r="L201" s="299"/>
       <c r="M201" s="300"/>
-      <c r="O201" s="618"/>
+      <c r="O201" s="587"/>
       <c r="P201" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -29215,7 +29356,7 @@
         <v/>
       </c>
       <c r="M202" s="12"/>
-      <c r="O202" s="618"/>
+      <c r="O202" s="587"/>
       <c r="P202" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -29248,7 +29389,7 @@
       </c>
       <c r="B203" s="10"/>
       <c r="M203" s="12"/>
-      <c r="O203" s="618"/>
+      <c r="O203" s="587"/>
       <c r="P203" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -29282,20 +29423,20 @@
       <c r="B204" s="301"/>
       <c r="C204" s="351"/>
       <c r="D204" s="323"/>
-      <c r="E204" s="577" t="s">
+      <c r="E204" s="620" t="s">
         <v>262</v>
       </c>
-      <c r="F204" s="579" t="s">
+      <c r="F204" s="622" t="s">
         <v>263</v>
       </c>
       <c r="G204" s="518" t="s">
         <v>264</v>
       </c>
-      <c r="H204" s="577" t="str">
+      <c r="H204" s="620" t="str">
         <f>R276</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="I204" s="581" t="str">
+      <c r="I204" s="624" t="str">
         <f>S276</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -29308,10 +29449,10 @@
       <c r="L204" s="135" t="s">
         <v>267</v>
       </c>
-      <c r="M204" s="583" t="s">
+      <c r="M204" s="626" t="s">
         <v>268</v>
       </c>
-      <c r="O204" s="618"/>
+      <c r="O204" s="587"/>
       <c r="P204" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -29349,11 +29490,11 @@
       <c r="D205" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="E205" s="578"/>
-      <c r="F205" s="580"/>
+      <c r="E205" s="621"/>
+      <c r="F205" s="623"/>
       <c r="G205" s="518"/>
-      <c r="H205" s="578"/>
-      <c r="I205" s="582"/>
+      <c r="H205" s="621"/>
+      <c r="I205" s="625"/>
       <c r="J205" s="519"/>
       <c r="K205" s="135" t="str">
         <f>U277</f>
@@ -29363,7 +29504,7 @@
         <f>V277</f>
         <v>mGy/min</v>
       </c>
-      <c r="M205" s="584"/>
+      <c r="M205" s="627"/>
       <c r="O205" s="13"/>
       <c r="Y205" s="14"/>
       <c r="AA205" s="2" t="s">
@@ -30007,7 +30148,7 @@
         <f>W286</f>
         <v/>
       </c>
-      <c r="O214" s="618" t="str">
+      <c r="O214" s="587" t="str">
         <f>$Q$139</f>
         <v>Auto 1</v>
       </c>
@@ -30063,7 +30204,7 @@
       <c r="K215" s="135"/>
       <c r="L215" s="135"/>
       <c r="M215" s="303"/>
-      <c r="O215" s="618"/>
+      <c r="O215" s="587"/>
       <c r="P215" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30109,7 +30250,7 @@
       <c r="K216" s="323"/>
       <c r="L216" s="323"/>
       <c r="M216" s="303"/>
-      <c r="O216" s="618"/>
+      <c r="O216" s="587"/>
       <c r="P216" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -30155,7 +30296,7 @@
       <c r="K217" s="368"/>
       <c r="L217" s="368"/>
       <c r="M217" s="369"/>
-      <c r="O217" s="618"/>
+      <c r="O217" s="587"/>
       <c r="P217" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -30202,7 +30343,7 @@
       <c r="K218" s="323"/>
       <c r="L218" s="323"/>
       <c r="M218" s="303"/>
-      <c r="O218" s="618"/>
+      <c r="O218" s="587"/>
       <c r="P218" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -30245,7 +30386,7 @@
       <c r="K219" s="323"/>
       <c r="L219" s="323"/>
       <c r="M219" s="327"/>
-      <c r="O219" s="618" t="str">
+      <c r="O219" s="587" t="str">
         <f>$T$139</f>
         <v/>
       </c>
@@ -30306,7 +30447,7 @@
         <v/>
       </c>
       <c r="M220" s="327"/>
-      <c r="O220" s="618"/>
+      <c r="O220" s="587"/>
       <c r="P220" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30349,7 +30490,7 @@
       <c r="K221" s="323"/>
       <c r="L221" s="323"/>
       <c r="M221" s="327"/>
-      <c r="O221" s="618"/>
+      <c r="O221" s="587"/>
       <c r="P221" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -30400,7 +30541,7 @@
       <c r="K222" s="323"/>
       <c r="L222" s="323"/>
       <c r="M222" s="327"/>
-      <c r="O222" s="618"/>
+      <c r="O222" s="587"/>
       <c r="P222" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -30457,7 +30598,7 @@
       <c r="K223" s="323"/>
       <c r="L223" s="323"/>
       <c r="M223" s="327"/>
-      <c r="O223" s="618"/>
+      <c r="O223" s="587"/>
       <c r="P223" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -30521,7 +30662,7 @@
       <c r="K224" s="323"/>
       <c r="L224" s="323"/>
       <c r="M224" s="327"/>
-      <c r="O224" s="618" t="str">
+      <c r="O224" s="587" t="str">
         <f>$W$139</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -30585,7 +30726,7 @@
       <c r="K225" s="323"/>
       <c r="L225" s="323"/>
       <c r="M225" s="327"/>
-      <c r="O225" s="618"/>
+      <c r="O225" s="587"/>
       <c r="P225" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30646,7 +30787,7 @@
       <c r="K226" s="323"/>
       <c r="L226" s="323"/>
       <c r="M226" s="327"/>
-      <c r="O226" s="618"/>
+      <c r="O226" s="587"/>
       <c r="P226" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -30707,7 +30848,7 @@
       <c r="K227" s="323"/>
       <c r="L227" s="323"/>
       <c r="M227" s="327"/>
-      <c r="O227" s="618"/>
+      <c r="O227" s="587"/>
       <c r="P227" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -30761,7 +30902,7 @@
       <c r="K228" s="323"/>
       <c r="L228" s="323"/>
       <c r="M228" s="327"/>
-      <c r="O228" s="618"/>
+      <c r="O228" s="587"/>
       <c r="P228" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -31314,7 +31455,7 @@
       <c r="K240" s="323"/>
       <c r="L240" s="323"/>
       <c r="M240" s="327"/>
-      <c r="O240" s="619" t="s">
+      <c r="O240" s="590" t="s">
         <v>294</v>
       </c>
       <c r="P240" s="167" t="s">
@@ -31373,7 +31514,7 @@
       <c r="K241" s="323"/>
       <c r="L241" s="323"/>
       <c r="M241" s="327"/>
-      <c r="O241" s="619"/>
+      <c r="O241" s="590"/>
       <c r="P241" s="172" t="s">
         <v>297</v>
       </c>
@@ -31430,7 +31571,7 @@
       <c r="K242" s="323"/>
       <c r="L242" s="323"/>
       <c r="M242" s="327"/>
-      <c r="O242" s="619" t="str">
+      <c r="O242" s="590" t="str">
         <f>IF($U$137=1,"Scatter - Pulse", "Scatter – Digital acq")</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -31490,7 +31631,7 @@
       <c r="K243" s="323"/>
       <c r="L243" s="323"/>
       <c r="M243" s="327"/>
-      <c r="O243" s="619"/>
+      <c r="O243" s="590"/>
       <c r="P243" s="172" t="s">
         <v>297</v>
       </c>
@@ -31899,7 +32040,7 @@
       <c r="L254" s="323"/>
       <c r="M254" s="327"/>
       <c r="O254" s="180">
-        <f>IF(OR(O252=0,O253=0),"",SQRT((O252^2)/(O253^2)))</f>
+        <f>IF(OR(O252=0,O253=0),"",(O252/O253)^2)</f>
         <v>1</v>
       </c>
       <c r="P254" s="17" t="s">
@@ -32020,17 +32161,17 @@
       <c r="P257" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="Q257" s="620" t="s">
+      <c r="Q257" s="591" t="s">
         <v>313</v>
       </c>
-      <c r="R257" s="620"/>
+      <c r="R257" s="591"/>
       <c r="S257" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="T257" s="620" t="s">
+      <c r="T257" s="591" t="s">
         <v>315</v>
       </c>
-      <c r="U257" s="620"/>
+      <c r="U257" s="591"/>
       <c r="V257" s="1" t="s">
         <v>316</v>
       </c>
@@ -32518,24 +32659,24 @@
         <f t="shared" si="43"/>
         <v>Attenuator</v>
       </c>
-      <c r="E269" s="612" t="str">
+      <c r="E269" s="592" t="str">
         <f>Q107</f>
         <v>Auto 1</v>
       </c>
-      <c r="F269" s="613"/>
-      <c r="G269" s="613"/>
-      <c r="H269" s="613" t="str">
+      <c r="F269" s="593"/>
+      <c r="G269" s="593"/>
+      <c r="H269" s="593" t="str">
         <f>T107</f>
         <v/>
       </c>
-      <c r="I269" s="613"/>
-      <c r="J269" s="613"/>
-      <c r="K269" s="614" t="str">
+      <c r="I269" s="593"/>
+      <c r="J269" s="593"/>
+      <c r="K269" s="594" t="str">
         <f>W107</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L269" s="614"/>
-      <c r="M269" s="615"/>
+      <c r="L269" s="594"/>
+      <c r="M269" s="595"/>
       <c r="O269" s="189" t="str">
         <f t="shared" si="44"/>
         <v/>
@@ -32637,7 +32778,7 @@
         <v>7</v>
       </c>
       <c r="B271" s="301"/>
-      <c r="C271" s="602" t="str">
+      <c r="C271" s="599" t="str">
         <f>O110&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -32713,7 +32854,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="301"/>
-      <c r="C272" s="602"/>
+      <c r="C272" s="599"/>
       <c r="D272" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -32779,7 +32920,7 @@
         <v>9</v>
       </c>
       <c r="B273" s="301"/>
-      <c r="C273" s="602"/>
+      <c r="C273" s="599"/>
       <c r="D273" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -32852,7 +32993,7 @@
         <v>10</v>
       </c>
       <c r="B274" s="301"/>
-      <c r="C274" s="602" t="str">
+      <c r="C274" s="599" t="str">
         <f>O113&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -32921,7 +33062,7 @@
         <v>11</v>
       </c>
       <c r="B275" s="301"/>
-      <c r="C275" s="602"/>
+      <c r="C275" s="599"/>
       <c r="D275" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -32994,7 +33135,7 @@
         <v>12</v>
       </c>
       <c r="B276" s="301"/>
-      <c r="C276" s="602"/>
+      <c r="C276" s="599"/>
       <c r="D276" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -33035,17 +33176,17 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="O276" s="616" t="s">
+      <c r="O276" s="600" t="s">
         <v>262</v>
       </c>
-      <c r="P276" s="617" t="s">
+      <c r="P276" s="601" t="s">
         <v>263</v>
       </c>
-      <c r="R276" s="617" t="str">
+      <c r="R276" s="601" t="str">
         <f>"Ind AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="S276" s="617" t="str">
+      <c r="S276" s="601" t="str">
         <f>"Meas AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -33067,7 +33208,7 @@
         <v>13</v>
       </c>
       <c r="B277" s="301"/>
-      <c r="C277" s="602" t="str">
+      <c r="C277" s="599" t="str">
         <f>O116&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33111,13 +33252,13 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="O277" s="616"/>
-      <c r="P277" s="617"/>
+      <c r="O277" s="600"/>
+      <c r="P277" s="601"/>
       <c r="Q277" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="R277" s="617"/>
-      <c r="S277" s="617"/>
+      <c r="R277" s="601"/>
+      <c r="S277" s="601"/>
       <c r="T277" s="1" t="s">
         <v>322</v>
       </c>
@@ -33149,7 +33290,7 @@
         <v>14</v>
       </c>
       <c r="B278" s="301"/>
-      <c r="C278" s="602"/>
+      <c r="C278" s="599"/>
       <c r="D278" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -33236,7 +33377,7 @@
         <v>15</v>
       </c>
       <c r="B279" s="301"/>
-      <c r="C279" s="602"/>
+      <c r="C279" s="599"/>
       <c r="D279" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -33330,7 +33471,7 @@
         <v>16</v>
       </c>
       <c r="B280" s="301"/>
-      <c r="C280" s="602" t="str">
+      <c r="C280" s="599" t="str">
         <f>O119&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33430,7 +33571,7 @@
         <v>17</v>
       </c>
       <c r="B281" s="301"/>
-      <c r="C281" s="602"/>
+      <c r="C281" s="599"/>
       <c r="D281" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -33517,7 +33658,7 @@
         <v>18</v>
       </c>
       <c r="B282" s="301"/>
-      <c r="C282" s="602"/>
+      <c r="C282" s="599"/>
       <c r="D282" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -33611,7 +33752,7 @@
         <v>19</v>
       </c>
       <c r="B283" s="301"/>
-      <c r="C283" s="602" t="str">
+      <c r="C283" s="599" t="str">
         <f>O122&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33701,7 +33842,7 @@
         <v>20</v>
       </c>
       <c r="B284" s="301"/>
-      <c r="C284" s="602"/>
+      <c r="C284" s="599"/>
       <c r="D284" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -33795,7 +33936,7 @@
         <v>21</v>
       </c>
       <c r="B285" s="301"/>
-      <c r="C285" s="602"/>
+      <c r="C285" s="599"/>
       <c r="D285" s="391">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -34230,12 +34371,12 @@
       <c r="L293" s="135"/>
       <c r="M293" s="303"/>
       <c r="O293" s="225"/>
-      <c r="P293" s="607" t="s">
+      <c r="P293" s="606" t="s">
         <v>328</v>
       </c>
-      <c r="Q293" s="607"/>
-      <c r="R293" s="607"/>
-      <c r="S293" s="607"/>
+      <c r="Q293" s="606"/>
+      <c r="R293" s="606"/>
+      <c r="S293" s="606"/>
       <c r="T293" s="223"/>
       <c r="U293" s="223"/>
       <c r="V293" s="223"/>
@@ -34612,12 +34753,12 @@
       <c r="L302" s="135"/>
       <c r="M302" s="303"/>
       <c r="O302" s="225"/>
-      <c r="P302" s="607" t="s">
+      <c r="P302" s="606" t="s">
         <v>328</v>
       </c>
-      <c r="Q302" s="607"/>
-      <c r="R302" s="607"/>
-      <c r="S302" s="607"/>
+      <c r="Q302" s="606"/>
+      <c r="R302" s="606"/>
+      <c r="S302" s="606"/>
       <c r="T302" s="223"/>
       <c r="U302" s="223"/>
       <c r="V302" s="223"/>
@@ -34639,7 +34780,7 @@
         <v>39</v>
       </c>
       <c r="B303" s="301"/>
-      <c r="C303" s="585" t="str">
+      <c r="C303" s="607" t="str">
         <f>O190</f>
         <v>Auto 1</v>
       </c>
@@ -34700,7 +34841,7 @@
         <v>40</v>
       </c>
       <c r="B304" s="301"/>
-      <c r="C304" s="586"/>
+      <c r="C304" s="608"/>
       <c r="D304" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -34770,7 +34911,7 @@
         <v>41</v>
       </c>
       <c r="B305" s="301"/>
-      <c r="C305" s="586"/>
+      <c r="C305" s="608"/>
       <c r="D305" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -34818,7 +34959,7 @@
         <v>42</v>
       </c>
       <c r="B306" s="301"/>
-      <c r="C306" s="586"/>
+      <c r="C306" s="608"/>
       <c r="D306" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -34870,7 +35011,7 @@
         <v>43</v>
       </c>
       <c r="B307" s="301"/>
-      <c r="C307" s="608"/>
+      <c r="C307" s="609"/>
       <c r="D307" s="436" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -34915,7 +35056,7 @@
         <v>44</v>
       </c>
       <c r="B308" s="301"/>
-      <c r="C308" s="585" t="str">
+      <c r="C308" s="607" t="str">
         <f>O195</f>
         <v/>
       </c>
@@ -34970,7 +35111,7 @@
         <v>45</v>
       </c>
       <c r="B309" s="301"/>
-      <c r="C309" s="586"/>
+      <c r="C309" s="608"/>
       <c r="D309" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35023,7 +35164,7 @@
         <v>46</v>
       </c>
       <c r="B310" s="301"/>
-      <c r="C310" s="586"/>
+      <c r="C310" s="608"/>
       <c r="D310" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35083,7 +35224,7 @@
         <v>47</v>
       </c>
       <c r="B311" s="301"/>
-      <c r="C311" s="586"/>
+      <c r="C311" s="608"/>
       <c r="D311" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35136,7 +35277,7 @@
         <v>48</v>
       </c>
       <c r="B312" s="301"/>
-      <c r="C312" s="587"/>
+      <c r="C312" s="610"/>
       <c r="D312" s="439" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35193,7 +35334,7 @@
         <v>49</v>
       </c>
       <c r="B313" s="301"/>
-      <c r="C313" s="609" t="str">
+      <c r="C313" s="611" t="str">
         <f>O200</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -35245,7 +35386,7 @@
         <v>50</v>
       </c>
       <c r="B314" s="301"/>
-      <c r="C314" s="586"/>
+      <c r="C314" s="608"/>
       <c r="D314" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35297,7 +35438,7 @@
         <v>51</v>
       </c>
       <c r="B315" s="301"/>
-      <c r="C315" s="586"/>
+      <c r="C315" s="608"/>
       <c r="D315" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35342,7 +35483,7 @@
         <v>52</v>
       </c>
       <c r="B316" s="301"/>
-      <c r="C316" s="586"/>
+      <c r="C316" s="608"/>
       <c r="D316" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35396,7 +35537,7 @@
         <v>53</v>
       </c>
       <c r="B317" s="301"/>
-      <c r="C317" s="587"/>
+      <c r="C317" s="610"/>
       <c r="D317" s="439" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35518,10 +35659,10 @@
       <c r="R319" s="246"/>
       <c r="S319" s="247"/>
       <c r="T319" s="247"/>
-      <c r="V319" s="610" t="s">
+      <c r="V319" s="586" t="s">
         <v>339</v>
       </c>
-      <c r="W319" s="610"/>
+      <c r="W319" s="586"/>
       <c r="X319" s="17" t="s">
         <v>340</v>
       </c>
@@ -35722,7 +35863,7 @@
         <v>60</v>
       </c>
       <c r="B324" s="301"/>
-      <c r="C324" s="591" t="str">
+      <c r="C324" s="596" t="str">
         <f>O240</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -35772,7 +35913,7 @@
         <v>61</v>
       </c>
       <c r="B325" s="301"/>
-      <c r="C325" s="592"/>
+      <c r="C325" s="597"/>
       <c r="D325" s="448" t="str">
         <f>P241</f>
         <v>Waist level</v>
@@ -35930,13 +36071,13 @@
         <v>347</v>
       </c>
       <c r="P329" s="53"/>
-      <c r="Q329" s="611" t="s">
+      <c r="Q329" s="598" t="s">
         <v>348</v>
       </c>
-      <c r="R329" s="611"/>
-      <c r="S329" s="611"/>
-      <c r="T329" s="611"/>
-      <c r="U329" s="611"/>
+      <c r="R329" s="598"/>
+      <c r="S329" s="598"/>
+      <c r="T329" s="598"/>
+      <c r="U329" s="598"/>
       <c r="Y329" s="14"/>
     </row>
     <row r="330" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -36119,24 +36260,24 @@
         <f t="shared" si="72"/>
         <v>Attenuator</v>
       </c>
-      <c r="E335" s="612" t="str">
+      <c r="E335" s="592" t="str">
         <f>Q139</f>
         <v>Auto 1</v>
       </c>
-      <c r="F335" s="613"/>
-      <c r="G335" s="613"/>
-      <c r="H335" s="613" t="str">
+      <c r="F335" s="593"/>
+      <c r="G335" s="593"/>
+      <c r="H335" s="593" t="str">
         <f>T139</f>
         <v/>
       </c>
-      <c r="I335" s="613"/>
-      <c r="J335" s="613"/>
-      <c r="K335" s="614" t="str">
+      <c r="I335" s="593"/>
+      <c r="J335" s="593"/>
+      <c r="K335" s="594" t="str">
         <f>W139</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L335" s="614"/>
-      <c r="M335" s="615"/>
+      <c r="L335" s="594"/>
+      <c r="M335" s="595"/>
       <c r="O335" s="130"/>
       <c r="P335" s="129" t="s">
         <v>354</v>
@@ -36213,7 +36354,7 @@
         <v>7</v>
       </c>
       <c r="B337" s="301"/>
-      <c r="C337" s="602" t="str">
+      <c r="C337" s="599" t="str">
         <f>O142&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -36273,7 +36414,7 @@
         <v>8</v>
       </c>
       <c r="B338" s="301"/>
-      <c r="C338" s="602"/>
+      <c r="C338" s="599"/>
       <c r="D338" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -36330,7 +36471,7 @@
         <v>9</v>
       </c>
       <c r="B339" s="301"/>
-      <c r="C339" s="602"/>
+      <c r="C339" s="599"/>
       <c r="D339" s="463">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -36387,7 +36528,7 @@
         <v>10</v>
       </c>
       <c r="B340" s="301"/>
-      <c r="C340" s="602" t="str">
+      <c r="C340" s="599" t="str">
         <f>O145&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -36447,7 +36588,7 @@
         <v>11</v>
       </c>
       <c r="B341" s="301"/>
-      <c r="C341" s="602"/>
+      <c r="C341" s="599"/>
       <c r="D341" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -36504,7 +36645,7 @@
         <v>12</v>
       </c>
       <c r="B342" s="301"/>
-      <c r="C342" s="602"/>
+      <c r="C342" s="599"/>
       <c r="D342" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -36561,7 +36702,7 @@
         <v>13</v>
       </c>
       <c r="B343" s="301"/>
-      <c r="C343" s="602" t="str">
+      <c r="C343" s="599" t="str">
         <f>O148&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -36613,7 +36754,7 @@
         <v>14</v>
       </c>
       <c r="B344" s="301"/>
-      <c r="C344" s="602"/>
+      <c r="C344" s="599"/>
       <c r="D344" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -36675,7 +36816,7 @@
         <v>15</v>
       </c>
       <c r="B345" s="301"/>
-      <c r="C345" s="602"/>
+      <c r="C345" s="599"/>
       <c r="D345" s="463">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -36738,7 +36879,7 @@
         <v>16</v>
       </c>
       <c r="B346" s="301"/>
-      <c r="C346" s="602" t="str">
+      <c r="C346" s="599" t="str">
         <f>O151&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -36801,7 +36942,7 @@
         <v>17</v>
       </c>
       <c r="B347" s="301"/>
-      <c r="C347" s="602"/>
+      <c r="C347" s="599"/>
       <c r="D347" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -36859,7 +37000,7 @@
         <v>18</v>
       </c>
       <c r="B348" s="301"/>
-      <c r="C348" s="602"/>
+      <c r="C348" s="599"/>
       <c r="D348" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -36937,7 +37078,7 @@
         <v>19</v>
       </c>
       <c r="B349" s="301"/>
-      <c r="C349" s="602" t="str">
+      <c r="C349" s="599" t="str">
         <f>O154&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37000,7 +37141,7 @@
         <v>20</v>
       </c>
       <c r="B350" s="301"/>
-      <c r="C350" s="602"/>
+      <c r="C350" s="599"/>
       <c r="D350" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37059,7 +37200,7 @@
         <v>21</v>
       </c>
       <c r="B351" s="301"/>
-      <c r="C351" s="602"/>
+      <c r="C351" s="599"/>
       <c r="D351" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37368,11 +37509,11 @@
         <f>IF(OR(V358="",V359="",V362=""),"",(V358-V359)*V362)</f>
         <v/>
       </c>
-      <c r="Q358" s="603" t="str">
+      <c r="Q358" s="602" t="str">
         <f>IF(OR(P358="",P359=""),"",(ABS(P358)+ABS(P359))/$O$355)</f>
         <v/>
       </c>
-      <c r="R358" s="604" t="str">
+      <c r="R358" s="603" t="str">
         <f>IF(OR(Q358="",Q360=""),"",Q358+Q360)</f>
         <v/>
       </c>
@@ -37411,8 +37552,8 @@
         <f>IF(OR(W358="",W359="",V362=""),"",(W358-W359)*V362)</f>
         <v/>
       </c>
-      <c r="Q359" s="603"/>
-      <c r="R359" s="603"/>
+      <c r="Q359" s="602"/>
+      <c r="R359" s="602"/>
       <c r="S359" s="146" t="str">
         <f>IF(AB171="","",AB171)</f>
         <v/>
@@ -37448,11 +37589,11 @@
         <f>IF(OR(X358="",X359="",V362=""),"",(X358-X359)*V362)</f>
         <v/>
       </c>
-      <c r="Q360" s="604" t="str">
+      <c r="Q360" s="603" t="str">
         <f>IF(OR(P360="",P361=""),"",(ABS(P360)+ABS(P361))/$O$355)</f>
         <v/>
       </c>
-      <c r="R360" s="604"/>
+      <c r="R360" s="603"/>
       <c r="S360" s="146" t="str">
         <f>IF(AB172="","",AB172)</f>
         <v/>
@@ -37494,8 +37635,8 @@
         <f>IF(OR(Y358="",Y359="",V362=""),"",(Y358-Y359)*V362)</f>
         <v/>
       </c>
-      <c r="Q361" s="604"/>
-      <c r="R361" s="604"/>
+      <c r="Q361" s="603"/>
+      <c r="R361" s="603"/>
       <c r="S361" s="148" t="str">
         <f>IF(AB173="","",AB173)</f>
         <v/>
@@ -37667,7 +37808,7 @@
         <v>36</v>
       </c>
       <c r="B366" s="301"/>
-      <c r="C366" s="605" t="str">
+      <c r="C366" s="604" t="str">
         <f>O214</f>
         <v>Auto 1</v>
       </c>
@@ -37718,7 +37859,7 @@
         <v>37</v>
       </c>
       <c r="B367" s="301"/>
-      <c r="C367" s="606"/>
+      <c r="C367" s="605"/>
       <c r="D367" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -37764,7 +37905,7 @@
         <v>38</v>
       </c>
       <c r="B368" s="301"/>
-      <c r="C368" s="606"/>
+      <c r="C368" s="605"/>
       <c r="D368" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -37799,7 +37940,7 @@
         <v>39</v>
       </c>
       <c r="B369" s="301"/>
-      <c r="C369" s="606"/>
+      <c r="C369" s="605"/>
       <c r="D369" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -37834,7 +37975,7 @@
         <v>40</v>
       </c>
       <c r="B370" s="301"/>
-      <c r="C370" s="606"/>
+      <c r="C370" s="605"/>
       <c r="D370" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -37879,7 +38020,7 @@
         <v>41</v>
       </c>
       <c r="B371" s="301"/>
-      <c r="C371" s="585" t="str">
+      <c r="C371" s="607" t="str">
         <f>O219</f>
         <v/>
       </c>
@@ -37929,7 +38070,7 @@
         <v>42</v>
       </c>
       <c r="B372" s="301"/>
-      <c r="C372" s="586"/>
+      <c r="C372" s="608"/>
       <c r="D372" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -37979,7 +38120,7 @@
         <v>43</v>
       </c>
       <c r="B373" s="301"/>
-      <c r="C373" s="586"/>
+      <c r="C373" s="608"/>
       <c r="D373" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38026,7 +38167,7 @@
         <v>44</v>
       </c>
       <c r="B374" s="301"/>
-      <c r="C374" s="586"/>
+      <c r="C374" s="608"/>
       <c r="D374" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38076,7 +38217,7 @@
         <v>45</v>
       </c>
       <c r="B375" s="301"/>
-      <c r="C375" s="587"/>
+      <c r="C375" s="610"/>
       <c r="D375" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38123,7 +38264,7 @@
         <v>46</v>
       </c>
       <c r="B376" s="301"/>
-      <c r="C376" s="588" t="str">
+      <c r="C376" s="628" t="str">
         <f>O224</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -38176,7 +38317,7 @@
         <v>47</v>
       </c>
       <c r="B377" s="301"/>
-      <c r="C377" s="589"/>
+      <c r="C377" s="629"/>
       <c r="D377" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38223,7 +38364,7 @@
         <v>48</v>
       </c>
       <c r="B378" s="301"/>
-      <c r="C378" s="589"/>
+      <c r="C378" s="629"/>
       <c r="D378" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38273,7 +38414,7 @@
         <v>49</v>
       </c>
       <c r="B379" s="301"/>
-      <c r="C379" s="589"/>
+      <c r="C379" s="629"/>
       <c r="D379" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38320,7 +38461,7 @@
         <v>50</v>
       </c>
       <c r="B380" s="301"/>
-      <c r="C380" s="590"/>
+      <c r="C380" s="630"/>
       <c r="D380" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38630,7 +38771,7 @@
         <v>58</v>
       </c>
       <c r="B388" s="301"/>
-      <c r="C388" s="591" t="str">
+      <c r="C388" s="596" t="str">
         <f>O242</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -38681,7 +38822,7 @@
         <v>59</v>
       </c>
       <c r="B389" s="301"/>
-      <c r="C389" s="592"/>
+      <c r="C389" s="597"/>
       <c r="D389" s="448" t="str">
         <f>P243</f>
         <v>Waist level</v>
@@ -39032,14 +39173,14 @@
       <c r="E399" s="299"/>
       <c r="F399" s="299"/>
       <c r="G399" s="299"/>
-      <c r="H399" s="593" t="s">
+      <c r="H399" s="631" t="s">
         <v>394</v>
       </c>
-      <c r="I399" s="593"/>
-      <c r="J399" s="593" t="s">
+      <c r="I399" s="631"/>
+      <c r="J399" s="631" t="s">
         <v>395</v>
       </c>
-      <c r="K399" s="593"/>
+      <c r="K399" s="631"/>
       <c r="L399" s="299"/>
       <c r="M399" s="300"/>
       <c r="O399" s="13"/>
@@ -39613,20 +39754,20 @@
       </c>
       <c r="B413" s="301"/>
       <c r="C413" s="42"/>
-      <c r="D413" s="594" t="s">
+      <c r="D413" s="612" t="s">
         <v>401</v>
       </c>
-      <c r="E413" s="594"/>
-      <c r="F413" s="594"/>
-      <c r="G413" s="594"/>
-      <c r="H413" s="594"/>
-      <c r="I413" s="594" t="s">
+      <c r="E413" s="612"/>
+      <c r="F413" s="612"/>
+      <c r="G413" s="612"/>
+      <c r="H413" s="612"/>
+      <c r="I413" s="612" t="s">
         <v>402</v>
       </c>
-      <c r="J413" s="594"/>
-      <c r="K413" s="594"/>
-      <c r="L413" s="594"/>
-      <c r="M413" s="595"/>
+      <c r="J413" s="612"/>
+      <c r="K413" s="612"/>
+      <c r="L413" s="612"/>
+      <c r="M413" s="613"/>
       <c r="O413" s="13"/>
       <c r="P413" s="2" t="s">
         <v>189</v>
@@ -41106,11 +41247,11 @@
         <f t="shared" si="95"/>
         <v/>
       </c>
-      <c r="F442" s="596" t="str">
+      <c r="F442" s="614" t="str">
         <f t="shared" si="95"/>
         <v/>
       </c>
-      <c r="G442" s="598" t="str">
+      <c r="G442" s="616" t="str">
         <f t="shared" si="95"/>
         <v/>
       </c>
@@ -41151,8 +41292,8 @@
         <f>P359</f>
         <v/>
       </c>
-      <c r="F443" s="597"/>
-      <c r="G443" s="599"/>
+      <c r="F443" s="615"/>
+      <c r="G443" s="617"/>
       <c r="H443" s="200"/>
       <c r="I443" s="82" t="str">
         <f>T360</f>
@@ -41192,11 +41333,11 @@
         <f>P360</f>
         <v/>
       </c>
-      <c r="F444" s="597" t="str">
+      <c r="F444" s="615" t="str">
         <f>Q360</f>
         <v/>
       </c>
-      <c r="G444" s="599"/>
+      <c r="G444" s="617"/>
       <c r="H444" s="135"/>
       <c r="I444" s="91" t="str">
         <f>T361</f>
@@ -41237,8 +41378,8 @@
         <f>P361</f>
         <v/>
       </c>
-      <c r="F445" s="601"/>
-      <c r="G445" s="600"/>
+      <c r="F445" s="619"/>
+      <c r="G445" s="618"/>
       <c r="H445" s="135"/>
       <c r="I445" s="135"/>
       <c r="J445" s="135"/>
@@ -47597,68 +47738,35 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="106">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="W107:Y107"/>
-    <mergeCell ref="Q139:S139"/>
-    <mergeCell ref="T139:V139"/>
-    <mergeCell ref="W139:Y139"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="T181:U181"/>
-    <mergeCell ref="O190:O194"/>
-    <mergeCell ref="O195:O199"/>
-    <mergeCell ref="O200:O204"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="Q107:S107"/>
-    <mergeCell ref="T107:V107"/>
-    <mergeCell ref="O214:O218"/>
-    <mergeCell ref="O219:O223"/>
-    <mergeCell ref="O224:O228"/>
-    <mergeCell ref="O240:O241"/>
-    <mergeCell ref="O242:O243"/>
-    <mergeCell ref="Q257:R257"/>
-    <mergeCell ref="T257:U257"/>
-    <mergeCell ref="E269:G269"/>
-    <mergeCell ref="H269:J269"/>
-    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="E204:E205"/>
+    <mergeCell ref="F204:F205"/>
+    <mergeCell ref="H204:H205"/>
+    <mergeCell ref="I204:I205"/>
+    <mergeCell ref="M204:M205"/>
+    <mergeCell ref="C371:C375"/>
+    <mergeCell ref="C376:C380"/>
+    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="H399:I399"/>
+    <mergeCell ref="J399:K399"/>
+    <mergeCell ref="D413:H413"/>
+    <mergeCell ref="I413:M413"/>
+    <mergeCell ref="F442:F443"/>
+    <mergeCell ref="G442:G445"/>
+    <mergeCell ref="F444:F445"/>
+    <mergeCell ref="C337:C339"/>
+    <mergeCell ref="C340:C342"/>
+    <mergeCell ref="C343:C345"/>
+    <mergeCell ref="C346:C348"/>
+    <mergeCell ref="C349:C351"/>
+    <mergeCell ref="Q358:Q359"/>
+    <mergeCell ref="R358:R361"/>
+    <mergeCell ref="Q360:Q361"/>
+    <mergeCell ref="C366:C370"/>
+    <mergeCell ref="P293:S293"/>
+    <mergeCell ref="P302:S302"/>
+    <mergeCell ref="C303:C307"/>
+    <mergeCell ref="C308:C312"/>
+    <mergeCell ref="C313:C317"/>
     <mergeCell ref="V319:W319"/>
     <mergeCell ref="C324:C325"/>
     <mergeCell ref="Q329:U329"/>
@@ -47674,35 +47782,68 @@
     <mergeCell ref="C277:C279"/>
     <mergeCell ref="C280:C282"/>
     <mergeCell ref="C283:C285"/>
-    <mergeCell ref="Q358:Q359"/>
-    <mergeCell ref="R358:R361"/>
-    <mergeCell ref="Q360:Q361"/>
-    <mergeCell ref="C366:C370"/>
-    <mergeCell ref="P293:S293"/>
-    <mergeCell ref="P302:S302"/>
-    <mergeCell ref="C303:C307"/>
-    <mergeCell ref="C308:C312"/>
-    <mergeCell ref="C313:C317"/>
-    <mergeCell ref="D413:H413"/>
-    <mergeCell ref="I413:M413"/>
-    <mergeCell ref="F442:F443"/>
-    <mergeCell ref="G442:G445"/>
-    <mergeCell ref="F444:F445"/>
-    <mergeCell ref="C337:C339"/>
-    <mergeCell ref="C340:C342"/>
-    <mergeCell ref="C343:C345"/>
-    <mergeCell ref="C346:C348"/>
-    <mergeCell ref="C349:C351"/>
-    <mergeCell ref="E204:E205"/>
-    <mergeCell ref="F204:F205"/>
-    <mergeCell ref="H204:H205"/>
-    <mergeCell ref="I204:I205"/>
-    <mergeCell ref="M204:M205"/>
-    <mergeCell ref="C371:C375"/>
-    <mergeCell ref="C376:C380"/>
-    <mergeCell ref="C388:C389"/>
-    <mergeCell ref="H399:I399"/>
-    <mergeCell ref="J399:K399"/>
+    <mergeCell ref="O214:O218"/>
+    <mergeCell ref="O219:O223"/>
+    <mergeCell ref="O224:O228"/>
+    <mergeCell ref="O240:O241"/>
+    <mergeCell ref="O242:O243"/>
+    <mergeCell ref="Q257:R257"/>
+    <mergeCell ref="T257:U257"/>
+    <mergeCell ref="E269:G269"/>
+    <mergeCell ref="H269:J269"/>
+    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="T181:U181"/>
+    <mergeCell ref="O190:O194"/>
+    <mergeCell ref="O195:O199"/>
+    <mergeCell ref="O200:O204"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="Q107:S107"/>
+    <mergeCell ref="T107:V107"/>
+    <mergeCell ref="W107:Y107"/>
+    <mergeCell ref="Q139:S139"/>
+    <mergeCell ref="T139:V139"/>
+    <mergeCell ref="W139:Y139"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
   </mergeCells>
   <conditionalFormatting sqref="S126 V126 Y126 S158 V158 Y158">
     <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
@@ -48022,39 +48163,39 @@
         <f>Fluoro!D269</f>
         <v>Attenuator</v>
       </c>
-      <c r="E5" s="613" t="str">
+      <c r="E5" s="593" t="str">
         <f>Fluoro!E269</f>
         <v>Auto 1</v>
       </c>
-      <c r="F5" s="613">
+      <c r="F5" s="593">
         <f>Fluoro!F269</f>
         <v>0</v>
       </c>
-      <c r="G5" s="613">
+      <c r="G5" s="593">
         <f>Fluoro!G269</f>
         <v>0</v>
       </c>
-      <c r="H5" s="613" t="str">
+      <c r="H5" s="593" t="str">
         <f>Fluoro!H269</f>
         <v/>
       </c>
-      <c r="I5" s="613">
+      <c r="I5" s="593">
         <f>Fluoro!I269</f>
         <v>0</v>
       </c>
-      <c r="J5" s="613">
+      <c r="J5" s="593">
         <f>Fluoro!J269</f>
         <v>0</v>
       </c>
-      <c r="K5" s="614" t="str">
+      <c r="K5" s="594" t="str">
         <f>Fluoro!K269</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L5" s="614">
+      <c r="L5" s="594">
         <f>Fluoro!L269</f>
         <v>0</v>
       </c>
-      <c r="M5" s="614">
+      <c r="M5" s="594">
         <f>Fluoro!M269</f>
         <v>0</v>
       </c>
@@ -48111,7 +48252,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="633" t="str">
+      <c r="C7" s="632" t="str">
         <f>Fluoro!C271</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -48161,7 +48302,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="633">
+      <c r="C8" s="632">
         <f>Fluoro!C272</f>
         <v>0</v>
       </c>
@@ -48211,7 +48352,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="633">
+      <c r="C9" s="632">
         <f>Fluoro!C273</f>
         <v>0</v>
       </c>
@@ -48261,7 +48402,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="633" t="str">
+      <c r="C10" s="632" t="str">
         <f>Fluoro!C274</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -48311,7 +48452,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="633">
+      <c r="C11" s="632">
         <f>Fluoro!C275</f>
         <v>0</v>
       </c>
@@ -48361,7 +48502,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="633">
+      <c r="C12" s="632">
         <f>Fluoro!C276</f>
         <v>0</v>
       </c>
@@ -48411,7 +48552,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="633" t="str">
+      <c r="C13" s="632" t="str">
         <f>Fluoro!C277</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -48461,7 +48602,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="633">
+      <c r="C14" s="632">
         <f>Fluoro!C278</f>
         <v>0</v>
       </c>
@@ -48511,7 +48652,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10"/>
-      <c r="C15" s="633">
+      <c r="C15" s="632">
         <f>Fluoro!C279</f>
         <v>0</v>
       </c>
@@ -48561,7 +48702,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10"/>
-      <c r="C16" s="633" t="str">
+      <c r="C16" s="632" t="str">
         <f>Fluoro!C280</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -48611,7 +48752,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="633">
+      <c r="C17" s="632">
         <f>Fluoro!C281</f>
         <v>0</v>
       </c>
@@ -48661,7 +48802,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="633">
+      <c r="C18" s="632">
         <f>Fluoro!C282</f>
         <v>0</v>
       </c>
@@ -48711,7 +48852,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="633" t="str">
+      <c r="C19" s="632" t="str">
         <f>Fluoro!C283</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -48761,7 +48902,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="633">
+      <c r="C20" s="632">
         <f>Fluoro!C284</f>
         <v>0</v>
       </c>
@@ -48811,7 +48952,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="633">
+      <c r="C21" s="632">
         <f>Fluoro!C285</f>
         <v>0</v>
       </c>
@@ -49235,39 +49376,39 @@
         <f>Fluoro!D335</f>
         <v>Attenuator</v>
       </c>
-      <c r="E37" s="613" t="str">
+      <c r="E37" s="593" t="str">
         <f>Fluoro!E335</f>
         <v>Auto 1</v>
       </c>
-      <c r="F37" s="613">
+      <c r="F37" s="593">
         <f>Fluoro!F335</f>
         <v>0</v>
       </c>
-      <c r="G37" s="613">
+      <c r="G37" s="593">
         <f>Fluoro!G335</f>
         <v>0</v>
       </c>
-      <c r="H37" s="613" t="str">
+      <c r="H37" s="593" t="str">
         <f>Fluoro!H335</f>
         <v/>
       </c>
-      <c r="I37" s="613">
+      <c r="I37" s="593">
         <f>Fluoro!I335</f>
         <v>0</v>
       </c>
-      <c r="J37" s="613">
+      <c r="J37" s="593">
         <f>Fluoro!J335</f>
         <v>0</v>
       </c>
-      <c r="K37" s="614" t="str">
+      <c r="K37" s="594" t="str">
         <f>Fluoro!K335</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L37" s="614">
+      <c r="L37" s="594">
         <f>Fluoro!L335</f>
         <v>0</v>
       </c>
-      <c r="M37" s="614">
+      <c r="M37" s="594">
         <f>Fluoro!M335</f>
         <v>0</v>
       </c>
@@ -49324,7 +49465,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="10"/>
-      <c r="C39" s="633" t="str">
+      <c r="C39" s="632" t="str">
         <f>Fluoro!C337</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49374,7 +49515,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="10"/>
-      <c r="C40" s="633">
+      <c r="C40" s="632">
         <f>Fluoro!C338</f>
         <v>0</v>
       </c>
@@ -49424,7 +49565,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="10"/>
-      <c r="C41" s="633">
+      <c r="C41" s="632">
         <f>Fluoro!C339</f>
         <v>0</v>
       </c>
@@ -49474,7 +49615,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="10"/>
-      <c r="C42" s="633" t="str">
+      <c r="C42" s="632" t="str">
         <f>Fluoro!C340</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49524,7 +49665,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="10"/>
-      <c r="C43" s="633">
+      <c r="C43" s="632">
         <f>Fluoro!C341</f>
         <v>0</v>
       </c>
@@ -49574,7 +49715,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="10"/>
-      <c r="C44" s="633">
+      <c r="C44" s="632">
         <f>Fluoro!C342</f>
         <v>0</v>
       </c>
@@ -49624,7 +49765,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="10"/>
-      <c r="C45" s="633" t="str">
+      <c r="C45" s="632" t="str">
         <f>Fluoro!C343</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49674,7 +49815,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="10"/>
-      <c r="C46" s="633">
+      <c r="C46" s="632">
         <f>Fluoro!C344</f>
         <v>0</v>
       </c>
@@ -49724,7 +49865,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="10"/>
-      <c r="C47" s="633">
+      <c r="C47" s="632">
         <f>Fluoro!C345</f>
         <v>0</v>
       </c>
@@ -49774,7 +49915,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="10"/>
-      <c r="C48" s="633" t="str">
+      <c r="C48" s="632" t="str">
         <f>Fluoro!C346</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49824,7 +49965,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="10"/>
-      <c r="C49" s="633">
+      <c r="C49" s="632">
         <f>Fluoro!C347</f>
         <v>0</v>
       </c>
@@ -49874,7 +50015,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="10"/>
-      <c r="C50" s="633">
+      <c r="C50" s="632">
         <f>Fluoro!C348</f>
         <v>0</v>
       </c>
@@ -49924,7 +50065,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="10"/>
-      <c r="C51" s="633" t="str">
+      <c r="C51" s="632" t="str">
         <f>Fluoro!C349</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49974,7 +50115,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="10"/>
-      <c r="C52" s="633">
+      <c r="C52" s="632">
         <f>Fluoro!C350</f>
         <v>0</v>
       </c>
@@ -50024,7 +50165,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="10"/>
-      <c r="C53" s="633">
+      <c r="C53" s="632">
         <f>Fluoro!C351</f>
         <v>0</v>
       </c>
@@ -50218,7 +50359,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="10"/>
-      <c r="C60" s="632"/>
+      <c r="C60" s="633"/>
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60"/>
@@ -50235,7 +50376,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="10"/>
-      <c r="C61" s="632"/>
+      <c r="C61" s="633"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>
@@ -50883,7 +51024,7 @@
     <row r="102" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102"/>
       <c r="B102"/>
-      <c r="C102" s="632"/>
+      <c r="C102" s="633"/>
       <c r="D102"/>
       <c r="E102"/>
       <c r="F102"/>
@@ -50898,7 +51039,7 @@
     <row r="103" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103"/>
       <c r="B103"/>
-      <c r="C103" s="632"/>
+      <c r="C103" s="633"/>
       <c r="D103"/>
       <c r="E103"/>
       <c r="F103"/>
@@ -50913,7 +51054,7 @@
     <row r="104" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104"/>
       <c r="B104"/>
-      <c r="C104" s="632"/>
+      <c r="C104" s="633"/>
       <c r="D104"/>
       <c r="E104"/>
       <c r="F104"/>
@@ -50928,7 +51069,7 @@
     <row r="105" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105"/>
       <c r="B105"/>
-      <c r="C105" s="632"/>
+      <c r="C105" s="633"/>
       <c r="D105"/>
       <c r="E105"/>
       <c r="F105"/>
@@ -50943,7 +51084,7 @@
     <row r="106" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106"/>
       <c r="B106"/>
-      <c r="C106" s="632"/>
+      <c r="C106" s="633"/>
       <c r="D106"/>
       <c r="E106"/>
       <c r="F106"/>
@@ -50958,7 +51099,7 @@
     <row r="107" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107"/>
       <c r="B107"/>
-      <c r="C107" s="632"/>
+      <c r="C107" s="633"/>
       <c r="D107"/>
       <c r="E107"/>
       <c r="F107"/>
@@ -50973,7 +51114,7 @@
     <row r="108" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108"/>
       <c r="B108"/>
-      <c r="C108" s="632"/>
+      <c r="C108" s="633"/>
       <c r="D108"/>
       <c r="E108"/>
       <c r="F108"/>
@@ -50988,7 +51129,7 @@
     <row r="109" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109"/>
       <c r="B109"/>
-      <c r="C109" s="632"/>
+      <c r="C109" s="633"/>
       <c r="D109"/>
       <c r="E109"/>
       <c r="F109"/>
@@ -51003,7 +51144,7 @@
     <row r="110" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110"/>
       <c r="B110"/>
-      <c r="C110" s="632"/>
+      <c r="C110" s="633"/>
       <c r="D110"/>
       <c r="E110"/>
       <c r="F110"/>
@@ -51018,7 +51159,7 @@
     <row r="111" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111"/>
       <c r="B111"/>
-      <c r="C111" s="632"/>
+      <c r="C111" s="633"/>
       <c r="D111"/>
       <c r="E111"/>
       <c r="F111"/>
@@ -51033,7 +51174,7 @@
     <row r="112" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112"/>
       <c r="B112"/>
-      <c r="C112" s="632"/>
+      <c r="C112" s="633"/>
       <c r="D112"/>
       <c r="E112"/>
       <c r="F112"/>
@@ -51048,7 +51189,7 @@
     <row r="113" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113"/>
       <c r="B113"/>
-      <c r="C113" s="632"/>
+      <c r="C113" s="633"/>
       <c r="D113"/>
       <c r="E113"/>
       <c r="F113"/>
@@ -51063,7 +51204,7 @@
     <row r="114" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114"/>
       <c r="B114"/>
-      <c r="C114" s="632"/>
+      <c r="C114" s="633"/>
       <c r="D114"/>
       <c r="E114"/>
       <c r="F114"/>
@@ -51078,7 +51219,7 @@
     <row r="115" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115"/>
       <c r="B115"/>
-      <c r="C115" s="632"/>
+      <c r="C115" s="633"/>
       <c r="D115"/>
       <c r="E115"/>
       <c r="F115"/>
@@ -51093,7 +51234,7 @@
     <row r="116" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116"/>
       <c r="B116"/>
-      <c r="C116" s="632"/>
+      <c r="C116" s="633"/>
       <c r="D116"/>
       <c r="E116"/>
       <c r="F116"/>
@@ -51213,7 +51354,7 @@
     <row r="124" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124"/>
       <c r="B124"/>
-      <c r="C124" s="632"/>
+      <c r="C124" s="633"/>
       <c r="D124"/>
       <c r="E124"/>
       <c r="F124"/>
@@ -51228,7 +51369,7 @@
     <row r="125" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125"/>
       <c r="B125"/>
-      <c r="C125" s="632"/>
+      <c r="C125" s="633"/>
       <c r="D125"/>
       <c r="E125"/>
       <c r="F125"/>
@@ -51360,17 +51501,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="21">
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C21"/>
     <mergeCell ref="C102:C106"/>
     <mergeCell ref="C107:C111"/>
     <mergeCell ref="C112:C116"/>
@@ -51381,6 +51511,17 @@
     <mergeCell ref="C48:C50"/>
     <mergeCell ref="C51:C53"/>
     <mergeCell ref="C60:C61"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="68" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -51412,29 +51553,29 @@
       </c>
       <c r="B1" s="634"/>
       <c r="N1" s="278"/>
-      <c r="O1" s="607" t="str">
+      <c r="O1" s="606" t="str">
         <f>Fluoro!O105</f>
         <v>Patient Entrance Exposure Rate (Fluoroscopy)*</v>
       </c>
-      <c r="P1" s="607"/>
-      <c r="Q1" s="607"/>
-      <c r="R1" s="607" t="s">
+      <c r="P1" s="606"/>
+      <c r="Q1" s="606"/>
+      <c r="R1" s="606" t="s">
         <v>407</v>
       </c>
-      <c r="S1" s="607"/>
-      <c r="T1" s="607"/>
+      <c r="S1" s="606"/>
+      <c r="T1" s="606"/>
       <c r="V1" s="278"/>
-      <c r="W1" s="607" t="str">
+      <c r="W1" s="606" t="str">
         <f>Fluoro!O137</f>
         <v>Patient Entrance Exposure Rate – Digital Acquisition</v>
       </c>
-      <c r="X1" s="607"/>
-      <c r="Y1" s="607"/>
-      <c r="Z1" s="607" t="s">
+      <c r="X1" s="606"/>
+      <c r="Y1" s="606"/>
+      <c r="Z1" s="606" t="s">
         <v>407</v>
       </c>
-      <c r="AA1" s="607"/>
-      <c r="AB1" s="607"/>
+      <c r="AA1" s="606"/>
+      <c r="AB1" s="606"/>
     </row>
     <row r="2" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="279">
@@ -55427,14 +55568,14 @@
       <c r="B75" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E75" s="607" t="s">
+      <c r="E75" s="606" t="s">
         <v>420</v>
       </c>
-      <c r="F75" s="607"/>
-      <c r="I75" s="607" t="s">
+      <c r="F75" s="606"/>
+      <c r="I75" s="606" t="s">
         <v>421</v>
       </c>
-      <c r="J75" s="607"/>
+      <c r="J75" s="606"/>
     </row>
     <row r="76" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">

</xml_diff>

<commit_message>
Integrate with Ocean Next data
</commit_message>
<xml_diff>
--- a/MUSCCArm.xlsx
+++ b/MUSCCArm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0927F91-23FF-4D09-BD90-383FA5D8654B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD8DA39-6632-4DB1-A508-CCDD1FC45F1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="473">
   <si>
     <t>Print Area</t>
   </si>
@@ -1520,9 +1520,6 @@
     <t>Calibration due:</t>
   </si>
   <si>
-    <t>Revision 1.5-20200128</t>
-  </si>
-  <si>
     <t>Exp rate (mGy/min)</t>
   </si>
   <si>
@@ -1549,6 +1546,48 @@
   <si>
     <t>Radcal 90-2123</t>
   </si>
+  <si>
+    <t>Measurements</t>
+  </si>
+  <si>
+    <t>Set kV_x000D_(kV)</t>
+  </si>
+  <si>
+    <t>Tube voltage_x000D_(kV)</t>
+  </si>
+  <si>
+    <t>Exposure_x000D_(mGy)</t>
+  </si>
+  <si>
+    <t>Exposure rate_x000D_(mGy/min)</t>
+  </si>
+  <si>
+    <t>HVL_x000D_(mm Al)</t>
+  </si>
+  <si>
+    <t>Total filtr._x000D_(mm Al)</t>
+  </si>
+  <si>
+    <t>Set frames/s_x000D_(FPS)</t>
+  </si>
+  <si>
+    <t>Frames/s_x000D_(FPS)</t>
+  </si>
+  <si>
+    <t>Exposure/frame_x000D_(µGy/frame)</t>
+  </si>
+  <si>
+    <t>Frame exp. rate_x000D_(mGy/s)</t>
+  </si>
+  <si>
+    <t>Pulse width_x000D_(ms)</t>
+  </si>
+  <si>
+    <t>Duty cycle ∆_x000D_(%)</t>
+  </si>
+  <si>
+    <t>Revision 1.6-20220428</t>
+  </si>
 </sst>
 </file>
 
@@ -1566,7 +1605,7 @@
     <numFmt numFmtId="172" formatCode="[$-409]d/mmm/yyyy;@"/>
     <numFmt numFmtId="173" formatCode="mmm/yyyy"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
@@ -1702,8 +1741,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1767,6 +1813,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4675,7 +4727,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="639">
+  <cellXfs count="642">
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6422,6 +6474,141 @@
     <xf numFmtId="172" fontId="3" fillId="5" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="200" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="222" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="223" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="127" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="155" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="182" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="149" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="150" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="175" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="151" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="176" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="154" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="180" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6440,30 +6627,12 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="200" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="201" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="149" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="150" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="151" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="183" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6473,127 +6642,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="193" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="127" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="155" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="182" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="175" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="176" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="154" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="180" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="222" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="223" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -20395,8 +20456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD792"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W103" sqref="W103"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20426,7 +20487,7 @@
       <c r="L1" s="299"/>
       <c r="M1" s="300"/>
       <c r="O1" s="6" t="s">
-        <v>450</v>
+        <v>472</v>
       </c>
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
@@ -20466,7 +20527,7 @@
       </c>
       <c r="Y2" s="14"/>
       <c r="AA2" s="15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20519,7 +20580,7 @@
         <v>3</v>
       </c>
       <c r="AB4" s="17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20707,21 +20768,21 @@
       <c r="E10" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="632" t="str">
+      <c r="F10" s="582" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="632"/>
+      <c r="G10" s="582"/>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
       <c r="J10" s="160" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="621" t="str">
+      <c r="K10" s="583" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="621"/>
+      <c r="L10" s="583"/>
       <c r="M10" s="312"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="2" t="s">
@@ -20764,21 +20825,21 @@
       <c r="E11" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="622" t="str">
+      <c r="F11" s="584" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="622"/>
+      <c r="G11" s="584"/>
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
       <c r="J11" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="622" t="str">
+      <c r="K11" s="584" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="622"/>
+      <c r="L11" s="584"/>
       <c r="M11" s="312"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="2" t="s">
@@ -20821,21 +20882,21 @@
       <c r="E12" s="160" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="622" t="str">
+      <c r="F12" s="584" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="622"/>
+      <c r="G12" s="584"/>
       <c r="H12" s="42"/>
       <c r="I12" s="42"/>
       <c r="J12" s="160" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="634" t="str">
+      <c r="K12" s="585" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="634"/>
+      <c r="L12" s="585"/>
       <c r="M12" s="312"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="2" t="s">
@@ -20878,21 +20939,21 @@
       <c r="E13" s="160" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="623" t="str">
+      <c r="F13" s="586" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="623"/>
+      <c r="G13" s="586"/>
       <c r="H13" s="42"/>
       <c r="I13" s="42"/>
       <c r="J13" s="160" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="623" t="str">
+      <c r="K13" s="586" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="623"/>
+      <c r="L13" s="586"/>
       <c r="M13" s="312"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="2" t="s">
@@ -21015,21 +21076,21 @@
       <c r="E16" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="632" t="str">
+      <c r="F16" s="582" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="632"/>
+      <c r="G16" s="582"/>
       <c r="H16" s="42"/>
       <c r="I16" s="42"/>
       <c r="J16" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="635" t="str">
+      <c r="K16" s="587" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="635"/>
+      <c r="L16" s="587"/>
       <c r="M16" s="312"/>
       <c r="O16" s="13"/>
       <c r="P16" s="50" t="s">
@@ -21059,21 +21120,21 @@
       <c r="E17" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="622" t="str">
+      <c r="F17" s="584" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="622"/>
+      <c r="G17" s="584"/>
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
       <c r="J17" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="623" t="str">
+      <c r="K17" s="586" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="623"/>
+      <c r="L17" s="586"/>
       <c r="M17" s="312"/>
       <c r="O17" s="13"/>
       <c r="Q17" s="2" t="s">
@@ -21116,21 +21177,21 @@
       <c r="E18" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="623" t="str">
+      <c r="F18" s="586" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="623"/>
+      <c r="G18" s="586"/>
       <c r="H18" s="42"/>
       <c r="I18" s="42"/>
       <c r="J18" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="623" t="str">
+      <c r="K18" s="586" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="623"/>
+      <c r="L18" s="586"/>
       <c r="M18" s="312"/>
       <c r="O18" s="13"/>
       <c r="Q18" s="2" t="s">
@@ -21178,11 +21239,11 @@
       <c r="J19" s="160" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="623" t="str">
+      <c r="K19" s="586" t="str">
         <f>IF(V20="","",V20)</f>
         <v/>
       </c>
-      <c r="L19" s="623"/>
+      <c r="L19" s="586"/>
       <c r="M19" s="312"/>
       <c r="O19" s="13"/>
       <c r="Q19" s="2" t="s">
@@ -21257,11 +21318,11 @@
       <c r="E21" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="632" t="str">
+      <c r="F21" s="582" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="632"/>
+      <c r="G21" s="582"/>
       <c r="H21" s="42"/>
       <c r="I21" s="42"/>
       <c r="J21" s="73" t="s">
@@ -21301,21 +21362,21 @@
       <c r="E22" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="633" t="str">
+      <c r="F22" s="588" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="633"/>
+      <c r="G22" s="588"/>
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
       <c r="J22" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="632" t="str">
+      <c r="K22" s="582" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="632"/>
+      <c r="L22" s="582"/>
       <c r="M22" s="312"/>
       <c r="O22" s="13"/>
       <c r="Q22" s="2" t="s">
@@ -21360,11 +21421,11 @@
       <c r="J23" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="622" t="str">
+      <c r="K23" s="584" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="622"/>
+      <c r="L23" s="584"/>
       <c r="M23" s="312"/>
       <c r="O23" s="13"/>
       <c r="Q23" s="2" t="s">
@@ -21407,21 +21468,21 @@
       <c r="E24" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="621" t="str">
+      <c r="F24" s="583" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="621"/>
+      <c r="G24" s="583"/>
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
       <c r="J24" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="622" t="str">
+      <c r="K24" s="584" t="str">
         <f>IF(V25="","",V25)</f>
         <v/>
       </c>
-      <c r="L24" s="622"/>
+      <c r="L24" s="584"/>
       <c r="M24" s="312"/>
       <c r="O24" s="13"/>
       <c r="P24" s="50" t="s">
@@ -21459,11 +21520,11 @@
       <c r="E25" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="623" t="str">
+      <c r="F25" s="586" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="623"/>
+      <c r="G25" s="586"/>
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
@@ -21511,11 +21572,11 @@
       <c r="E26" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="623" t="str">
+      <c r="F26" s="586" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="623"/>
+      <c r="G26" s="586"/>
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
       <c r="J26" s="313" t="s">
@@ -21564,11 +21625,11 @@
       <c r="J27" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="632" t="str">
+      <c r="K27" s="582" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="632"/>
+      <c r="L27" s="582"/>
       <c r="M27" s="312"/>
       <c r="O27" s="13"/>
       <c r="Q27" s="2" t="s">
@@ -21606,21 +21667,21 @@
       <c r="E28" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="621" t="str">
+      <c r="F28" s="583" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="621"/>
+      <c r="G28" s="583"/>
       <c r="H28" s="42"/>
       <c r="I28" s="42"/>
       <c r="J28" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="622" t="str">
+      <c r="K28" s="584" t="str">
         <f>IF(V29="","",V29)</f>
         <v/>
       </c>
-      <c r="L28" s="622"/>
+      <c r="L28" s="584"/>
       <c r="M28" s="312"/>
       <c r="O28" s="13"/>
       <c r="P28" s="50" t="s">
@@ -21649,11 +21710,11 @@
       <c r="E29" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="623" t="str">
+      <c r="F29" s="586" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="623"/>
+      <c r="G29" s="586"/>
       <c r="H29" s="42"/>
       <c r="I29" s="42"/>
       <c r="J29" s="42"/>
@@ -21701,11 +21762,11 @@
       <c r="E30" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="623" t="str">
+      <c r="F30" s="586" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="623"/>
+      <c r="G30" s="586"/>
       <c r="H30" s="42"/>
       <c r="I30" s="42"/>
       <c r="J30" s="42"/>
@@ -21820,11 +21881,11 @@
       <c r="E33" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="632" t="str">
+      <c r="F33" s="582" t="str">
         <f>IF(R34="","",R34)</f>
         <v/>
       </c>
-      <c r="G33" s="632"/>
+      <c r="G33" s="582"/>
       <c r="H33" s="42"/>
       <c r="I33" s="42"/>
       <c r="J33" s="73" t="s">
@@ -21861,21 +21922,21 @@
       <c r="E34" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="633" t="str">
+      <c r="F34" s="588" t="str">
         <f>IF(R35="","",R35)</f>
         <v/>
       </c>
-      <c r="G34" s="633"/>
+      <c r="G34" s="588"/>
       <c r="H34" s="42"/>
       <c r="I34" s="42"/>
       <c r="J34" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="632" t="str">
+      <c r="K34" s="582" t="str">
         <f>IF(V35="","",V35)</f>
         <v/>
       </c>
-      <c r="L34" s="632"/>
+      <c r="L34" s="582"/>
       <c r="M34" s="312"/>
       <c r="O34" s="13"/>
       <c r="Q34" s="2" t="s">
@@ -21920,11 +21981,11 @@
       <c r="J35" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="K35" s="622" t="str">
+      <c r="K35" s="584" t="str">
         <f>IF(V36="","",V36)</f>
         <v/>
       </c>
-      <c r="L35" s="622"/>
+      <c r="L35" s="584"/>
       <c r="M35" s="312"/>
       <c r="O35" s="13"/>
       <c r="Q35" s="2" t="s">
@@ -21967,21 +22028,21 @@
       <c r="E36" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="621" t="str">
+      <c r="F36" s="583" t="str">
         <f>IF(R37="","",R37)</f>
         <v/>
       </c>
-      <c r="G36" s="621"/>
+      <c r="G36" s="583"/>
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
       <c r="J36" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="K36" s="622" t="str">
+      <c r="K36" s="584" t="str">
         <f>IF(V37="","",V37)</f>
         <v/>
       </c>
-      <c r="L36" s="622"/>
+      <c r="L36" s="584"/>
       <c r="M36" s="312"/>
       <c r="O36" s="13"/>
       <c r="P36" s="50" t="s">
@@ -22019,11 +22080,11 @@
       <c r="E37" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="623" t="str">
+      <c r="F37" s="586" t="str">
         <f>IF(R38="","",R38)</f>
         <v/>
       </c>
-      <c r="G37" s="623"/>
+      <c r="G37" s="586"/>
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
       <c r="J37" s="42"/>
@@ -22071,11 +22132,11 @@
       <c r="E38" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="623" t="str">
+      <c r="F38" s="586" t="str">
         <f>IF(R39="","",R39)</f>
         <v/>
       </c>
-      <c r="G38" s="623"/>
+      <c r="G38" s="586"/>
       <c r="H38" s="42"/>
       <c r="I38" s="42"/>
       <c r="J38" s="313" t="s">
@@ -22122,11 +22183,11 @@
       <c r="J39" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="K39" s="632" t="str">
+      <c r="K39" s="582" t="str">
         <f>IF(V40="","",V40)</f>
         <v/>
       </c>
-      <c r="L39" s="632"/>
+      <c r="L39" s="582"/>
       <c r="M39" s="312"/>
       <c r="O39" s="13"/>
       <c r="Q39" s="2" t="s">
@@ -22164,21 +22225,21 @@
       <c r="E40" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="621" t="str">
+      <c r="F40" s="583" t="str">
         <f>IF(R41="","",R41)</f>
         <v/>
       </c>
-      <c r="G40" s="621"/>
+      <c r="G40" s="583"/>
       <c r="H40" s="42"/>
       <c r="I40" s="42"/>
       <c r="J40" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K40" s="622" t="str">
+      <c r="K40" s="584" t="str">
         <f>IF(V41="","",V41)</f>
         <v/>
       </c>
-      <c r="L40" s="622"/>
+      <c r="L40" s="584"/>
       <c r="M40" s="312"/>
       <c r="O40" s="13"/>
       <c r="P40" s="50" t="s">
@@ -22216,11 +22277,11 @@
       <c r="E41" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="623" t="str">
+      <c r="F41" s="586" t="str">
         <f>IF(R42="","",R42)</f>
         <v/>
       </c>
-      <c r="G41" s="623"/>
+      <c r="G41" s="586"/>
       <c r="H41" s="42"/>
       <c r="I41" s="42"/>
       <c r="J41" s="42"/>
@@ -22268,11 +22329,11 @@
       <c r="E42" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="623" t="str">
+      <c r="F42" s="586" t="str">
         <f>IF(R43="","",R43)</f>
         <v/>
       </c>
-      <c r="G42" s="623"/>
+      <c r="G42" s="586"/>
       <c r="H42" s="42"/>
       <c r="I42" s="42"/>
       <c r="J42" s="42"/>
@@ -22454,7 +22515,7 @@
         <v>2</v>
       </c>
       <c r="Q48" s="335" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="S48" s="53"/>
       <c r="T48" s="49" t="s">
@@ -22515,7 +22576,7 @@
       </c>
       <c r="O50" s="56"/>
       <c r="P50" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="U50" s="53"/>
       <c r="W50" s="17" t="s">
@@ -23039,10 +23100,10 @@
       <c r="I69" s="299"/>
       <c r="J69" s="299"/>
       <c r="K69" s="299"/>
-      <c r="L69" s="624" t="s">
+      <c r="L69" s="593" t="s">
         <v>83</v>
       </c>
-      <c r="M69" s="625"/>
+      <c r="M69" s="594"/>
       <c r="O69" s="56"/>
       <c r="P69" s="17" t="s">
         <v>84</v>
@@ -23115,7 +23176,7 @@
       </c>
       <c r="D71" s="135"/>
       <c r="E71" s="70" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F71" s="135"/>
       <c r="G71" s="135"/>
@@ -24357,7 +24418,7 @@
         <v>Radcal 90-2123</v>
       </c>
       <c r="W100" s="579" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="X100" s="1" t="s">
         <v>445</v>
@@ -24711,24 +24772,24 @@
       <c r="P107" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="Q107" s="626" t="str">
+      <c r="Q107" s="590" t="str">
         <f>IF(Q106&lt;&gt;"",Q106,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R107" s="626"/>
-      <c r="S107" s="626"/>
-      <c r="T107" s="627" t="str">
+      <c r="R107" s="590"/>
+      <c r="S107" s="590"/>
+      <c r="T107" s="589" t="str">
         <f>IF(T106&lt;&gt;"",T106,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v/>
       </c>
-      <c r="U107" s="627"/>
-      <c r="V107" s="627"/>
-      <c r="W107" s="627" t="str">
+      <c r="U107" s="589"/>
+      <c r="V107" s="589"/>
+      <c r="W107" s="589" t="str">
         <f>IF(W106&lt;&gt;"",W106,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="X107" s="627"/>
-      <c r="Y107" s="627"/>
+      <c r="X107" s="589"/>
+      <c r="Y107" s="589"/>
       <c r="AA107" s="2" t="s">
         <v>152</v>
       </c>
@@ -26720,24 +26781,24 @@
       <c r="P139" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="Q139" s="626" t="str">
+      <c r="Q139" s="590" t="str">
         <f>IF(Q138&lt;&gt;"",Q138,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R139" s="626"/>
-      <c r="S139" s="626"/>
-      <c r="T139" s="627" t="str">
+      <c r="R139" s="590"/>
+      <c r="S139" s="590"/>
+      <c r="T139" s="589" t="str">
         <f>IF(T138&lt;&gt;"",T138,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v/>
       </c>
-      <c r="U139" s="627"/>
-      <c r="V139" s="627"/>
-      <c r="W139" s="627" t="str">
+      <c r="U139" s="589"/>
+      <c r="V139" s="589"/>
+      <c r="W139" s="589" t="str">
         <f>IF(W138&lt;&gt;"",W138,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="X139" s="627"/>
-      <c r="Y139" s="627"/>
+      <c r="X139" s="589"/>
+      <c r="Y139" s="589"/>
       <c r="AA139" s="2" t="str">
         <f>$T$139&amp;" Mag 4"</f>
         <v xml:space="preserve"> Mag 4</v>
@@ -29081,10 +29142,10 @@
       <c r="P181" s="135"/>
       <c r="Q181" s="137"/>
       <c r="R181" s="128"/>
-      <c r="T181" s="609" t="s">
+      <c r="T181" s="591" t="s">
         <v>244</v>
       </c>
-      <c r="U181" s="609"/>
+      <c r="U181" s="591"/>
       <c r="W181" s="2" t="s">
         <v>198</v>
       </c>
@@ -29455,7 +29516,7 @@
       <c r="K190" s="323"/>
       <c r="L190" s="323"/>
       <c r="M190" s="327"/>
-      <c r="O190" s="618" t="str">
+      <c r="O190" s="592" t="str">
         <f>$Q$107</f>
         <v>Auto 1</v>
       </c>
@@ -29505,7 +29566,7 @@
       <c r="K191" s="323"/>
       <c r="L191" s="323"/>
       <c r="M191" s="303"/>
-      <c r="O191" s="618"/>
+      <c r="O191" s="592"/>
       <c r="P191" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -29551,7 +29612,7 @@
       <c r="K192" s="135"/>
       <c r="L192" s="135"/>
       <c r="M192" s="303"/>
-      <c r="O192" s="618"/>
+      <c r="O192" s="592"/>
       <c r="P192" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -29597,7 +29658,7 @@
       <c r="K193" s="135"/>
       <c r="L193" s="135"/>
       <c r="M193" s="303"/>
-      <c r="O193" s="618"/>
+      <c r="O193" s="592"/>
       <c r="P193" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -29640,7 +29701,7 @@
       <c r="K194" s="135"/>
       <c r="L194" s="135"/>
       <c r="M194" s="303"/>
-      <c r="O194" s="618"/>
+      <c r="O194" s="592"/>
       <c r="P194" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -29683,7 +29744,7 @@
       <c r="K195" s="135"/>
       <c r="L195" s="135"/>
       <c r="M195" s="303"/>
-      <c r="O195" s="618" t="str">
+      <c r="O195" s="592" t="str">
         <f>$T$107</f>
         <v/>
       </c>
@@ -29729,7 +29790,7 @@
       <c r="K196" s="305"/>
       <c r="L196" s="305"/>
       <c r="M196" s="306"/>
-      <c r="O196" s="618"/>
+      <c r="O196" s="592"/>
       <c r="P196" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -29774,7 +29835,7 @@
         <f>IF($X$7="","",$X$7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="O197" s="618"/>
+      <c r="O197" s="592"/>
       <c r="P197" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -29819,7 +29880,7 @@
         <f>IF($R$13="","",$R$13)</f>
         <v/>
       </c>
-      <c r="O198" s="618"/>
+      <c r="O198" s="592"/>
       <c r="P198" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -29865,7 +29926,7 @@
         <f>$H$2</f>
         <v>Medical University of South Carolina</v>
       </c>
-      <c r="O199" s="618"/>
+      <c r="O199" s="592"/>
       <c r="P199" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -29914,7 +29975,7 @@
         <f>$H$5</f>
         <v>Fluoroscopy System Compliance Inspection</v>
       </c>
-      <c r="O200" s="618" t="str">
+      <c r="O200" s="592" t="str">
         <f>$W$107</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -29963,7 +30024,7 @@
       <c r="K201" s="299"/>
       <c r="L201" s="299"/>
       <c r="M201" s="300"/>
-      <c r="O201" s="618"/>
+      <c r="O201" s="592"/>
       <c r="P201" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30000,24 +30061,24 @@
       </c>
       <c r="D202" s="66" t="str">
         <f>IF(R266="","",R266)</f>
-        <v/>
+        <v>Radcal 90-2123</v>
       </c>
       <c r="F202" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="G202" s="513" t="str">
+      <c r="G202" s="513">
         <f>IF(U266="","",U266)</f>
-        <v/>
+        <v>44540</v>
       </c>
       <c r="I202" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="J202" s="513" t="str">
+      <c r="J202" s="513">
         <f>IF(X266="","",X266)</f>
-        <v/>
+        <v>44905</v>
       </c>
       <c r="M202" s="12"/>
-      <c r="O202" s="618"/>
+      <c r="O202" s="592"/>
       <c r="P202" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -30050,7 +30111,7 @@
       </c>
       <c r="B203" s="10"/>
       <c r="M203" s="12"/>
-      <c r="O203" s="618"/>
+      <c r="O203" s="592"/>
       <c r="P203" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -30084,20 +30145,20 @@
       <c r="B204" s="301"/>
       <c r="C204" s="351"/>
       <c r="D204" s="323"/>
-      <c r="E204" s="588" t="s">
+      <c r="E204" s="595" t="s">
         <v>261</v>
       </c>
-      <c r="F204" s="590" t="s">
+      <c r="F204" s="632" t="s">
         <v>262</v>
       </c>
       <c r="G204" s="518" t="s">
         <v>263</v>
       </c>
-      <c r="H204" s="588" t="str">
+      <c r="H204" s="595" t="str">
         <f>R276</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="I204" s="628" t="str">
+      <c r="I204" s="597" t="str">
         <f>S276</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -30110,10 +30171,10 @@
       <c r="L204" s="135" t="s">
         <v>266</v>
       </c>
-      <c r="M204" s="630" t="s">
+      <c r="M204" s="599" t="s">
         <v>267</v>
       </c>
-      <c r="O204" s="618"/>
+      <c r="O204" s="592"/>
       <c r="P204" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -30151,11 +30212,11 @@
       <c r="D205" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="E205" s="589"/>
-      <c r="F205" s="591"/>
+      <c r="E205" s="596"/>
+      <c r="F205" s="633"/>
       <c r="G205" s="518"/>
-      <c r="H205" s="589"/>
-      <c r="I205" s="629"/>
+      <c r="H205" s="596"/>
+      <c r="I205" s="598"/>
       <c r="J205" s="519"/>
       <c r="K205" s="135" t="str">
         <f>U277</f>
@@ -30165,7 +30226,7 @@
         <f>V277</f>
         <v>mGy/min</v>
       </c>
-      <c r="M205" s="631"/>
+      <c r="M205" s="600"/>
       <c r="O205" s="13"/>
       <c r="Y205" s="14"/>
       <c r="AA205" s="2" t="s">
@@ -30809,7 +30870,7 @@
         <f>W286</f>
         <v/>
       </c>
-      <c r="O214" s="618" t="str">
+      <c r="O214" s="592" t="str">
         <f>$Q$139</f>
         <v>Auto 1</v>
       </c>
@@ -30865,7 +30926,7 @@
       <c r="K215" s="135"/>
       <c r="L215" s="135"/>
       <c r="M215" s="303"/>
-      <c r="O215" s="618"/>
+      <c r="O215" s="592"/>
       <c r="P215" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30911,7 +30972,7 @@
       <c r="K216" s="323"/>
       <c r="L216" s="323"/>
       <c r="M216" s="303"/>
-      <c r="O216" s="618"/>
+      <c r="O216" s="592"/>
       <c r="P216" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -30957,7 +31018,7 @@
       <c r="K217" s="368"/>
       <c r="L217" s="368"/>
       <c r="M217" s="369"/>
-      <c r="O217" s="618"/>
+      <c r="O217" s="592"/>
       <c r="P217" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31004,7 +31065,7 @@
       <c r="K218" s="323"/>
       <c r="L218" s="323"/>
       <c r="M218" s="303"/>
-      <c r="O218" s="618"/>
+      <c r="O218" s="592"/>
       <c r="P218" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -31047,7 +31108,7 @@
       <c r="K219" s="323"/>
       <c r="L219" s="323"/>
       <c r="M219" s="327"/>
-      <c r="O219" s="618" t="str">
+      <c r="O219" s="592" t="str">
         <f>$T$139</f>
         <v/>
       </c>
@@ -31108,7 +31169,7 @@
         <v/>
       </c>
       <c r="M220" s="327"/>
-      <c r="O220" s="618"/>
+      <c r="O220" s="592"/>
       <c r="P220" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -31151,7 +31212,7 @@
       <c r="K221" s="323"/>
       <c r="L221" s="323"/>
       <c r="M221" s="327"/>
-      <c r="O221" s="618"/>
+      <c r="O221" s="592"/>
       <c r="P221" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -31189,7 +31250,7 @@
       </c>
       <c r="E222" s="323"/>
       <c r="F222" s="323" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G222" s="323"/>
       <c r="H222" s="323"/>
@@ -31197,12 +31258,12 @@
         <v>271</v>
       </c>
       <c r="J222" s="323" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K222" s="323"/>
       <c r="L222" s="323"/>
       <c r="M222" s="327"/>
-      <c r="O222" s="618"/>
+      <c r="O222" s="592"/>
       <c r="P222" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31244,7 +31305,7 @@
         <v>273</v>
       </c>
       <c r="F223" s="561" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G223" s="323"/>
       <c r="H223" s="380" t="s">
@@ -31254,12 +31315,12 @@
         <v>227</v>
       </c>
       <c r="J223" s="561" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K223" s="323"/>
       <c r="L223" s="323"/>
       <c r="M223" s="327"/>
-      <c r="O223" s="618"/>
+      <c r="O223" s="592"/>
       <c r="P223" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -31323,7 +31384,7 @@
       <c r="K224" s="323"/>
       <c r="L224" s="323"/>
       <c r="M224" s="327"/>
-      <c r="O224" s="618" t="str">
+      <c r="O224" s="592" t="str">
         <f>$W$139</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -31387,7 +31448,7 @@
       <c r="K225" s="323"/>
       <c r="L225" s="323"/>
       <c r="M225" s="327"/>
-      <c r="O225" s="618"/>
+      <c r="O225" s="592"/>
       <c r="P225" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -31448,7 +31509,7 @@
       <c r="K226" s="323"/>
       <c r="L226" s="323"/>
       <c r="M226" s="327"/>
-      <c r="O226" s="618"/>
+      <c r="O226" s="592"/>
       <c r="P226" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -31509,7 +31570,7 @@
       <c r="K227" s="323"/>
       <c r="L227" s="323"/>
       <c r="M227" s="327"/>
-      <c r="O227" s="618"/>
+      <c r="O227" s="592"/>
       <c r="P227" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31563,7 +31624,7 @@
       <c r="K228" s="323"/>
       <c r="L228" s="323"/>
       <c r="M228" s="327"/>
-      <c r="O228" s="618"/>
+      <c r="O228" s="592"/>
       <c r="P228" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -32116,7 +32177,7 @@
       <c r="K240" s="323"/>
       <c r="L240" s="323"/>
       <c r="M240" s="327"/>
-      <c r="O240" s="619" t="s">
+      <c r="O240" s="601" t="s">
         <v>293</v>
       </c>
       <c r="P240" s="167" t="s">
@@ -32175,7 +32236,7 @@
       <c r="K241" s="323"/>
       <c r="L241" s="323"/>
       <c r="M241" s="327"/>
-      <c r="O241" s="619"/>
+      <c r="O241" s="601"/>
       <c r="P241" s="172" t="s">
         <v>296</v>
       </c>
@@ -32232,7 +32293,7 @@
       <c r="K242" s="323"/>
       <c r="L242" s="323"/>
       <c r="M242" s="327"/>
-      <c r="O242" s="619" t="str">
+      <c r="O242" s="601" t="str">
         <f>IF($U$137=1,"Scatter - Pulse", "Scatter – Digital acq")</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -32292,7 +32353,7 @@
       <c r="K243" s="323"/>
       <c r="L243" s="323"/>
       <c r="M243" s="327"/>
-      <c r="O243" s="619"/>
+      <c r="O243" s="601"/>
       <c r="P243" s="172" t="s">
         <v>296</v>
       </c>
@@ -32822,17 +32883,17 @@
       <c r="P257" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="Q257" s="620" t="s">
+      <c r="Q257" s="602" t="s">
         <v>312</v>
       </c>
-      <c r="R257" s="620"/>
+      <c r="R257" s="602"/>
       <c r="S257" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="T257" s="620" t="s">
+      <c r="T257" s="602" t="s">
         <v>314</v>
       </c>
-      <c r="U257" s="620"/>
+      <c r="U257" s="602"/>
       <c r="V257" s="1" t="s">
         <v>315</v>
       </c>
@@ -33186,15 +33247,24 @@
       <c r="Q266" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="R266" s="527"/>
+      <c r="R266" s="527" t="str">
+        <f>V100</f>
+        <v>Radcal 90-2123</v>
+      </c>
       <c r="T266" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="U266" s="528"/>
+      <c r="U266" s="528">
+        <f>V101</f>
+        <v>44540</v>
+      </c>
       <c r="W266" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="X266" s="528"/>
+      <c r="X266" s="528">
+        <f>V102</f>
+        <v>44905</v>
+      </c>
       <c r="Y266" s="14"/>
       <c r="AB266" s="71"/>
       <c r="AD266" s="71"/>
@@ -33320,24 +33390,24 @@
         <f t="shared" si="43"/>
         <v>Attenuator</v>
       </c>
-      <c r="E269" s="611" t="str">
+      <c r="E269" s="603" t="str">
         <f>Q107</f>
         <v>Auto 1</v>
       </c>
-      <c r="F269" s="612"/>
-      <c r="G269" s="612"/>
-      <c r="H269" s="612" t="str">
+      <c r="F269" s="604"/>
+      <c r="G269" s="604"/>
+      <c r="H269" s="604" t="str">
         <f>T107</f>
         <v/>
       </c>
-      <c r="I269" s="612"/>
-      <c r="J269" s="612"/>
-      <c r="K269" s="613" t="str">
+      <c r="I269" s="604"/>
+      <c r="J269" s="604"/>
+      <c r="K269" s="605" t="str">
         <f>W107</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L269" s="613"/>
-      <c r="M269" s="614"/>
+      <c r="L269" s="605"/>
+      <c r="M269" s="606"/>
       <c r="O269" s="189" t="str">
         <f t="shared" si="44"/>
         <v/>
@@ -33439,7 +33509,7 @@
         <v>7</v>
       </c>
       <c r="B271" s="301"/>
-      <c r="C271" s="587" t="str">
+      <c r="C271" s="610" t="str">
         <f>O110&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33515,7 +33585,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="301"/>
-      <c r="C272" s="587"/>
+      <c r="C272" s="610"/>
       <c r="D272" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -33581,7 +33651,7 @@
         <v>9</v>
       </c>
       <c r="B273" s="301"/>
-      <c r="C273" s="587"/>
+      <c r="C273" s="610"/>
       <c r="D273" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -33654,7 +33724,7 @@
         <v>10</v>
       </c>
       <c r="B274" s="301"/>
-      <c r="C274" s="587" t="str">
+      <c r="C274" s="610" t="str">
         <f>O113&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33723,7 +33793,7 @@
         <v>11</v>
       </c>
       <c r="B275" s="301"/>
-      <c r="C275" s="587"/>
+      <c r="C275" s="610"/>
       <c r="D275" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -33796,7 +33866,7 @@
         <v>12</v>
       </c>
       <c r="B276" s="301"/>
-      <c r="C276" s="587"/>
+      <c r="C276" s="610"/>
       <c r="D276" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -33837,17 +33907,17 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="O276" s="615" t="s">
+      <c r="O276" s="611" t="s">
         <v>261</v>
       </c>
-      <c r="P276" s="616" t="s">
+      <c r="P276" s="612" t="s">
         <v>262</v>
       </c>
-      <c r="R276" s="616" t="str">
+      <c r="R276" s="612" t="str">
         <f>"Ind AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="S276" s="616" t="str">
+      <c r="S276" s="612" t="str">
         <f>"Meas AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -33869,7 +33939,7 @@
         <v>13</v>
       </c>
       <c r="B277" s="301"/>
-      <c r="C277" s="587" t="str">
+      <c r="C277" s="610" t="str">
         <f>O116&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33913,13 +33983,13 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="O277" s="615"/>
-      <c r="P277" s="616"/>
+      <c r="O277" s="611"/>
+      <c r="P277" s="612"/>
       <c r="Q277" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="R277" s="616"/>
-      <c r="S277" s="616"/>
+      <c r="R277" s="612"/>
+      <c r="S277" s="612"/>
       <c r="T277" s="1" t="s">
         <v>321</v>
       </c>
@@ -33951,7 +34021,7 @@
         <v>14</v>
       </c>
       <c r="B278" s="301"/>
-      <c r="C278" s="587"/>
+      <c r="C278" s="610"/>
       <c r="D278" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -34038,7 +34108,7 @@
         <v>15</v>
       </c>
       <c r="B279" s="301"/>
-      <c r="C279" s="587"/>
+      <c r="C279" s="610"/>
       <c r="D279" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -34132,7 +34202,7 @@
         <v>16</v>
       </c>
       <c r="B280" s="301"/>
-      <c r="C280" s="587" t="str">
+      <c r="C280" s="610" t="str">
         <f>O119&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -34232,7 +34302,7 @@
         <v>17</v>
       </c>
       <c r="B281" s="301"/>
-      <c r="C281" s="587"/>
+      <c r="C281" s="610"/>
       <c r="D281" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -34319,7 +34389,7 @@
         <v>18</v>
       </c>
       <c r="B282" s="301"/>
-      <c r="C282" s="587"/>
+      <c r="C282" s="610"/>
       <c r="D282" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -34413,7 +34483,7 @@
         <v>19</v>
       </c>
       <c r="B283" s="301"/>
-      <c r="C283" s="587" t="str">
+      <c r="C283" s="610" t="str">
         <f>O122&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -34503,7 +34573,7 @@
         <v>20</v>
       </c>
       <c r="B284" s="301"/>
-      <c r="C284" s="587"/>
+      <c r="C284" s="610"/>
       <c r="D284" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -34597,7 +34667,7 @@
         <v>21</v>
       </c>
       <c r="B285" s="301"/>
-      <c r="C285" s="587"/>
+      <c r="C285" s="610"/>
       <c r="D285" s="391">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -35032,13 +35102,13 @@
       <c r="L293" s="135"/>
       <c r="M293" s="303"/>
       <c r="O293" s="225"/>
-      <c r="P293" s="617" t="s">
+      <c r="P293" s="613" t="s">
         <v>327</v>
       </c>
-      <c r="Q293" s="617"/>
-      <c r="R293" s="617"/>
-      <c r="S293" s="617"/>
-      <c r="T293" s="617"/>
+      <c r="Q293" s="613"/>
+      <c r="R293" s="613"/>
+      <c r="S293" s="613"/>
+      <c r="T293" s="613"/>
       <c r="U293" s="223"/>
       <c r="V293" s="223"/>
       <c r="W293" s="223"/>
@@ -35073,10 +35143,10 @@
         <v>227</v>
       </c>
       <c r="Q294" s="575" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="R294" s="558" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="S294" s="1" t="s">
         <v>148</v>
@@ -35124,13 +35194,29 @@
       <c r="L295" s="420"/>
       <c r="M295" s="421"/>
       <c r="O295" s="230">
+        <f>IF(DataEntry!M4="","",DataEntry!M4)</f>
         <v>60</v>
       </c>
-      <c r="P295" s="125"/>
-      <c r="Q295" s="126"/>
-      <c r="R295" s="126"/>
-      <c r="S295" s="126"/>
-      <c r="T295" s="246"/>
+      <c r="P295" s="125" t="str">
+        <f>IF(DataEntry!N4="","",DataEntry!N4)</f>
+        <v/>
+      </c>
+      <c r="Q295" s="126" t="str">
+        <f>IF(DataEntry!O4="","",DataEntry!O4)</f>
+        <v/>
+      </c>
+      <c r="R295" s="126" t="str">
+        <f>IF(DataEntry!P4="","",DataEntry!P4)</f>
+        <v/>
+      </c>
+      <c r="S295" s="126" t="str">
+        <f>IF(DataEntry!Q4="","",DataEntry!Q4)</f>
+        <v/>
+      </c>
+      <c r="T295" s="246" t="str">
+        <f>IF(DataEntry!R4="","",DataEntry!R4)</f>
+        <v/>
+      </c>
       <c r="U295" s="536" t="str">
         <f>IF(OR(O295="",P295=""),"",IF(AND(O295&gt;0,P295&gt;0),(P295-O295)/O295,""))</f>
         <v/>
@@ -35162,13 +35248,29 @@
       <c r="L296" s="423"/>
       <c r="M296" s="424"/>
       <c r="O296" s="232">
+        <f>IF(DataEntry!M5="","",DataEntry!M5)</f>
         <v>80</v>
       </c>
-      <c r="P296" s="248"/>
-      <c r="Q296" s="249"/>
-      <c r="R296" s="249"/>
-      <c r="S296" s="249"/>
-      <c r="T296" s="250"/>
+      <c r="P296" s="248" t="str">
+        <f>IF(DataEntry!N5="","",DataEntry!N5)</f>
+        <v/>
+      </c>
+      <c r="Q296" s="249" t="str">
+        <f>IF(DataEntry!O5="","",DataEntry!O5)</f>
+        <v/>
+      </c>
+      <c r="R296" s="249" t="str">
+        <f>IF(DataEntry!P5="","",DataEntry!P5)</f>
+        <v/>
+      </c>
+      <c r="S296" s="249" t="str">
+        <f>IF(DataEntry!Q5="","",DataEntry!Q5)</f>
+        <v/>
+      </c>
+      <c r="T296" s="250" t="str">
+        <f>IF(DataEntry!R5="","",DataEntry!R5)</f>
+        <v/>
+      </c>
       <c r="U296" s="537" t="str">
         <f>IF(OR(O296="",P296=""),"",IF(AND(O296&gt;0,P296&gt;0),(P296-O296)/O296,""))</f>
         <v/>
@@ -35207,13 +35309,29 @@
       <c r="L297" s="423"/>
       <c r="M297" s="424"/>
       <c r="O297" s="232">
+        <f>IF(DataEntry!M10="","",DataEntry!M10)</f>
         <v>100</v>
       </c>
-      <c r="P297" s="248"/>
-      <c r="Q297" s="249"/>
-      <c r="R297" s="249"/>
-      <c r="S297" s="249"/>
-      <c r="T297" s="250"/>
+      <c r="P297" s="248" t="str">
+        <f>IF(DataEntry!N10="","",DataEntry!N10)</f>
+        <v/>
+      </c>
+      <c r="Q297" s="249" t="str">
+        <f>IF(DataEntry!O10="","",DataEntry!O10)</f>
+        <v/>
+      </c>
+      <c r="R297" s="249" t="str">
+        <f>IF(DataEntry!P10="","",DataEntry!P10)</f>
+        <v/>
+      </c>
+      <c r="S297" s="249" t="str">
+        <f>IF(DataEntry!Q10="","",DataEntry!Q10)</f>
+        <v/>
+      </c>
+      <c r="T297" s="250" t="str">
+        <f>IF(DataEntry!R10="","",DataEntry!R10)</f>
+        <v/>
+      </c>
       <c r="U297" s="537" t="str">
         <f>IF(OR(O297="",P297=""),"",IF(AND(O297&gt;0,P297&gt;0),(P297-O297)/O297,""))</f>
         <v/>
@@ -35242,13 +35360,29 @@
       <c r="L298" s="417"/>
       <c r="M298" s="418"/>
       <c r="O298" s="132">
+        <f>IF(DataEntry!M11="","",DataEntry!M11)</f>
         <v>120</v>
       </c>
-      <c r="P298" s="254"/>
-      <c r="Q298" s="255"/>
-      <c r="R298" s="255"/>
-      <c r="S298" s="255"/>
-      <c r="T298" s="256"/>
+      <c r="P298" s="254" t="str">
+        <f>IF(DataEntry!N11="","",DataEntry!N11)</f>
+        <v/>
+      </c>
+      <c r="Q298" s="255" t="str">
+        <f>IF(DataEntry!O11="","",DataEntry!O11)</f>
+        <v/>
+      </c>
+      <c r="R298" s="255" t="str">
+        <f>IF(DataEntry!P11="","",DataEntry!P11)</f>
+        <v/>
+      </c>
+      <c r="S298" s="255" t="str">
+        <f>IF(DataEntry!Q11="","",DataEntry!Q11)</f>
+        <v/>
+      </c>
+      <c r="T298" s="256" t="str">
+        <f>IF(DataEntry!R11="","",DataEntry!R11)</f>
+        <v/>
+      </c>
       <c r="U298" s="538" t="str">
         <f>IF(OR(O298="",P298=""),"",IF(AND(O298&gt;0,P298&gt;0),(P298-O298)/O298,""))</f>
         <v/>
@@ -35415,13 +35549,13 @@
       <c r="L302" s="135"/>
       <c r="M302" s="303"/>
       <c r="O302" s="225"/>
-      <c r="P302" s="617" t="s">
+      <c r="P302" s="613" t="s">
         <v>327</v>
       </c>
-      <c r="Q302" s="617"/>
-      <c r="R302" s="617"/>
-      <c r="S302" s="617"/>
-      <c r="T302" s="617"/>
+      <c r="Q302" s="613"/>
+      <c r="R302" s="613"/>
+      <c r="S302" s="613"/>
+      <c r="T302" s="613"/>
       <c r="U302" s="223"/>
       <c r="V302" s="223"/>
       <c r="W302" s="223"/>
@@ -35442,7 +35576,7 @@
         <v>39</v>
       </c>
       <c r="B303" s="301"/>
-      <c r="C303" s="592" t="str">
+      <c r="C303" s="618" t="str">
         <f>O190</f>
         <v>Auto 1</v>
       </c>
@@ -35481,10 +35615,10 @@
         <v>227</v>
       </c>
       <c r="Q303" s="575" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="R303" s="558" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="S303" s="1" t="s">
         <v>148</v>
@@ -35505,7 +35639,7 @@
         <v>40</v>
       </c>
       <c r="B304" s="301"/>
-      <c r="C304" s="593"/>
+      <c r="C304" s="619"/>
       <c r="D304" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35578,7 +35712,7 @@
         <v>41</v>
       </c>
       <c r="B305" s="301"/>
-      <c r="C305" s="593"/>
+      <c r="C305" s="619"/>
       <c r="D305" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35608,11 +35742,26 @@
       <c r="L305" s="135"/>
       <c r="M305" s="303"/>
       <c r="O305" s="225"/>
-      <c r="P305" s="87"/>
-      <c r="Q305" s="88"/>
-      <c r="R305" s="88"/>
-      <c r="S305" s="88"/>
-      <c r="T305" s="89"/>
+      <c r="P305" s="87" t="str">
+        <f>IF(DataEntry!N6="","",DataEntry!N6)</f>
+        <v/>
+      </c>
+      <c r="Q305" s="88" t="str">
+        <f>IF(DataEntry!O6="","",DataEntry!O6)</f>
+        <v/>
+      </c>
+      <c r="R305" s="88" t="str">
+        <f>IF(DataEntry!P6="","",DataEntry!P6)</f>
+        <v/>
+      </c>
+      <c r="S305" s="88" t="str">
+        <f>IF(DataEntry!Q6="","",DataEntry!Q6)</f>
+        <v/>
+      </c>
+      <c r="T305" s="89" t="str">
+        <f>IF(DataEntry!R6="","",DataEntry!R6)</f>
+        <v/>
+      </c>
       <c r="U305" s="223"/>
       <c r="V305" s="223"/>
       <c r="W305" s="223"/>
@@ -35626,7 +35775,7 @@
         <v>42</v>
       </c>
       <c r="B306" s="301"/>
-      <c r="C306" s="593"/>
+      <c r="C306" s="619"/>
       <c r="D306" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35653,11 +35802,26 @@
       <c r="L306" s="135"/>
       <c r="M306" s="303"/>
       <c r="O306" s="225"/>
-      <c r="P306" s="87"/>
-      <c r="Q306" s="88"/>
-      <c r="R306" s="88"/>
-      <c r="S306" s="88"/>
-      <c r="T306" s="89"/>
+      <c r="P306" s="87" t="str">
+        <f>IF(DataEntry!N7="","",DataEntry!N7)</f>
+        <v/>
+      </c>
+      <c r="Q306" s="88" t="str">
+        <f>IF(DataEntry!O7="","",DataEntry!O7)</f>
+        <v/>
+      </c>
+      <c r="R306" s="88" t="str">
+        <f>IF(DataEntry!P7="","",DataEntry!P7)</f>
+        <v/>
+      </c>
+      <c r="S306" s="88" t="str">
+        <f>IF(DataEntry!Q7="","",DataEntry!Q7)</f>
+        <v/>
+      </c>
+      <c r="T306" s="89" t="str">
+        <f>IF(DataEntry!R7="","",DataEntry!R7)</f>
+        <v/>
+      </c>
       <c r="U306" s="223"/>
       <c r="V306" s="223"/>
       <c r="W306" s="223"/>
@@ -35678,7 +35842,7 @@
         <v>43</v>
       </c>
       <c r="B307" s="301"/>
-      <c r="C307" s="604"/>
+      <c r="C307" s="620"/>
       <c r="D307" s="436" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35705,11 +35869,26 @@
       <c r="L307" s="135"/>
       <c r="M307" s="303"/>
       <c r="O307" s="225"/>
-      <c r="P307" s="87"/>
-      <c r="Q307" s="88"/>
-      <c r="R307" s="88"/>
-      <c r="S307" s="88"/>
-      <c r="T307" s="89"/>
+      <c r="P307" s="87" t="str">
+        <f>IF(DataEntry!N8="","",DataEntry!N8)</f>
+        <v/>
+      </c>
+      <c r="Q307" s="88" t="str">
+        <f>IF(DataEntry!O8="","",DataEntry!O8)</f>
+        <v/>
+      </c>
+      <c r="R307" s="88" t="str">
+        <f>IF(DataEntry!P8="","",DataEntry!P8)</f>
+        <v/>
+      </c>
+      <c r="S307" s="88" t="str">
+        <f>IF(DataEntry!Q8="","",DataEntry!Q8)</f>
+        <v/>
+      </c>
+      <c r="T307" s="89" t="str">
+        <f>IF(DataEntry!R8="","",DataEntry!R8)</f>
+        <v/>
+      </c>
       <c r="U307" s="223"/>
       <c r="V307" s="223"/>
       <c r="W307" s="223"/>
@@ -35723,7 +35902,7 @@
         <v>44</v>
       </c>
       <c r="B308" s="301"/>
-      <c r="C308" s="592" t="str">
+      <c r="C308" s="618" t="str">
         <f>O195</f>
         <v/>
       </c>
@@ -35753,11 +35932,26 @@
       <c r="L308" s="135"/>
       <c r="M308" s="303"/>
       <c r="O308" s="225"/>
-      <c r="P308" s="92"/>
-      <c r="Q308" s="93"/>
-      <c r="R308" s="93"/>
-      <c r="S308" s="93"/>
-      <c r="T308" s="94"/>
+      <c r="P308" s="92" t="str">
+        <f>IF(DataEntry!N9="","",DataEntry!N9)</f>
+        <v/>
+      </c>
+      <c r="Q308" s="93" t="str">
+        <f>IF(DataEntry!O9="","",DataEntry!O9)</f>
+        <v/>
+      </c>
+      <c r="R308" s="93" t="str">
+        <f>IF(DataEntry!P9="","",DataEntry!P9)</f>
+        <v/>
+      </c>
+      <c r="S308" s="93" t="str">
+        <f>IF(DataEntry!Q9="","",DataEntry!Q9)</f>
+        <v/>
+      </c>
+      <c r="T308" s="94" t="str">
+        <f>IF(DataEntry!R9="","",DataEntry!R9)</f>
+        <v/>
+      </c>
       <c r="U308" s="223"/>
       <c r="V308" s="223"/>
       <c r="W308" s="223"/>
@@ -35778,7 +35972,7 @@
         <v>45</v>
       </c>
       <c r="B309" s="301"/>
-      <c r="C309" s="593"/>
+      <c r="C309" s="619"/>
       <c r="D309" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35830,7 +36024,7 @@
         <v>46</v>
       </c>
       <c r="B310" s="301"/>
-      <c r="C310" s="593"/>
+      <c r="C310" s="619"/>
       <c r="D310" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35889,7 +36083,7 @@
         <v>47</v>
       </c>
       <c r="B311" s="301"/>
-      <c r="C311" s="593"/>
+      <c r="C311" s="619"/>
       <c r="D311" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35941,7 +36135,7 @@
         <v>48</v>
       </c>
       <c r="B312" s="301"/>
-      <c r="C312" s="594"/>
+      <c r="C312" s="621"/>
       <c r="D312" s="439" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35997,7 +36191,7 @@
         <v>49</v>
       </c>
       <c r="B313" s="301"/>
-      <c r="C313" s="605" t="str">
+      <c r="C313" s="622" t="str">
         <f>O200</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -36049,7 +36243,7 @@
         <v>50</v>
       </c>
       <c r="B314" s="301"/>
-      <c r="C314" s="593"/>
+      <c r="C314" s="619"/>
       <c r="D314" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36101,7 +36295,7 @@
         <v>51</v>
       </c>
       <c r="B315" s="301"/>
-      <c r="C315" s="593"/>
+      <c r="C315" s="619"/>
       <c r="D315" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36146,7 +36340,7 @@
         <v>52</v>
       </c>
       <c r="B316" s="301"/>
-      <c r="C316" s="593"/>
+      <c r="C316" s="619"/>
       <c r="D316" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36200,7 +36394,7 @@
         <v>53</v>
       </c>
       <c r="B317" s="301"/>
-      <c r="C317" s="594"/>
+      <c r="C317" s="621"/>
       <c r="D317" s="439" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36282,7 +36476,7 @@
       <c r="X318" s="53"/>
       <c r="Y318" s="181"/>
       <c r="AA318" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AB318" s="28">
         <v>1</v>
@@ -36324,10 +36518,10 @@
       <c r="R319" s="246"/>
       <c r="S319" s="247"/>
       <c r="T319" s="247"/>
-      <c r="V319" s="609" t="s">
+      <c r="V319" s="591" t="s">
         <v>338</v>
       </c>
-      <c r="W319" s="609"/>
+      <c r="W319" s="591"/>
       <c r="X319" s="17" t="s">
         <v>339</v>
       </c>
@@ -36528,7 +36722,7 @@
         <v>60</v>
       </c>
       <c r="B324" s="301"/>
-      <c r="C324" s="598" t="str">
+      <c r="C324" s="607" t="str">
         <f>O240</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -36578,7 +36772,7 @@
         <v>61</v>
       </c>
       <c r="B325" s="301"/>
-      <c r="C325" s="599"/>
+      <c r="C325" s="608"/>
       <c r="D325" s="448" t="str">
         <f>P241</f>
         <v>Waist level</v>
@@ -36736,13 +36930,13 @@
         <v>346</v>
       </c>
       <c r="P329" s="53"/>
-      <c r="Q329" s="610" t="s">
+      <c r="Q329" s="609" t="s">
         <v>347</v>
       </c>
-      <c r="R329" s="610"/>
-      <c r="S329" s="610"/>
-      <c r="T329" s="610"/>
-      <c r="U329" s="610"/>
+      <c r="R329" s="609"/>
+      <c r="S329" s="609"/>
+      <c r="T329" s="609"/>
+      <c r="U329" s="609"/>
       <c r="Y329" s="14"/>
     </row>
     <row r="330" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -36925,24 +37119,24 @@
         <f t="shared" si="72"/>
         <v>Attenuator</v>
       </c>
-      <c r="E335" s="611" t="str">
+      <c r="E335" s="603" t="str">
         <f>Q139</f>
         <v>Auto 1</v>
       </c>
-      <c r="F335" s="612"/>
-      <c r="G335" s="612"/>
-      <c r="H335" s="612" t="str">
+      <c r="F335" s="604"/>
+      <c r="G335" s="604"/>
+      <c r="H335" s="604" t="str">
         <f>T139</f>
         <v/>
       </c>
-      <c r="I335" s="612"/>
-      <c r="J335" s="612"/>
-      <c r="K335" s="613" t="str">
+      <c r="I335" s="604"/>
+      <c r="J335" s="604"/>
+      <c r="K335" s="605" t="str">
         <f>W139</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L335" s="613"/>
-      <c r="M335" s="614"/>
+      <c r="L335" s="605"/>
+      <c r="M335" s="606"/>
       <c r="O335" s="130"/>
       <c r="P335" s="129" t="s">
         <v>353</v>
@@ -37019,7 +37213,7 @@
         <v>7</v>
       </c>
       <c r="B337" s="301"/>
-      <c r="C337" s="587" t="str">
+      <c r="C337" s="610" t="str">
         <f>O142&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37079,7 +37273,7 @@
         <v>8</v>
       </c>
       <c r="B338" s="301"/>
-      <c r="C338" s="587"/>
+      <c r="C338" s="610"/>
       <c r="D338" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37136,7 +37330,7 @@
         <v>9</v>
       </c>
       <c r="B339" s="301"/>
-      <c r="C339" s="587"/>
+      <c r="C339" s="610"/>
       <c r="D339" s="463">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37193,7 +37387,7 @@
         <v>10</v>
       </c>
       <c r="B340" s="301"/>
-      <c r="C340" s="587" t="str">
+      <c r="C340" s="610" t="str">
         <f>O145&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37253,7 +37447,7 @@
         <v>11</v>
       </c>
       <c r="B341" s="301"/>
-      <c r="C341" s="587"/>
+      <c r="C341" s="610"/>
       <c r="D341" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37310,7 +37504,7 @@
         <v>12</v>
       </c>
       <c r="B342" s="301"/>
-      <c r="C342" s="587"/>
+      <c r="C342" s="610"/>
       <c r="D342" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37367,7 +37561,7 @@
         <v>13</v>
       </c>
       <c r="B343" s="301"/>
-      <c r="C343" s="587" t="str">
+      <c r="C343" s="610" t="str">
         <f>O148&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37419,7 +37613,7 @@
         <v>14</v>
       </c>
       <c r="B344" s="301"/>
-      <c r="C344" s="587"/>
+      <c r="C344" s="610"/>
       <c r="D344" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37481,7 +37675,7 @@
         <v>15</v>
       </c>
       <c r="B345" s="301"/>
-      <c r="C345" s="587"/>
+      <c r="C345" s="610"/>
       <c r="D345" s="463">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37544,7 +37738,7 @@
         <v>16</v>
       </c>
       <c r="B346" s="301"/>
-      <c r="C346" s="587" t="str">
+      <c r="C346" s="610" t="str">
         <f>O151&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37607,7 +37801,7 @@
         <v>17</v>
       </c>
       <c r="B347" s="301"/>
-      <c r="C347" s="587"/>
+      <c r="C347" s="610"/>
       <c r="D347" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37665,7 +37859,7 @@
         <v>18</v>
       </c>
       <c r="B348" s="301"/>
-      <c r="C348" s="587"/>
+      <c r="C348" s="610"/>
       <c r="D348" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37743,7 +37937,7 @@
         <v>19</v>
       </c>
       <c r="B349" s="301"/>
-      <c r="C349" s="587" t="str">
+      <c r="C349" s="610" t="str">
         <f>O154&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37806,7 +38000,7 @@
         <v>20</v>
       </c>
       <c r="B350" s="301"/>
-      <c r="C350" s="587"/>
+      <c r="C350" s="610"/>
       <c r="D350" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37865,7 +38059,7 @@
         <v>21</v>
       </c>
       <c r="B351" s="301"/>
-      <c r="C351" s="587"/>
+      <c r="C351" s="610"/>
       <c r="D351" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -38174,11 +38368,11 @@
         <f>IF(OR(V358="",V359="",V362=""),"",(V358-V359)*V362)</f>
         <v/>
       </c>
-      <c r="Q358" s="600" t="str">
+      <c r="Q358" s="614" t="str">
         <f>IF(OR(P358="",P359=""),"",(ABS(P358)+ABS(P359))/$O$355)</f>
         <v/>
       </c>
-      <c r="R358" s="601" t="str">
+      <c r="R358" s="615" t="str">
         <f>IF(OR(Q358="",Q360=""),"",Q358+Q360)</f>
         <v/>
       </c>
@@ -38217,8 +38411,8 @@
         <f>IF(OR(W358="",W359="",V362=""),"",(W358-W359)*V362)</f>
         <v/>
       </c>
-      <c r="Q359" s="600"/>
-      <c r="R359" s="600"/>
+      <c r="Q359" s="614"/>
+      <c r="R359" s="614"/>
       <c r="S359" s="146" t="str">
         <f>IF(AB171="","",AB171)</f>
         <v/>
@@ -38254,11 +38448,11 @@
         <f>IF(OR(X358="",X359="",V362=""),"",(X358-X359)*V362)</f>
         <v/>
       </c>
-      <c r="Q360" s="601" t="str">
+      <c r="Q360" s="615" t="str">
         <f>IF(OR(P360="",P361=""),"",(ABS(P360)+ABS(P361))/$O$355)</f>
         <v/>
       </c>
-      <c r="R360" s="601"/>
+      <c r="R360" s="615"/>
       <c r="S360" s="146" t="str">
         <f>IF(AB172="","",AB172)</f>
         <v/>
@@ -38300,8 +38494,8 @@
         <f>IF(OR(Y358="",Y359="",V362=""),"",(Y358-Y359)*V362)</f>
         <v/>
       </c>
-      <c r="Q361" s="601"/>
-      <c r="R361" s="601"/>
+      <c r="Q361" s="615"/>
+      <c r="R361" s="615"/>
       <c r="S361" s="148" t="str">
         <f>IF(AB173="","",AB173)</f>
         <v/>
@@ -38473,7 +38667,7 @@
         <v>36</v>
       </c>
       <c r="B366" s="301"/>
-      <c r="C366" s="602" t="str">
+      <c r="C366" s="616" t="str">
         <f>O214</f>
         <v>Auto 1</v>
       </c>
@@ -38524,7 +38718,7 @@
         <v>37</v>
       </c>
       <c r="B367" s="301"/>
-      <c r="C367" s="603"/>
+      <c r="C367" s="617"/>
       <c r="D367" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38570,7 +38764,7 @@
         <v>38</v>
       </c>
       <c r="B368" s="301"/>
-      <c r="C368" s="603"/>
+      <c r="C368" s="617"/>
       <c r="D368" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38605,7 +38799,7 @@
         <v>39</v>
       </c>
       <c r="B369" s="301"/>
-      <c r="C369" s="603"/>
+      <c r="C369" s="617"/>
       <c r="D369" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38640,7 +38834,7 @@
         <v>40</v>
       </c>
       <c r="B370" s="301"/>
-      <c r="C370" s="603"/>
+      <c r="C370" s="617"/>
       <c r="D370" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38685,7 +38879,7 @@
         <v>41</v>
       </c>
       <c r="B371" s="301"/>
-      <c r="C371" s="592" t="str">
+      <c r="C371" s="618" t="str">
         <f>O219</f>
         <v/>
       </c>
@@ -38735,7 +38929,7 @@
         <v>42</v>
       </c>
       <c r="B372" s="301"/>
-      <c r="C372" s="593"/>
+      <c r="C372" s="619"/>
       <c r="D372" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38785,7 +38979,7 @@
         <v>43</v>
       </c>
       <c r="B373" s="301"/>
-      <c r="C373" s="593"/>
+      <c r="C373" s="619"/>
       <c r="D373" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38832,7 +39026,7 @@
         <v>44</v>
       </c>
       <c r="B374" s="301"/>
-      <c r="C374" s="593"/>
+      <c r="C374" s="619"/>
       <c r="D374" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38882,7 +39076,7 @@
         <v>45</v>
       </c>
       <c r="B375" s="301"/>
-      <c r="C375" s="594"/>
+      <c r="C375" s="621"/>
       <c r="D375" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38929,7 +39123,7 @@
         <v>46</v>
       </c>
       <c r="B376" s="301"/>
-      <c r="C376" s="595" t="str">
+      <c r="C376" s="634" t="str">
         <f>O224</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -38982,7 +39176,7 @@
         <v>47</v>
       </c>
       <c r="B377" s="301"/>
-      <c r="C377" s="596"/>
+      <c r="C377" s="635"/>
       <c r="D377" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39029,7 +39223,7 @@
         <v>48</v>
       </c>
       <c r="B378" s="301"/>
-      <c r="C378" s="596"/>
+      <c r="C378" s="635"/>
       <c r="D378" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39079,7 +39273,7 @@
         <v>49</v>
       </c>
       <c r="B379" s="301"/>
-      <c r="C379" s="596"/>
+      <c r="C379" s="635"/>
       <c r="D379" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39126,7 +39320,7 @@
         <v>50</v>
       </c>
       <c r="B380" s="301"/>
-      <c r="C380" s="597"/>
+      <c r="C380" s="636"/>
       <c r="D380" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39436,7 +39630,7 @@
         <v>58</v>
       </c>
       <c r="B388" s="301"/>
-      <c r="C388" s="598" t="str">
+      <c r="C388" s="607" t="str">
         <f>O242</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -39487,7 +39681,7 @@
         <v>59</v>
       </c>
       <c r="B389" s="301"/>
-      <c r="C389" s="599"/>
+      <c r="C389" s="608"/>
       <c r="D389" s="448" t="str">
         <f>P243</f>
         <v>Waist level</v>
@@ -39838,14 +40032,14 @@
       <c r="E399" s="299"/>
       <c r="F399" s="299"/>
       <c r="G399" s="299"/>
-      <c r="H399" s="608" t="s">
+      <c r="H399" s="625" t="s">
         <v>393</v>
       </c>
-      <c r="I399" s="608"/>
-      <c r="J399" s="608" t="s">
+      <c r="I399" s="625"/>
+      <c r="J399" s="625" t="s">
         <v>394</v>
       </c>
-      <c r="K399" s="608"/>
+      <c r="K399" s="625"/>
       <c r="L399" s="299"/>
       <c r="M399" s="300"/>
       <c r="O399" s="13"/>
@@ -40419,20 +40613,20 @@
       </c>
       <c r="B413" s="301"/>
       <c r="C413" s="42"/>
-      <c r="D413" s="606" t="s">
+      <c r="D413" s="623" t="s">
         <v>400</v>
       </c>
-      <c r="E413" s="606"/>
-      <c r="F413" s="606"/>
-      <c r="G413" s="606"/>
-      <c r="H413" s="606"/>
-      <c r="I413" s="606" t="s">
+      <c r="E413" s="623"/>
+      <c r="F413" s="623"/>
+      <c r="G413" s="623"/>
+      <c r="H413" s="623"/>
+      <c r="I413" s="623" t="s">
         <v>401</v>
       </c>
-      <c r="J413" s="606"/>
-      <c r="K413" s="606"/>
-      <c r="L413" s="606"/>
-      <c r="M413" s="607"/>
+      <c r="J413" s="623"/>
+      <c r="K413" s="623"/>
+      <c r="L413" s="623"/>
+      <c r="M413" s="624"/>
       <c r="O413" s="13"/>
       <c r="P413" s="2" t="s">
         <v>188</v>
@@ -41912,11 +42106,11 @@
         <f t="shared" si="95"/>
         <v/>
       </c>
-      <c r="F442" s="581" t="str">
+      <c r="F442" s="626" t="str">
         <f t="shared" si="95"/>
         <v/>
       </c>
-      <c r="G442" s="583" t="str">
+      <c r="G442" s="628" t="str">
         <f t="shared" si="95"/>
         <v/>
       </c>
@@ -41957,8 +42151,8 @@
         <f>P359</f>
         <v/>
       </c>
-      <c r="F443" s="582"/>
-      <c r="G443" s="584"/>
+      <c r="F443" s="627"/>
+      <c r="G443" s="629"/>
       <c r="H443" s="200"/>
       <c r="I443" s="82" t="str">
         <f>T360</f>
@@ -41998,11 +42192,11 @@
         <f>P360</f>
         <v/>
       </c>
-      <c r="F444" s="582" t="str">
+      <c r="F444" s="627" t="str">
         <f>Q360</f>
         <v/>
       </c>
-      <c r="G444" s="584"/>
+      <c r="G444" s="629"/>
       <c r="H444" s="135"/>
       <c r="I444" s="91" t="str">
         <f>T361</f>
@@ -42043,8 +42237,8 @@
         <f>P361</f>
         <v/>
       </c>
-      <c r="F445" s="586"/>
-      <c r="G445" s="585"/>
+      <c r="F445" s="631"/>
+      <c r="G445" s="630"/>
       <c r="H445" s="135"/>
       <c r="I445" s="135"/>
       <c r="J445" s="135"/>
@@ -48403,71 +48597,30 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="106">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="W107:Y107"/>
-    <mergeCell ref="Q139:S139"/>
-    <mergeCell ref="T139:V139"/>
-    <mergeCell ref="W139:Y139"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="T181:U181"/>
-    <mergeCell ref="O190:O194"/>
-    <mergeCell ref="O195:O199"/>
-    <mergeCell ref="O200:O204"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="Q107:S107"/>
-    <mergeCell ref="T107:V107"/>
-    <mergeCell ref="H204:H205"/>
-    <mergeCell ref="I204:I205"/>
-    <mergeCell ref="M204:M205"/>
-    <mergeCell ref="O214:O218"/>
-    <mergeCell ref="O219:O223"/>
-    <mergeCell ref="O224:O228"/>
-    <mergeCell ref="O240:O241"/>
-    <mergeCell ref="O242:O243"/>
-    <mergeCell ref="Q257:R257"/>
-    <mergeCell ref="T257:U257"/>
-    <mergeCell ref="E269:G269"/>
-    <mergeCell ref="H269:J269"/>
-    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="F442:F443"/>
+    <mergeCell ref="G442:G445"/>
+    <mergeCell ref="F444:F445"/>
+    <mergeCell ref="C337:C339"/>
+    <mergeCell ref="C340:C342"/>
+    <mergeCell ref="C343:C345"/>
+    <mergeCell ref="C346:C348"/>
+    <mergeCell ref="C349:C351"/>
+    <mergeCell ref="E204:E205"/>
+    <mergeCell ref="F204:F205"/>
+    <mergeCell ref="C371:C375"/>
+    <mergeCell ref="C376:C380"/>
+    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="Q358:Q359"/>
+    <mergeCell ref="R358:R361"/>
+    <mergeCell ref="Q360:Q361"/>
+    <mergeCell ref="C366:C370"/>
+    <mergeCell ref="C303:C307"/>
+    <mergeCell ref="C308:C312"/>
+    <mergeCell ref="C313:C317"/>
+    <mergeCell ref="D413:H413"/>
+    <mergeCell ref="I413:M413"/>
+    <mergeCell ref="H399:I399"/>
+    <mergeCell ref="J399:K399"/>
     <mergeCell ref="V319:W319"/>
     <mergeCell ref="C324:C325"/>
     <mergeCell ref="Q329:U329"/>
@@ -48485,30 +48638,71 @@
     <mergeCell ref="C283:C285"/>
     <mergeCell ref="P302:T302"/>
     <mergeCell ref="P293:T293"/>
-    <mergeCell ref="Q358:Q359"/>
-    <mergeCell ref="R358:R361"/>
-    <mergeCell ref="Q360:Q361"/>
-    <mergeCell ref="C366:C370"/>
-    <mergeCell ref="C303:C307"/>
-    <mergeCell ref="C308:C312"/>
-    <mergeCell ref="C313:C317"/>
-    <mergeCell ref="D413:H413"/>
-    <mergeCell ref="I413:M413"/>
-    <mergeCell ref="H399:I399"/>
-    <mergeCell ref="J399:K399"/>
-    <mergeCell ref="F442:F443"/>
-    <mergeCell ref="G442:G445"/>
-    <mergeCell ref="F444:F445"/>
-    <mergeCell ref="C337:C339"/>
-    <mergeCell ref="C340:C342"/>
-    <mergeCell ref="C343:C345"/>
-    <mergeCell ref="C346:C348"/>
-    <mergeCell ref="C349:C351"/>
-    <mergeCell ref="E204:E205"/>
-    <mergeCell ref="F204:F205"/>
-    <mergeCell ref="C371:C375"/>
-    <mergeCell ref="C376:C380"/>
-    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="O214:O218"/>
+    <mergeCell ref="O219:O223"/>
+    <mergeCell ref="O224:O228"/>
+    <mergeCell ref="O240:O241"/>
+    <mergeCell ref="O242:O243"/>
+    <mergeCell ref="Q257:R257"/>
+    <mergeCell ref="T257:U257"/>
+    <mergeCell ref="E269:G269"/>
+    <mergeCell ref="H269:J269"/>
+    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="T181:U181"/>
+    <mergeCell ref="O190:O194"/>
+    <mergeCell ref="O195:O199"/>
+    <mergeCell ref="O200:O204"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="Q107:S107"/>
+    <mergeCell ref="T107:V107"/>
+    <mergeCell ref="H204:H205"/>
+    <mergeCell ref="I204:I205"/>
+    <mergeCell ref="M204:M205"/>
+    <mergeCell ref="W107:Y107"/>
+    <mergeCell ref="Q139:S139"/>
+    <mergeCell ref="T139:V139"/>
+    <mergeCell ref="W139:Y139"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
   </mergeCells>
   <conditionalFormatting sqref="S126 V126 Y126 S158 V158 Y158">
     <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
@@ -48826,39 +49020,39 @@
         <f>Fluoro!D269</f>
         <v>Attenuator</v>
       </c>
-      <c r="E5" s="612" t="str">
+      <c r="E5" s="604" t="str">
         <f>Fluoro!E269</f>
         <v>Auto 1</v>
       </c>
-      <c r="F5" s="612">
+      <c r="F5" s="604">
         <f>Fluoro!F269</f>
         <v>0</v>
       </c>
-      <c r="G5" s="612">
+      <c r="G5" s="604">
         <f>Fluoro!G269</f>
         <v>0</v>
       </c>
-      <c r="H5" s="612" t="str">
+      <c r="H5" s="604" t="str">
         <f>Fluoro!H269</f>
         <v/>
       </c>
-      <c r="I5" s="612">
+      <c r="I5" s="604">
         <f>Fluoro!I269</f>
         <v>0</v>
       </c>
-      <c r="J5" s="612">
+      <c r="J5" s="604">
         <f>Fluoro!J269</f>
         <v>0</v>
       </c>
-      <c r="K5" s="613" t="str">
+      <c r="K5" s="605" t="str">
         <f>Fluoro!K269</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L5" s="613">
+      <c r="L5" s="605">
         <f>Fluoro!L269</f>
         <v>0</v>
       </c>
-      <c r="M5" s="613">
+      <c r="M5" s="605">
         <f>Fluoro!M269</f>
         <v>0</v>
       </c>
@@ -50039,39 +50233,39 @@
         <f>Fluoro!D335</f>
         <v>Attenuator</v>
       </c>
-      <c r="E37" s="612" t="str">
+      <c r="E37" s="604" t="str">
         <f>Fluoro!E335</f>
         <v>Auto 1</v>
       </c>
-      <c r="F37" s="612">
+      <c r="F37" s="604">
         <f>Fluoro!F335</f>
         <v>0</v>
       </c>
-      <c r="G37" s="612">
+      <c r="G37" s="604">
         <f>Fluoro!G335</f>
         <v>0</v>
       </c>
-      <c r="H37" s="612" t="str">
+      <c r="H37" s="604" t="str">
         <f>Fluoro!H335</f>
         <v/>
       </c>
-      <c r="I37" s="612">
+      <c r="I37" s="604">
         <f>Fluoro!I335</f>
         <v>0</v>
       </c>
-      <c r="J37" s="612">
+      <c r="J37" s="604">
         <f>Fluoro!J335</f>
         <v>0</v>
       </c>
-      <c r="K37" s="613" t="str">
+      <c r="K37" s="605" t="str">
         <f>Fluoro!K335</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L37" s="613">
+      <c r="L37" s="605">
         <f>Fluoro!L335</f>
         <v>0</v>
       </c>
-      <c r="M37" s="613">
+      <c r="M37" s="605">
         <f>Fluoro!M335</f>
         <v>0</v>
       </c>
@@ -51022,7 +51216,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="10"/>
-      <c r="C60" s="636"/>
+      <c r="C60" s="638"/>
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60"/>
@@ -51039,7 +51233,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="10"/>
-      <c r="C61" s="636"/>
+      <c r="C61" s="638"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>
@@ -51174,23 +51368,23 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="17">
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C51:C53"/>
     <mergeCell ref="E37:G37"/>
     <mergeCell ref="H37:J37"/>
     <mergeCell ref="K37:M37"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="68" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -51214,34 +51408,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="638" t="s">
+      <c r="A1" s="639" t="s">
         <v>405</v>
       </c>
-      <c r="B1" s="638"/>
+      <c r="B1" s="639"/>
       <c r="N1" s="278"/>
-      <c r="O1" s="617" t="str">
+      <c r="O1" s="613" t="str">
         <f>Fluoro!O105</f>
         <v>Patient Entrance Exposure Rate (Fluoroscopy)*</v>
       </c>
-      <c r="P1" s="617"/>
-      <c r="Q1" s="617"/>
-      <c r="R1" s="617" t="s">
+      <c r="P1" s="613"/>
+      <c r="Q1" s="613"/>
+      <c r="R1" s="613" t="s">
         <v>406</v>
       </c>
-      <c r="S1" s="617"/>
-      <c r="T1" s="617"/>
+      <c r="S1" s="613"/>
+      <c r="T1" s="613"/>
       <c r="V1" s="278"/>
-      <c r="W1" s="617" t="str">
+      <c r="W1" s="613" t="str">
         <f>Fluoro!O137</f>
         <v>Patient Entrance Exposure Rate – Digital Acquisition</v>
       </c>
-      <c r="X1" s="617"/>
-      <c r="Y1" s="617"/>
-      <c r="Z1" s="617" t="s">
+      <c r="X1" s="613"/>
+      <c r="Y1" s="613"/>
+      <c r="Z1" s="613" t="s">
         <v>406</v>
       </c>
-      <c r="AA1" s="617"/>
-      <c r="AB1" s="617"/>
+      <c r="AA1" s="613"/>
+      <c r="AB1" s="613"/>
     </row>
     <row r="2" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="279">
@@ -51444,10 +51638,10 @@
       <c r="AB6" s="278"/>
     </row>
     <row r="7" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="638" t="s">
+      <c r="A7" s="639" t="s">
         <v>409</v>
       </c>
-      <c r="B7" s="638"/>
+      <c r="B7" s="639"/>
       <c r="D7" s="203" t="s">
         <v>410</v>
       </c>
@@ -55234,14 +55428,14 @@
       <c r="B75" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="E75" s="617" t="s">
+      <c r="E75" s="613" t="s">
         <v>419</v>
       </c>
-      <c r="F75" s="617"/>
-      <c r="I75" s="617" t="s">
+      <c r="F75" s="613"/>
+      <c r="I75" s="613" t="s">
         <v>420</v>
       </c>
-      <c r="J75" s="617"/>
+      <c r="J75" s="613"/>
     </row>
     <row r="76" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
@@ -56969,16 +57163,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:AF41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:AF11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1025" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="80" t="s">
         <v>155</v>
       </c>
@@ -56992,8 +57188,32 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="14"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M1" s="640" t="s">
+        <v>459</v>
+      </c>
+      <c r="N1" s="581"/>
+      <c r="O1" s="581"/>
+      <c r="P1" s="581"/>
+      <c r="Q1" s="581"/>
+      <c r="R1" s="581"/>
+      <c r="S1" s="581"/>
+      <c r="T1" s="581"/>
+      <c r="U1" s="640" t="s">
+        <v>459</v>
+      </c>
+      <c r="V1" s="581"/>
+      <c r="W1" s="581"/>
+      <c r="X1" s="581"/>
+      <c r="Y1" s="581"/>
+      <c r="Z1" s="581"/>
+      <c r="AA1" s="581"/>
+      <c r="AB1" s="581"/>
+      <c r="AC1" s="581"/>
+      <c r="AD1" s="581"/>
+      <c r="AE1" s="581"/>
+      <c r="AF1" s="581"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
         <v>158</v>
       </c>
@@ -57019,8 +57239,28 @@
       </c>
       <c r="J2" s="48"/>
       <c r="K2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="581"/>
+      <c r="N2" s="581"/>
+      <c r="O2" s="581"/>
+      <c r="P2" s="581"/>
+      <c r="Q2" s="581"/>
+      <c r="R2" s="581"/>
+      <c r="S2" s="581"/>
+      <c r="T2" s="581"/>
+      <c r="U2" s="581"/>
+      <c r="V2" s="581"/>
+      <c r="W2" s="581"/>
+      <c r="X2" s="581"/>
+      <c r="Y2" s="581"/>
+      <c r="Z2" s="581"/>
+      <c r="AA2" s="581"/>
+      <c r="AB2" s="581"/>
+      <c r="AC2" s="581"/>
+      <c r="AD2" s="581"/>
+      <c r="AE2" s="581"/>
+      <c r="AF2" s="581"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="81" t="s">
         <v>161</v>
       </c>
@@ -57036,8 +57276,64 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="14"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="641" t="s">
+        <v>460</v>
+      </c>
+      <c r="N3" s="641" t="s">
+        <v>461</v>
+      </c>
+      <c r="O3" s="641" t="s">
+        <v>462</v>
+      </c>
+      <c r="P3" s="641" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q3" s="641" t="s">
+        <v>464</v>
+      </c>
+      <c r="R3" s="641" t="s">
+        <v>465</v>
+      </c>
+      <c r="S3" s="581"/>
+      <c r="T3" s="581"/>
+      <c r="U3" s="641" t="s">
+        <v>460</v>
+      </c>
+      <c r="V3" s="641" t="s">
+        <v>461</v>
+      </c>
+      <c r="W3" s="641" t="s">
+        <v>462</v>
+      </c>
+      <c r="X3" s="641" t="s">
+        <v>463</v>
+      </c>
+      <c r="Y3" s="641" t="s">
+        <v>464</v>
+      </c>
+      <c r="Z3" s="641" t="s">
+        <v>465</v>
+      </c>
+      <c r="AA3" s="641" t="s">
+        <v>466</v>
+      </c>
+      <c r="AB3" s="641" t="s">
+        <v>467</v>
+      </c>
+      <c r="AC3" s="641" t="s">
+        <v>468</v>
+      </c>
+      <c r="AD3" s="641" t="s">
+        <v>469</v>
+      </c>
+      <c r="AE3" s="641" t="s">
+        <v>470</v>
+      </c>
+      <c r="AF3" s="641" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="81" t="str">
         <f>IF(Fluoro!O104="","","("&amp;Fluoro!O104&amp;")")</f>
         <v>(cm)</v>
@@ -57072,8 +57368,32 @@
       <c r="K4" s="14" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="581">
+        <v>60</v>
+      </c>
+      <c r="N4" s="581"/>
+      <c r="O4" s="581"/>
+      <c r="P4" s="581"/>
+      <c r="Q4" s="581"/>
+      <c r="R4" s="581"/>
+      <c r="S4" s="581"/>
+      <c r="T4" s="581"/>
+      <c r="U4" s="581">
+        <v>60</v>
+      </c>
+      <c r="V4" s="581"/>
+      <c r="W4" s="581"/>
+      <c r="X4" s="581"/>
+      <c r="Y4" s="581"/>
+      <c r="Z4" s="581"/>
+      <c r="AA4" s="581"/>
+      <c r="AB4" s="581"/>
+      <c r="AC4" s="581"/>
+      <c r="AD4" s="581"/>
+      <c r="AE4" s="581"/>
+      <c r="AF4" s="581"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="82" t="s">
         <v>169</v>
       </c>
@@ -57089,8 +57409,32 @@
       <c r="I5" s="83"/>
       <c r="J5" s="84"/>
       <c r="K5" s="85"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="581">
+        <v>80</v>
+      </c>
+      <c r="N5" s="581"/>
+      <c r="O5" s="581"/>
+      <c r="P5" s="581"/>
+      <c r="Q5" s="581"/>
+      <c r="R5" s="581"/>
+      <c r="S5" s="581"/>
+      <c r="T5" s="581"/>
+      <c r="U5" s="581">
+        <v>80</v>
+      </c>
+      <c r="V5" s="581"/>
+      <c r="W5" s="581"/>
+      <c r="X5" s="581"/>
+      <c r="Y5" s="581"/>
+      <c r="Z5" s="581"/>
+      <c r="AA5" s="581"/>
+      <c r="AB5" s="581"/>
+      <c r="AC5" s="581"/>
+      <c r="AD5" s="581"/>
+      <c r="AE5" s="581"/>
+      <c r="AF5" s="581"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="86" t="str">
         <f>Fluoro!O110</f>
         <v/>
@@ -57107,8 +57451,32 @@
       <c r="I6" s="87"/>
       <c r="J6" s="88"/>
       <c r="K6" s="89"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="581">
+        <v>80</v>
+      </c>
+      <c r="N6" s="581"/>
+      <c r="O6" s="581"/>
+      <c r="P6" s="581"/>
+      <c r="Q6" s="581"/>
+      <c r="R6" s="581"/>
+      <c r="S6" s="581"/>
+      <c r="T6" s="581"/>
+      <c r="U6" s="581">
+        <v>80</v>
+      </c>
+      <c r="V6" s="581"/>
+      <c r="W6" s="581"/>
+      <c r="X6" s="581"/>
+      <c r="Y6" s="581"/>
+      <c r="Z6" s="581"/>
+      <c r="AA6" s="581"/>
+      <c r="AB6" s="581"/>
+      <c r="AC6" s="581"/>
+      <c r="AD6" s="581"/>
+      <c r="AE6" s="581"/>
+      <c r="AF6" s="581"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="90"/>
       <c r="B7" s="91">
         <v>30</v>
@@ -57122,8 +57490,32 @@
       <c r="I7" s="92"/>
       <c r="J7" s="93"/>
       <c r="K7" s="94"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="581">
+        <v>80</v>
+      </c>
+      <c r="N7" s="581"/>
+      <c r="O7" s="581"/>
+      <c r="P7" s="581"/>
+      <c r="Q7" s="581"/>
+      <c r="R7" s="581"/>
+      <c r="S7" s="581"/>
+      <c r="T7" s="581"/>
+      <c r="U7" s="581">
+        <v>80</v>
+      </c>
+      <c r="V7" s="581"/>
+      <c r="W7" s="581"/>
+      <c r="X7" s="581"/>
+      <c r="Y7" s="581"/>
+      <c r="Z7" s="581"/>
+      <c r="AA7" s="581"/>
+      <c r="AB7" s="581"/>
+      <c r="AC7" s="581"/>
+      <c r="AD7" s="581"/>
+      <c r="AE7" s="581"/>
+      <c r="AF7" s="581"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="82" t="s">
         <v>172</v>
       </c>
@@ -57139,8 +57531,32 @@
       <c r="I8" s="83"/>
       <c r="J8" s="84"/>
       <c r="K8" s="85"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="581">
+        <v>80</v>
+      </c>
+      <c r="N8" s="581"/>
+      <c r="O8" s="581"/>
+      <c r="P8" s="581"/>
+      <c r="Q8" s="581"/>
+      <c r="R8" s="581"/>
+      <c r="S8" s="581"/>
+      <c r="T8" s="581"/>
+      <c r="U8" s="581">
+        <v>80</v>
+      </c>
+      <c r="V8" s="581"/>
+      <c r="W8" s="581"/>
+      <c r="X8" s="581"/>
+      <c r="Y8" s="581"/>
+      <c r="Z8" s="581"/>
+      <c r="AA8" s="581"/>
+      <c r="AB8" s="581"/>
+      <c r="AC8" s="581"/>
+      <c r="AD8" s="581"/>
+      <c r="AE8" s="581"/>
+      <c r="AF8" s="581"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="86" t="str">
         <f>Fluoro!O113</f>
         <v/>
@@ -57157,8 +57573,32 @@
       <c r="I9" s="87"/>
       <c r="J9" s="88"/>
       <c r="K9" s="89"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="581">
+        <v>80</v>
+      </c>
+      <c r="N9" s="581"/>
+      <c r="O9" s="581"/>
+      <c r="P9" s="581"/>
+      <c r="Q9" s="581"/>
+      <c r="R9" s="581"/>
+      <c r="S9" s="581"/>
+      <c r="T9" s="581"/>
+      <c r="U9" s="581">
+        <v>80</v>
+      </c>
+      <c r="V9" s="581"/>
+      <c r="W9" s="581"/>
+      <c r="X9" s="581"/>
+      <c r="Y9" s="581"/>
+      <c r="Z9" s="581"/>
+      <c r="AA9" s="581"/>
+      <c r="AB9" s="581"/>
+      <c r="AC9" s="581"/>
+      <c r="AD9" s="581"/>
+      <c r="AE9" s="581"/>
+      <c r="AF9" s="581"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="90"/>
       <c r="B10" s="91">
         <v>30</v>
@@ -57172,8 +57612,32 @@
       <c r="I10" s="92"/>
       <c r="J10" s="93"/>
       <c r="K10" s="94"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="581">
+        <v>100</v>
+      </c>
+      <c r="N10" s="581"/>
+      <c r="O10" s="581"/>
+      <c r="P10" s="581"/>
+      <c r="Q10" s="581"/>
+      <c r="R10" s="581"/>
+      <c r="S10" s="581"/>
+      <c r="T10" s="581"/>
+      <c r="U10" s="581">
+        <v>100</v>
+      </c>
+      <c r="V10" s="581"/>
+      <c r="W10" s="581"/>
+      <c r="X10" s="581"/>
+      <c r="Y10" s="581"/>
+      <c r="Z10" s="581"/>
+      <c r="AA10" s="581"/>
+      <c r="AB10" s="581"/>
+      <c r="AC10" s="581"/>
+      <c r="AD10" s="581"/>
+      <c r="AE10" s="581"/>
+      <c r="AF10" s="581"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="82" t="s">
         <v>173</v>
       </c>
@@ -57189,8 +57653,32 @@
       <c r="I11" s="83"/>
       <c r="J11" s="84"/>
       <c r="K11" s="85"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11" s="581">
+        <v>120</v>
+      </c>
+      <c r="N11" s="581"/>
+      <c r="O11" s="581"/>
+      <c r="P11" s="581"/>
+      <c r="Q11" s="581"/>
+      <c r="R11" s="581"/>
+      <c r="S11" s="581"/>
+      <c r="T11" s="581"/>
+      <c r="U11" s="581">
+        <v>120</v>
+      </c>
+      <c r="V11" s="581"/>
+      <c r="W11" s="581"/>
+      <c r="X11" s="581"/>
+      <c r="Y11" s="581"/>
+      <c r="Z11" s="581"/>
+      <c r="AA11" s="581"/>
+      <c r="AB11" s="581"/>
+      <c r="AC11" s="581"/>
+      <c r="AD11" s="581"/>
+      <c r="AE11" s="581"/>
+      <c r="AF11" s="581"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="86" t="str">
         <f>Fluoro!O116</f>
         <v/>
@@ -57208,7 +57696,7 @@
       <c r="J12" s="88"/>
       <c r="K12" s="89"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="90"/>
       <c r="B13" s="91">
         <v>30</v>
@@ -57223,7 +57711,7 @@
       <c r="J13" s="93"/>
       <c r="K13" s="94"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="82" t="s">
         <v>174</v>
       </c>
@@ -57240,7 +57728,7 @@
       <c r="J14" s="84"/>
       <c r="K14" s="85"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="86" t="str">
         <f>Fluoro!O119</f>
         <v/>
@@ -57258,7 +57746,7 @@
       <c r="J15" s="88"/>
       <c r="K15" s="89"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="90"/>
       <c r="B16" s="91">
         <v>30</v>

</xml_diff>

<commit_message>
Remove accidentally saved test data
</commit_message>
<xml_diff>
--- a/MUSCCArm.xlsx
+++ b/MUSCCArm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD8DA39-6632-4DB1-A508-CCDD1FC45F1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE8926C-5E8C-416F-9393-AE9205F9EF3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6477,184 +6477,184 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="122" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="123" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="124" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="200" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="201" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="149" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="150" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="151" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="183" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="192" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="193" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="127" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="155" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="182" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="175" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="176" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="154" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="180" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="222" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="223" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="200" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="222" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="223" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="127" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="155" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="182" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="149" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="150" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="175" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="151" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="176" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="154" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="180" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="122" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="123" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="124" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="201" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="183" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="192" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="193" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -20456,9 +20456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD792"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20768,21 +20766,21 @@
       <c r="E10" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="582" t="str">
+      <c r="F10" s="635" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="582"/>
+      <c r="G10" s="635"/>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
       <c r="J10" s="160" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="583" t="str">
+      <c r="K10" s="624" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="583"/>
+      <c r="L10" s="624"/>
       <c r="M10" s="312"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="2" t="s">
@@ -20825,21 +20823,21 @@
       <c r="E11" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="584" t="str">
+      <c r="F11" s="625" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="584"/>
+      <c r="G11" s="625"/>
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
       <c r="J11" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="584" t="str">
+      <c r="K11" s="625" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="584"/>
+      <c r="L11" s="625"/>
       <c r="M11" s="312"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="2" t="s">
@@ -20882,21 +20880,21 @@
       <c r="E12" s="160" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="584" t="str">
+      <c r="F12" s="625" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="584"/>
+      <c r="G12" s="625"/>
       <c r="H12" s="42"/>
       <c r="I12" s="42"/>
       <c r="J12" s="160" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="585" t="str">
+      <c r="K12" s="637" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="585"/>
+      <c r="L12" s="637"/>
       <c r="M12" s="312"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="2" t="s">
@@ -20939,21 +20937,21 @@
       <c r="E13" s="160" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="586" t="str">
+      <c r="F13" s="626" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="586"/>
+      <c r="G13" s="626"/>
       <c r="H13" s="42"/>
       <c r="I13" s="42"/>
       <c r="J13" s="160" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="586" t="str">
+      <c r="K13" s="626" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="586"/>
+      <c r="L13" s="626"/>
       <c r="M13" s="312"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="2" t="s">
@@ -21076,21 +21074,21 @@
       <c r="E16" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="582" t="str">
+      <c r="F16" s="635" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="582"/>
+      <c r="G16" s="635"/>
       <c r="H16" s="42"/>
       <c r="I16" s="42"/>
       <c r="J16" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="587" t="str">
+      <c r="K16" s="638" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="587"/>
+      <c r="L16" s="638"/>
       <c r="M16" s="312"/>
       <c r="O16" s="13"/>
       <c r="P16" s="50" t="s">
@@ -21120,21 +21118,21 @@
       <c r="E17" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="584" t="str">
+      <c r="F17" s="625" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="584"/>
+      <c r="G17" s="625"/>
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
       <c r="J17" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="586" t="str">
+      <c r="K17" s="626" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="586"/>
+      <c r="L17" s="626"/>
       <c r="M17" s="312"/>
       <c r="O17" s="13"/>
       <c r="Q17" s="2" t="s">
@@ -21177,21 +21175,21 @@
       <c r="E18" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="586" t="str">
+      <c r="F18" s="626" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="586"/>
+      <c r="G18" s="626"/>
       <c r="H18" s="42"/>
       <c r="I18" s="42"/>
       <c r="J18" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="586" t="str">
+      <c r="K18" s="626" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="586"/>
+      <c r="L18" s="626"/>
       <c r="M18" s="312"/>
       <c r="O18" s="13"/>
       <c r="Q18" s="2" t="s">
@@ -21239,11 +21237,11 @@
       <c r="J19" s="160" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="586" t="str">
+      <c r="K19" s="626" t="str">
         <f>IF(V20="","",V20)</f>
         <v/>
       </c>
-      <c r="L19" s="586"/>
+      <c r="L19" s="626"/>
       <c r="M19" s="312"/>
       <c r="O19" s="13"/>
       <c r="Q19" s="2" t="s">
@@ -21318,11 +21316,11 @@
       <c r="E21" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="582" t="str">
+      <c r="F21" s="635" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="582"/>
+      <c r="G21" s="635"/>
       <c r="H21" s="42"/>
       <c r="I21" s="42"/>
       <c r="J21" s="73" t="s">
@@ -21362,21 +21360,21 @@
       <c r="E22" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="588" t="str">
+      <c r="F22" s="636" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="588"/>
+      <c r="G22" s="636"/>
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
       <c r="J22" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="582" t="str">
+      <c r="K22" s="635" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="582"/>
+      <c r="L22" s="635"/>
       <c r="M22" s="312"/>
       <c r="O22" s="13"/>
       <c r="Q22" s="2" t="s">
@@ -21421,11 +21419,11 @@
       <c r="J23" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="584" t="str">
+      <c r="K23" s="625" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="584"/>
+      <c r="L23" s="625"/>
       <c r="M23" s="312"/>
       <c r="O23" s="13"/>
       <c r="Q23" s="2" t="s">
@@ -21468,21 +21466,21 @@
       <c r="E24" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="583" t="str">
+      <c r="F24" s="624" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="583"/>
+      <c r="G24" s="624"/>
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
       <c r="J24" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="584" t="str">
+      <c r="K24" s="625" t="str">
         <f>IF(V25="","",V25)</f>
         <v/>
       </c>
-      <c r="L24" s="584"/>
+      <c r="L24" s="625"/>
       <c r="M24" s="312"/>
       <c r="O24" s="13"/>
       <c r="P24" s="50" t="s">
@@ -21520,11 +21518,11 @@
       <c r="E25" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="586" t="str">
+      <c r="F25" s="626" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="586"/>
+      <c r="G25" s="626"/>
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
@@ -21572,11 +21570,11 @@
       <c r="E26" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="586" t="str">
+      <c r="F26" s="626" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="586"/>
+      <c r="G26" s="626"/>
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
       <c r="J26" s="313" t="s">
@@ -21625,11 +21623,11 @@
       <c r="J27" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="582" t="str">
+      <c r="K27" s="635" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="582"/>
+      <c r="L27" s="635"/>
       <c r="M27" s="312"/>
       <c r="O27" s="13"/>
       <c r="Q27" s="2" t="s">
@@ -21667,21 +21665,21 @@
       <c r="E28" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="583" t="str">
+      <c r="F28" s="624" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="583"/>
+      <c r="G28" s="624"/>
       <c r="H28" s="42"/>
       <c r="I28" s="42"/>
       <c r="J28" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="584" t="str">
+      <c r="K28" s="625" t="str">
         <f>IF(V29="","",V29)</f>
         <v/>
       </c>
-      <c r="L28" s="584"/>
+      <c r="L28" s="625"/>
       <c r="M28" s="312"/>
       <c r="O28" s="13"/>
       <c r="P28" s="50" t="s">
@@ -21710,11 +21708,11 @@
       <c r="E29" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="586" t="str">
+      <c r="F29" s="626" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="586"/>
+      <c r="G29" s="626"/>
       <c r="H29" s="42"/>
       <c r="I29" s="42"/>
       <c r="J29" s="42"/>
@@ -21762,11 +21760,11 @@
       <c r="E30" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="586" t="str">
+      <c r="F30" s="626" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="586"/>
+      <c r="G30" s="626"/>
       <c r="H30" s="42"/>
       <c r="I30" s="42"/>
       <c r="J30" s="42"/>
@@ -21881,11 +21879,11 @@
       <c r="E33" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="582" t="str">
+      <c r="F33" s="635" t="str">
         <f>IF(R34="","",R34)</f>
         <v/>
       </c>
-      <c r="G33" s="582"/>
+      <c r="G33" s="635"/>
       <c r="H33" s="42"/>
       <c r="I33" s="42"/>
       <c r="J33" s="73" t="s">
@@ -21922,21 +21920,21 @@
       <c r="E34" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="588" t="str">
+      <c r="F34" s="636" t="str">
         <f>IF(R35="","",R35)</f>
         <v/>
       </c>
-      <c r="G34" s="588"/>
+      <c r="G34" s="636"/>
       <c r="H34" s="42"/>
       <c r="I34" s="42"/>
       <c r="J34" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="582" t="str">
+      <c r="K34" s="635" t="str">
         <f>IF(V35="","",V35)</f>
         <v/>
       </c>
-      <c r="L34" s="582"/>
+      <c r="L34" s="635"/>
       <c r="M34" s="312"/>
       <c r="O34" s="13"/>
       <c r="Q34" s="2" t="s">
@@ -21981,11 +21979,11 @@
       <c r="J35" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="K35" s="584" t="str">
+      <c r="K35" s="625" t="str">
         <f>IF(V36="","",V36)</f>
         <v/>
       </c>
-      <c r="L35" s="584"/>
+      <c r="L35" s="625"/>
       <c r="M35" s="312"/>
       <c r="O35" s="13"/>
       <c r="Q35" s="2" t="s">
@@ -22028,21 +22026,21 @@
       <c r="E36" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="583" t="str">
+      <c r="F36" s="624" t="str">
         <f>IF(R37="","",R37)</f>
         <v/>
       </c>
-      <c r="G36" s="583"/>
+      <c r="G36" s="624"/>
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
       <c r="J36" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="K36" s="584" t="str">
+      <c r="K36" s="625" t="str">
         <f>IF(V37="","",V37)</f>
         <v/>
       </c>
-      <c r="L36" s="584"/>
+      <c r="L36" s="625"/>
       <c r="M36" s="312"/>
       <c r="O36" s="13"/>
       <c r="P36" s="50" t="s">
@@ -22080,11 +22078,11 @@
       <c r="E37" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="586" t="str">
+      <c r="F37" s="626" t="str">
         <f>IF(R38="","",R38)</f>
         <v/>
       </c>
-      <c r="G37" s="586"/>
+      <c r="G37" s="626"/>
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
       <c r="J37" s="42"/>
@@ -22132,11 +22130,11 @@
       <c r="E38" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="586" t="str">
+      <c r="F38" s="626" t="str">
         <f>IF(R39="","",R39)</f>
         <v/>
       </c>
-      <c r="G38" s="586"/>
+      <c r="G38" s="626"/>
       <c r="H38" s="42"/>
       <c r="I38" s="42"/>
       <c r="J38" s="313" t="s">
@@ -22183,11 +22181,11 @@
       <c r="J39" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="K39" s="582" t="str">
+      <c r="K39" s="635" t="str">
         <f>IF(V40="","",V40)</f>
         <v/>
       </c>
-      <c r="L39" s="582"/>
+      <c r="L39" s="635"/>
       <c r="M39" s="312"/>
       <c r="O39" s="13"/>
       <c r="Q39" s="2" t="s">
@@ -22225,21 +22223,21 @@
       <c r="E40" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="583" t="str">
+      <c r="F40" s="624" t="str">
         <f>IF(R41="","",R41)</f>
         <v/>
       </c>
-      <c r="G40" s="583"/>
+      <c r="G40" s="624"/>
       <c r="H40" s="42"/>
       <c r="I40" s="42"/>
       <c r="J40" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K40" s="584" t="str">
+      <c r="K40" s="625" t="str">
         <f>IF(V41="","",V41)</f>
         <v/>
       </c>
-      <c r="L40" s="584"/>
+      <c r="L40" s="625"/>
       <c r="M40" s="312"/>
       <c r="O40" s="13"/>
       <c r="P40" s="50" t="s">
@@ -22277,11 +22275,11 @@
       <c r="E41" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="586" t="str">
+      <c r="F41" s="626" t="str">
         <f>IF(R42="","",R42)</f>
         <v/>
       </c>
-      <c r="G41" s="586"/>
+      <c r="G41" s="626"/>
       <c r="H41" s="42"/>
       <c r="I41" s="42"/>
       <c r="J41" s="42"/>
@@ -22329,11 +22327,11 @@
       <c r="E42" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="586" t="str">
+      <c r="F42" s="626" t="str">
         <f>IF(R43="","",R43)</f>
         <v/>
       </c>
-      <c r="G42" s="586"/>
+      <c r="G42" s="626"/>
       <c r="H42" s="42"/>
       <c r="I42" s="42"/>
       <c r="J42" s="42"/>
@@ -23100,10 +23098,10 @@
       <c r="I69" s="299"/>
       <c r="J69" s="299"/>
       <c r="K69" s="299"/>
-      <c r="L69" s="593" t="s">
+      <c r="L69" s="627" t="s">
         <v>83</v>
       </c>
-      <c r="M69" s="594"/>
+      <c r="M69" s="628"/>
       <c r="O69" s="56"/>
       <c r="P69" s="17" t="s">
         <v>84</v>
@@ -24772,24 +24770,24 @@
       <c r="P107" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="Q107" s="590" t="str">
+      <c r="Q107" s="629" t="str">
         <f>IF(Q106&lt;&gt;"",Q106,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R107" s="590"/>
-      <c r="S107" s="590"/>
-      <c r="T107" s="589" t="str">
+      <c r="R107" s="629"/>
+      <c r="S107" s="629"/>
+      <c r="T107" s="630" t="str">
         <f>IF(T106&lt;&gt;"",T106,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v/>
       </c>
-      <c r="U107" s="589"/>
-      <c r="V107" s="589"/>
-      <c r="W107" s="589" t="str">
+      <c r="U107" s="630"/>
+      <c r="V107" s="630"/>
+      <c r="W107" s="630" t="str">
         <f>IF(W106&lt;&gt;"",W106,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="X107" s="589"/>
-      <c r="Y107" s="589"/>
+      <c r="X107" s="630"/>
+      <c r="Y107" s="630"/>
       <c r="AA107" s="2" t="s">
         <v>152</v>
       </c>
@@ -25593,7 +25591,7 @@
         <f>DataEntry!D14</f>
         <v>0</v>
       </c>
-      <c r="S118" s="85">
+      <c r="S118" s="128">
         <f>DataEntry!E14</f>
         <v>0</v>
       </c>
@@ -25605,7 +25603,7 @@
         <f>DataEntry!G14</f>
         <v>0</v>
       </c>
-      <c r="V118" s="85">
+      <c r="V118" s="128">
         <f>DataEntry!H14</f>
         <v>0</v>
       </c>
@@ -25617,7 +25615,7 @@
         <f>DataEntry!J14</f>
         <v>0</v>
       </c>
-      <c r="Y118" s="85">
+      <c r="Y118" s="128">
         <f>DataEntry!K14</f>
         <v>0</v>
       </c>
@@ -25738,7 +25736,7 @@
         <f>DataEntry!D16</f>
         <v>0</v>
       </c>
-      <c r="S120" s="94">
+      <c r="S120" s="133">
         <f>DataEntry!E16</f>
         <v>0</v>
       </c>
@@ -25750,7 +25748,7 @@
         <f>DataEntry!G16</f>
         <v>0</v>
       </c>
-      <c r="V120" s="94">
+      <c r="V120" s="133">
         <f>DataEntry!H16</f>
         <v>0</v>
       </c>
@@ -25762,7 +25760,7 @@
         <f>DataEntry!J16</f>
         <v>0</v>
       </c>
-      <c r="Y120" s="94">
+      <c r="Y120" s="133">
         <f>DataEntry!K16</f>
         <v>0</v>
       </c>
@@ -25818,7 +25816,7 @@
         <f>DataEntry!D17</f>
         <v>0</v>
       </c>
-      <c r="S121" s="85">
+      <c r="S121" s="128">
         <f>DataEntry!E17</f>
         <v>0</v>
       </c>
@@ -25830,7 +25828,7 @@
         <f>DataEntry!G17</f>
         <v>0</v>
       </c>
-      <c r="V121" s="85">
+      <c r="V121" s="128">
         <f>DataEntry!H17</f>
         <v>0</v>
       </c>
@@ -25842,7 +25840,7 @@
         <f>DataEntry!J17</f>
         <v>0</v>
       </c>
-      <c r="Y121" s="85">
+      <c r="Y121" s="128">
         <f>DataEntry!K17</f>
         <v>0</v>
       </c>
@@ -25977,7 +25975,7 @@
         <f>DataEntry!D19</f>
         <v>0</v>
       </c>
-      <c r="S123" s="94">
+      <c r="S123" s="133">
         <f>DataEntry!E19</f>
         <v>0</v>
       </c>
@@ -25989,7 +25987,7 @@
         <f>DataEntry!G19</f>
         <v>0</v>
       </c>
-      <c r="V123" s="94">
+      <c r="V123" s="133">
         <f>DataEntry!H19</f>
         <v>0</v>
       </c>
@@ -26001,7 +25999,7 @@
         <f>DataEntry!J19</f>
         <v>0</v>
       </c>
-      <c r="Y123" s="94">
+      <c r="Y123" s="133">
         <f>DataEntry!K19</f>
         <v>0</v>
       </c>
@@ -26781,24 +26779,24 @@
       <c r="P139" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="Q139" s="590" t="str">
+      <c r="Q139" s="629" t="str">
         <f>IF(Q138&lt;&gt;"",Q138,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R139" s="590"/>
-      <c r="S139" s="590"/>
-      <c r="T139" s="589" t="str">
+      <c r="R139" s="629"/>
+      <c r="S139" s="629"/>
+      <c r="T139" s="630" t="str">
         <f>IF(T138&lt;&gt;"",T138,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v/>
       </c>
-      <c r="U139" s="589"/>
-      <c r="V139" s="589"/>
-      <c r="W139" s="589" t="str">
+      <c r="U139" s="630"/>
+      <c r="V139" s="630"/>
+      <c r="W139" s="630" t="str">
         <f>IF(W138&lt;&gt;"",W138,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="X139" s="589"/>
-      <c r="Y139" s="589"/>
+      <c r="X139" s="630"/>
+      <c r="Y139" s="630"/>
       <c r="AA139" s="2" t="str">
         <f>$T$139&amp;" Mag 4"</f>
         <v xml:space="preserve"> Mag 4</v>
@@ -29142,10 +29140,10 @@
       <c r="P181" s="135"/>
       <c r="Q181" s="137"/>
       <c r="R181" s="128"/>
-      <c r="T181" s="591" t="s">
+      <c r="T181" s="612" t="s">
         <v>244</v>
       </c>
-      <c r="U181" s="591"/>
+      <c r="U181" s="612"/>
       <c r="W181" s="2" t="s">
         <v>198</v>
       </c>
@@ -29516,7 +29514,7 @@
       <c r="K190" s="323"/>
       <c r="L190" s="323"/>
       <c r="M190" s="327"/>
-      <c r="O190" s="592" t="str">
+      <c r="O190" s="621" t="str">
         <f>$Q$107</f>
         <v>Auto 1</v>
       </c>
@@ -29566,7 +29564,7 @@
       <c r="K191" s="323"/>
       <c r="L191" s="323"/>
       <c r="M191" s="303"/>
-      <c r="O191" s="592"/>
+      <c r="O191" s="621"/>
       <c r="P191" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -29612,7 +29610,7 @@
       <c r="K192" s="135"/>
       <c r="L192" s="135"/>
       <c r="M192" s="303"/>
-      <c r="O192" s="592"/>
+      <c r="O192" s="621"/>
       <c r="P192" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -29658,7 +29656,7 @@
       <c r="K193" s="135"/>
       <c r="L193" s="135"/>
       <c r="M193" s="303"/>
-      <c r="O193" s="592"/>
+      <c r="O193" s="621"/>
       <c r="P193" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -29701,7 +29699,7 @@
       <c r="K194" s="135"/>
       <c r="L194" s="135"/>
       <c r="M194" s="303"/>
-      <c r="O194" s="592"/>
+      <c r="O194" s="621"/>
       <c r="P194" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -29744,7 +29742,7 @@
       <c r="K195" s="135"/>
       <c r="L195" s="135"/>
       <c r="M195" s="303"/>
-      <c r="O195" s="592" t="str">
+      <c r="O195" s="621" t="str">
         <f>$T$107</f>
         <v/>
       </c>
@@ -29790,7 +29788,7 @@
       <c r="K196" s="305"/>
       <c r="L196" s="305"/>
       <c r="M196" s="306"/>
-      <c r="O196" s="592"/>
+      <c r="O196" s="621"/>
       <c r="P196" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -29835,7 +29833,7 @@
         <f>IF($X$7="","",$X$7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="O197" s="592"/>
+      <c r="O197" s="621"/>
       <c r="P197" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -29880,7 +29878,7 @@
         <f>IF($R$13="","",$R$13)</f>
         <v/>
       </c>
-      <c r="O198" s="592"/>
+      <c r="O198" s="621"/>
       <c r="P198" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -29926,7 +29924,7 @@
         <f>$H$2</f>
         <v>Medical University of South Carolina</v>
       </c>
-      <c r="O199" s="592"/>
+      <c r="O199" s="621"/>
       <c r="P199" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -29975,7 +29973,7 @@
         <f>$H$5</f>
         <v>Fluoroscopy System Compliance Inspection</v>
       </c>
-      <c r="O200" s="592" t="str">
+      <c r="O200" s="621" t="str">
         <f>$W$107</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -30024,7 +30022,7 @@
       <c r="K201" s="299"/>
       <c r="L201" s="299"/>
       <c r="M201" s="300"/>
-      <c r="O201" s="592"/>
+      <c r="O201" s="621"/>
       <c r="P201" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30078,7 +30076,7 @@
         <v>44905</v>
       </c>
       <c r="M202" s="12"/>
-      <c r="O202" s="592"/>
+      <c r="O202" s="621"/>
       <c r="P202" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -30111,7 +30109,7 @@
       </c>
       <c r="B203" s="10"/>
       <c r="M203" s="12"/>
-      <c r="O203" s="592"/>
+      <c r="O203" s="621"/>
       <c r="P203" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -30145,20 +30143,20 @@
       <c r="B204" s="301"/>
       <c r="C204" s="351"/>
       <c r="D204" s="323"/>
-      <c r="E204" s="595" t="s">
+      <c r="E204" s="591" t="s">
         <v>261</v>
       </c>
-      <c r="F204" s="632" t="s">
+      <c r="F204" s="593" t="s">
         <v>262</v>
       </c>
       <c r="G204" s="518" t="s">
         <v>263</v>
       </c>
-      <c r="H204" s="595" t="str">
+      <c r="H204" s="591" t="str">
         <f>R276</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="I204" s="597" t="str">
+      <c r="I204" s="631" t="str">
         <f>S276</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -30171,10 +30169,10 @@
       <c r="L204" s="135" t="s">
         <v>266</v>
       </c>
-      <c r="M204" s="599" t="s">
+      <c r="M204" s="633" t="s">
         <v>267</v>
       </c>
-      <c r="O204" s="592"/>
+      <c r="O204" s="621"/>
       <c r="P204" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -30212,11 +30210,11 @@
       <c r="D205" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="E205" s="596"/>
-      <c r="F205" s="633"/>
+      <c r="E205" s="592"/>
+      <c r="F205" s="594"/>
       <c r="G205" s="518"/>
-      <c r="H205" s="596"/>
-      <c r="I205" s="598"/>
+      <c r="H205" s="592"/>
+      <c r="I205" s="632"/>
       <c r="J205" s="519"/>
       <c r="K205" s="135" t="str">
         <f>U277</f>
@@ -30226,7 +30224,7 @@
         <f>V277</f>
         <v>mGy/min</v>
       </c>
-      <c r="M205" s="600"/>
+      <c r="M205" s="634"/>
       <c r="O205" s="13"/>
       <c r="Y205" s="14"/>
       <c r="AA205" s="2" t="s">
@@ -30870,7 +30868,7 @@
         <f>W286</f>
         <v/>
       </c>
-      <c r="O214" s="592" t="str">
+      <c r="O214" s="621" t="str">
         <f>$Q$139</f>
         <v>Auto 1</v>
       </c>
@@ -30926,7 +30924,7 @@
       <c r="K215" s="135"/>
       <c r="L215" s="135"/>
       <c r="M215" s="303"/>
-      <c r="O215" s="592"/>
+      <c r="O215" s="621"/>
       <c r="P215" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30972,7 +30970,7 @@
       <c r="K216" s="323"/>
       <c r="L216" s="323"/>
       <c r="M216" s="303"/>
-      <c r="O216" s="592"/>
+      <c r="O216" s="621"/>
       <c r="P216" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -31018,7 +31016,7 @@
       <c r="K217" s="368"/>
       <c r="L217" s="368"/>
       <c r="M217" s="369"/>
-      <c r="O217" s="592"/>
+      <c r="O217" s="621"/>
       <c r="P217" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31065,7 +31063,7 @@
       <c r="K218" s="323"/>
       <c r="L218" s="323"/>
       <c r="M218" s="303"/>
-      <c r="O218" s="592"/>
+      <c r="O218" s="621"/>
       <c r="P218" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -31108,7 +31106,7 @@
       <c r="K219" s="323"/>
       <c r="L219" s="323"/>
       <c r="M219" s="327"/>
-      <c r="O219" s="592" t="str">
+      <c r="O219" s="621" t="str">
         <f>$T$139</f>
         <v/>
       </c>
@@ -31169,7 +31167,7 @@
         <v/>
       </c>
       <c r="M220" s="327"/>
-      <c r="O220" s="592"/>
+      <c r="O220" s="621"/>
       <c r="P220" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -31212,7 +31210,7 @@
       <c r="K221" s="323"/>
       <c r="L221" s="323"/>
       <c r="M221" s="327"/>
-      <c r="O221" s="592"/>
+      <c r="O221" s="621"/>
       <c r="P221" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -31263,7 +31261,7 @@
       <c r="K222" s="323"/>
       <c r="L222" s="323"/>
       <c r="M222" s="327"/>
-      <c r="O222" s="592"/>
+      <c r="O222" s="621"/>
       <c r="P222" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31320,7 +31318,7 @@
       <c r="K223" s="323"/>
       <c r="L223" s="323"/>
       <c r="M223" s="327"/>
-      <c r="O223" s="592"/>
+      <c r="O223" s="621"/>
       <c r="P223" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -31384,7 +31382,7 @@
       <c r="K224" s="323"/>
       <c r="L224" s="323"/>
       <c r="M224" s="327"/>
-      <c r="O224" s="592" t="str">
+      <c r="O224" s="621" t="str">
         <f>$W$139</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -31448,7 +31446,7 @@
       <c r="K225" s="323"/>
       <c r="L225" s="323"/>
       <c r="M225" s="327"/>
-      <c r="O225" s="592"/>
+      <c r="O225" s="621"/>
       <c r="P225" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -31509,7 +31507,7 @@
       <c r="K226" s="323"/>
       <c r="L226" s="323"/>
       <c r="M226" s="327"/>
-      <c r="O226" s="592"/>
+      <c r="O226" s="621"/>
       <c r="P226" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -31570,7 +31568,7 @@
       <c r="K227" s="323"/>
       <c r="L227" s="323"/>
       <c r="M227" s="327"/>
-      <c r="O227" s="592"/>
+      <c r="O227" s="621"/>
       <c r="P227" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31624,7 +31622,7 @@
       <c r="K228" s="323"/>
       <c r="L228" s="323"/>
       <c r="M228" s="327"/>
-      <c r="O228" s="592"/>
+      <c r="O228" s="621"/>
       <c r="P228" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -32177,7 +32175,7 @@
       <c r="K240" s="323"/>
       <c r="L240" s="323"/>
       <c r="M240" s="327"/>
-      <c r="O240" s="601" t="s">
+      <c r="O240" s="622" t="s">
         <v>293</v>
       </c>
       <c r="P240" s="167" t="s">
@@ -32236,7 +32234,7 @@
       <c r="K241" s="323"/>
       <c r="L241" s="323"/>
       <c r="M241" s="327"/>
-      <c r="O241" s="601"/>
+      <c r="O241" s="622"/>
       <c r="P241" s="172" t="s">
         <v>296</v>
       </c>
@@ -32293,7 +32291,7 @@
       <c r="K242" s="323"/>
       <c r="L242" s="323"/>
       <c r="M242" s="327"/>
-      <c r="O242" s="601" t="str">
+      <c r="O242" s="622" t="str">
         <f>IF($U$137=1,"Scatter - Pulse", "Scatter – Digital acq")</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -32353,7 +32351,7 @@
       <c r="K243" s="323"/>
       <c r="L243" s="323"/>
       <c r="M243" s="327"/>
-      <c r="O243" s="601"/>
+      <c r="O243" s="622"/>
       <c r="P243" s="172" t="s">
         <v>296</v>
       </c>
@@ -32883,17 +32881,17 @@
       <c r="P257" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="Q257" s="602" t="s">
+      <c r="Q257" s="623" t="s">
         <v>312</v>
       </c>
-      <c r="R257" s="602"/>
+      <c r="R257" s="623"/>
       <c r="S257" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="T257" s="602" t="s">
+      <c r="T257" s="623" t="s">
         <v>314</v>
       </c>
-      <c r="U257" s="602"/>
+      <c r="U257" s="623"/>
       <c r="V257" s="1" t="s">
         <v>315</v>
       </c>
@@ -33390,24 +33388,24 @@
         <f t="shared" si="43"/>
         <v>Attenuator</v>
       </c>
-      <c r="E269" s="603" t="str">
+      <c r="E269" s="614" t="str">
         <f>Q107</f>
         <v>Auto 1</v>
       </c>
-      <c r="F269" s="604"/>
-      <c r="G269" s="604"/>
-      <c r="H269" s="604" t="str">
+      <c r="F269" s="615"/>
+      <c r="G269" s="615"/>
+      <c r="H269" s="615" t="str">
         <f>T107</f>
         <v/>
       </c>
-      <c r="I269" s="604"/>
-      <c r="J269" s="604"/>
-      <c r="K269" s="605" t="str">
+      <c r="I269" s="615"/>
+      <c r="J269" s="615"/>
+      <c r="K269" s="616" t="str">
         <f>W107</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L269" s="605"/>
-      <c r="M269" s="606"/>
+      <c r="L269" s="616"/>
+      <c r="M269" s="617"/>
       <c r="O269" s="189" t="str">
         <f t="shared" si="44"/>
         <v/>
@@ -33509,7 +33507,7 @@
         <v>7</v>
       </c>
       <c r="B271" s="301"/>
-      <c r="C271" s="610" t="str">
+      <c r="C271" s="590" t="str">
         <f>O110&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33585,7 +33583,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="301"/>
-      <c r="C272" s="610"/>
+      <c r="C272" s="590"/>
       <c r="D272" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -33651,7 +33649,7 @@
         <v>9</v>
       </c>
       <c r="B273" s="301"/>
-      <c r="C273" s="610"/>
+      <c r="C273" s="590"/>
       <c r="D273" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -33724,7 +33722,7 @@
         <v>10</v>
       </c>
       <c r="B274" s="301"/>
-      <c r="C274" s="610" t="str">
+      <c r="C274" s="590" t="str">
         <f>O113&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33793,7 +33791,7 @@
         <v>11</v>
       </c>
       <c r="B275" s="301"/>
-      <c r="C275" s="610"/>
+      <c r="C275" s="590"/>
       <c r="D275" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -33866,7 +33864,7 @@
         <v>12</v>
       </c>
       <c r="B276" s="301"/>
-      <c r="C276" s="610"/>
+      <c r="C276" s="590"/>
       <c r="D276" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -33907,17 +33905,17 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="O276" s="611" t="s">
+      <c r="O276" s="618" t="s">
         <v>261</v>
       </c>
-      <c r="P276" s="612" t="s">
+      <c r="P276" s="619" t="s">
         <v>262</v>
       </c>
-      <c r="R276" s="612" t="str">
+      <c r="R276" s="619" t="str">
         <f>"Ind AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="S276" s="612" t="str">
+      <c r="S276" s="619" t="str">
         <f>"Meas AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -33939,7 +33937,7 @@
         <v>13</v>
       </c>
       <c r="B277" s="301"/>
-      <c r="C277" s="610" t="str">
+      <c r="C277" s="590" t="str">
         <f>O116&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33983,13 +33981,13 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="O277" s="611"/>
-      <c r="P277" s="612"/>
+      <c r="O277" s="618"/>
+      <c r="P277" s="619"/>
       <c r="Q277" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="R277" s="612"/>
-      <c r="S277" s="612"/>
+      <c r="R277" s="619"/>
+      <c r="S277" s="619"/>
       <c r="T277" s="1" t="s">
         <v>321</v>
       </c>
@@ -34021,7 +34019,7 @@
         <v>14</v>
       </c>
       <c r="B278" s="301"/>
-      <c r="C278" s="610"/>
+      <c r="C278" s="590"/>
       <c r="D278" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -34108,7 +34106,7 @@
         <v>15</v>
       </c>
       <c r="B279" s="301"/>
-      <c r="C279" s="610"/>
+      <c r="C279" s="590"/>
       <c r="D279" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -34202,7 +34200,7 @@
         <v>16</v>
       </c>
       <c r="B280" s="301"/>
-      <c r="C280" s="610" t="str">
+      <c r="C280" s="590" t="str">
         <f>O119&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -34302,7 +34300,7 @@
         <v>17</v>
       </c>
       <c r="B281" s="301"/>
-      <c r="C281" s="610"/>
+      <c r="C281" s="590"/>
       <c r="D281" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -34389,7 +34387,7 @@
         <v>18</v>
       </c>
       <c r="B282" s="301"/>
-      <c r="C282" s="610"/>
+      <c r="C282" s="590"/>
       <c r="D282" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -34483,7 +34481,7 @@
         <v>19</v>
       </c>
       <c r="B283" s="301"/>
-      <c r="C283" s="610" t="str">
+      <c r="C283" s="590" t="str">
         <f>O122&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -34573,7 +34571,7 @@
         <v>20</v>
       </c>
       <c r="B284" s="301"/>
-      <c r="C284" s="610"/>
+      <c r="C284" s="590"/>
       <c r="D284" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -34667,7 +34665,7 @@
         <v>21</v>
       </c>
       <c r="B285" s="301"/>
-      <c r="C285" s="610"/>
+      <c r="C285" s="590"/>
       <c r="D285" s="391">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -35102,13 +35100,13 @@
       <c r="L293" s="135"/>
       <c r="M293" s="303"/>
       <c r="O293" s="225"/>
-      <c r="P293" s="613" t="s">
+      <c r="P293" s="620" t="s">
         <v>327</v>
       </c>
-      <c r="Q293" s="613"/>
-      <c r="R293" s="613"/>
-      <c r="S293" s="613"/>
-      <c r="T293" s="613"/>
+      <c r="Q293" s="620"/>
+      <c r="R293" s="620"/>
+      <c r="S293" s="620"/>
+      <c r="T293" s="620"/>
       <c r="U293" s="223"/>
       <c r="V293" s="223"/>
       <c r="W293" s="223"/>
@@ -35549,13 +35547,13 @@
       <c r="L302" s="135"/>
       <c r="M302" s="303"/>
       <c r="O302" s="225"/>
-      <c r="P302" s="613" t="s">
+      <c r="P302" s="620" t="s">
         <v>327</v>
       </c>
-      <c r="Q302" s="613"/>
-      <c r="R302" s="613"/>
-      <c r="S302" s="613"/>
-      <c r="T302" s="613"/>
+      <c r="Q302" s="620"/>
+      <c r="R302" s="620"/>
+      <c r="S302" s="620"/>
+      <c r="T302" s="620"/>
       <c r="U302" s="223"/>
       <c r="V302" s="223"/>
       <c r="W302" s="223"/>
@@ -35576,7 +35574,7 @@
         <v>39</v>
       </c>
       <c r="B303" s="301"/>
-      <c r="C303" s="618" t="str">
+      <c r="C303" s="595" t="str">
         <f>O190</f>
         <v>Auto 1</v>
       </c>
@@ -35639,7 +35637,7 @@
         <v>40</v>
       </c>
       <c r="B304" s="301"/>
-      <c r="C304" s="619"/>
+      <c r="C304" s="596"/>
       <c r="D304" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35712,7 +35710,7 @@
         <v>41</v>
       </c>
       <c r="B305" s="301"/>
-      <c r="C305" s="619"/>
+      <c r="C305" s="596"/>
       <c r="D305" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35775,7 +35773,7 @@
         <v>42</v>
       </c>
       <c r="B306" s="301"/>
-      <c r="C306" s="619"/>
+      <c r="C306" s="596"/>
       <c r="D306" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35842,7 +35840,7 @@
         <v>43</v>
       </c>
       <c r="B307" s="301"/>
-      <c r="C307" s="620"/>
+      <c r="C307" s="607"/>
       <c r="D307" s="436" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35902,7 +35900,7 @@
         <v>44</v>
       </c>
       <c r="B308" s="301"/>
-      <c r="C308" s="618" t="str">
+      <c r="C308" s="595" t="str">
         <f>O195</f>
         <v/>
       </c>
@@ -35972,7 +35970,7 @@
         <v>45</v>
       </c>
       <c r="B309" s="301"/>
-      <c r="C309" s="619"/>
+      <c r="C309" s="596"/>
       <c r="D309" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36024,7 +36022,7 @@
         <v>46</v>
       </c>
       <c r="B310" s="301"/>
-      <c r="C310" s="619"/>
+      <c r="C310" s="596"/>
       <c r="D310" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36083,7 +36081,7 @@
         <v>47</v>
       </c>
       <c r="B311" s="301"/>
-      <c r="C311" s="619"/>
+      <c r="C311" s="596"/>
       <c r="D311" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36135,7 +36133,7 @@
         <v>48</v>
       </c>
       <c r="B312" s="301"/>
-      <c r="C312" s="621"/>
+      <c r="C312" s="597"/>
       <c r="D312" s="439" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36191,7 +36189,7 @@
         <v>49</v>
       </c>
       <c r="B313" s="301"/>
-      <c r="C313" s="622" t="str">
+      <c r="C313" s="608" t="str">
         <f>O200</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -36243,7 +36241,7 @@
         <v>50</v>
       </c>
       <c r="B314" s="301"/>
-      <c r="C314" s="619"/>
+      <c r="C314" s="596"/>
       <c r="D314" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36295,7 +36293,7 @@
         <v>51</v>
       </c>
       <c r="B315" s="301"/>
-      <c r="C315" s="619"/>
+      <c r="C315" s="596"/>
       <c r="D315" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36340,7 +36338,7 @@
         <v>52</v>
       </c>
       <c r="B316" s="301"/>
-      <c r="C316" s="619"/>
+      <c r="C316" s="596"/>
       <c r="D316" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36394,7 +36392,7 @@
         <v>53</v>
       </c>
       <c r="B317" s="301"/>
-      <c r="C317" s="621"/>
+      <c r="C317" s="597"/>
       <c r="D317" s="439" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36478,9 +36476,7 @@
       <c r="AA318" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="AB318" s="28">
-        <v>1</v>
-      </c>
+      <c r="AB318" s="28"/>
       <c r="AC318" s="29" t="str">
         <f>IF(AB318&lt;&gt;AD318,"Change","")</f>
         <v>Change</v>
@@ -36518,10 +36514,10 @@
       <c r="R319" s="246"/>
       <c r="S319" s="247"/>
       <c r="T319" s="247"/>
-      <c r="V319" s="591" t="s">
+      <c r="V319" s="612" t="s">
         <v>338</v>
       </c>
-      <c r="W319" s="591"/>
+      <c r="W319" s="612"/>
       <c r="X319" s="17" t="s">
         <v>339</v>
       </c>
@@ -36722,7 +36718,7 @@
         <v>60</v>
       </c>
       <c r="B324" s="301"/>
-      <c r="C324" s="607" t="str">
+      <c r="C324" s="601" t="str">
         <f>O240</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -36772,7 +36768,7 @@
         <v>61</v>
       </c>
       <c r="B325" s="301"/>
-      <c r="C325" s="608"/>
+      <c r="C325" s="602"/>
       <c r="D325" s="448" t="str">
         <f>P241</f>
         <v>Waist level</v>
@@ -36930,13 +36926,13 @@
         <v>346</v>
       </c>
       <c r="P329" s="53"/>
-      <c r="Q329" s="609" t="s">
+      <c r="Q329" s="613" t="s">
         <v>347</v>
       </c>
-      <c r="R329" s="609"/>
-      <c r="S329" s="609"/>
-      <c r="T329" s="609"/>
-      <c r="U329" s="609"/>
+      <c r="R329" s="613"/>
+      <c r="S329" s="613"/>
+      <c r="T329" s="613"/>
+      <c r="U329" s="613"/>
       <c r="Y329" s="14"/>
     </row>
     <row r="330" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37119,24 +37115,24 @@
         <f t="shared" si="72"/>
         <v>Attenuator</v>
       </c>
-      <c r="E335" s="603" t="str">
+      <c r="E335" s="614" t="str">
         <f>Q139</f>
         <v>Auto 1</v>
       </c>
-      <c r="F335" s="604"/>
-      <c r="G335" s="604"/>
-      <c r="H335" s="604" t="str">
+      <c r="F335" s="615"/>
+      <c r="G335" s="615"/>
+      <c r="H335" s="615" t="str">
         <f>T139</f>
         <v/>
       </c>
-      <c r="I335" s="604"/>
-      <c r="J335" s="604"/>
-      <c r="K335" s="605" t="str">
+      <c r="I335" s="615"/>
+      <c r="J335" s="615"/>
+      <c r="K335" s="616" t="str">
         <f>W139</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L335" s="605"/>
-      <c r="M335" s="606"/>
+      <c r="L335" s="616"/>
+      <c r="M335" s="617"/>
       <c r="O335" s="130"/>
       <c r="P335" s="129" t="s">
         <v>353</v>
@@ -37213,7 +37209,7 @@
         <v>7</v>
       </c>
       <c r="B337" s="301"/>
-      <c r="C337" s="610" t="str">
+      <c r="C337" s="590" t="str">
         <f>O142&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37273,7 +37269,7 @@
         <v>8</v>
       </c>
       <c r="B338" s="301"/>
-      <c r="C338" s="610"/>
+      <c r="C338" s="590"/>
       <c r="D338" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37330,7 +37326,7 @@
         <v>9</v>
       </c>
       <c r="B339" s="301"/>
-      <c r="C339" s="610"/>
+      <c r="C339" s="590"/>
       <c r="D339" s="463">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37387,7 +37383,7 @@
         <v>10</v>
       </c>
       <c r="B340" s="301"/>
-      <c r="C340" s="610" t="str">
+      <c r="C340" s="590" t="str">
         <f>O145&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37447,7 +37443,7 @@
         <v>11</v>
       </c>
       <c r="B341" s="301"/>
-      <c r="C341" s="610"/>
+      <c r="C341" s="590"/>
       <c r="D341" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37504,7 +37500,7 @@
         <v>12</v>
       </c>
       <c r="B342" s="301"/>
-      <c r="C342" s="610"/>
+      <c r="C342" s="590"/>
       <c r="D342" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37561,7 +37557,7 @@
         <v>13</v>
       </c>
       <c r="B343" s="301"/>
-      <c r="C343" s="610" t="str">
+      <c r="C343" s="590" t="str">
         <f>O148&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37613,7 +37609,7 @@
         <v>14</v>
       </c>
       <c r="B344" s="301"/>
-      <c r="C344" s="610"/>
+      <c r="C344" s="590"/>
       <c r="D344" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37675,7 +37671,7 @@
         <v>15</v>
       </c>
       <c r="B345" s="301"/>
-      <c r="C345" s="610"/>
+      <c r="C345" s="590"/>
       <c r="D345" s="463">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37738,7 +37734,7 @@
         <v>16</v>
       </c>
       <c r="B346" s="301"/>
-      <c r="C346" s="610" t="str">
+      <c r="C346" s="590" t="str">
         <f>O151&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37801,7 +37797,7 @@
         <v>17</v>
       </c>
       <c r="B347" s="301"/>
-      <c r="C347" s="610"/>
+      <c r="C347" s="590"/>
       <c r="D347" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37859,7 +37855,7 @@
         <v>18</v>
       </c>
       <c r="B348" s="301"/>
-      <c r="C348" s="610"/>
+      <c r="C348" s="590"/>
       <c r="D348" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37937,7 +37933,7 @@
         <v>19</v>
       </c>
       <c r="B349" s="301"/>
-      <c r="C349" s="610" t="str">
+      <c r="C349" s="590" t="str">
         <f>O154&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -38000,7 +37996,7 @@
         <v>20</v>
       </c>
       <c r="B350" s="301"/>
-      <c r="C350" s="610"/>
+      <c r="C350" s="590"/>
       <c r="D350" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -38059,7 +38055,7 @@
         <v>21</v>
       </c>
       <c r="B351" s="301"/>
-      <c r="C351" s="610"/>
+      <c r="C351" s="590"/>
       <c r="D351" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -38368,11 +38364,11 @@
         <f>IF(OR(V358="",V359="",V362=""),"",(V358-V359)*V362)</f>
         <v/>
       </c>
-      <c r="Q358" s="614" t="str">
+      <c r="Q358" s="603" t="str">
         <f>IF(OR(P358="",P359=""),"",(ABS(P358)+ABS(P359))/$O$355)</f>
         <v/>
       </c>
-      <c r="R358" s="615" t="str">
+      <c r="R358" s="604" t="str">
         <f>IF(OR(Q358="",Q360=""),"",Q358+Q360)</f>
         <v/>
       </c>
@@ -38411,8 +38407,8 @@
         <f>IF(OR(W358="",W359="",V362=""),"",(W358-W359)*V362)</f>
         <v/>
       </c>
-      <c r="Q359" s="614"/>
-      <c r="R359" s="614"/>
+      <c r="Q359" s="603"/>
+      <c r="R359" s="603"/>
       <c r="S359" s="146" t="str">
         <f>IF(AB171="","",AB171)</f>
         <v/>
@@ -38448,11 +38444,11 @@
         <f>IF(OR(X358="",X359="",V362=""),"",(X358-X359)*V362)</f>
         <v/>
       </c>
-      <c r="Q360" s="615" t="str">
+      <c r="Q360" s="604" t="str">
         <f>IF(OR(P360="",P361=""),"",(ABS(P360)+ABS(P361))/$O$355)</f>
         <v/>
       </c>
-      <c r="R360" s="615"/>
+      <c r="R360" s="604"/>
       <c r="S360" s="146" t="str">
         <f>IF(AB172="","",AB172)</f>
         <v/>
@@ -38494,8 +38490,8 @@
         <f>IF(OR(Y358="",Y359="",V362=""),"",(Y358-Y359)*V362)</f>
         <v/>
       </c>
-      <c r="Q361" s="615"/>
-      <c r="R361" s="615"/>
+      <c r="Q361" s="604"/>
+      <c r="R361" s="604"/>
       <c r="S361" s="148" t="str">
         <f>IF(AB173="","",AB173)</f>
         <v/>
@@ -38667,7 +38663,7 @@
         <v>36</v>
       </c>
       <c r="B366" s="301"/>
-      <c r="C366" s="616" t="str">
+      <c r="C366" s="605" t="str">
         <f>O214</f>
         <v>Auto 1</v>
       </c>
@@ -38718,7 +38714,7 @@
         <v>37</v>
       </c>
       <c r="B367" s="301"/>
-      <c r="C367" s="617"/>
+      <c r="C367" s="606"/>
       <c r="D367" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38764,7 +38760,7 @@
         <v>38</v>
       </c>
       <c r="B368" s="301"/>
-      <c r="C368" s="617"/>
+      <c r="C368" s="606"/>
       <c r="D368" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38799,7 +38795,7 @@
         <v>39</v>
       </c>
       <c r="B369" s="301"/>
-      <c r="C369" s="617"/>
+      <c r="C369" s="606"/>
       <c r="D369" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38834,7 +38830,7 @@
         <v>40</v>
       </c>
       <c r="B370" s="301"/>
-      <c r="C370" s="617"/>
+      <c r="C370" s="606"/>
       <c r="D370" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38879,7 +38875,7 @@
         <v>41</v>
       </c>
       <c r="B371" s="301"/>
-      <c r="C371" s="618" t="str">
+      <c r="C371" s="595" t="str">
         <f>O219</f>
         <v/>
       </c>
@@ -38929,7 +38925,7 @@
         <v>42</v>
       </c>
       <c r="B372" s="301"/>
-      <c r="C372" s="619"/>
+      <c r="C372" s="596"/>
       <c r="D372" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38979,7 +38975,7 @@
         <v>43</v>
       </c>
       <c r="B373" s="301"/>
-      <c r="C373" s="619"/>
+      <c r="C373" s="596"/>
       <c r="D373" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39026,7 +39022,7 @@
         <v>44</v>
       </c>
       <c r="B374" s="301"/>
-      <c r="C374" s="619"/>
+      <c r="C374" s="596"/>
       <c r="D374" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39076,7 +39072,7 @@
         <v>45</v>
       </c>
       <c r="B375" s="301"/>
-      <c r="C375" s="621"/>
+      <c r="C375" s="597"/>
       <c r="D375" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39123,7 +39119,7 @@
         <v>46</v>
       </c>
       <c r="B376" s="301"/>
-      <c r="C376" s="634" t="str">
+      <c r="C376" s="598" t="str">
         <f>O224</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -39176,7 +39172,7 @@
         <v>47</v>
       </c>
       <c r="B377" s="301"/>
-      <c r="C377" s="635"/>
+      <c r="C377" s="599"/>
       <c r="D377" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39223,7 +39219,7 @@
         <v>48</v>
       </c>
       <c r="B378" s="301"/>
-      <c r="C378" s="635"/>
+      <c r="C378" s="599"/>
       <c r="D378" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39273,7 +39269,7 @@
         <v>49</v>
       </c>
       <c r="B379" s="301"/>
-      <c r="C379" s="635"/>
+      <c r="C379" s="599"/>
       <c r="D379" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39320,7 +39316,7 @@
         <v>50</v>
       </c>
       <c r="B380" s="301"/>
-      <c r="C380" s="636"/>
+      <c r="C380" s="600"/>
       <c r="D380" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39630,7 +39626,7 @@
         <v>58</v>
       </c>
       <c r="B388" s="301"/>
-      <c r="C388" s="607" t="str">
+      <c r="C388" s="601" t="str">
         <f>O242</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -39681,7 +39677,7 @@
         <v>59</v>
       </c>
       <c r="B389" s="301"/>
-      <c r="C389" s="608"/>
+      <c r="C389" s="602"/>
       <c r="D389" s="448" t="str">
         <f>P243</f>
         <v>Waist level</v>
@@ -40032,14 +40028,14 @@
       <c r="E399" s="299"/>
       <c r="F399" s="299"/>
       <c r="G399" s="299"/>
-      <c r="H399" s="625" t="s">
+      <c r="H399" s="611" t="s">
         <v>393</v>
       </c>
-      <c r="I399" s="625"/>
-      <c r="J399" s="625" t="s">
+      <c r="I399" s="611"/>
+      <c r="J399" s="611" t="s">
         <v>394</v>
       </c>
-      <c r="K399" s="625"/>
+      <c r="K399" s="611"/>
       <c r="L399" s="299"/>
       <c r="M399" s="300"/>
       <c r="O399" s="13"/>
@@ -40613,20 +40609,20 @@
       </c>
       <c r="B413" s="301"/>
       <c r="C413" s="42"/>
-      <c r="D413" s="623" t="s">
+      <c r="D413" s="609" t="s">
         <v>400</v>
       </c>
-      <c r="E413" s="623"/>
-      <c r="F413" s="623"/>
-      <c r="G413" s="623"/>
-      <c r="H413" s="623"/>
-      <c r="I413" s="623" t="s">
+      <c r="E413" s="609"/>
+      <c r="F413" s="609"/>
+      <c r="G413" s="609"/>
+      <c r="H413" s="609"/>
+      <c r="I413" s="609" t="s">
         <v>401</v>
       </c>
-      <c r="J413" s="623"/>
-      <c r="K413" s="623"/>
-      <c r="L413" s="623"/>
-      <c r="M413" s="624"/>
+      <c r="J413" s="609"/>
+      <c r="K413" s="609"/>
+      <c r="L413" s="609"/>
+      <c r="M413" s="610"/>
       <c r="O413" s="13"/>
       <c r="P413" s="2" t="s">
         <v>188</v>
@@ -42106,11 +42102,11 @@
         <f t="shared" si="95"/>
         <v/>
       </c>
-      <c r="F442" s="626" t="str">
+      <c r="F442" s="584" t="str">
         <f t="shared" si="95"/>
         <v/>
       </c>
-      <c r="G442" s="628" t="str">
+      <c r="G442" s="586" t="str">
         <f t="shared" si="95"/>
         <v/>
       </c>
@@ -42151,8 +42147,8 @@
         <f>P359</f>
         <v/>
       </c>
-      <c r="F443" s="627"/>
-      <c r="G443" s="629"/>
+      <c r="F443" s="585"/>
+      <c r="G443" s="587"/>
       <c r="H443" s="200"/>
       <c r="I443" s="82" t="str">
         <f>T360</f>
@@ -42192,11 +42188,11 @@
         <f>P360</f>
         <v/>
       </c>
-      <c r="F444" s="627" t="str">
+      <c r="F444" s="585" t="str">
         <f>Q360</f>
         <v/>
       </c>
-      <c r="G444" s="629"/>
+      <c r="G444" s="587"/>
       <c r="H444" s="135"/>
       <c r="I444" s="91" t="str">
         <f>T361</f>
@@ -42237,8 +42233,8 @@
         <f>P361</f>
         <v/>
       </c>
-      <c r="F445" s="631"/>
-      <c r="G445" s="630"/>
+      <c r="F445" s="589"/>
+      <c r="G445" s="588"/>
       <c r="H445" s="135"/>
       <c r="I445" s="135"/>
       <c r="J445" s="135"/>
@@ -48597,30 +48593,71 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="106">
-    <mergeCell ref="F442:F443"/>
-    <mergeCell ref="G442:G445"/>
-    <mergeCell ref="F444:F445"/>
-    <mergeCell ref="C337:C339"/>
-    <mergeCell ref="C340:C342"/>
-    <mergeCell ref="C343:C345"/>
-    <mergeCell ref="C346:C348"/>
-    <mergeCell ref="C349:C351"/>
-    <mergeCell ref="E204:E205"/>
-    <mergeCell ref="F204:F205"/>
-    <mergeCell ref="C371:C375"/>
-    <mergeCell ref="C376:C380"/>
-    <mergeCell ref="C388:C389"/>
-    <mergeCell ref="Q358:Q359"/>
-    <mergeCell ref="R358:R361"/>
-    <mergeCell ref="Q360:Q361"/>
-    <mergeCell ref="C366:C370"/>
-    <mergeCell ref="C303:C307"/>
-    <mergeCell ref="C308:C312"/>
-    <mergeCell ref="C313:C317"/>
-    <mergeCell ref="D413:H413"/>
-    <mergeCell ref="I413:M413"/>
-    <mergeCell ref="H399:I399"/>
-    <mergeCell ref="J399:K399"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="W107:Y107"/>
+    <mergeCell ref="Q139:S139"/>
+    <mergeCell ref="T139:V139"/>
+    <mergeCell ref="W139:Y139"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="T181:U181"/>
+    <mergeCell ref="O190:O194"/>
+    <mergeCell ref="O195:O199"/>
+    <mergeCell ref="O200:O204"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="Q107:S107"/>
+    <mergeCell ref="T107:V107"/>
+    <mergeCell ref="H204:H205"/>
+    <mergeCell ref="I204:I205"/>
+    <mergeCell ref="M204:M205"/>
+    <mergeCell ref="O214:O218"/>
+    <mergeCell ref="O219:O223"/>
+    <mergeCell ref="O224:O228"/>
+    <mergeCell ref="O240:O241"/>
+    <mergeCell ref="O242:O243"/>
+    <mergeCell ref="Q257:R257"/>
+    <mergeCell ref="T257:U257"/>
+    <mergeCell ref="E269:G269"/>
+    <mergeCell ref="H269:J269"/>
+    <mergeCell ref="K269:M269"/>
     <mergeCell ref="V319:W319"/>
     <mergeCell ref="C324:C325"/>
     <mergeCell ref="Q329:U329"/>
@@ -48638,71 +48675,30 @@
     <mergeCell ref="C283:C285"/>
     <mergeCell ref="P302:T302"/>
     <mergeCell ref="P293:T293"/>
-    <mergeCell ref="O214:O218"/>
-    <mergeCell ref="O219:O223"/>
-    <mergeCell ref="O224:O228"/>
-    <mergeCell ref="O240:O241"/>
-    <mergeCell ref="O242:O243"/>
-    <mergeCell ref="Q257:R257"/>
-    <mergeCell ref="T257:U257"/>
-    <mergeCell ref="E269:G269"/>
-    <mergeCell ref="H269:J269"/>
-    <mergeCell ref="K269:M269"/>
-    <mergeCell ref="T181:U181"/>
-    <mergeCell ref="O190:O194"/>
-    <mergeCell ref="O195:O199"/>
-    <mergeCell ref="O200:O204"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="Q107:S107"/>
-    <mergeCell ref="T107:V107"/>
-    <mergeCell ref="H204:H205"/>
-    <mergeCell ref="I204:I205"/>
-    <mergeCell ref="M204:M205"/>
-    <mergeCell ref="W107:Y107"/>
-    <mergeCell ref="Q139:S139"/>
-    <mergeCell ref="T139:V139"/>
-    <mergeCell ref="W139:Y139"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="Q358:Q359"/>
+    <mergeCell ref="R358:R361"/>
+    <mergeCell ref="Q360:Q361"/>
+    <mergeCell ref="C366:C370"/>
+    <mergeCell ref="C303:C307"/>
+    <mergeCell ref="C308:C312"/>
+    <mergeCell ref="C313:C317"/>
+    <mergeCell ref="D413:H413"/>
+    <mergeCell ref="I413:M413"/>
+    <mergeCell ref="H399:I399"/>
+    <mergeCell ref="J399:K399"/>
+    <mergeCell ref="F442:F443"/>
+    <mergeCell ref="G442:G445"/>
+    <mergeCell ref="F444:F445"/>
+    <mergeCell ref="C337:C339"/>
+    <mergeCell ref="C340:C342"/>
+    <mergeCell ref="C343:C345"/>
+    <mergeCell ref="C346:C348"/>
+    <mergeCell ref="C349:C351"/>
+    <mergeCell ref="E204:E205"/>
+    <mergeCell ref="F204:F205"/>
+    <mergeCell ref="C371:C375"/>
+    <mergeCell ref="C376:C380"/>
+    <mergeCell ref="C388:C389"/>
   </mergeCells>
   <conditionalFormatting sqref="S126 V126 Y126 S158 V158 Y158">
     <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
@@ -49020,39 +49016,39 @@
         <f>Fluoro!D269</f>
         <v>Attenuator</v>
       </c>
-      <c r="E5" s="604" t="str">
+      <c r="E5" s="615" t="str">
         <f>Fluoro!E269</f>
         <v>Auto 1</v>
       </c>
-      <c r="F5" s="604">
+      <c r="F5" s="615">
         <f>Fluoro!F269</f>
         <v>0</v>
       </c>
-      <c r="G5" s="604">
+      <c r="G5" s="615">
         <f>Fluoro!G269</f>
         <v>0</v>
       </c>
-      <c r="H5" s="604" t="str">
+      <c r="H5" s="615" t="str">
         <f>Fluoro!H269</f>
         <v/>
       </c>
-      <c r="I5" s="604">
+      <c r="I5" s="615">
         <f>Fluoro!I269</f>
         <v>0</v>
       </c>
-      <c r="J5" s="604">
+      <c r="J5" s="615">
         <f>Fluoro!J269</f>
         <v>0</v>
       </c>
-      <c r="K5" s="605" t="str">
+      <c r="K5" s="616" t="str">
         <f>Fluoro!K269</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L5" s="605">
+      <c r="L5" s="616">
         <f>Fluoro!L269</f>
         <v>0</v>
       </c>
-      <c r="M5" s="605">
+      <c r="M5" s="616">
         <f>Fluoro!M269</f>
         <v>0</v>
       </c>
@@ -49109,7 +49105,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="637" t="str">
+      <c r="C7" s="640" t="str">
         <f>Fluoro!C271</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49159,7 +49155,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="637">
+      <c r="C8" s="640">
         <f>Fluoro!C272</f>
         <v>0</v>
       </c>
@@ -49209,7 +49205,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="637">
+      <c r="C9" s="640">
         <f>Fluoro!C273</f>
         <v>0</v>
       </c>
@@ -49259,7 +49255,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="637" t="str">
+      <c r="C10" s="640" t="str">
         <f>Fluoro!C274</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49309,7 +49305,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="637">
+      <c r="C11" s="640">
         <f>Fluoro!C275</f>
         <v>0</v>
       </c>
@@ -49359,7 +49355,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="637">
+      <c r="C12" s="640">
         <f>Fluoro!C276</f>
         <v>0</v>
       </c>
@@ -49409,7 +49405,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="637" t="str">
+      <c r="C13" s="640" t="str">
         <f>Fluoro!C277</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49459,7 +49455,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="637">
+      <c r="C14" s="640">
         <f>Fluoro!C278</f>
         <v>0</v>
       </c>
@@ -49509,7 +49505,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10"/>
-      <c r="C15" s="637">
+      <c r="C15" s="640">
         <f>Fluoro!C279</f>
         <v>0</v>
       </c>
@@ -49559,7 +49555,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10"/>
-      <c r="C16" s="637" t="str">
+      <c r="C16" s="640" t="str">
         <f>Fluoro!C280</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49609,7 +49605,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="637">
+      <c r="C17" s="640">
         <f>Fluoro!C281</f>
         <v>0</v>
       </c>
@@ -49659,7 +49655,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="637">
+      <c r="C18" s="640">
         <f>Fluoro!C282</f>
         <v>0</v>
       </c>
@@ -49709,7 +49705,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="637" t="str">
+      <c r="C19" s="640" t="str">
         <f>Fluoro!C283</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49759,7 +49755,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="637">
+      <c r="C20" s="640">
         <f>Fluoro!C284</f>
         <v>0</v>
       </c>
@@ -49809,7 +49805,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="637">
+      <c r="C21" s="640">
         <f>Fluoro!C285</f>
         <v>0</v>
       </c>
@@ -50233,39 +50229,39 @@
         <f>Fluoro!D335</f>
         <v>Attenuator</v>
       </c>
-      <c r="E37" s="604" t="str">
+      <c r="E37" s="615" t="str">
         <f>Fluoro!E335</f>
         <v>Auto 1</v>
       </c>
-      <c r="F37" s="604">
+      <c r="F37" s="615">
         <f>Fluoro!F335</f>
         <v>0</v>
       </c>
-      <c r="G37" s="604">
+      <c r="G37" s="615">
         <f>Fluoro!G335</f>
         <v>0</v>
       </c>
-      <c r="H37" s="604" t="str">
+      <c r="H37" s="615" t="str">
         <f>Fluoro!H335</f>
         <v/>
       </c>
-      <c r="I37" s="604">
+      <c r="I37" s="615">
         <f>Fluoro!I335</f>
         <v>0</v>
       </c>
-      <c r="J37" s="604">
+      <c r="J37" s="615">
         <f>Fluoro!J335</f>
         <v>0</v>
       </c>
-      <c r="K37" s="605" t="str">
+      <c r="K37" s="616" t="str">
         <f>Fluoro!K335</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L37" s="605">
+      <c r="L37" s="616">
         <f>Fluoro!L335</f>
         <v>0</v>
       </c>
-      <c r="M37" s="605">
+      <c r="M37" s="616">
         <f>Fluoro!M335</f>
         <v>0</v>
       </c>
@@ -50322,7 +50318,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="10"/>
-      <c r="C39" s="637" t="str">
+      <c r="C39" s="640" t="str">
         <f>Fluoro!C337</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50372,7 +50368,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="10"/>
-      <c r="C40" s="637">
+      <c r="C40" s="640">
         <f>Fluoro!C338</f>
         <v>0</v>
       </c>
@@ -50422,7 +50418,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="10"/>
-      <c r="C41" s="637">
+      <c r="C41" s="640">
         <f>Fluoro!C339</f>
         <v>0</v>
       </c>
@@ -50472,7 +50468,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="10"/>
-      <c r="C42" s="637" t="str">
+      <c r="C42" s="640" t="str">
         <f>Fluoro!C340</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50522,7 +50518,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="10"/>
-      <c r="C43" s="637">
+      <c r="C43" s="640">
         <f>Fluoro!C341</f>
         <v>0</v>
       </c>
@@ -50572,7 +50568,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="10"/>
-      <c r="C44" s="637">
+      <c r="C44" s="640">
         <f>Fluoro!C342</f>
         <v>0</v>
       </c>
@@ -50622,7 +50618,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="10"/>
-      <c r="C45" s="637" t="str">
+      <c r="C45" s="640" t="str">
         <f>Fluoro!C343</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50672,7 +50668,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="10"/>
-      <c r="C46" s="637">
+      <c r="C46" s="640">
         <f>Fluoro!C344</f>
         <v>0</v>
       </c>
@@ -50722,7 +50718,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="10"/>
-      <c r="C47" s="637">
+      <c r="C47" s="640">
         <f>Fluoro!C345</f>
         <v>0</v>
       </c>
@@ -50772,7 +50768,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="10"/>
-      <c r="C48" s="637" t="str">
+      <c r="C48" s="640" t="str">
         <f>Fluoro!C346</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50822,7 +50818,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="10"/>
-      <c r="C49" s="637">
+      <c r="C49" s="640">
         <f>Fluoro!C347</f>
         <v>0</v>
       </c>
@@ -50872,7 +50868,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="10"/>
-      <c r="C50" s="637">
+      <c r="C50" s="640">
         <f>Fluoro!C348</f>
         <v>0</v>
       </c>
@@ -50922,7 +50918,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="10"/>
-      <c r="C51" s="637" t="str">
+      <c r="C51" s="640" t="str">
         <f>Fluoro!C349</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50972,7 +50968,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="10"/>
-      <c r="C52" s="637">
+      <c r="C52" s="640">
         <f>Fluoro!C350</f>
         <v>0</v>
       </c>
@@ -51022,7 +51018,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="10"/>
-      <c r="C53" s="637">
+      <c r="C53" s="640">
         <f>Fluoro!C351</f>
         <v>0</v>
       </c>
@@ -51216,7 +51212,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="10"/>
-      <c r="C60" s="638"/>
+      <c r="C60" s="639"/>
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60"/>
@@ -51233,7 +51229,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="10"/>
-      <c r="C61" s="638"/>
+      <c r="C61" s="639"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>
@@ -51368,23 +51364,23 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="17">
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C21"/>
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="C42:C44"/>
     <mergeCell ref="C45:C47"/>
     <mergeCell ref="C48:C50"/>
     <mergeCell ref="C51:C53"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="68" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -51408,34 +51404,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="639" t="s">
+      <c r="A1" s="641" t="s">
         <v>405</v>
       </c>
-      <c r="B1" s="639"/>
+      <c r="B1" s="641"/>
       <c r="N1" s="278"/>
-      <c r="O1" s="613" t="str">
+      <c r="O1" s="620" t="str">
         <f>Fluoro!O105</f>
         <v>Patient Entrance Exposure Rate (Fluoroscopy)*</v>
       </c>
-      <c r="P1" s="613"/>
-      <c r="Q1" s="613"/>
-      <c r="R1" s="613" t="s">
+      <c r="P1" s="620"/>
+      <c r="Q1" s="620"/>
+      <c r="R1" s="620" t="s">
         <v>406</v>
       </c>
-      <c r="S1" s="613"/>
-      <c r="T1" s="613"/>
+      <c r="S1" s="620"/>
+      <c r="T1" s="620"/>
       <c r="V1" s="278"/>
-      <c r="W1" s="613" t="str">
+      <c r="W1" s="620" t="str">
         <f>Fluoro!O137</f>
         <v>Patient Entrance Exposure Rate – Digital Acquisition</v>
       </c>
-      <c r="X1" s="613"/>
-      <c r="Y1" s="613"/>
-      <c r="Z1" s="613" t="s">
+      <c r="X1" s="620"/>
+      <c r="Y1" s="620"/>
+      <c r="Z1" s="620" t="s">
         <v>406</v>
       </c>
-      <c r="AA1" s="613"/>
-      <c r="AB1" s="613"/>
+      <c r="AA1" s="620"/>
+      <c r="AB1" s="620"/>
     </row>
     <row r="2" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="279">
@@ -51638,10 +51634,10 @@
       <c r="AB6" s="278"/>
     </row>
     <row r="7" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="639" t="s">
+      <c r="A7" s="641" t="s">
         <v>409</v>
       </c>
-      <c r="B7" s="639"/>
+      <c r="B7" s="641"/>
       <c r="D7" s="203" t="s">
         <v>410</v>
       </c>
@@ -55428,14 +55424,14 @@
       <c r="B75" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="E75" s="613" t="s">
+      <c r="E75" s="620" t="s">
         <v>419</v>
       </c>
-      <c r="F75" s="613"/>
-      <c r="I75" s="613" t="s">
+      <c r="F75" s="620"/>
+      <c r="I75" s="620" t="s">
         <v>420</v>
       </c>
-      <c r="J75" s="613"/>
+      <c r="J75" s="620"/>
     </row>
     <row r="76" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
@@ -57188,7 +57184,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="14"/>
-      <c r="M1" s="640" t="s">
+      <c r="M1" s="582" t="s">
         <v>459</v>
       </c>
       <c r="N1" s="581"/>
@@ -57198,7 +57194,7 @@
       <c r="R1" s="581"/>
       <c r="S1" s="581"/>
       <c r="T1" s="581"/>
-      <c r="U1" s="640" t="s">
+      <c r="U1" s="582" t="s">
         <v>459</v>
       </c>
       <c r="V1" s="581"/>
@@ -57276,60 +57272,60 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="14"/>
-      <c r="M3" s="641" t="s">
+      <c r="M3" s="583" t="s">
         <v>460</v>
       </c>
-      <c r="N3" s="641" t="s">
+      <c r="N3" s="583" t="s">
         <v>461</v>
       </c>
-      <c r="O3" s="641" t="s">
+      <c r="O3" s="583" t="s">
         <v>462</v>
       </c>
-      <c r="P3" s="641" t="s">
+      <c r="P3" s="583" t="s">
         <v>463</v>
       </c>
-      <c r="Q3" s="641" t="s">
+      <c r="Q3" s="583" t="s">
         <v>464</v>
       </c>
-      <c r="R3" s="641" t="s">
+      <c r="R3" s="583" t="s">
         <v>465</v>
       </c>
       <c r="S3" s="581"/>
       <c r="T3" s="581"/>
-      <c r="U3" s="641" t="s">
+      <c r="U3" s="583" t="s">
         <v>460</v>
       </c>
-      <c r="V3" s="641" t="s">
+      <c r="V3" s="583" t="s">
         <v>461</v>
       </c>
-      <c r="W3" s="641" t="s">
+      <c r="W3" s="583" t="s">
         <v>462</v>
       </c>
-      <c r="X3" s="641" t="s">
+      <c r="X3" s="583" t="s">
         <v>463</v>
       </c>
-      <c r="Y3" s="641" t="s">
+      <c r="Y3" s="583" t="s">
         <v>464</v>
       </c>
-      <c r="Z3" s="641" t="s">
+      <c r="Z3" s="583" t="s">
         <v>465</v>
       </c>
-      <c r="AA3" s="641" t="s">
+      <c r="AA3" s="583" t="s">
         <v>466</v>
       </c>
-      <c r="AB3" s="641" t="s">
+      <c r="AB3" s="583" t="s">
         <v>467</v>
       </c>
-      <c r="AC3" s="641" t="s">
+      <c r="AC3" s="583" t="s">
         <v>468</v>
       </c>
-      <c r="AD3" s="641" t="s">
+      <c r="AD3" s="583" t="s">
         <v>469</v>
       </c>
-      <c r="AE3" s="641" t="s">
+      <c r="AE3" s="583" t="s">
         <v>470</v>
       </c>
-      <c r="AF3" s="641" t="s">
+      <c r="AF3" s="583" t="s">
         <v>471</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix cell references for graph legends
</commit_message>
<xml_diff>
--- a/MUSCCArm.xlsx
+++ b/MUSCCArm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE8926C-5E8C-416F-9393-AE9205F9EF3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9FA454-96D4-416F-9E7D-7A20A2FEE42B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6483,6 +6483,138 @@
     <xf numFmtId="2" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="200" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="222" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="223" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="127" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="155" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="182" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="149" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="150" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="175" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="151" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="176" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="154" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="180" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6501,30 +6633,12 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="200" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="201" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="149" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="150" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="151" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="183" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6534,124 +6648,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="193" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="127" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="155" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="182" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="175" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="176" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="154" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="180" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="222" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="223" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -20766,21 +20766,21 @@
       <c r="E10" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="635" t="str">
+      <c r="F10" s="584" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="635"/>
+      <c r="G10" s="584"/>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
       <c r="J10" s="160" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="624" t="str">
+      <c r="K10" s="585" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="624"/>
+      <c r="L10" s="585"/>
       <c r="M10" s="312"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="2" t="s">
@@ -20823,21 +20823,21 @@
       <c r="E11" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="625" t="str">
+      <c r="F11" s="586" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="625"/>
+      <c r="G11" s="586"/>
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
       <c r="J11" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="625" t="str">
+      <c r="K11" s="586" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="625"/>
+      <c r="L11" s="586"/>
       <c r="M11" s="312"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="2" t="s">
@@ -20880,21 +20880,21 @@
       <c r="E12" s="160" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="625" t="str">
+      <c r="F12" s="586" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="625"/>
+      <c r="G12" s="586"/>
       <c r="H12" s="42"/>
       <c r="I12" s="42"/>
       <c r="J12" s="160" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="637" t="str">
+      <c r="K12" s="587" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="637"/>
+      <c r="L12" s="587"/>
       <c r="M12" s="312"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="2" t="s">
@@ -20937,21 +20937,21 @@
       <c r="E13" s="160" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="626" t="str">
+      <c r="F13" s="588" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="626"/>
+      <c r="G13" s="588"/>
       <c r="H13" s="42"/>
       <c r="I13" s="42"/>
       <c r="J13" s="160" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="626" t="str">
+      <c r="K13" s="588" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="626"/>
+      <c r="L13" s="588"/>
       <c r="M13" s="312"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="2" t="s">
@@ -21074,21 +21074,21 @@
       <c r="E16" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="635" t="str">
+      <c r="F16" s="584" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="635"/>
+      <c r="G16" s="584"/>
       <c r="H16" s="42"/>
       <c r="I16" s="42"/>
       <c r="J16" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="638" t="str">
+      <c r="K16" s="589" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="638"/>
+      <c r="L16" s="589"/>
       <c r="M16" s="312"/>
       <c r="O16" s="13"/>
       <c r="P16" s="50" t="s">
@@ -21118,21 +21118,21 @@
       <c r="E17" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="625" t="str">
+      <c r="F17" s="586" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="625"/>
+      <c r="G17" s="586"/>
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
       <c r="J17" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="626" t="str">
+      <c r="K17" s="588" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="626"/>
+      <c r="L17" s="588"/>
       <c r="M17" s="312"/>
       <c r="O17" s="13"/>
       <c r="Q17" s="2" t="s">
@@ -21175,21 +21175,21 @@
       <c r="E18" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="626" t="str">
+      <c r="F18" s="588" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="626"/>
+      <c r="G18" s="588"/>
       <c r="H18" s="42"/>
       <c r="I18" s="42"/>
       <c r="J18" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="626" t="str">
+      <c r="K18" s="588" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="626"/>
+      <c r="L18" s="588"/>
       <c r="M18" s="312"/>
       <c r="O18" s="13"/>
       <c r="Q18" s="2" t="s">
@@ -21237,11 +21237,11 @@
       <c r="J19" s="160" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="626" t="str">
+      <c r="K19" s="588" t="str">
         <f>IF(V20="","",V20)</f>
         <v/>
       </c>
-      <c r="L19" s="626"/>
+      <c r="L19" s="588"/>
       <c r="M19" s="312"/>
       <c r="O19" s="13"/>
       <c r="Q19" s="2" t="s">
@@ -21316,11 +21316,11 @@
       <c r="E21" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="635" t="str">
+      <c r="F21" s="584" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="635"/>
+      <c r="G21" s="584"/>
       <c r="H21" s="42"/>
       <c r="I21" s="42"/>
       <c r="J21" s="73" t="s">
@@ -21360,21 +21360,21 @@
       <c r="E22" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="636" t="str">
+      <c r="F22" s="590" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="636"/>
+      <c r="G22" s="590"/>
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
       <c r="J22" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="635" t="str">
+      <c r="K22" s="584" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="635"/>
+      <c r="L22" s="584"/>
       <c r="M22" s="312"/>
       <c r="O22" s="13"/>
       <c r="Q22" s="2" t="s">
@@ -21419,11 +21419,11 @@
       <c r="J23" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="625" t="str">
+      <c r="K23" s="586" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="625"/>
+      <c r="L23" s="586"/>
       <c r="M23" s="312"/>
       <c r="O23" s="13"/>
       <c r="Q23" s="2" t="s">
@@ -21466,21 +21466,21 @@
       <c r="E24" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="624" t="str">
+      <c r="F24" s="585" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="624"/>
+      <c r="G24" s="585"/>
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
       <c r="J24" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="625" t="str">
+      <c r="K24" s="586" t="str">
         <f>IF(V25="","",V25)</f>
         <v/>
       </c>
-      <c r="L24" s="625"/>
+      <c r="L24" s="586"/>
       <c r="M24" s="312"/>
       <c r="O24" s="13"/>
       <c r="P24" s="50" t="s">
@@ -21518,11 +21518,11 @@
       <c r="E25" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="626" t="str">
+      <c r="F25" s="588" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="626"/>
+      <c r="G25" s="588"/>
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
@@ -21570,11 +21570,11 @@
       <c r="E26" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="626" t="str">
+      <c r="F26" s="588" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="626"/>
+      <c r="G26" s="588"/>
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
       <c r="J26" s="313" t="s">
@@ -21623,11 +21623,11 @@
       <c r="J27" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="635" t="str">
+      <c r="K27" s="584" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="635"/>
+      <c r="L27" s="584"/>
       <c r="M27" s="312"/>
       <c r="O27" s="13"/>
       <c r="Q27" s="2" t="s">
@@ -21665,21 +21665,21 @@
       <c r="E28" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="624" t="str">
+      <c r="F28" s="585" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="624"/>
+      <c r="G28" s="585"/>
       <c r="H28" s="42"/>
       <c r="I28" s="42"/>
       <c r="J28" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="625" t="str">
+      <c r="K28" s="586" t="str">
         <f>IF(V29="","",V29)</f>
         <v/>
       </c>
-      <c r="L28" s="625"/>
+      <c r="L28" s="586"/>
       <c r="M28" s="312"/>
       <c r="O28" s="13"/>
       <c r="P28" s="50" t="s">
@@ -21708,11 +21708,11 @@
       <c r="E29" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="626" t="str">
+      <c r="F29" s="588" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="626"/>
+      <c r="G29" s="588"/>
       <c r="H29" s="42"/>
       <c r="I29" s="42"/>
       <c r="J29" s="42"/>
@@ -21760,11 +21760,11 @@
       <c r="E30" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="626" t="str">
+      <c r="F30" s="588" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="626"/>
+      <c r="G30" s="588"/>
       <c r="H30" s="42"/>
       <c r="I30" s="42"/>
       <c r="J30" s="42"/>
@@ -21879,11 +21879,11 @@
       <c r="E33" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="635" t="str">
+      <c r="F33" s="584" t="str">
         <f>IF(R34="","",R34)</f>
         <v/>
       </c>
-      <c r="G33" s="635"/>
+      <c r="G33" s="584"/>
       <c r="H33" s="42"/>
       <c r="I33" s="42"/>
       <c r="J33" s="73" t="s">
@@ -21920,21 +21920,21 @@
       <c r="E34" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="636" t="str">
+      <c r="F34" s="590" t="str">
         <f>IF(R35="","",R35)</f>
         <v/>
       </c>
-      <c r="G34" s="636"/>
+      <c r="G34" s="590"/>
       <c r="H34" s="42"/>
       <c r="I34" s="42"/>
       <c r="J34" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="635" t="str">
+      <c r="K34" s="584" t="str">
         <f>IF(V35="","",V35)</f>
         <v/>
       </c>
-      <c r="L34" s="635"/>
+      <c r="L34" s="584"/>
       <c r="M34" s="312"/>
       <c r="O34" s="13"/>
       <c r="Q34" s="2" t="s">
@@ -21979,11 +21979,11 @@
       <c r="J35" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="K35" s="625" t="str">
+      <c r="K35" s="586" t="str">
         <f>IF(V36="","",V36)</f>
         <v/>
       </c>
-      <c r="L35" s="625"/>
+      <c r="L35" s="586"/>
       <c r="M35" s="312"/>
       <c r="O35" s="13"/>
       <c r="Q35" s="2" t="s">
@@ -22026,21 +22026,21 @@
       <c r="E36" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="624" t="str">
+      <c r="F36" s="585" t="str">
         <f>IF(R37="","",R37)</f>
         <v/>
       </c>
-      <c r="G36" s="624"/>
+      <c r="G36" s="585"/>
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
       <c r="J36" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="K36" s="625" t="str">
+      <c r="K36" s="586" t="str">
         <f>IF(V37="","",V37)</f>
         <v/>
       </c>
-      <c r="L36" s="625"/>
+      <c r="L36" s="586"/>
       <c r="M36" s="312"/>
       <c r="O36" s="13"/>
       <c r="P36" s="50" t="s">
@@ -22078,11 +22078,11 @@
       <c r="E37" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="626" t="str">
+      <c r="F37" s="588" t="str">
         <f>IF(R38="","",R38)</f>
         <v/>
       </c>
-      <c r="G37" s="626"/>
+      <c r="G37" s="588"/>
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
       <c r="J37" s="42"/>
@@ -22130,11 +22130,11 @@
       <c r="E38" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="626" t="str">
+      <c r="F38" s="588" t="str">
         <f>IF(R39="","",R39)</f>
         <v/>
       </c>
-      <c r="G38" s="626"/>
+      <c r="G38" s="588"/>
       <c r="H38" s="42"/>
       <c r="I38" s="42"/>
       <c r="J38" s="313" t="s">
@@ -22181,11 +22181,11 @@
       <c r="J39" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="K39" s="635" t="str">
+      <c r="K39" s="584" t="str">
         <f>IF(V40="","",V40)</f>
         <v/>
       </c>
-      <c r="L39" s="635"/>
+      <c r="L39" s="584"/>
       <c r="M39" s="312"/>
       <c r="O39" s="13"/>
       <c r="Q39" s="2" t="s">
@@ -22223,21 +22223,21 @@
       <c r="E40" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="624" t="str">
+      <c r="F40" s="585" t="str">
         <f>IF(R41="","",R41)</f>
         <v/>
       </c>
-      <c r="G40" s="624"/>
+      <c r="G40" s="585"/>
       <c r="H40" s="42"/>
       <c r="I40" s="42"/>
       <c r="J40" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K40" s="625" t="str">
+      <c r="K40" s="586" t="str">
         <f>IF(V41="","",V41)</f>
         <v/>
       </c>
-      <c r="L40" s="625"/>
+      <c r="L40" s="586"/>
       <c r="M40" s="312"/>
       <c r="O40" s="13"/>
       <c r="P40" s="50" t="s">
@@ -22275,11 +22275,11 @@
       <c r="E41" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="626" t="str">
+      <c r="F41" s="588" t="str">
         <f>IF(R42="","",R42)</f>
         <v/>
       </c>
-      <c r="G41" s="626"/>
+      <c r="G41" s="588"/>
       <c r="H41" s="42"/>
       <c r="I41" s="42"/>
       <c r="J41" s="42"/>
@@ -22327,11 +22327,11 @@
       <c r="E42" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="626" t="str">
+      <c r="F42" s="588" t="str">
         <f>IF(R43="","",R43)</f>
         <v/>
       </c>
-      <c r="G42" s="626"/>
+      <c r="G42" s="588"/>
       <c r="H42" s="42"/>
       <c r="I42" s="42"/>
       <c r="J42" s="42"/>
@@ -23098,10 +23098,10 @@
       <c r="I69" s="299"/>
       <c r="J69" s="299"/>
       <c r="K69" s="299"/>
-      <c r="L69" s="627" t="s">
+      <c r="L69" s="595" t="s">
         <v>83</v>
       </c>
-      <c r="M69" s="628"/>
+      <c r="M69" s="596"/>
       <c r="O69" s="56"/>
       <c r="P69" s="17" t="s">
         <v>84</v>
@@ -24770,24 +24770,24 @@
       <c r="P107" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="Q107" s="629" t="str">
+      <c r="Q107" s="592" t="str">
         <f>IF(Q106&lt;&gt;"",Q106,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R107" s="629"/>
-      <c r="S107" s="629"/>
-      <c r="T107" s="630" t="str">
+      <c r="R107" s="592"/>
+      <c r="S107" s="592"/>
+      <c r="T107" s="591" t="str">
         <f>IF(T106&lt;&gt;"",T106,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v/>
       </c>
-      <c r="U107" s="630"/>
-      <c r="V107" s="630"/>
-      <c r="W107" s="630" t="str">
+      <c r="U107" s="591"/>
+      <c r="V107" s="591"/>
+      <c r="W107" s="591" t="str">
         <f>IF(W106&lt;&gt;"",W106,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="X107" s="630"/>
-      <c r="Y107" s="630"/>
+      <c r="X107" s="591"/>
+      <c r="Y107" s="591"/>
       <c r="AA107" s="2" t="s">
         <v>152</v>
       </c>
@@ -26779,24 +26779,24 @@
       <c r="P139" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="Q139" s="629" t="str">
+      <c r="Q139" s="592" t="str">
         <f>IF(Q138&lt;&gt;"",Q138,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R139" s="629"/>
-      <c r="S139" s="629"/>
-      <c r="T139" s="630" t="str">
+      <c r="R139" s="592"/>
+      <c r="S139" s="592"/>
+      <c r="T139" s="591" t="str">
         <f>IF(T138&lt;&gt;"",T138,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v/>
       </c>
-      <c r="U139" s="630"/>
-      <c r="V139" s="630"/>
-      <c r="W139" s="630" t="str">
+      <c r="U139" s="591"/>
+      <c r="V139" s="591"/>
+      <c r="W139" s="591" t="str">
         <f>IF(W138&lt;&gt;"",W138,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="X139" s="630"/>
-      <c r="Y139" s="630"/>
+      <c r="X139" s="591"/>
+      <c r="Y139" s="591"/>
       <c r="AA139" s="2" t="str">
         <f>$T$139&amp;" Mag 4"</f>
         <v xml:space="preserve"> Mag 4</v>
@@ -29140,10 +29140,10 @@
       <c r="P181" s="135"/>
       <c r="Q181" s="137"/>
       <c r="R181" s="128"/>
-      <c r="T181" s="612" t="s">
+      <c r="T181" s="593" t="s">
         <v>244</v>
       </c>
-      <c r="U181" s="612"/>
+      <c r="U181" s="593"/>
       <c r="W181" s="2" t="s">
         <v>198</v>
       </c>
@@ -29514,7 +29514,7 @@
       <c r="K190" s="323"/>
       <c r="L190" s="323"/>
       <c r="M190" s="327"/>
-      <c r="O190" s="621" t="str">
+      <c r="O190" s="594" t="str">
         <f>$Q$107</f>
         <v>Auto 1</v>
       </c>
@@ -29564,7 +29564,7 @@
       <c r="K191" s="323"/>
       <c r="L191" s="323"/>
       <c r="M191" s="303"/>
-      <c r="O191" s="621"/>
+      <c r="O191" s="594"/>
       <c r="P191" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -29610,7 +29610,7 @@
       <c r="K192" s="135"/>
       <c r="L192" s="135"/>
       <c r="M192" s="303"/>
-      <c r="O192" s="621"/>
+      <c r="O192" s="594"/>
       <c r="P192" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -29656,7 +29656,7 @@
       <c r="K193" s="135"/>
       <c r="L193" s="135"/>
       <c r="M193" s="303"/>
-      <c r="O193" s="621"/>
+      <c r="O193" s="594"/>
       <c r="P193" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -29699,7 +29699,7 @@
       <c r="K194" s="135"/>
       <c r="L194" s="135"/>
       <c r="M194" s="303"/>
-      <c r="O194" s="621"/>
+      <c r="O194" s="594"/>
       <c r="P194" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -29742,7 +29742,7 @@
       <c r="K195" s="135"/>
       <c r="L195" s="135"/>
       <c r="M195" s="303"/>
-      <c r="O195" s="621" t="str">
+      <c r="O195" s="594" t="str">
         <f>$T$107</f>
         <v/>
       </c>
@@ -29788,7 +29788,7 @@
       <c r="K196" s="305"/>
       <c r="L196" s="305"/>
       <c r="M196" s="306"/>
-      <c r="O196" s="621"/>
+      <c r="O196" s="594"/>
       <c r="P196" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -29833,7 +29833,7 @@
         <f>IF($X$7="","",$X$7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="O197" s="621"/>
+      <c r="O197" s="594"/>
       <c r="P197" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -29878,7 +29878,7 @@
         <f>IF($R$13="","",$R$13)</f>
         <v/>
       </c>
-      <c r="O198" s="621"/>
+      <c r="O198" s="594"/>
       <c r="P198" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -29924,7 +29924,7 @@
         <f>$H$2</f>
         <v>Medical University of South Carolina</v>
       </c>
-      <c r="O199" s="621"/>
+      <c r="O199" s="594"/>
       <c r="P199" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -29973,7 +29973,7 @@
         <f>$H$5</f>
         <v>Fluoroscopy System Compliance Inspection</v>
       </c>
-      <c r="O200" s="621" t="str">
+      <c r="O200" s="594" t="str">
         <f>$W$107</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -30022,7 +30022,7 @@
       <c r="K201" s="299"/>
       <c r="L201" s="299"/>
       <c r="M201" s="300"/>
-      <c r="O201" s="621"/>
+      <c r="O201" s="594"/>
       <c r="P201" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30076,7 +30076,7 @@
         <v>44905</v>
       </c>
       <c r="M202" s="12"/>
-      <c r="O202" s="621"/>
+      <c r="O202" s="594"/>
       <c r="P202" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -30109,7 +30109,7 @@
       </c>
       <c r="B203" s="10"/>
       <c r="M203" s="12"/>
-      <c r="O203" s="621"/>
+      <c r="O203" s="594"/>
       <c r="P203" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -30143,20 +30143,20 @@
       <c r="B204" s="301"/>
       <c r="C204" s="351"/>
       <c r="D204" s="323"/>
-      <c r="E204" s="591" t="s">
+      <c r="E204" s="597" t="s">
         <v>261</v>
       </c>
-      <c r="F204" s="593" t="s">
+      <c r="F204" s="634" t="s">
         <v>262</v>
       </c>
       <c r="G204" s="518" t="s">
         <v>263</v>
       </c>
-      <c r="H204" s="591" t="str">
+      <c r="H204" s="597" t="str">
         <f>R276</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="I204" s="631" t="str">
+      <c r="I204" s="599" t="str">
         <f>S276</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -30169,10 +30169,10 @@
       <c r="L204" s="135" t="s">
         <v>266</v>
       </c>
-      <c r="M204" s="633" t="s">
+      <c r="M204" s="601" t="s">
         <v>267</v>
       </c>
-      <c r="O204" s="621"/>
+      <c r="O204" s="594"/>
       <c r="P204" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -30210,11 +30210,11 @@
       <c r="D205" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="E205" s="592"/>
-      <c r="F205" s="594"/>
+      <c r="E205" s="598"/>
+      <c r="F205" s="635"/>
       <c r="G205" s="518"/>
-      <c r="H205" s="592"/>
-      <c r="I205" s="632"/>
+      <c r="H205" s="598"/>
+      <c r="I205" s="600"/>
       <c r="J205" s="519"/>
       <c r="K205" s="135" t="str">
         <f>U277</f>
@@ -30224,7 +30224,7 @@
         <f>V277</f>
         <v>mGy/min</v>
       </c>
-      <c r="M205" s="634"/>
+      <c r="M205" s="602"/>
       <c r="O205" s="13"/>
       <c r="Y205" s="14"/>
       <c r="AA205" s="2" t="s">
@@ -30868,7 +30868,7 @@
         <f>W286</f>
         <v/>
       </c>
-      <c r="O214" s="621" t="str">
+      <c r="O214" s="594" t="str">
         <f>$Q$139</f>
         <v>Auto 1</v>
       </c>
@@ -30924,7 +30924,7 @@
       <c r="K215" s="135"/>
       <c r="L215" s="135"/>
       <c r="M215" s="303"/>
-      <c r="O215" s="621"/>
+      <c r="O215" s="594"/>
       <c r="P215" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30970,7 +30970,7 @@
       <c r="K216" s="323"/>
       <c r="L216" s="323"/>
       <c r="M216" s="303"/>
-      <c r="O216" s="621"/>
+      <c r="O216" s="594"/>
       <c r="P216" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -31016,7 +31016,7 @@
       <c r="K217" s="368"/>
       <c r="L217" s="368"/>
       <c r="M217" s="369"/>
-      <c r="O217" s="621"/>
+      <c r="O217" s="594"/>
       <c r="P217" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31063,7 +31063,7 @@
       <c r="K218" s="323"/>
       <c r="L218" s="323"/>
       <c r="M218" s="303"/>
-      <c r="O218" s="621"/>
+      <c r="O218" s="594"/>
       <c r="P218" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -31106,7 +31106,7 @@
       <c r="K219" s="323"/>
       <c r="L219" s="323"/>
       <c r="M219" s="327"/>
-      <c r="O219" s="621" t="str">
+      <c r="O219" s="594" t="str">
         <f>$T$139</f>
         <v/>
       </c>
@@ -31167,7 +31167,7 @@
         <v/>
       </c>
       <c r="M220" s="327"/>
-      <c r="O220" s="621"/>
+      <c r="O220" s="594"/>
       <c r="P220" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -31210,7 +31210,7 @@
       <c r="K221" s="323"/>
       <c r="L221" s="323"/>
       <c r="M221" s="327"/>
-      <c r="O221" s="621"/>
+      <c r="O221" s="594"/>
       <c r="P221" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -31261,7 +31261,7 @@
       <c r="K222" s="323"/>
       <c r="L222" s="323"/>
       <c r="M222" s="327"/>
-      <c r="O222" s="621"/>
+      <c r="O222" s="594"/>
       <c r="P222" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31318,7 +31318,7 @@
       <c r="K223" s="323"/>
       <c r="L223" s="323"/>
       <c r="M223" s="327"/>
-      <c r="O223" s="621"/>
+      <c r="O223" s="594"/>
       <c r="P223" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -31382,7 +31382,7 @@
       <c r="K224" s="323"/>
       <c r="L224" s="323"/>
       <c r="M224" s="327"/>
-      <c r="O224" s="621" t="str">
+      <c r="O224" s="594" t="str">
         <f>$W$139</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -31446,7 +31446,7 @@
       <c r="K225" s="323"/>
       <c r="L225" s="323"/>
       <c r="M225" s="327"/>
-      <c r="O225" s="621"/>
+      <c r="O225" s="594"/>
       <c r="P225" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -31507,7 +31507,7 @@
       <c r="K226" s="323"/>
       <c r="L226" s="323"/>
       <c r="M226" s="327"/>
-      <c r="O226" s="621"/>
+      <c r="O226" s="594"/>
       <c r="P226" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -31568,7 +31568,7 @@
       <c r="K227" s="323"/>
       <c r="L227" s="323"/>
       <c r="M227" s="327"/>
-      <c r="O227" s="621"/>
+      <c r="O227" s="594"/>
       <c r="P227" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31622,7 +31622,7 @@
       <c r="K228" s="323"/>
       <c r="L228" s="323"/>
       <c r="M228" s="327"/>
-      <c r="O228" s="621"/>
+      <c r="O228" s="594"/>
       <c r="P228" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -32175,7 +32175,7 @@
       <c r="K240" s="323"/>
       <c r="L240" s="323"/>
       <c r="M240" s="327"/>
-      <c r="O240" s="622" t="s">
+      <c r="O240" s="603" t="s">
         <v>293</v>
       </c>
       <c r="P240" s="167" t="s">
@@ -32234,7 +32234,7 @@
       <c r="K241" s="323"/>
       <c r="L241" s="323"/>
       <c r="M241" s="327"/>
-      <c r="O241" s="622"/>
+      <c r="O241" s="603"/>
       <c r="P241" s="172" t="s">
         <v>296</v>
       </c>
@@ -32291,7 +32291,7 @@
       <c r="K242" s="323"/>
       <c r="L242" s="323"/>
       <c r="M242" s="327"/>
-      <c r="O242" s="622" t="str">
+      <c r="O242" s="603" t="str">
         <f>IF($U$137=1,"Scatter - Pulse", "Scatter – Digital acq")</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -32351,7 +32351,7 @@
       <c r="K243" s="323"/>
       <c r="L243" s="323"/>
       <c r="M243" s="327"/>
-      <c r="O243" s="622"/>
+      <c r="O243" s="603"/>
       <c r="P243" s="172" t="s">
         <v>296</v>
       </c>
@@ -32881,17 +32881,17 @@
       <c r="P257" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="Q257" s="623" t="s">
+      <c r="Q257" s="604" t="s">
         <v>312</v>
       </c>
-      <c r="R257" s="623"/>
+      <c r="R257" s="604"/>
       <c r="S257" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="T257" s="623" t="s">
+      <c r="T257" s="604" t="s">
         <v>314</v>
       </c>
-      <c r="U257" s="623"/>
+      <c r="U257" s="604"/>
       <c r="V257" s="1" t="s">
         <v>315</v>
       </c>
@@ -33388,24 +33388,24 @@
         <f t="shared" si="43"/>
         <v>Attenuator</v>
       </c>
-      <c r="E269" s="614" t="str">
+      <c r="E269" s="605" t="str">
         <f>Q107</f>
         <v>Auto 1</v>
       </c>
-      <c r="F269" s="615"/>
-      <c r="G269" s="615"/>
-      <c r="H269" s="615" t="str">
+      <c r="F269" s="606"/>
+      <c r="G269" s="606"/>
+      <c r="H269" s="606" t="str">
         <f>T107</f>
         <v/>
       </c>
-      <c r="I269" s="615"/>
-      <c r="J269" s="615"/>
-      <c r="K269" s="616" t="str">
+      <c r="I269" s="606"/>
+      <c r="J269" s="606"/>
+      <c r="K269" s="607" t="str">
         <f>W107</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L269" s="616"/>
-      <c r="M269" s="617"/>
+      <c r="L269" s="607"/>
+      <c r="M269" s="608"/>
       <c r="O269" s="189" t="str">
         <f t="shared" si="44"/>
         <v/>
@@ -33507,7 +33507,7 @@
         <v>7</v>
       </c>
       <c r="B271" s="301"/>
-      <c r="C271" s="590" t="str">
+      <c r="C271" s="612" t="str">
         <f>O110&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33583,7 +33583,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="301"/>
-      <c r="C272" s="590"/>
+      <c r="C272" s="612"/>
       <c r="D272" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -33649,7 +33649,7 @@
         <v>9</v>
       </c>
       <c r="B273" s="301"/>
-      <c r="C273" s="590"/>
+      <c r="C273" s="612"/>
       <c r="D273" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -33722,7 +33722,7 @@
         <v>10</v>
       </c>
       <c r="B274" s="301"/>
-      <c r="C274" s="590" t="str">
+      <c r="C274" s="612" t="str">
         <f>O113&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33791,7 +33791,7 @@
         <v>11</v>
       </c>
       <c r="B275" s="301"/>
-      <c r="C275" s="590"/>
+      <c r="C275" s="612"/>
       <c r="D275" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -33864,7 +33864,7 @@
         <v>12</v>
       </c>
       <c r="B276" s="301"/>
-      <c r="C276" s="590"/>
+      <c r="C276" s="612"/>
       <c r="D276" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -33905,17 +33905,17 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="O276" s="618" t="s">
+      <c r="O276" s="613" t="s">
         <v>261</v>
       </c>
-      <c r="P276" s="619" t="s">
+      <c r="P276" s="614" t="s">
         <v>262</v>
       </c>
-      <c r="R276" s="619" t="str">
+      <c r="R276" s="614" t="str">
         <f>"Ind AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="S276" s="619" t="str">
+      <c r="S276" s="614" t="str">
         <f>"Meas AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -33937,7 +33937,7 @@
         <v>13</v>
       </c>
       <c r="B277" s="301"/>
-      <c r="C277" s="590" t="str">
+      <c r="C277" s="612" t="str">
         <f>O116&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33981,13 +33981,13 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
-      <c r="O277" s="618"/>
-      <c r="P277" s="619"/>
+      <c r="O277" s="613"/>
+      <c r="P277" s="614"/>
       <c r="Q277" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="R277" s="619"/>
-      <c r="S277" s="619"/>
+      <c r="R277" s="614"/>
+      <c r="S277" s="614"/>
       <c r="T277" s="1" t="s">
         <v>321</v>
       </c>
@@ -34019,7 +34019,7 @@
         <v>14</v>
       </c>
       <c r="B278" s="301"/>
-      <c r="C278" s="590"/>
+      <c r="C278" s="612"/>
       <c r="D278" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -34106,7 +34106,7 @@
         <v>15</v>
       </c>
       <c r="B279" s="301"/>
-      <c r="C279" s="590"/>
+      <c r="C279" s="612"/>
       <c r="D279" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -34200,7 +34200,7 @@
         <v>16</v>
       </c>
       <c r="B280" s="301"/>
-      <c r="C280" s="590" t="str">
+      <c r="C280" s="612" t="str">
         <f>O119&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -34300,7 +34300,7 @@
         <v>17</v>
       </c>
       <c r="B281" s="301"/>
-      <c r="C281" s="590"/>
+      <c r="C281" s="612"/>
       <c r="D281" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -34387,7 +34387,7 @@
         <v>18</v>
       </c>
       <c r="B282" s="301"/>
-      <c r="C282" s="590"/>
+      <c r="C282" s="612"/>
       <c r="D282" s="394">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -34481,7 +34481,7 @@
         <v>19</v>
       </c>
       <c r="B283" s="301"/>
-      <c r="C283" s="590" t="str">
+      <c r="C283" s="612" t="str">
         <f>O122&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -34571,7 +34571,7 @@
         <v>20</v>
       </c>
       <c r="B284" s="301"/>
-      <c r="C284" s="590"/>
+      <c r="C284" s="612"/>
       <c r="D284" s="391">
         <f t="shared" si="45"/>
         <v>20</v>
@@ -34665,7 +34665,7 @@
         <v>21</v>
       </c>
       <c r="B285" s="301"/>
-      <c r="C285" s="590"/>
+      <c r="C285" s="612"/>
       <c r="D285" s="391">
         <f t="shared" si="45"/>
         <v>30</v>
@@ -35100,13 +35100,13 @@
       <c r="L293" s="135"/>
       <c r="M293" s="303"/>
       <c r="O293" s="225"/>
-      <c r="P293" s="620" t="s">
+      <c r="P293" s="615" t="s">
         <v>327</v>
       </c>
-      <c r="Q293" s="620"/>
-      <c r="R293" s="620"/>
-      <c r="S293" s="620"/>
-      <c r="T293" s="620"/>
+      <c r="Q293" s="615"/>
+      <c r="R293" s="615"/>
+      <c r="S293" s="615"/>
+      <c r="T293" s="615"/>
       <c r="U293" s="223"/>
       <c r="V293" s="223"/>
       <c r="W293" s="223"/>
@@ -35547,13 +35547,13 @@
       <c r="L302" s="135"/>
       <c r="M302" s="303"/>
       <c r="O302" s="225"/>
-      <c r="P302" s="620" t="s">
+      <c r="P302" s="615" t="s">
         <v>327</v>
       </c>
-      <c r="Q302" s="620"/>
-      <c r="R302" s="620"/>
-      <c r="S302" s="620"/>
-      <c r="T302" s="620"/>
+      <c r="Q302" s="615"/>
+      <c r="R302" s="615"/>
+      <c r="S302" s="615"/>
+      <c r="T302" s="615"/>
       <c r="U302" s="223"/>
       <c r="V302" s="223"/>
       <c r="W302" s="223"/>
@@ -35574,7 +35574,7 @@
         <v>39</v>
       </c>
       <c r="B303" s="301"/>
-      <c r="C303" s="595" t="str">
+      <c r="C303" s="620" t="str">
         <f>O190</f>
         <v>Auto 1</v>
       </c>
@@ -35637,7 +35637,7 @@
         <v>40</v>
       </c>
       <c r="B304" s="301"/>
-      <c r="C304" s="596"/>
+      <c r="C304" s="621"/>
       <c r="D304" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35710,7 +35710,7 @@
         <v>41</v>
       </c>
       <c r="B305" s="301"/>
-      <c r="C305" s="596"/>
+      <c r="C305" s="621"/>
       <c r="D305" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35773,7 +35773,7 @@
         <v>42</v>
       </c>
       <c r="B306" s="301"/>
-      <c r="C306" s="596"/>
+      <c r="C306" s="621"/>
       <c r="D306" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35840,7 +35840,7 @@
         <v>43</v>
       </c>
       <c r="B307" s="301"/>
-      <c r="C307" s="607"/>
+      <c r="C307" s="622"/>
       <c r="D307" s="436" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -35900,7 +35900,7 @@
         <v>44</v>
       </c>
       <c r="B308" s="301"/>
-      <c r="C308" s="595" t="str">
+      <c r="C308" s="620" t="str">
         <f>O195</f>
         <v/>
       </c>
@@ -35970,7 +35970,7 @@
         <v>45</v>
       </c>
       <c r="B309" s="301"/>
-      <c r="C309" s="596"/>
+      <c r="C309" s="621"/>
       <c r="D309" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36022,7 +36022,7 @@
         <v>46</v>
       </c>
       <c r="B310" s="301"/>
-      <c r="C310" s="596"/>
+      <c r="C310" s="621"/>
       <c r="D310" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36081,7 +36081,7 @@
         <v>47</v>
       </c>
       <c r="B311" s="301"/>
-      <c r="C311" s="596"/>
+      <c r="C311" s="621"/>
       <c r="D311" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36133,7 +36133,7 @@
         <v>48</v>
       </c>
       <c r="B312" s="301"/>
-      <c r="C312" s="597"/>
+      <c r="C312" s="623"/>
       <c r="D312" s="439" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36189,7 +36189,7 @@
         <v>49</v>
       </c>
       <c r="B313" s="301"/>
-      <c r="C313" s="608" t="str">
+      <c r="C313" s="624" t="str">
         <f>O200</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -36241,7 +36241,7 @@
         <v>50</v>
       </c>
       <c r="B314" s="301"/>
-      <c r="C314" s="596"/>
+      <c r="C314" s="621"/>
       <c r="D314" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36293,7 +36293,7 @@
         <v>51</v>
       </c>
       <c r="B315" s="301"/>
-      <c r="C315" s="596"/>
+      <c r="C315" s="621"/>
       <c r="D315" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36338,7 +36338,7 @@
         <v>52</v>
       </c>
       <c r="B316" s="301"/>
-      <c r="C316" s="596"/>
+      <c r="C316" s="621"/>
       <c r="D316" s="433" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36392,7 +36392,7 @@
         <v>53</v>
       </c>
       <c r="B317" s="301"/>
-      <c r="C317" s="597"/>
+      <c r="C317" s="623"/>
       <c r="D317" s="439" t="str">
         <f t="shared" si="64"/>
         <v/>
@@ -36514,10 +36514,10 @@
       <c r="R319" s="246"/>
       <c r="S319" s="247"/>
       <c r="T319" s="247"/>
-      <c r="V319" s="612" t="s">
+      <c r="V319" s="593" t="s">
         <v>338</v>
       </c>
-      <c r="W319" s="612"/>
+      <c r="W319" s="593"/>
       <c r="X319" s="17" t="s">
         <v>339</v>
       </c>
@@ -36718,7 +36718,7 @@
         <v>60</v>
       </c>
       <c r="B324" s="301"/>
-      <c r="C324" s="601" t="str">
+      <c r="C324" s="609" t="str">
         <f>O240</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -36768,7 +36768,7 @@
         <v>61</v>
       </c>
       <c r="B325" s="301"/>
-      <c r="C325" s="602"/>
+      <c r="C325" s="610"/>
       <c r="D325" s="448" t="str">
         <f>P241</f>
         <v>Waist level</v>
@@ -36926,13 +36926,13 @@
         <v>346</v>
       </c>
       <c r="P329" s="53"/>
-      <c r="Q329" s="613" t="s">
+      <c r="Q329" s="611" t="s">
         <v>347</v>
       </c>
-      <c r="R329" s="613"/>
-      <c r="S329" s="613"/>
-      <c r="T329" s="613"/>
-      <c r="U329" s="613"/>
+      <c r="R329" s="611"/>
+      <c r="S329" s="611"/>
+      <c r="T329" s="611"/>
+      <c r="U329" s="611"/>
       <c r="Y329" s="14"/>
     </row>
     <row r="330" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37115,24 +37115,24 @@
         <f t="shared" si="72"/>
         <v>Attenuator</v>
       </c>
-      <c r="E335" s="614" t="str">
+      <c r="E335" s="605" t="str">
         <f>Q139</f>
         <v>Auto 1</v>
       </c>
-      <c r="F335" s="615"/>
-      <c r="G335" s="615"/>
-      <c r="H335" s="615" t="str">
+      <c r="F335" s="606"/>
+      <c r="G335" s="606"/>
+      <c r="H335" s="606" t="str">
         <f>T139</f>
         <v/>
       </c>
-      <c r="I335" s="615"/>
-      <c r="J335" s="615"/>
-      <c r="K335" s="616" t="str">
+      <c r="I335" s="606"/>
+      <c r="J335" s="606"/>
+      <c r="K335" s="607" t="str">
         <f>W139</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L335" s="616"/>
-      <c r="M335" s="617"/>
+      <c r="L335" s="607"/>
+      <c r="M335" s="608"/>
       <c r="O335" s="130"/>
       <c r="P335" s="129" t="s">
         <v>353</v>
@@ -37209,7 +37209,7 @@
         <v>7</v>
       </c>
       <c r="B337" s="301"/>
-      <c r="C337" s="590" t="str">
+      <c r="C337" s="612" t="str">
         <f>O142&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37269,7 +37269,7 @@
         <v>8</v>
       </c>
       <c r="B338" s="301"/>
-      <c r="C338" s="590"/>
+      <c r="C338" s="612"/>
       <c r="D338" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37326,7 +37326,7 @@
         <v>9</v>
       </c>
       <c r="B339" s="301"/>
-      <c r="C339" s="590"/>
+      <c r="C339" s="612"/>
       <c r="D339" s="463">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37383,7 +37383,7 @@
         <v>10</v>
       </c>
       <c r="B340" s="301"/>
-      <c r="C340" s="590" t="str">
+      <c r="C340" s="612" t="str">
         <f>O145&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37443,7 +37443,7 @@
         <v>11</v>
       </c>
       <c r="B341" s="301"/>
-      <c r="C341" s="590"/>
+      <c r="C341" s="612"/>
       <c r="D341" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37500,7 +37500,7 @@
         <v>12</v>
       </c>
       <c r="B342" s="301"/>
-      <c r="C342" s="590"/>
+      <c r="C342" s="612"/>
       <c r="D342" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37557,7 +37557,7 @@
         <v>13</v>
       </c>
       <c r="B343" s="301"/>
-      <c r="C343" s="590" t="str">
+      <c r="C343" s="612" t="str">
         <f>O148&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37609,7 +37609,7 @@
         <v>14</v>
       </c>
       <c r="B344" s="301"/>
-      <c r="C344" s="590"/>
+      <c r="C344" s="612"/>
       <c r="D344" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37671,7 +37671,7 @@
         <v>15</v>
       </c>
       <c r="B345" s="301"/>
-      <c r="C345" s="590"/>
+      <c r="C345" s="612"/>
       <c r="D345" s="463">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37734,7 +37734,7 @@
         <v>16</v>
       </c>
       <c r="B346" s="301"/>
-      <c r="C346" s="590" t="str">
+      <c r="C346" s="612" t="str">
         <f>O151&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37797,7 +37797,7 @@
         <v>17</v>
       </c>
       <c r="B347" s="301"/>
-      <c r="C347" s="590"/>
+      <c r="C347" s="612"/>
       <c r="D347" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -37855,7 +37855,7 @@
         <v>18</v>
       </c>
       <c r="B348" s="301"/>
-      <c r="C348" s="590"/>
+      <c r="C348" s="612"/>
       <c r="D348" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -37933,7 +37933,7 @@
         <v>19</v>
       </c>
       <c r="B349" s="301"/>
-      <c r="C349" s="590" t="str">
+      <c r="C349" s="612" t="str">
         <f>O154&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37996,7 +37996,7 @@
         <v>20</v>
       </c>
       <c r="B350" s="301"/>
-      <c r="C350" s="590"/>
+      <c r="C350" s="612"/>
       <c r="D350" s="462">
         <f t="shared" si="73"/>
         <v>20</v>
@@ -38055,7 +38055,7 @@
         <v>21</v>
       </c>
       <c r="B351" s="301"/>
-      <c r="C351" s="590"/>
+      <c r="C351" s="612"/>
       <c r="D351" s="464">
         <f t="shared" si="73"/>
         <v>30</v>
@@ -38364,11 +38364,11 @@
         <f>IF(OR(V358="",V359="",V362=""),"",(V358-V359)*V362)</f>
         <v/>
       </c>
-      <c r="Q358" s="603" t="str">
+      <c r="Q358" s="616" t="str">
         <f>IF(OR(P358="",P359=""),"",(ABS(P358)+ABS(P359))/$O$355)</f>
         <v/>
       </c>
-      <c r="R358" s="604" t="str">
+      <c r="R358" s="617" t="str">
         <f>IF(OR(Q358="",Q360=""),"",Q358+Q360)</f>
         <v/>
       </c>
@@ -38407,8 +38407,8 @@
         <f>IF(OR(W358="",W359="",V362=""),"",(W358-W359)*V362)</f>
         <v/>
       </c>
-      <c r="Q359" s="603"/>
-      <c r="R359" s="603"/>
+      <c r="Q359" s="616"/>
+      <c r="R359" s="616"/>
       <c r="S359" s="146" t="str">
         <f>IF(AB171="","",AB171)</f>
         <v/>
@@ -38444,11 +38444,11 @@
         <f>IF(OR(X358="",X359="",V362=""),"",(X358-X359)*V362)</f>
         <v/>
       </c>
-      <c r="Q360" s="604" t="str">
+      <c r="Q360" s="617" t="str">
         <f>IF(OR(P360="",P361=""),"",(ABS(P360)+ABS(P361))/$O$355)</f>
         <v/>
       </c>
-      <c r="R360" s="604"/>
+      <c r="R360" s="617"/>
       <c r="S360" s="146" t="str">
         <f>IF(AB172="","",AB172)</f>
         <v/>
@@ -38490,8 +38490,8 @@
         <f>IF(OR(Y358="",Y359="",V362=""),"",(Y358-Y359)*V362)</f>
         <v/>
       </c>
-      <c r="Q361" s="604"/>
-      <c r="R361" s="604"/>
+      <c r="Q361" s="617"/>
+      <c r="R361" s="617"/>
       <c r="S361" s="148" t="str">
         <f>IF(AB173="","",AB173)</f>
         <v/>
@@ -38663,7 +38663,7 @@
         <v>36</v>
       </c>
       <c r="B366" s="301"/>
-      <c r="C366" s="605" t="str">
+      <c r="C366" s="618" t="str">
         <f>O214</f>
         <v>Auto 1</v>
       </c>
@@ -38714,7 +38714,7 @@
         <v>37</v>
       </c>
       <c r="B367" s="301"/>
-      <c r="C367" s="606"/>
+      <c r="C367" s="619"/>
       <c r="D367" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38760,7 +38760,7 @@
         <v>38</v>
       </c>
       <c r="B368" s="301"/>
-      <c r="C368" s="606"/>
+      <c r="C368" s="619"/>
       <c r="D368" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38795,7 +38795,7 @@
         <v>39</v>
       </c>
       <c r="B369" s="301"/>
-      <c r="C369" s="606"/>
+      <c r="C369" s="619"/>
       <c r="D369" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38830,7 +38830,7 @@
         <v>40</v>
       </c>
       <c r="B370" s="301"/>
-      <c r="C370" s="606"/>
+      <c r="C370" s="619"/>
       <c r="D370" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38875,7 +38875,7 @@
         <v>41</v>
       </c>
       <c r="B371" s="301"/>
-      <c r="C371" s="595" t="str">
+      <c r="C371" s="620" t="str">
         <f>O219</f>
         <v/>
       </c>
@@ -38925,7 +38925,7 @@
         <v>42</v>
       </c>
       <c r="B372" s="301"/>
-      <c r="C372" s="596"/>
+      <c r="C372" s="621"/>
       <c r="D372" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -38975,7 +38975,7 @@
         <v>43</v>
       </c>
       <c r="B373" s="301"/>
-      <c r="C373" s="596"/>
+      <c r="C373" s="621"/>
       <c r="D373" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39022,7 +39022,7 @@
         <v>44</v>
       </c>
       <c r="B374" s="301"/>
-      <c r="C374" s="596"/>
+      <c r="C374" s="621"/>
       <c r="D374" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39072,7 +39072,7 @@
         <v>45</v>
       </c>
       <c r="B375" s="301"/>
-      <c r="C375" s="597"/>
+      <c r="C375" s="623"/>
       <c r="D375" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39119,7 +39119,7 @@
         <v>46</v>
       </c>
       <c r="B376" s="301"/>
-      <c r="C376" s="598" t="str">
+      <c r="C376" s="636" t="str">
         <f>O224</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -39172,7 +39172,7 @@
         <v>47</v>
       </c>
       <c r="B377" s="301"/>
-      <c r="C377" s="599"/>
+      <c r="C377" s="637"/>
       <c r="D377" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39219,7 +39219,7 @@
         <v>48</v>
       </c>
       <c r="B378" s="301"/>
-      <c r="C378" s="599"/>
+      <c r="C378" s="637"/>
       <c r="D378" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39269,7 +39269,7 @@
         <v>49</v>
       </c>
       <c r="B379" s="301"/>
-      <c r="C379" s="599"/>
+      <c r="C379" s="637"/>
       <c r="D379" s="433" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39316,7 +39316,7 @@
         <v>50</v>
       </c>
       <c r="B380" s="301"/>
-      <c r="C380" s="600"/>
+      <c r="C380" s="638"/>
       <c r="D380" s="439" t="str">
         <f t="shared" si="83"/>
         <v/>
@@ -39626,7 +39626,7 @@
         <v>58</v>
       </c>
       <c r="B388" s="301"/>
-      <c r="C388" s="601" t="str">
+      <c r="C388" s="609" t="str">
         <f>O242</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -39677,7 +39677,7 @@
         <v>59</v>
       </c>
       <c r="B389" s="301"/>
-      <c r="C389" s="602"/>
+      <c r="C389" s="610"/>
       <c r="D389" s="448" t="str">
         <f>P243</f>
         <v>Waist level</v>
@@ -40028,14 +40028,14 @@
       <c r="E399" s="299"/>
       <c r="F399" s="299"/>
       <c r="G399" s="299"/>
-      <c r="H399" s="611" t="s">
+      <c r="H399" s="627" t="s">
         <v>393</v>
       </c>
-      <c r="I399" s="611"/>
-      <c r="J399" s="611" t="s">
+      <c r="I399" s="627"/>
+      <c r="J399" s="627" t="s">
         <v>394</v>
       </c>
-      <c r="K399" s="611"/>
+      <c r="K399" s="627"/>
       <c r="L399" s="299"/>
       <c r="M399" s="300"/>
       <c r="O399" s="13"/>
@@ -40609,20 +40609,20 @@
       </c>
       <c r="B413" s="301"/>
       <c r="C413" s="42"/>
-      <c r="D413" s="609" t="s">
+      <c r="D413" s="625" t="s">
         <v>400</v>
       </c>
-      <c r="E413" s="609"/>
-      <c r="F413" s="609"/>
-      <c r="G413" s="609"/>
-      <c r="H413" s="609"/>
-      <c r="I413" s="609" t="s">
+      <c r="E413" s="625"/>
+      <c r="F413" s="625"/>
+      <c r="G413" s="625"/>
+      <c r="H413" s="625"/>
+      <c r="I413" s="625" t="s">
         <v>401</v>
       </c>
-      <c r="J413" s="609"/>
-      <c r="K413" s="609"/>
-      <c r="L413" s="609"/>
-      <c r="M413" s="610"/>
+      <c r="J413" s="625"/>
+      <c r="K413" s="625"/>
+      <c r="L413" s="625"/>
+      <c r="M413" s="626"/>
       <c r="O413" s="13"/>
       <c r="P413" s="2" t="s">
         <v>188</v>
@@ -42102,11 +42102,11 @@
         <f t="shared" si="95"/>
         <v/>
       </c>
-      <c r="F442" s="584" t="str">
+      <c r="F442" s="628" t="str">
         <f t="shared" si="95"/>
         <v/>
       </c>
-      <c r="G442" s="586" t="str">
+      <c r="G442" s="630" t="str">
         <f t="shared" si="95"/>
         <v/>
       </c>
@@ -42147,8 +42147,8 @@
         <f>P359</f>
         <v/>
       </c>
-      <c r="F443" s="585"/>
-      <c r="G443" s="587"/>
+      <c r="F443" s="629"/>
+      <c r="G443" s="631"/>
       <c r="H443" s="200"/>
       <c r="I443" s="82" t="str">
         <f>T360</f>
@@ -42188,11 +42188,11 @@
         <f>P360</f>
         <v/>
       </c>
-      <c r="F444" s="585" t="str">
+      <c r="F444" s="629" t="str">
         <f>Q360</f>
         <v/>
       </c>
-      <c r="G444" s="587"/>
+      <c r="G444" s="631"/>
       <c r="H444" s="135"/>
       <c r="I444" s="91" t="str">
         <f>T361</f>
@@ -42233,8 +42233,8 @@
         <f>P361</f>
         <v/>
       </c>
-      <c r="F445" s="589"/>
-      <c r="G445" s="588"/>
+      <c r="F445" s="633"/>
+      <c r="G445" s="632"/>
       <c r="H445" s="135"/>
       <c r="I445" s="135"/>
       <c r="J445" s="135"/>
@@ -48593,71 +48593,30 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="106">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="W107:Y107"/>
-    <mergeCell ref="Q139:S139"/>
-    <mergeCell ref="T139:V139"/>
-    <mergeCell ref="W139:Y139"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="T181:U181"/>
-    <mergeCell ref="O190:O194"/>
-    <mergeCell ref="O195:O199"/>
-    <mergeCell ref="O200:O204"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="Q107:S107"/>
-    <mergeCell ref="T107:V107"/>
-    <mergeCell ref="H204:H205"/>
-    <mergeCell ref="I204:I205"/>
-    <mergeCell ref="M204:M205"/>
-    <mergeCell ref="O214:O218"/>
-    <mergeCell ref="O219:O223"/>
-    <mergeCell ref="O224:O228"/>
-    <mergeCell ref="O240:O241"/>
-    <mergeCell ref="O242:O243"/>
-    <mergeCell ref="Q257:R257"/>
-    <mergeCell ref="T257:U257"/>
-    <mergeCell ref="E269:G269"/>
-    <mergeCell ref="H269:J269"/>
-    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="F442:F443"/>
+    <mergeCell ref="G442:G445"/>
+    <mergeCell ref="F444:F445"/>
+    <mergeCell ref="C337:C339"/>
+    <mergeCell ref="C340:C342"/>
+    <mergeCell ref="C343:C345"/>
+    <mergeCell ref="C346:C348"/>
+    <mergeCell ref="C349:C351"/>
+    <mergeCell ref="E204:E205"/>
+    <mergeCell ref="F204:F205"/>
+    <mergeCell ref="C371:C375"/>
+    <mergeCell ref="C376:C380"/>
+    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="Q358:Q359"/>
+    <mergeCell ref="R358:R361"/>
+    <mergeCell ref="Q360:Q361"/>
+    <mergeCell ref="C366:C370"/>
+    <mergeCell ref="C303:C307"/>
+    <mergeCell ref="C308:C312"/>
+    <mergeCell ref="C313:C317"/>
+    <mergeCell ref="D413:H413"/>
+    <mergeCell ref="I413:M413"/>
+    <mergeCell ref="H399:I399"/>
+    <mergeCell ref="J399:K399"/>
     <mergeCell ref="V319:W319"/>
     <mergeCell ref="C324:C325"/>
     <mergeCell ref="Q329:U329"/>
@@ -48675,30 +48634,71 @@
     <mergeCell ref="C283:C285"/>
     <mergeCell ref="P302:T302"/>
     <mergeCell ref="P293:T293"/>
-    <mergeCell ref="Q358:Q359"/>
-    <mergeCell ref="R358:R361"/>
-    <mergeCell ref="Q360:Q361"/>
-    <mergeCell ref="C366:C370"/>
-    <mergeCell ref="C303:C307"/>
-    <mergeCell ref="C308:C312"/>
-    <mergeCell ref="C313:C317"/>
-    <mergeCell ref="D413:H413"/>
-    <mergeCell ref="I413:M413"/>
-    <mergeCell ref="H399:I399"/>
-    <mergeCell ref="J399:K399"/>
-    <mergeCell ref="F442:F443"/>
-    <mergeCell ref="G442:G445"/>
-    <mergeCell ref="F444:F445"/>
-    <mergeCell ref="C337:C339"/>
-    <mergeCell ref="C340:C342"/>
-    <mergeCell ref="C343:C345"/>
-    <mergeCell ref="C346:C348"/>
-    <mergeCell ref="C349:C351"/>
-    <mergeCell ref="E204:E205"/>
-    <mergeCell ref="F204:F205"/>
-    <mergeCell ref="C371:C375"/>
-    <mergeCell ref="C376:C380"/>
-    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="O214:O218"/>
+    <mergeCell ref="O219:O223"/>
+    <mergeCell ref="O224:O228"/>
+    <mergeCell ref="O240:O241"/>
+    <mergeCell ref="O242:O243"/>
+    <mergeCell ref="Q257:R257"/>
+    <mergeCell ref="T257:U257"/>
+    <mergeCell ref="E269:G269"/>
+    <mergeCell ref="H269:J269"/>
+    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="T181:U181"/>
+    <mergeCell ref="O190:O194"/>
+    <mergeCell ref="O195:O199"/>
+    <mergeCell ref="O200:O204"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="Q107:S107"/>
+    <mergeCell ref="T107:V107"/>
+    <mergeCell ref="H204:H205"/>
+    <mergeCell ref="I204:I205"/>
+    <mergeCell ref="M204:M205"/>
+    <mergeCell ref="W107:Y107"/>
+    <mergeCell ref="Q139:S139"/>
+    <mergeCell ref="T139:V139"/>
+    <mergeCell ref="W139:Y139"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
   </mergeCells>
   <conditionalFormatting sqref="S126 V126 Y126 S158 V158 Y158">
     <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
@@ -49016,39 +49016,39 @@
         <f>Fluoro!D269</f>
         <v>Attenuator</v>
       </c>
-      <c r="E5" s="615" t="str">
+      <c r="E5" s="606" t="str">
         <f>Fluoro!E269</f>
         <v>Auto 1</v>
       </c>
-      <c r="F5" s="615">
+      <c r="F5" s="606">
         <f>Fluoro!F269</f>
         <v>0</v>
       </c>
-      <c r="G5" s="615">
+      <c r="G5" s="606">
         <f>Fluoro!G269</f>
         <v>0</v>
       </c>
-      <c r="H5" s="615" t="str">
+      <c r="H5" s="606" t="str">
         <f>Fluoro!H269</f>
         <v/>
       </c>
-      <c r="I5" s="615">
+      <c r="I5" s="606">
         <f>Fluoro!I269</f>
         <v>0</v>
       </c>
-      <c r="J5" s="615">
+      <c r="J5" s="606">
         <f>Fluoro!J269</f>
         <v>0</v>
       </c>
-      <c r="K5" s="616" t="str">
+      <c r="K5" s="607" t="str">
         <f>Fluoro!K269</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L5" s="616">
+      <c r="L5" s="607">
         <f>Fluoro!L269</f>
         <v>0</v>
       </c>
-      <c r="M5" s="616">
+      <c r="M5" s="607">
         <f>Fluoro!M269</f>
         <v>0</v>
       </c>
@@ -49105,7 +49105,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="640" t="str">
+      <c r="C7" s="639" t="str">
         <f>Fluoro!C271</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49155,7 +49155,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="640">
+      <c r="C8" s="639">
         <f>Fluoro!C272</f>
         <v>0</v>
       </c>
@@ -49205,7 +49205,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="640">
+      <c r="C9" s="639">
         <f>Fluoro!C273</f>
         <v>0</v>
       </c>
@@ -49255,7 +49255,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="640" t="str">
+      <c r="C10" s="639" t="str">
         <f>Fluoro!C274</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49305,7 +49305,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="640">
+      <c r="C11" s="639">
         <f>Fluoro!C275</f>
         <v>0</v>
       </c>
@@ -49355,7 +49355,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="640">
+      <c r="C12" s="639">
         <f>Fluoro!C276</f>
         <v>0</v>
       </c>
@@ -49405,7 +49405,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="640" t="str">
+      <c r="C13" s="639" t="str">
         <f>Fluoro!C277</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49455,7 +49455,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="640">
+      <c r="C14" s="639">
         <f>Fluoro!C278</f>
         <v>0</v>
       </c>
@@ -49505,7 +49505,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10"/>
-      <c r="C15" s="640">
+      <c r="C15" s="639">
         <f>Fluoro!C279</f>
         <v>0</v>
       </c>
@@ -49555,7 +49555,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10"/>
-      <c r="C16" s="640" t="str">
+      <c r="C16" s="639" t="str">
         <f>Fluoro!C280</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49605,7 +49605,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="640">
+      <c r="C17" s="639">
         <f>Fluoro!C281</f>
         <v>0</v>
       </c>
@@ -49655,7 +49655,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="640">
+      <c r="C18" s="639">
         <f>Fluoro!C282</f>
         <v>0</v>
       </c>
@@ -49705,7 +49705,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="640" t="str">
+      <c r="C19" s="639" t="str">
         <f>Fluoro!C283</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49755,7 +49755,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="640">
+      <c r="C20" s="639">
         <f>Fluoro!C284</f>
         <v>0</v>
       </c>
@@ -49805,7 +49805,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="640">
+      <c r="C21" s="639">
         <f>Fluoro!C285</f>
         <v>0</v>
       </c>
@@ -50229,39 +50229,39 @@
         <f>Fluoro!D335</f>
         <v>Attenuator</v>
       </c>
-      <c r="E37" s="615" t="str">
+      <c r="E37" s="606" t="str">
         <f>Fluoro!E335</f>
         <v>Auto 1</v>
       </c>
-      <c r="F37" s="615">
+      <c r="F37" s="606">
         <f>Fluoro!F335</f>
         <v>0</v>
       </c>
-      <c r="G37" s="615">
+      <c r="G37" s="606">
         <f>Fluoro!G335</f>
         <v>0</v>
       </c>
-      <c r="H37" s="615" t="str">
+      <c r="H37" s="606" t="str">
         <f>Fluoro!H335</f>
         <v/>
       </c>
-      <c r="I37" s="615">
+      <c r="I37" s="606">
         <f>Fluoro!I335</f>
         <v>0</v>
       </c>
-      <c r="J37" s="615">
+      <c r="J37" s="606">
         <f>Fluoro!J335</f>
         <v>0</v>
       </c>
-      <c r="K37" s="616" t="str">
+      <c r="K37" s="607" t="str">
         <f>Fluoro!K335</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L37" s="616">
+      <c r="L37" s="607">
         <f>Fluoro!L335</f>
         <v>0</v>
       </c>
-      <c r="M37" s="616">
+      <c r="M37" s="607">
         <f>Fluoro!M335</f>
         <v>0</v>
       </c>
@@ -50318,7 +50318,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="10"/>
-      <c r="C39" s="640" t="str">
+      <c r="C39" s="639" t="str">
         <f>Fluoro!C337</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50368,7 +50368,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="10"/>
-      <c r="C40" s="640">
+      <c r="C40" s="639">
         <f>Fluoro!C338</f>
         <v>0</v>
       </c>
@@ -50418,7 +50418,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="10"/>
-      <c r="C41" s="640">
+      <c r="C41" s="639">
         <f>Fluoro!C339</f>
         <v>0</v>
       </c>
@@ -50468,7 +50468,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="10"/>
-      <c r="C42" s="640" t="str">
+      <c r="C42" s="639" t="str">
         <f>Fluoro!C340</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50518,7 +50518,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="10"/>
-      <c r="C43" s="640">
+      <c r="C43" s="639">
         <f>Fluoro!C341</f>
         <v>0</v>
       </c>
@@ -50568,7 +50568,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="10"/>
-      <c r="C44" s="640">
+      <c r="C44" s="639">
         <f>Fluoro!C342</f>
         <v>0</v>
       </c>
@@ -50618,7 +50618,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="10"/>
-      <c r="C45" s="640" t="str">
+      <c r="C45" s="639" t="str">
         <f>Fluoro!C343</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50668,7 +50668,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="10"/>
-      <c r="C46" s="640">
+      <c r="C46" s="639">
         <f>Fluoro!C344</f>
         <v>0</v>
       </c>
@@ -50718,7 +50718,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="10"/>
-      <c r="C47" s="640">
+      <c r="C47" s="639">
         <f>Fluoro!C345</f>
         <v>0</v>
       </c>
@@ -50768,7 +50768,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="10"/>
-      <c r="C48" s="640" t="str">
+      <c r="C48" s="639" t="str">
         <f>Fluoro!C346</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50818,7 +50818,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="10"/>
-      <c r="C49" s="640">
+      <c r="C49" s="639">
         <f>Fluoro!C347</f>
         <v>0</v>
       </c>
@@ -50868,7 +50868,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="10"/>
-      <c r="C50" s="640">
+      <c r="C50" s="639">
         <f>Fluoro!C348</f>
         <v>0</v>
       </c>
@@ -50918,7 +50918,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="10"/>
-      <c r="C51" s="640" t="str">
+      <c r="C51" s="639" t="str">
         <f>Fluoro!C349</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50968,7 +50968,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="10"/>
-      <c r="C52" s="640">
+      <c r="C52" s="639">
         <f>Fluoro!C350</f>
         <v>0</v>
       </c>
@@ -51018,7 +51018,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="10"/>
-      <c r="C53" s="640">
+      <c r="C53" s="639">
         <f>Fluoro!C351</f>
         <v>0</v>
       </c>
@@ -51212,7 +51212,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="10"/>
-      <c r="C60" s="639"/>
+      <c r="C60" s="640"/>
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60"/>
@@ -51229,7 +51229,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="10"/>
-      <c r="C61" s="639"/>
+      <c r="C61" s="640"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>
@@ -51364,23 +51364,23 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="17">
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C51:C53"/>
     <mergeCell ref="E37:G37"/>
     <mergeCell ref="H37:J37"/>
     <mergeCell ref="K37:M37"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="68" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -51394,8 +51394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB143"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -51409,29 +51409,29 @@
       </c>
       <c r="B1" s="641"/>
       <c r="N1" s="278"/>
-      <c r="O1" s="620" t="str">
+      <c r="O1" s="615" t="str">
         <f>Fluoro!O105</f>
         <v>Patient Entrance Exposure Rate (Fluoroscopy)*</v>
       </c>
-      <c r="P1" s="620"/>
-      <c r="Q1" s="620"/>
-      <c r="R1" s="620" t="s">
+      <c r="P1" s="615"/>
+      <c r="Q1" s="615"/>
+      <c r="R1" s="615" t="s">
         <v>406</v>
       </c>
-      <c r="S1" s="620"/>
-      <c r="T1" s="620"/>
+      <c r="S1" s="615"/>
+      <c r="T1" s="615"/>
       <c r="V1" s="278"/>
-      <c r="W1" s="620" t="str">
+      <c r="W1" s="615" t="str">
         <f>Fluoro!O137</f>
         <v>Patient Entrance Exposure Rate – Digital Acquisition</v>
       </c>
-      <c r="X1" s="620"/>
-      <c r="Y1" s="620"/>
-      <c r="Z1" s="620" t="s">
+      <c r="X1" s="615"/>
+      <c r="Y1" s="615"/>
+      <c r="Z1" s="615" t="s">
         <v>406</v>
       </c>
-      <c r="AA1" s="620"/>
-      <c r="AB1" s="620"/>
+      <c r="AA1" s="615"/>
+      <c r="AB1" s="615"/>
     </row>
     <row r="2" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="279">
@@ -55424,14 +55424,14 @@
       <c r="B75" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="E75" s="620" t="s">
+      <c r="E75" s="615" t="s">
         <v>419</v>
       </c>
-      <c r="F75" s="620"/>
-      <c r="I75" s="620" t="s">
+      <c r="F75" s="615"/>
+      <c r="I75" s="615" t="s">
         <v>420</v>
       </c>
-      <c r="J75" s="620"/>
+      <c r="J75" s="615"/>
     </row>
     <row r="76" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
@@ -56216,63 +56216,63 @@
         <v>Attenuator</v>
       </c>
       <c r="B104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$S$141:$S$143)=0,"Not Avail.",Fluoro!$Q$107)</f>
+        <f>IF(MAX(Fluoro!$S$141:$S$143)=0,"Not Avail.",Fluoro!$Q$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="C104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$S$144:$S$146)=0,"Not Avail.",Fluoro!$Q$107)</f>
+        <f>IF(MAX(Fluoro!$S$144:$S$146)=0,"Not Avail.",Fluoro!$Q$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="D104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$S$147:$S$149)=0,"Not Avail.",Fluoro!$Q$107)</f>
+        <f>IF(MAX(Fluoro!$S$147:$S$149)=0,"Not Avail.",Fluoro!$Q$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="E104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$S$150:$S$152)=0,"Not Avail.",Fluoro!$Q$107)</f>
+        <f>IF(MAX(Fluoro!$S$150:$S$152)=0,"Not Avail.",Fluoro!$Q$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="F104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$S$153:$S$155)=0,"Not Avail.",Fluoro!$Q$107)</f>
+        <f>IF(MAX(Fluoro!$S$153:$S$155)=0,"Not Avail.",Fluoro!$Q$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="G104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$V$141:$V$143)=0,"Not Avail.",Fluoro!$T$107)</f>
+        <f>IF(MAX(Fluoro!$V$141:$V$143)=0,"Not Avail.",Fluoro!$T$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="H104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$V$144:$V$146)=0,"Not Avail.",Fluoro!$T$107)</f>
+        <f>IF(MAX(Fluoro!$V$144:$V$146)=0,"Not Avail.",Fluoro!$T$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="I104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$V$147:$V$149)=0,"Not Avail.",Fluoro!$T$107)</f>
+        <f>IF(MAX(Fluoro!$V$147:$V$149)=0,"Not Avail.",Fluoro!$T$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="J104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$V$150:$V$152)=0,"Not Avail.",Fluoro!$T$107)</f>
+        <f>IF(MAX(Fluoro!$V$150:$V$152)=0,"Not Avail.",Fluoro!$T$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="K104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$V$153:$V$155)=0,"Not Avail.",Fluoro!$T$107)</f>
+        <f>IF(MAX(Fluoro!$V$153:$V$155)=0,"Not Avail.",Fluoro!$T$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="L104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$Y$141:$Y$143)=0,"Not Avail.",Fluoro!$W$107)</f>
+        <f>IF(MAX(Fluoro!$Y$141:$Y$143)=0,"Not Avail.",Fluoro!$W$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="M104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$Y$144:$Y$146)=0,"Not Avail.",Fluoro!$W$107)</f>
+        <f>IF(MAX(Fluoro!$Y$144:$Y$146)=0,"Not Avail.",Fluoro!$W$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="N104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$Y$147:$Y$149)=0,"Not Avail.",Fluoro!$W$107)</f>
+        <f>IF(MAX(Fluoro!$Y$147:$Y$149)=0,"Not Avail.",Fluoro!$W$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="O104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$Y$150:$Y$152)=0,"Not Avail.",Fluoro!$W$107)</f>
+        <f>IF(MAX(Fluoro!$Y$150:$Y$152)=0,"Not Avail.",Fluoro!$W$139)</f>
         <v>Not Avail.</v>
       </c>
       <c r="P104" s="223" t="str">
-        <f>IF(MAX(Fluoro!$Y$153:$Y$155)=0,"Not Avail.",Fluoro!$W$107)</f>
+        <f>IF(MAX(Fluoro!$Y$153:$Y$155)=0,"Not Avail.",Fluoro!$W$139)</f>
         <v>Not Avail.</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjust beam profile pass/fail formula
</commit_message>
<xml_diff>
--- a/MUSCCArm.xlsx
+++ b/MUSCCArm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1DD7EE-9B70-43B5-ADB2-CEDAC4C8BA4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C05385-C07C-4A11-B360-10AE0B261464}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="480">
   <si>
     <t>Print Area</t>
   </si>
@@ -1605,6 +1605,9 @@
   </si>
   <si>
     <t>Revision 1.7-20220928</t>
+  </si>
+  <si>
+    <t>Minimum of 0.25 mm lead equivalent shielding (i.e. drapes or sliding panels)</t>
   </si>
 </sst>
 </file>
@@ -6589,6 +6592,138 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="150" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="200" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="222" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="223" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="127" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="155" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="182" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="149" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="150" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="175" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="151" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="176" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="154" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="180" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6607,30 +6742,12 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="117" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="200" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="201" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="149" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="150" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="151" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="183" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6640,124 +6757,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="193" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="125" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="127" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="155" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="182" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="175" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="176" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="154" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="180" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="108" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="222" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="223" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="139" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -20413,7 +20416,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD792"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I92" sqref="I92"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20723,21 +20728,21 @@
       <c r="E10" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="664" t="str">
+      <c r="F10" s="613" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="664"/>
+      <c r="G10" s="613"/>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
       <c r="J10" s="160" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="653" t="str">
+      <c r="K10" s="614" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="653"/>
+      <c r="L10" s="614"/>
       <c r="M10" s="309"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="2" t="s">
@@ -20780,21 +20785,21 @@
       <c r="E11" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="654" t="str">
+      <c r="F11" s="615" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="654"/>
+      <c r="G11" s="615"/>
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
       <c r="J11" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="654" t="str">
+      <c r="K11" s="615" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="654"/>
+      <c r="L11" s="615"/>
       <c r="M11" s="309"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="2" t="s">
@@ -20837,21 +20842,21 @@
       <c r="E12" s="160" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="654" t="str">
+      <c r="F12" s="615" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="654"/>
+      <c r="G12" s="615"/>
       <c r="H12" s="42"/>
       <c r="I12" s="42"/>
       <c r="J12" s="160" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="666" t="str">
+      <c r="K12" s="616" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="666"/>
+      <c r="L12" s="616"/>
       <c r="M12" s="309"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="2" t="s">
@@ -20894,21 +20899,21 @@
       <c r="E13" s="160" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="655" t="str">
+      <c r="F13" s="617" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="655"/>
+      <c r="G13" s="617"/>
       <c r="H13" s="42"/>
       <c r="I13" s="42"/>
       <c r="J13" s="160" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="655" t="str">
+      <c r="K13" s="617" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="L13" s="655"/>
+      <c r="L13" s="617"/>
       <c r="M13" s="309"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="2" t="s">
@@ -21031,21 +21036,21 @@
       <c r="E16" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="664" t="str">
+      <c r="F16" s="613" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="664"/>
+      <c r="G16" s="613"/>
       <c r="H16" s="42"/>
       <c r="I16" s="42"/>
       <c r="J16" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="667" t="str">
+      <c r="K16" s="618" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="667"/>
+      <c r="L16" s="618"/>
       <c r="M16" s="309"/>
       <c r="O16" s="13"/>
       <c r="P16" s="50" t="s">
@@ -21075,21 +21080,21 @@
       <c r="E17" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="654" t="str">
+      <c r="F17" s="615" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="654"/>
+      <c r="G17" s="615"/>
       <c r="H17" s="42"/>
       <c r="I17" s="42"/>
       <c r="J17" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="K17" s="655" t="str">
+      <c r="K17" s="617" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="655"/>
+      <c r="L17" s="617"/>
       <c r="M17" s="309"/>
       <c r="O17" s="13"/>
       <c r="Q17" s="2" t="s">
@@ -21132,21 +21137,21 @@
       <c r="E18" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="655" t="str">
+      <c r="F18" s="617" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="655"/>
+      <c r="G18" s="617"/>
       <c r="H18" s="42"/>
       <c r="I18" s="42"/>
       <c r="J18" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="655" t="str">
+      <c r="K18" s="617" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="655"/>
+      <c r="L18" s="617"/>
       <c r="M18" s="309"/>
       <c r="O18" s="13"/>
       <c r="Q18" s="2" t="s">
@@ -21194,11 +21199,11 @@
       <c r="J19" s="160" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="655" t="str">
+      <c r="K19" s="617" t="str">
         <f>IF(V20="","",V20)</f>
         <v/>
       </c>
-      <c r="L19" s="655"/>
+      <c r="L19" s="617"/>
       <c r="M19" s="309"/>
       <c r="O19" s="13"/>
       <c r="Q19" s="2" t="s">
@@ -21273,11 +21278,11 @@
       <c r="E21" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="664" t="str">
+      <c r="F21" s="613" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="664"/>
+      <c r="G21" s="613"/>
       <c r="H21" s="42"/>
       <c r="I21" s="42"/>
       <c r="J21" s="73" t="s">
@@ -21317,21 +21322,21 @@
       <c r="E22" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="665" t="str">
+      <c r="F22" s="619" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="665"/>
+      <c r="G22" s="619"/>
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
       <c r="J22" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="664" t="str">
+      <c r="K22" s="613" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="664"/>
+      <c r="L22" s="613"/>
       <c r="M22" s="309"/>
       <c r="O22" s="13"/>
       <c r="Q22" s="2" t="s">
@@ -21376,11 +21381,11 @@
       <c r="J23" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="K23" s="654" t="str">
+      <c r="K23" s="615" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="654"/>
+      <c r="L23" s="615"/>
       <c r="M23" s="309"/>
       <c r="O23" s="13"/>
       <c r="Q23" s="2" t="s">
@@ -21423,21 +21428,21 @@
       <c r="E24" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="653" t="str">
+      <c r="F24" s="614" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="653"/>
+      <c r="G24" s="614"/>
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
       <c r="J24" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="K24" s="654" t="str">
+      <c r="K24" s="615" t="str">
         <f>IF(V25="","",V25)</f>
         <v/>
       </c>
-      <c r="L24" s="654"/>
+      <c r="L24" s="615"/>
       <c r="M24" s="309"/>
       <c r="O24" s="13"/>
       <c r="P24" s="50" t="s">
@@ -21475,11 +21480,11 @@
       <c r="E25" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="655" t="str">
+      <c r="F25" s="617" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="655"/>
+      <c r="G25" s="617"/>
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
@@ -21527,11 +21532,11 @@
       <c r="E26" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="655" t="str">
+      <c r="F26" s="617" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="655"/>
+      <c r="G26" s="617"/>
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
       <c r="J26" s="310" t="s">
@@ -21580,11 +21585,11 @@
       <c r="J27" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="664" t="str">
+      <c r="K27" s="613" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="664"/>
+      <c r="L27" s="613"/>
       <c r="M27" s="309"/>
       <c r="O27" s="13"/>
       <c r="Q27" s="2" t="s">
@@ -21622,21 +21627,21 @@
       <c r="E28" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="653" t="str">
+      <c r="F28" s="614" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="653"/>
+      <c r="G28" s="614"/>
       <c r="H28" s="42"/>
       <c r="I28" s="42"/>
       <c r="J28" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="654" t="str">
+      <c r="K28" s="615" t="str">
         <f>IF(V29="","",V29)</f>
         <v/>
       </c>
-      <c r="L28" s="654"/>
+      <c r="L28" s="615"/>
       <c r="M28" s="309"/>
       <c r="O28" s="13"/>
       <c r="P28" s="50" t="s">
@@ -21665,11 +21670,11 @@
       <c r="E29" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="655" t="str">
+      <c r="F29" s="617" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="655"/>
+      <c r="G29" s="617"/>
       <c r="H29" s="42"/>
       <c r="I29" s="42"/>
       <c r="J29" s="42"/>
@@ -21717,11 +21722,11 @@
       <c r="E30" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="655" t="str">
+      <c r="F30" s="617" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="655"/>
+      <c r="G30" s="617"/>
       <c r="H30" s="42"/>
       <c r="I30" s="42"/>
       <c r="J30" s="42"/>
@@ -21836,11 +21841,11 @@
       <c r="E33" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="664" t="str">
+      <c r="F33" s="613" t="str">
         <f>IF(R34="","",R34)</f>
         <v/>
       </c>
-      <c r="G33" s="664"/>
+      <c r="G33" s="613"/>
       <c r="H33" s="42"/>
       <c r="I33" s="42"/>
       <c r="J33" s="73" t="s">
@@ -21877,21 +21882,21 @@
       <c r="E34" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="665" t="str">
+      <c r="F34" s="619" t="str">
         <f>IF(R35="","",R35)</f>
         <v/>
       </c>
-      <c r="G34" s="665"/>
+      <c r="G34" s="619"/>
       <c r="H34" s="42"/>
       <c r="I34" s="42"/>
       <c r="J34" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="664" t="str">
+      <c r="K34" s="613" t="str">
         <f>IF(V35="","",V35)</f>
         <v/>
       </c>
-      <c r="L34" s="664"/>
+      <c r="L34" s="613"/>
       <c r="M34" s="309"/>
       <c r="O34" s="13"/>
       <c r="Q34" s="2" t="s">
@@ -21936,11 +21941,11 @@
       <c r="J35" s="160" t="s">
         <v>41</v>
       </c>
-      <c r="K35" s="654" t="str">
+      <c r="K35" s="615" t="str">
         <f>IF(V36="","",V36)</f>
         <v/>
       </c>
-      <c r="L35" s="654"/>
+      <c r="L35" s="615"/>
       <c r="M35" s="309"/>
       <c r="O35" s="13"/>
       <c r="Q35" s="2" t="s">
@@ -21983,21 +21988,21 @@
       <c r="E36" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="653" t="str">
+      <c r="F36" s="614" t="str">
         <f>IF(R37="","",R37)</f>
         <v/>
       </c>
-      <c r="G36" s="653"/>
+      <c r="G36" s="614"/>
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
       <c r="J36" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="K36" s="654" t="str">
+      <c r="K36" s="615" t="str">
         <f>IF(V37="","",V37)</f>
         <v/>
       </c>
-      <c r="L36" s="654"/>
+      <c r="L36" s="615"/>
       <c r="M36" s="309"/>
       <c r="O36" s="13"/>
       <c r="P36" s="50" t="s">
@@ -22035,11 +22040,11 @@
       <c r="E37" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="655" t="str">
+      <c r="F37" s="617" t="str">
         <f>IF(R38="","",R38)</f>
         <v/>
       </c>
-      <c r="G37" s="655"/>
+      <c r="G37" s="617"/>
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
       <c r="J37" s="42"/>
@@ -22087,11 +22092,11 @@
       <c r="E38" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="655" t="str">
+      <c r="F38" s="617" t="str">
         <f>IF(R39="","",R39)</f>
         <v/>
       </c>
-      <c r="G38" s="655"/>
+      <c r="G38" s="617"/>
       <c r="H38" s="42"/>
       <c r="I38" s="42"/>
       <c r="J38" s="310" t="s">
@@ -22138,11 +22143,11 @@
       <c r="J39" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="K39" s="664" t="str">
+      <c r="K39" s="613" t="str">
         <f>IF(V40="","",V40)</f>
         <v/>
       </c>
-      <c r="L39" s="664"/>
+      <c r="L39" s="613"/>
       <c r="M39" s="309"/>
       <c r="O39" s="13"/>
       <c r="Q39" s="2" t="s">
@@ -22180,21 +22185,21 @@
       <c r="E40" s="160" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="653" t="str">
+      <c r="F40" s="614" t="str">
         <f>IF(R41="","",R41)</f>
         <v/>
       </c>
-      <c r="G40" s="653"/>
+      <c r="G40" s="614"/>
       <c r="H40" s="42"/>
       <c r="I40" s="42"/>
       <c r="J40" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K40" s="654" t="str">
+      <c r="K40" s="615" t="str">
         <f>IF(V41="","",V41)</f>
         <v/>
       </c>
-      <c r="L40" s="654"/>
+      <c r="L40" s="615"/>
       <c r="M40" s="309"/>
       <c r="O40" s="13"/>
       <c r="P40" s="50" t="s">
@@ -22232,11 +22237,11 @@
       <c r="E41" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="655" t="str">
+      <c r="F41" s="617" t="str">
         <f>IF(R42="","",R42)</f>
         <v/>
       </c>
-      <c r="G41" s="655"/>
+      <c r="G41" s="617"/>
       <c r="H41" s="42"/>
       <c r="I41" s="42"/>
       <c r="J41" s="42"/>
@@ -22284,11 +22289,11 @@
       <c r="E42" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="655" t="str">
+      <c r="F42" s="617" t="str">
         <f>IF(R43="","",R43)</f>
         <v/>
       </c>
-      <c r="G42" s="655"/>
+      <c r="G42" s="617"/>
       <c r="H42" s="42"/>
       <c r="I42" s="42"/>
       <c r="J42" s="42"/>
@@ -23055,10 +23060,10 @@
       <c r="I69" s="296"/>
       <c r="J69" s="296"/>
       <c r="K69" s="296"/>
-      <c r="L69" s="656" t="s">
+      <c r="L69" s="624" t="s">
         <v>83</v>
       </c>
-      <c r="M69" s="657"/>
+      <c r="M69" s="625"/>
       <c r="O69" s="56"/>
       <c r="P69" s="17" t="s">
         <v>84</v>
@@ -23981,7 +23986,7 @@
       </c>
       <c r="D92" s="135"/>
       <c r="E92" s="70" t="s">
-        <v>69</v>
+        <v>479</v>
       </c>
       <c r="F92" s="135"/>
       <c r="G92" s="135"/>
@@ -24727,24 +24732,24 @@
       <c r="P107" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="Q107" s="658" t="str">
+      <c r="Q107" s="621" t="str">
         <f>IF(Q106&lt;&gt;"",Q106,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R107" s="658"/>
-      <c r="S107" s="658"/>
-      <c r="T107" s="659" t="str">
+      <c r="R107" s="621"/>
+      <c r="S107" s="621"/>
+      <c r="T107" s="620" t="str">
         <f>IF(T106&lt;&gt;"",T106,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v/>
       </c>
-      <c r="U107" s="659"/>
-      <c r="V107" s="659"/>
-      <c r="W107" s="659" t="str">
+      <c r="U107" s="620"/>
+      <c r="V107" s="620"/>
+      <c r="W107" s="620" t="str">
         <f>IF(W106&lt;&gt;"",W106,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="X107" s="659"/>
-      <c r="Y107" s="659"/>
+      <c r="X107" s="620"/>
+      <c r="Y107" s="620"/>
       <c r="AA107" s="2" t="s">
         <v>152</v>
       </c>
@@ -26736,24 +26741,24 @@
       <c r="P139" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="Q139" s="658" t="str">
+      <c r="Q139" s="621" t="str">
         <f>IF(Q138&lt;&gt;"",Q138,IF($Q$99=1,"Manual 1",IF(AUTO_MA="","",AUTO_MA&amp;" 1")))</f>
         <v>Auto 1</v>
       </c>
-      <c r="R139" s="658"/>
-      <c r="S139" s="658"/>
-      <c r="T139" s="659" t="str">
+      <c r="R139" s="621"/>
+      <c r="S139" s="621"/>
+      <c r="T139" s="620" t="str">
         <f>IF(T138&lt;&gt;"",T138,IF($R$1399=1,"Manual 2",IF(OR(AUTO_MA="",O101="",O101=1),"",AUTO_MA&amp;" "&amp;IF(O101=2,2,IF(AND(O102=2,O101&gt;2),ROUND(O101/2,0),O101)))))</f>
         <v/>
       </c>
-      <c r="U139" s="659"/>
-      <c r="V139" s="659"/>
-      <c r="W139" s="659" t="str">
+      <c r="U139" s="620"/>
+      <c r="V139" s="620"/>
+      <c r="W139" s="620" t="str">
         <f>IF(W138&lt;&gt;"",W138,IF(OR(O102=1,O101&lt;3),IF(O102=1,"High Level","No High Level"),IF(AUTO_MA="","",AUTO_MA&amp;" "&amp;O101)))</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="X139" s="659"/>
-      <c r="Y139" s="659"/>
+      <c r="X139" s="620"/>
+      <c r="Y139" s="620"/>
       <c r="AA139" s="2" t="str">
         <f>$T$139&amp;" Mag 4"</f>
         <v xml:space="preserve"> Mag 4</v>
@@ -29097,10 +29102,10 @@
       <c r="P181" s="135"/>
       <c r="Q181" s="137"/>
       <c r="R181" s="128"/>
-      <c r="T181" s="641" t="s">
+      <c r="T181" s="622" t="s">
         <v>244</v>
       </c>
-      <c r="U181" s="641"/>
+      <c r="U181" s="622"/>
       <c r="W181" s="2" t="s">
         <v>198</v>
       </c>
@@ -29471,7 +29476,7 @@
       <c r="K190" s="320"/>
       <c r="L190" s="320"/>
       <c r="M190" s="324"/>
-      <c r="O190" s="650" t="str">
+      <c r="O190" s="623" t="str">
         <f>$Q$107</f>
         <v>Auto 1</v>
       </c>
@@ -29521,7 +29526,7 @@
       <c r="K191" s="320"/>
       <c r="L191" s="320"/>
       <c r="M191" s="300"/>
-      <c r="O191" s="650"/>
+      <c r="O191" s="623"/>
       <c r="P191" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -29567,7 +29572,7 @@
       <c r="K192" s="135"/>
       <c r="L192" s="135"/>
       <c r="M192" s="300"/>
-      <c r="O192" s="650"/>
+      <c r="O192" s="623"/>
       <c r="P192" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -29613,7 +29618,7 @@
       <c r="K193" s="135"/>
       <c r="L193" s="135"/>
       <c r="M193" s="300"/>
-      <c r="O193" s="650"/>
+      <c r="O193" s="623"/>
       <c r="P193" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -29656,7 +29661,7 @@
       <c r="K194" s="135"/>
       <c r="L194" s="135"/>
       <c r="M194" s="300"/>
-      <c r="O194" s="650"/>
+      <c r="O194" s="623"/>
       <c r="P194" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -29699,7 +29704,7 @@
       <c r="K195" s="135"/>
       <c r="L195" s="135"/>
       <c r="M195" s="300"/>
-      <c r="O195" s="650" t="str">
+      <c r="O195" s="623" t="str">
         <f>$T$107</f>
         <v/>
       </c>
@@ -29745,7 +29750,7 @@
       <c r="K196" s="302"/>
       <c r="L196" s="302"/>
       <c r="M196" s="303"/>
-      <c r="O196" s="650"/>
+      <c r="O196" s="623"/>
       <c r="P196" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -29790,7 +29795,7 @@
         <f>IF($X$7="","",$X$7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="O197" s="650"/>
+      <c r="O197" s="623"/>
       <c r="P197" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -29835,7 +29840,7 @@
         <f>IF($R$13="","",$R$13)</f>
         <v/>
       </c>
-      <c r="O198" s="650"/>
+      <c r="O198" s="623"/>
       <c r="P198" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -29881,7 +29886,7 @@
         <f>$H$2</f>
         <v>Medical University of South Carolina</v>
       </c>
-      <c r="O199" s="650"/>
+      <c r="O199" s="623"/>
       <c r="P199" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -29930,7 +29935,7 @@
         <f>$H$5</f>
         <v>Fluoroscopy System Compliance Inspection</v>
       </c>
-      <c r="O200" s="650" t="str">
+      <c r="O200" s="623" t="str">
         <f>$W$107</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -29979,7 +29984,7 @@
       <c r="K201" s="296"/>
       <c r="L201" s="296"/>
       <c r="M201" s="297"/>
-      <c r="O201" s="650"/>
+      <c r="O201" s="623"/>
       <c r="P201" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30033,7 +30038,7 @@
         <v>44905</v>
       </c>
       <c r="M202" s="12"/>
-      <c r="O202" s="650"/>
+      <c r="O202" s="623"/>
       <c r="P202" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -30066,7 +30071,7 @@
       </c>
       <c r="B203" s="10"/>
       <c r="M203" s="12"/>
-      <c r="O203" s="650"/>
+      <c r="O203" s="623"/>
       <c r="P203" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -30100,20 +30105,20 @@
       <c r="B204" s="298"/>
       <c r="C204" s="348"/>
       <c r="D204" s="320"/>
-      <c r="E204" s="620" t="s">
+      <c r="E204" s="626" t="s">
         <v>261</v>
       </c>
-      <c r="F204" s="622" t="s">
+      <c r="F204" s="663" t="s">
         <v>262</v>
       </c>
       <c r="G204" s="512" t="s">
         <v>263</v>
       </c>
-      <c r="H204" s="620" t="str">
+      <c r="H204" s="626" t="str">
         <f>R276</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="I204" s="660" t="str">
+      <c r="I204" s="628" t="str">
         <f>S276</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -30126,10 +30131,10 @@
       <c r="L204" s="135" t="s">
         <v>266</v>
       </c>
-      <c r="M204" s="662" t="s">
+      <c r="M204" s="630" t="s">
         <v>267</v>
       </c>
-      <c r="O204" s="650"/>
+      <c r="O204" s="623"/>
       <c r="P204" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -30167,11 +30172,11 @@
       <c r="D205" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="E205" s="621"/>
-      <c r="F205" s="623"/>
+      <c r="E205" s="627"/>
+      <c r="F205" s="664"/>
       <c r="G205" s="512"/>
-      <c r="H205" s="621"/>
-      <c r="I205" s="661"/>
+      <c r="H205" s="627"/>
+      <c r="I205" s="629"/>
       <c r="J205" s="513"/>
       <c r="K205" s="135" t="str">
         <f>U277</f>
@@ -30181,7 +30186,7 @@
         <f>V277</f>
         <v>mGy/min</v>
       </c>
-      <c r="M205" s="663"/>
+      <c r="M205" s="631"/>
       <c r="O205" s="13"/>
       <c r="Y205" s="14"/>
       <c r="AA205" s="2" t="s">
@@ -30825,7 +30830,7 @@
         <f>W286</f>
         <v/>
       </c>
-      <c r="O214" s="650" t="str">
+      <c r="O214" s="623" t="str">
         <f>$Q$139</f>
         <v>Auto 1</v>
       </c>
@@ -30881,7 +30886,7 @@
       <c r="K215" s="135"/>
       <c r="L215" s="135"/>
       <c r="M215" s="300"/>
-      <c r="O215" s="650"/>
+      <c r="O215" s="623"/>
       <c r="P215" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -30927,7 +30932,7 @@
       <c r="K216" s="320"/>
       <c r="L216" s="320"/>
       <c r="M216" s="300"/>
-      <c r="O216" s="650"/>
+      <c r="O216" s="623"/>
       <c r="P216" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -30973,7 +30978,7 @@
       <c r="K217" s="365"/>
       <c r="L217" s="365"/>
       <c r="M217" s="366"/>
-      <c r="O217" s="650"/>
+      <c r="O217" s="623"/>
       <c r="P217" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31019,7 +31024,7 @@
       <c r="K218" s="320"/>
       <c r="L218" s="320"/>
       <c r="M218" s="300"/>
-      <c r="O218" s="650"/>
+      <c r="O218" s="623"/>
       <c r="P218" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -31062,7 +31067,7 @@
       <c r="K219" s="320"/>
       <c r="L219" s="320"/>
       <c r="M219" s="324"/>
-      <c r="O219" s="650" t="str">
+      <c r="O219" s="623" t="str">
         <f>$T$139</f>
         <v/>
       </c>
@@ -31123,7 +31128,7 @@
         <v/>
       </c>
       <c r="M220" s="324"/>
-      <c r="O220" s="650"/>
+      <c r="O220" s="623"/>
       <c r="P220" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -31166,7 +31171,7 @@
       <c r="K221" s="320"/>
       <c r="L221" s="320"/>
       <c r="M221" s="324"/>
-      <c r="O221" s="650"/>
+      <c r="O221" s="623"/>
       <c r="P221" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -31215,7 +31220,7 @@
       </c>
       <c r="L222" s="320"/>
       <c r="M222" s="324"/>
-      <c r="O222" s="650"/>
+      <c r="O222" s="623"/>
       <c r="P222" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31273,7 +31278,7 @@
       </c>
       <c r="L223" s="320"/>
       <c r="M223" s="324"/>
-      <c r="O223" s="650"/>
+      <c r="O223" s="623"/>
       <c r="P223" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -31339,7 +31344,7 @@
       </c>
       <c r="L224" s="320"/>
       <c r="M224" s="324"/>
-      <c r="O224" s="650" t="str">
+      <c r="O224" s="623" t="str">
         <f>$W$139</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -31405,7 +31410,7 @@
       </c>
       <c r="L225" s="320"/>
       <c r="M225" s="324"/>
-      <c r="O225" s="650"/>
+      <c r="O225" s="623"/>
       <c r="P225" s="144" t="str">
         <f>IF($O$113="","",$O$113)</f>
         <v/>
@@ -31468,7 +31473,7 @@
       </c>
       <c r="L226" s="320"/>
       <c r="M226" s="324"/>
-      <c r="O226" s="650"/>
+      <c r="O226" s="623"/>
       <c r="P226" s="144" t="str">
         <f>IF($O$116="","",$O$116)</f>
         <v/>
@@ -31531,7 +31536,7 @@
       </c>
       <c r="L227" s="320"/>
       <c r="M227" s="324"/>
-      <c r="O227" s="650"/>
+      <c r="O227" s="623"/>
       <c r="P227" s="144" t="str">
         <f>IF($O$119="","",$O$119)</f>
         <v/>
@@ -31584,7 +31589,7 @@
       </c>
       <c r="L228" s="320"/>
       <c r="M228" s="324"/>
-      <c r="O228" s="650"/>
+      <c r="O228" s="623"/>
       <c r="P228" s="134" t="str">
         <f>IF($O$122="","",$O$122)</f>
         <v/>
@@ -32162,7 +32167,7 @@
       <c r="K240" s="320"/>
       <c r="L240" s="320"/>
       <c r="M240" s="324"/>
-      <c r="O240" s="651" t="s">
+      <c r="O240" s="632" t="s">
         <v>293</v>
       </c>
       <c r="P240" s="165" t="s">
@@ -32227,7 +32232,7 @@
       <c r="K241" s="320"/>
       <c r="L241" s="320"/>
       <c r="M241" s="324"/>
-      <c r="O241" s="651"/>
+      <c r="O241" s="632"/>
       <c r="P241" s="170" t="s">
         <v>296</v>
       </c>
@@ -32290,7 +32295,7 @@
       <c r="K242" s="320"/>
       <c r="L242" s="320"/>
       <c r="M242" s="324"/>
-      <c r="O242" s="651" t="str">
+      <c r="O242" s="632" t="str">
         <f>IF($U$137=1,"Scatter - Pulse", "Scatter – Digital acq")</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -32355,7 +32360,7 @@
       <c r="K243" s="320"/>
       <c r="L243" s="320"/>
       <c r="M243" s="324"/>
-      <c r="O243" s="651"/>
+      <c r="O243" s="632"/>
       <c r="P243" s="170" t="s">
         <v>296</v>
       </c>
@@ -32889,17 +32894,17 @@
       <c r="P257" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="Q257" s="652" t="s">
+      <c r="Q257" s="633" t="s">
         <v>312</v>
       </c>
-      <c r="R257" s="652"/>
+      <c r="R257" s="633"/>
       <c r="S257" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="T257" s="652" t="s">
+      <c r="T257" s="633" t="s">
         <v>314</v>
       </c>
-      <c r="U257" s="652"/>
+      <c r="U257" s="633"/>
       <c r="V257" s="1" t="s">
         <v>315</v>
       </c>
@@ -33396,24 +33401,24 @@
         <f t="shared" si="46"/>
         <v>Attenuator</v>
       </c>
-      <c r="E269" s="643" t="str">
+      <c r="E269" s="634" t="str">
         <f>Q107</f>
         <v>Auto 1</v>
       </c>
-      <c r="F269" s="644"/>
-      <c r="G269" s="644"/>
-      <c r="H269" s="644" t="str">
+      <c r="F269" s="635"/>
+      <c r="G269" s="635"/>
+      <c r="H269" s="635" t="str">
         <f>T107</f>
         <v/>
       </c>
-      <c r="I269" s="644"/>
-      <c r="J269" s="644"/>
-      <c r="K269" s="645" t="str">
+      <c r="I269" s="635"/>
+      <c r="J269" s="635"/>
+      <c r="K269" s="636" t="str">
         <f>W107</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L269" s="645"/>
-      <c r="M269" s="646"/>
+      <c r="L269" s="636"/>
+      <c r="M269" s="637"/>
       <c r="O269" s="187" t="str">
         <f t="shared" si="47"/>
         <v/>
@@ -33515,7 +33520,7 @@
         <v>7</v>
       </c>
       <c r="B271" s="298"/>
-      <c r="C271" s="619" t="str">
+      <c r="C271" s="641" t="str">
         <f>O110&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33591,7 +33596,7 @@
         <v>8</v>
       </c>
       <c r="B272" s="298"/>
-      <c r="C272" s="619"/>
+      <c r="C272" s="641"/>
       <c r="D272" s="385">
         <f t="shared" si="48"/>
         <v>20</v>
@@ -33657,7 +33662,7 @@
         <v>9</v>
       </c>
       <c r="B273" s="298"/>
-      <c r="C273" s="619"/>
+      <c r="C273" s="641"/>
       <c r="D273" s="388">
         <f t="shared" si="48"/>
         <v>30</v>
@@ -33730,7 +33735,7 @@
         <v>10</v>
       </c>
       <c r="B274" s="298"/>
-      <c r="C274" s="619" t="str">
+      <c r="C274" s="641" t="str">
         <f>O113&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33799,7 +33804,7 @@
         <v>11</v>
       </c>
       <c r="B275" s="298"/>
-      <c r="C275" s="619"/>
+      <c r="C275" s="641"/>
       <c r="D275" s="385">
         <f t="shared" si="48"/>
         <v>20</v>
@@ -33872,7 +33877,7 @@
         <v>12</v>
       </c>
       <c r="B276" s="298"/>
-      <c r="C276" s="619"/>
+      <c r="C276" s="641"/>
       <c r="D276" s="388">
         <f t="shared" si="48"/>
         <v>30</v>
@@ -33913,17 +33918,17 @@
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="O276" s="647" t="s">
+      <c r="O276" s="642" t="s">
         <v>261</v>
       </c>
-      <c r="P276" s="648" t="s">
+      <c r="P276" s="643" t="s">
         <v>262</v>
       </c>
-      <c r="R276" s="648" t="str">
+      <c r="R276" s="643" t="str">
         <f>"Ind AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Ind AK @ Ref Pt (mGy)</v>
       </c>
-      <c r="S276" s="648" t="str">
+      <c r="S276" s="643" t="str">
         <f>"Meas AK @ Ref Pt ("&amp;T257&amp;")"</f>
         <v>Meas AK @ Ref Pt (mGy)</v>
       </c>
@@ -33945,7 +33950,7 @@
         <v>13</v>
       </c>
       <c r="B277" s="298"/>
-      <c r="C277" s="619" t="str">
+      <c r="C277" s="641" t="str">
         <f>O116&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -33989,13 +33994,13 @@
         <f t="shared" si="57"/>
         <v>0</v>
       </c>
-      <c r="O277" s="647"/>
-      <c r="P277" s="648"/>
+      <c r="O277" s="642"/>
+      <c r="P277" s="643"/>
       <c r="Q277" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="R277" s="648"/>
-      <c r="S277" s="648"/>
+      <c r="R277" s="643"/>
+      <c r="S277" s="643"/>
       <c r="T277" s="1" t="s">
         <v>321</v>
       </c>
@@ -34027,7 +34032,7 @@
         <v>14</v>
       </c>
       <c r="B278" s="298"/>
-      <c r="C278" s="619"/>
+      <c r="C278" s="641"/>
       <c r="D278" s="385">
         <f t="shared" si="48"/>
         <v>20</v>
@@ -34114,7 +34119,7 @@
         <v>15</v>
       </c>
       <c r="B279" s="298"/>
-      <c r="C279" s="619"/>
+      <c r="C279" s="641"/>
       <c r="D279" s="388">
         <f t="shared" si="48"/>
         <v>30</v>
@@ -34208,7 +34213,7 @@
         <v>16</v>
       </c>
       <c r="B280" s="298"/>
-      <c r="C280" s="619" t="str">
+      <c r="C280" s="641" t="str">
         <f>O119&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -34308,7 +34313,7 @@
         <v>17</v>
       </c>
       <c r="B281" s="298"/>
-      <c r="C281" s="619"/>
+      <c r="C281" s="641"/>
       <c r="D281" s="385">
         <f t="shared" si="48"/>
         <v>20</v>
@@ -34395,7 +34400,7 @@
         <v>18</v>
       </c>
       <c r="B282" s="298"/>
-      <c r="C282" s="619"/>
+      <c r="C282" s="641"/>
       <c r="D282" s="388">
         <f t="shared" si="48"/>
         <v>30</v>
@@ -34489,7 +34494,7 @@
         <v>19</v>
       </c>
       <c r="B283" s="298"/>
-      <c r="C283" s="619" t="str">
+      <c r="C283" s="641" t="str">
         <f>O122&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -34579,7 +34584,7 @@
         <v>20</v>
       </c>
       <c r="B284" s="298"/>
-      <c r="C284" s="619"/>
+      <c r="C284" s="641"/>
       <c r="D284" s="385">
         <f t="shared" si="48"/>
         <v>20</v>
@@ -34673,7 +34678,7 @@
         <v>21</v>
       </c>
       <c r="B285" s="298"/>
-      <c r="C285" s="619"/>
+      <c r="C285" s="641"/>
       <c r="D285" s="385">
         <f t="shared" si="48"/>
         <v>30</v>
@@ -35108,13 +35113,13 @@
       <c r="L293" s="135"/>
       <c r="M293" s="300"/>
       <c r="O293" s="223"/>
-      <c r="P293" s="649" t="s">
+      <c r="P293" s="644" t="s">
         <v>327</v>
       </c>
-      <c r="Q293" s="649"/>
-      <c r="R293" s="649"/>
-      <c r="S293" s="649"/>
-      <c r="T293" s="649"/>
+      <c r="Q293" s="644"/>
+      <c r="R293" s="644"/>
+      <c r="S293" s="644"/>
+      <c r="T293" s="644"/>
       <c r="U293" s="221"/>
       <c r="V293" s="221"/>
       <c r="W293" s="221"/>
@@ -35568,13 +35573,13 @@
       <c r="L302" s="135"/>
       <c r="M302" s="300"/>
       <c r="O302" s="223"/>
-      <c r="P302" s="649" t="s">
+      <c r="P302" s="644" t="s">
         <v>327</v>
       </c>
-      <c r="Q302" s="649"/>
-      <c r="R302" s="649"/>
-      <c r="S302" s="649"/>
-      <c r="T302" s="649"/>
+      <c r="Q302" s="644"/>
+      <c r="R302" s="644"/>
+      <c r="S302" s="644"/>
+      <c r="T302" s="644"/>
       <c r="U302" s="221"/>
       <c r="V302" s="161" t="s">
         <v>472</v>
@@ -35597,7 +35602,7 @@
         <v>39</v>
       </c>
       <c r="B303" s="298"/>
-      <c r="C303" s="624" t="str">
+      <c r="C303" s="649" t="str">
         <f>O190</f>
         <v>Auto 1</v>
       </c>
@@ -35666,7 +35671,7 @@
         <v>40</v>
       </c>
       <c r="B304" s="298"/>
-      <c r="C304" s="625"/>
+      <c r="C304" s="650"/>
       <c r="D304" s="427" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -35748,7 +35753,7 @@
         <v>41</v>
       </c>
       <c r="B305" s="298"/>
-      <c r="C305" s="625"/>
+      <c r="C305" s="650"/>
       <c r="D305" s="427" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -35817,7 +35822,7 @@
         <v>42</v>
       </c>
       <c r="B306" s="298"/>
-      <c r="C306" s="625"/>
+      <c r="C306" s="650"/>
       <c r="D306" s="427" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -35890,7 +35895,7 @@
         <v>43</v>
       </c>
       <c r="B307" s="298"/>
-      <c r="C307" s="636"/>
+      <c r="C307" s="651"/>
       <c r="D307" s="430" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -35956,7 +35961,7 @@
         <v>44</v>
       </c>
       <c r="B308" s="298"/>
-      <c r="C308" s="624" t="str">
+      <c r="C308" s="649" t="str">
         <f>O195</f>
         <v/>
       </c>
@@ -36031,7 +36036,7 @@
         <v>45</v>
       </c>
       <c r="B309" s="298"/>
-      <c r="C309" s="625"/>
+      <c r="C309" s="650"/>
       <c r="D309" s="427" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -36088,7 +36093,7 @@
         <v>46</v>
       </c>
       <c r="B310" s="298"/>
-      <c r="C310" s="625"/>
+      <c r="C310" s="650"/>
       <c r="D310" s="427" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -36151,7 +36156,7 @@
         <v>47</v>
       </c>
       <c r="B311" s="298"/>
-      <c r="C311" s="625"/>
+      <c r="C311" s="650"/>
       <c r="D311" s="427" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -36203,7 +36208,7 @@
         <v>48</v>
       </c>
       <c r="B312" s="298"/>
-      <c r="C312" s="626"/>
+      <c r="C312" s="652"/>
       <c r="D312" s="433" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -36259,7 +36264,7 @@
         <v>49</v>
       </c>
       <c r="B313" s="298"/>
-      <c r="C313" s="637" t="str">
+      <c r="C313" s="653" t="str">
         <f>O200</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -36311,7 +36316,7 @@
         <v>50</v>
       </c>
       <c r="B314" s="298"/>
-      <c r="C314" s="625"/>
+      <c r="C314" s="650"/>
       <c r="D314" s="427" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -36363,7 +36368,7 @@
         <v>51</v>
       </c>
       <c r="B315" s="298"/>
-      <c r="C315" s="625"/>
+      <c r="C315" s="650"/>
       <c r="D315" s="427" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -36408,7 +36413,7 @@
         <v>52</v>
       </c>
       <c r="B316" s="298"/>
-      <c r="C316" s="625"/>
+      <c r="C316" s="650"/>
       <c r="D316" s="427" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -36462,7 +36467,7 @@
         <v>53</v>
       </c>
       <c r="B317" s="298"/>
-      <c r="C317" s="626"/>
+      <c r="C317" s="652"/>
       <c r="D317" s="433" t="str">
         <f t="shared" si="67"/>
         <v/>
@@ -36584,10 +36589,10 @@
       <c r="R319" s="243"/>
       <c r="S319" s="244"/>
       <c r="T319" s="244"/>
-      <c r="V319" s="641" t="s">
+      <c r="V319" s="622" t="s">
         <v>338</v>
       </c>
-      <c r="W319" s="641"/>
+      <c r="W319" s="622"/>
       <c r="X319" s="17" t="s">
         <v>339</v>
       </c>
@@ -36788,7 +36793,7 @@
         <v>60</v>
       </c>
       <c r="B324" s="298"/>
-      <c r="C324" s="630" t="str">
+      <c r="C324" s="638" t="str">
         <f>O240</f>
         <v>Scatter – Fluoro</v>
       </c>
@@ -36838,7 +36843,7 @@
         <v>61</v>
       </c>
       <c r="B325" s="298"/>
-      <c r="C325" s="631"/>
+      <c r="C325" s="639"/>
       <c r="D325" s="442" t="str">
         <f>P241</f>
         <v>Waist level</v>
@@ -36996,13 +37001,13 @@
         <v>346</v>
       </c>
       <c r="P329" s="53"/>
-      <c r="Q329" s="642" t="s">
+      <c r="Q329" s="640" t="s">
         <v>347</v>
       </c>
-      <c r="R329" s="642"/>
-      <c r="S329" s="642"/>
-      <c r="T329" s="642"/>
-      <c r="U329" s="642"/>
+      <c r="R329" s="640"/>
+      <c r="S329" s="640"/>
+      <c r="T329" s="640"/>
+      <c r="U329" s="640"/>
       <c r="Y329" s="14"/>
     </row>
     <row r="330" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37185,24 +37190,24 @@
         <f t="shared" si="75"/>
         <v>Attenuator</v>
       </c>
-      <c r="E335" s="643" t="str">
+      <c r="E335" s="634" t="str">
         <f>Q139</f>
         <v>Auto 1</v>
       </c>
-      <c r="F335" s="644"/>
-      <c r="G335" s="644"/>
-      <c r="H335" s="644" t="str">
+      <c r="F335" s="635"/>
+      <c r="G335" s="635"/>
+      <c r="H335" s="635" t="str">
         <f>T139</f>
         <v/>
       </c>
-      <c r="I335" s="644"/>
-      <c r="J335" s="644"/>
-      <c r="K335" s="645" t="str">
+      <c r="I335" s="635"/>
+      <c r="J335" s="635"/>
+      <c r="K335" s="636" t="str">
         <f>W139</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L335" s="645"/>
-      <c r="M335" s="646"/>
+      <c r="L335" s="636"/>
+      <c r="M335" s="637"/>
       <c r="O335" s="130"/>
       <c r="P335" s="129" t="s">
         <v>353</v>
@@ -37279,7 +37284,7 @@
         <v>7</v>
       </c>
       <c r="B337" s="298"/>
-      <c r="C337" s="619" t="str">
+      <c r="C337" s="641" t="str">
         <f>O142&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37339,7 +37344,7 @@
         <v>8</v>
       </c>
       <c r="B338" s="298"/>
-      <c r="C338" s="619"/>
+      <c r="C338" s="641"/>
       <c r="D338" s="456">
         <f t="shared" si="76"/>
         <v>20</v>
@@ -37396,7 +37401,7 @@
         <v>9</v>
       </c>
       <c r="B339" s="298"/>
-      <c r="C339" s="619"/>
+      <c r="C339" s="641"/>
       <c r="D339" s="457">
         <f t="shared" si="76"/>
         <v>30</v>
@@ -37453,7 +37458,7 @@
         <v>10</v>
       </c>
       <c r="B340" s="298"/>
-      <c r="C340" s="619" t="str">
+      <c r="C340" s="641" t="str">
         <f>O145&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37513,7 +37518,7 @@
         <v>11</v>
       </c>
       <c r="B341" s="298"/>
-      <c r="C341" s="619"/>
+      <c r="C341" s="641"/>
       <c r="D341" s="456">
         <f t="shared" si="76"/>
         <v>20</v>
@@ -37570,7 +37575,7 @@
         <v>12</v>
       </c>
       <c r="B342" s="298"/>
-      <c r="C342" s="619"/>
+      <c r="C342" s="641"/>
       <c r="D342" s="458">
         <f t="shared" si="76"/>
         <v>30</v>
@@ -37627,7 +37632,7 @@
         <v>13</v>
       </c>
       <c r="B343" s="298"/>
-      <c r="C343" s="619" t="str">
+      <c r="C343" s="641" t="str">
         <f>O148&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37679,7 +37684,7 @@
         <v>14</v>
       </c>
       <c r="B344" s="298"/>
-      <c r="C344" s="619"/>
+      <c r="C344" s="641"/>
       <c r="D344" s="456">
         <f t="shared" si="76"/>
         <v>20</v>
@@ -37741,7 +37746,7 @@
         <v>15</v>
       </c>
       <c r="B345" s="298"/>
-      <c r="C345" s="619"/>
+      <c r="C345" s="641"/>
       <c r="D345" s="457">
         <f t="shared" si="76"/>
         <v>30</v>
@@ -37804,7 +37809,7 @@
         <v>16</v>
       </c>
       <c r="B346" s="298"/>
-      <c r="C346" s="619" t="str">
+      <c r="C346" s="641" t="str">
         <f>O151&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -37867,7 +37872,7 @@
         <v>17</v>
       </c>
       <c r="B347" s="298"/>
-      <c r="C347" s="619"/>
+      <c r="C347" s="641"/>
       <c r="D347" s="456">
         <f t="shared" si="76"/>
         <v>20</v>
@@ -37925,7 +37930,7 @@
         <v>18</v>
       </c>
       <c r="B348" s="298"/>
-      <c r="C348" s="619"/>
+      <c r="C348" s="641"/>
       <c r="D348" s="458">
         <f t="shared" si="76"/>
         <v>30</v>
@@ -38003,7 +38008,7 @@
         <v>19</v>
       </c>
       <c r="B349" s="298"/>
-      <c r="C349" s="619" t="str">
+      <c r="C349" s="641" t="str">
         <f>O154&amp;" "&amp;flocm_in</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -38066,7 +38071,7 @@
         <v>20</v>
       </c>
       <c r="B350" s="298"/>
-      <c r="C350" s="619"/>
+      <c r="C350" s="641"/>
       <c r="D350" s="456">
         <f t="shared" si="76"/>
         <v>20</v>
@@ -38125,7 +38130,7 @@
         <v>21</v>
       </c>
       <c r="B351" s="298"/>
-      <c r="C351" s="619"/>
+      <c r="C351" s="641"/>
       <c r="D351" s="458">
         <f t="shared" si="76"/>
         <v>30</v>
@@ -38434,11 +38439,11 @@
         <f>IF(OR(V358="",V359="",V362=""),"",(V358-V359)*V362)</f>
         <v/>
       </c>
-      <c r="Q358" s="632" t="str">
+      <c r="Q358" s="645" t="str">
         <f>IF(OR(P358="",P359=""),"",(ABS(P358)+ABS(P359))/$O$355)</f>
         <v/>
       </c>
-      <c r="R358" s="633" t="str">
+      <c r="R358" s="646" t="str">
         <f>IF(OR(Q358="",Q360=""),"",Q358+Q360)</f>
         <v/>
       </c>
@@ -38477,8 +38482,8 @@
         <f>IF(OR(W358="",W359="",V362=""),"",(W358-W359)*V362)</f>
         <v/>
       </c>
-      <c r="Q359" s="632"/>
-      <c r="R359" s="632"/>
+      <c r="Q359" s="645"/>
+      <c r="R359" s="645"/>
       <c r="S359" s="146" t="str">
         <f>IF(AB171="","",AB171)</f>
         <v/>
@@ -38514,11 +38519,11 @@
         <f>IF(OR(X358="",X359="",V362=""),"",(X358-X359)*V362)</f>
         <v/>
       </c>
-      <c r="Q360" s="633" t="str">
+      <c r="Q360" s="646" t="str">
         <f>IF(OR(P360="",P361=""),"",(ABS(P360)+ABS(P361))/$O$355)</f>
         <v/>
       </c>
-      <c r="R360" s="633"/>
+      <c r="R360" s="646"/>
       <c r="S360" s="146" t="str">
         <f>IF(AB172="","",AB172)</f>
         <v/>
@@ -38560,8 +38565,8 @@
         <f>IF(OR(Y358="",Y359="",V362=""),"",(Y358-Y359)*V362)</f>
         <v/>
       </c>
-      <c r="Q361" s="633"/>
-      <c r="R361" s="633"/>
+      <c r="Q361" s="646"/>
+      <c r="R361" s="646"/>
       <c r="S361" s="148" t="str">
         <f>IF(AB173="","",AB173)</f>
         <v/>
@@ -38733,7 +38738,7 @@
         <v>36</v>
       </c>
       <c r="B366" s="298"/>
-      <c r="C366" s="634" t="str">
+      <c r="C366" s="647" t="str">
         <f>O214</f>
         <v>Auto 1</v>
       </c>
@@ -38784,7 +38789,7 @@
         <v>37</v>
       </c>
       <c r="B367" s="298"/>
-      <c r="C367" s="635"/>
+      <c r="C367" s="648"/>
       <c r="D367" s="427" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -38830,7 +38835,7 @@
         <v>38</v>
       </c>
       <c r="B368" s="298"/>
-      <c r="C368" s="635"/>
+      <c r="C368" s="648"/>
       <c r="D368" s="427" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -38865,7 +38870,7 @@
         <v>39</v>
       </c>
       <c r="B369" s="298"/>
-      <c r="C369" s="635"/>
+      <c r="C369" s="648"/>
       <c r="D369" s="427" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -38900,7 +38905,7 @@
         <v>40</v>
       </c>
       <c r="B370" s="298"/>
-      <c r="C370" s="635"/>
+      <c r="C370" s="648"/>
       <c r="D370" s="433" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -38945,7 +38950,7 @@
         <v>41</v>
       </c>
       <c r="B371" s="298"/>
-      <c r="C371" s="624" t="str">
+      <c r="C371" s="649" t="str">
         <f>O219</f>
         <v/>
       </c>
@@ -38995,7 +39000,7 @@
         <v>42</v>
       </c>
       <c r="B372" s="298"/>
-      <c r="C372" s="625"/>
+      <c r="C372" s="650"/>
       <c r="D372" s="427" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -39045,7 +39050,7 @@
         <v>43</v>
       </c>
       <c r="B373" s="298"/>
-      <c r="C373" s="625"/>
+      <c r="C373" s="650"/>
       <c r="D373" s="427" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -39092,7 +39097,7 @@
         <v>44</v>
       </c>
       <c r="B374" s="298"/>
-      <c r="C374" s="625"/>
+      <c r="C374" s="650"/>
       <c r="D374" s="427" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -39142,7 +39147,7 @@
         <v>45</v>
       </c>
       <c r="B375" s="298"/>
-      <c r="C375" s="626"/>
+      <c r="C375" s="652"/>
       <c r="D375" s="433" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -39189,7 +39194,7 @@
         <v>46</v>
       </c>
       <c r="B376" s="298"/>
-      <c r="C376" s="627" t="str">
+      <c r="C376" s="665" t="str">
         <f>O224</f>
         <v xml:space="preserve">Auto </v>
       </c>
@@ -39242,7 +39247,7 @@
         <v>47</v>
       </c>
       <c r="B377" s="298"/>
-      <c r="C377" s="628"/>
+      <c r="C377" s="666"/>
       <c r="D377" s="427" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -39289,7 +39294,7 @@
         <v>48</v>
       </c>
       <c r="B378" s="298"/>
-      <c r="C378" s="628"/>
+      <c r="C378" s="666"/>
       <c r="D378" s="427" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -39339,7 +39344,7 @@
         <v>49</v>
       </c>
       <c r="B379" s="298"/>
-      <c r="C379" s="628"/>
+      <c r="C379" s="666"/>
       <c r="D379" s="427" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -39386,7 +39391,7 @@
         <v>50</v>
       </c>
       <c r="B380" s="298"/>
-      <c r="C380" s="629"/>
+      <c r="C380" s="667"/>
       <c r="D380" s="433" t="str">
         <f t="shared" si="86"/>
         <v/>
@@ -39696,7 +39701,7 @@
         <v>58</v>
       </c>
       <c r="B388" s="298"/>
-      <c r="C388" s="630" t="str">
+      <c r="C388" s="638" t="str">
         <f>O242</f>
         <v>Scatter – Digital acq</v>
       </c>
@@ -39747,7 +39752,7 @@
         <v>59</v>
       </c>
       <c r="B389" s="298"/>
-      <c r="C389" s="631"/>
+      <c r="C389" s="639"/>
       <c r="D389" s="442" t="str">
         <f>P243</f>
         <v>Waist level</v>
@@ -40098,14 +40103,14 @@
       <c r="E399" s="296"/>
       <c r="F399" s="296"/>
       <c r="G399" s="296"/>
-      <c r="H399" s="640" t="s">
+      <c r="H399" s="656" t="s">
         <v>393</v>
       </c>
-      <c r="I399" s="640"/>
-      <c r="J399" s="640" t="s">
+      <c r="I399" s="656"/>
+      <c r="J399" s="656" t="s">
         <v>394</v>
       </c>
-      <c r="K399" s="640"/>
+      <c r="K399" s="656"/>
       <c r="L399" s="296"/>
       <c r="M399" s="297"/>
       <c r="O399" s="13"/>
@@ -40679,20 +40684,20 @@
       </c>
       <c r="B413" s="298"/>
       <c r="C413" s="42"/>
-      <c r="D413" s="638" t="s">
+      <c r="D413" s="654" t="s">
         <v>400</v>
       </c>
-      <c r="E413" s="638"/>
-      <c r="F413" s="638"/>
-      <c r="G413" s="638"/>
-      <c r="H413" s="638"/>
-      <c r="I413" s="638" t="s">
+      <c r="E413" s="654"/>
+      <c r="F413" s="654"/>
+      <c r="G413" s="654"/>
+      <c r="H413" s="654"/>
+      <c r="I413" s="654" t="s">
         <v>401</v>
       </c>
-      <c r="J413" s="638"/>
-      <c r="K413" s="638"/>
-      <c r="L413" s="638"/>
-      <c r="M413" s="639"/>
+      <c r="J413" s="654"/>
+      <c r="K413" s="654"/>
+      <c r="L413" s="654"/>
+      <c r="M413" s="655"/>
       <c r="O413" s="13"/>
       <c r="P413" s="2" t="s">
         <v>188</v>
@@ -42172,11 +42177,11 @@
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="F442" s="613" t="str">
+      <c r="F442" s="657" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
-      <c r="G442" s="615" t="str">
+      <c r="G442" s="659" t="str">
         <f t="shared" si="98"/>
         <v/>
       </c>
@@ -42217,8 +42222,8 @@
         <f>P359</f>
         <v/>
       </c>
-      <c r="F443" s="614"/>
-      <c r="G443" s="616"/>
+      <c r="F443" s="658"/>
+      <c r="G443" s="660"/>
       <c r="H443" s="198"/>
       <c r="I443" s="82" t="str">
         <f>T360</f>
@@ -42258,11 +42263,11 @@
         <f>P360</f>
         <v/>
       </c>
-      <c r="F444" s="614" t="str">
+      <c r="F444" s="658" t="str">
         <f>Q360</f>
         <v/>
       </c>
-      <c r="G444" s="616"/>
+      <c r="G444" s="660"/>
       <c r="H444" s="135"/>
       <c r="I444" s="91" t="str">
         <f>T361</f>
@@ -42303,8 +42308,8 @@
         <f>P361</f>
         <v/>
       </c>
-      <c r="F445" s="618"/>
-      <c r="G445" s="617"/>
+      <c r="F445" s="662"/>
+      <c r="G445" s="661"/>
       <c r="H445" s="135"/>
       <c r="I445" s="135"/>
       <c r="J445" s="135"/>
@@ -48663,71 +48668,30 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="106">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="W107:Y107"/>
-    <mergeCell ref="Q139:S139"/>
-    <mergeCell ref="T139:V139"/>
-    <mergeCell ref="W139:Y139"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="T181:U181"/>
-    <mergeCell ref="O190:O194"/>
-    <mergeCell ref="O195:O199"/>
-    <mergeCell ref="O200:O204"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="Q107:S107"/>
-    <mergeCell ref="T107:V107"/>
-    <mergeCell ref="H204:H205"/>
-    <mergeCell ref="I204:I205"/>
-    <mergeCell ref="M204:M205"/>
-    <mergeCell ref="O214:O218"/>
-    <mergeCell ref="O219:O223"/>
-    <mergeCell ref="O224:O228"/>
-    <mergeCell ref="O240:O241"/>
-    <mergeCell ref="O242:O243"/>
-    <mergeCell ref="Q257:R257"/>
-    <mergeCell ref="T257:U257"/>
-    <mergeCell ref="E269:G269"/>
-    <mergeCell ref="H269:J269"/>
-    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="F442:F443"/>
+    <mergeCell ref="G442:G445"/>
+    <mergeCell ref="F444:F445"/>
+    <mergeCell ref="C337:C339"/>
+    <mergeCell ref="C340:C342"/>
+    <mergeCell ref="C343:C345"/>
+    <mergeCell ref="C346:C348"/>
+    <mergeCell ref="C349:C351"/>
+    <mergeCell ref="E204:E205"/>
+    <mergeCell ref="F204:F205"/>
+    <mergeCell ref="C371:C375"/>
+    <mergeCell ref="C376:C380"/>
+    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="Q358:Q359"/>
+    <mergeCell ref="R358:R361"/>
+    <mergeCell ref="Q360:Q361"/>
+    <mergeCell ref="C366:C370"/>
+    <mergeCell ref="C303:C307"/>
+    <mergeCell ref="C308:C312"/>
+    <mergeCell ref="C313:C317"/>
+    <mergeCell ref="D413:H413"/>
+    <mergeCell ref="I413:M413"/>
+    <mergeCell ref="H399:I399"/>
+    <mergeCell ref="J399:K399"/>
     <mergeCell ref="V319:W319"/>
     <mergeCell ref="C324:C325"/>
     <mergeCell ref="Q329:U329"/>
@@ -48745,30 +48709,71 @@
     <mergeCell ref="C283:C285"/>
     <mergeCell ref="P302:T302"/>
     <mergeCell ref="P293:T293"/>
-    <mergeCell ref="Q358:Q359"/>
-    <mergeCell ref="R358:R361"/>
-    <mergeCell ref="Q360:Q361"/>
-    <mergeCell ref="C366:C370"/>
-    <mergeCell ref="C303:C307"/>
-    <mergeCell ref="C308:C312"/>
-    <mergeCell ref="C313:C317"/>
-    <mergeCell ref="D413:H413"/>
-    <mergeCell ref="I413:M413"/>
-    <mergeCell ref="H399:I399"/>
-    <mergeCell ref="J399:K399"/>
-    <mergeCell ref="F442:F443"/>
-    <mergeCell ref="G442:G445"/>
-    <mergeCell ref="F444:F445"/>
-    <mergeCell ref="C337:C339"/>
-    <mergeCell ref="C340:C342"/>
-    <mergeCell ref="C343:C345"/>
-    <mergeCell ref="C346:C348"/>
-    <mergeCell ref="C349:C351"/>
-    <mergeCell ref="E204:E205"/>
-    <mergeCell ref="F204:F205"/>
-    <mergeCell ref="C371:C375"/>
-    <mergeCell ref="C376:C380"/>
-    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="O214:O218"/>
+    <mergeCell ref="O219:O223"/>
+    <mergeCell ref="O224:O228"/>
+    <mergeCell ref="O240:O241"/>
+    <mergeCell ref="O242:O243"/>
+    <mergeCell ref="Q257:R257"/>
+    <mergeCell ref="T257:U257"/>
+    <mergeCell ref="E269:G269"/>
+    <mergeCell ref="H269:J269"/>
+    <mergeCell ref="K269:M269"/>
+    <mergeCell ref="T181:U181"/>
+    <mergeCell ref="O190:O194"/>
+    <mergeCell ref="O195:O199"/>
+    <mergeCell ref="O200:O204"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="Q107:S107"/>
+    <mergeCell ref="T107:V107"/>
+    <mergeCell ref="H204:H205"/>
+    <mergeCell ref="I204:I205"/>
+    <mergeCell ref="M204:M205"/>
+    <mergeCell ref="W107:Y107"/>
+    <mergeCell ref="Q139:S139"/>
+    <mergeCell ref="T139:V139"/>
+    <mergeCell ref="W139:Y139"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
   </mergeCells>
   <conditionalFormatting sqref="S126 V126 Y126 S158 V158 Y158">
     <cfRule type="cellIs" dxfId="21" priority="42" operator="equal">
@@ -49044,39 +49049,39 @@
         <f>Fluoro!D269</f>
         <v>Attenuator</v>
       </c>
-      <c r="E5" s="644" t="str">
+      <c r="E5" s="635" t="str">
         <f>Fluoro!E269</f>
         <v>Auto 1</v>
       </c>
-      <c r="F5" s="644">
+      <c r="F5" s="635">
         <f>Fluoro!F269</f>
         <v>0</v>
       </c>
-      <c r="G5" s="644">
+      <c r="G5" s="635">
         <f>Fluoro!G269</f>
         <v>0</v>
       </c>
-      <c r="H5" s="644" t="str">
+      <c r="H5" s="635" t="str">
         <f>Fluoro!H269</f>
         <v/>
       </c>
-      <c r="I5" s="644">
+      <c r="I5" s="635">
         <f>Fluoro!I269</f>
         <v>0</v>
       </c>
-      <c r="J5" s="644">
+      <c r="J5" s="635">
         <f>Fluoro!J269</f>
         <v>0</v>
       </c>
-      <c r="K5" s="645" t="str">
+      <c r="K5" s="636" t="str">
         <f>Fluoro!K269</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L5" s="645">
+      <c r="L5" s="636">
         <f>Fluoro!L269</f>
         <v>0</v>
       </c>
-      <c r="M5" s="645">
+      <c r="M5" s="636">
         <f>Fluoro!M269</f>
         <v>0</v>
       </c>
@@ -49133,7 +49138,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="669" t="str">
+      <c r="C7" s="668" t="str">
         <f>Fluoro!C271</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49183,7 +49188,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="669">
+      <c r="C8" s="668">
         <f>Fluoro!C272</f>
         <v>0</v>
       </c>
@@ -49233,7 +49238,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="669">
+      <c r="C9" s="668">
         <f>Fluoro!C273</f>
         <v>0</v>
       </c>
@@ -49283,7 +49288,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="669" t="str">
+      <c r="C10" s="668" t="str">
         <f>Fluoro!C274</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49333,7 +49338,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="669">
+      <c r="C11" s="668">
         <f>Fluoro!C275</f>
         <v>0</v>
       </c>
@@ -49383,7 +49388,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="669">
+      <c r="C12" s="668">
         <f>Fluoro!C276</f>
         <v>0</v>
       </c>
@@ -49433,7 +49438,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="669" t="str">
+      <c r="C13" s="668" t="str">
         <f>Fluoro!C277</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49483,7 +49488,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="669">
+      <c r="C14" s="668">
         <f>Fluoro!C278</f>
         <v>0</v>
       </c>
@@ -49533,7 +49538,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="10"/>
-      <c r="C15" s="669">
+      <c r="C15" s="668">
         <f>Fluoro!C279</f>
         <v>0</v>
       </c>
@@ -49583,7 +49588,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="10"/>
-      <c r="C16" s="669" t="str">
+      <c r="C16" s="668" t="str">
         <f>Fluoro!C280</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49633,7 +49638,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="669">
+      <c r="C17" s="668">
         <f>Fluoro!C281</f>
         <v>0</v>
       </c>
@@ -49683,7 +49688,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="669">
+      <c r="C18" s="668">
         <f>Fluoro!C282</f>
         <v>0</v>
       </c>
@@ -49733,7 +49738,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="669" t="str">
+      <c r="C19" s="668" t="str">
         <f>Fluoro!C283</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -49783,7 +49788,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="669">
+      <c r="C20" s="668">
         <f>Fluoro!C284</f>
         <v>0</v>
       </c>
@@ -49833,7 +49838,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="669">
+      <c r="C21" s="668">
         <f>Fluoro!C285</f>
         <v>0</v>
       </c>
@@ -50257,39 +50262,39 @@
         <f>Fluoro!D335</f>
         <v>Attenuator</v>
       </c>
-      <c r="E37" s="644" t="str">
+      <c r="E37" s="635" t="str">
         <f>Fluoro!E335</f>
         <v>Auto 1</v>
       </c>
-      <c r="F37" s="644">
+      <c r="F37" s="635">
         <f>Fluoro!F335</f>
         <v>0</v>
       </c>
-      <c r="G37" s="644">
+      <c r="G37" s="635">
         <f>Fluoro!G335</f>
         <v>0</v>
       </c>
-      <c r="H37" s="644" t="str">
+      <c r="H37" s="635" t="str">
         <f>Fluoro!H335</f>
         <v/>
       </c>
-      <c r="I37" s="644">
+      <c r="I37" s="635">
         <f>Fluoro!I335</f>
         <v>0</v>
       </c>
-      <c r="J37" s="644">
+      <c r="J37" s="635">
         <f>Fluoro!J335</f>
         <v>0</v>
       </c>
-      <c r="K37" s="645" t="str">
+      <c r="K37" s="636" t="str">
         <f>Fluoro!K335</f>
         <v xml:space="preserve">Auto </v>
       </c>
-      <c r="L37" s="645">
+      <c r="L37" s="636">
         <f>Fluoro!L335</f>
         <v>0</v>
       </c>
-      <c r="M37" s="645">
+      <c r="M37" s="636">
         <f>Fluoro!M335</f>
         <v>0</v>
       </c>
@@ -50346,7 +50351,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="10"/>
-      <c r="C39" s="669" t="str">
+      <c r="C39" s="668" t="str">
         <f>Fluoro!C337</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50396,7 +50401,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="10"/>
-      <c r="C40" s="669">
+      <c r="C40" s="668">
         <f>Fluoro!C338</f>
         <v>0</v>
       </c>
@@ -50446,7 +50451,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="10"/>
-      <c r="C41" s="669">
+      <c r="C41" s="668">
         <f>Fluoro!C339</f>
         <v>0</v>
       </c>
@@ -50496,7 +50501,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="10"/>
-      <c r="C42" s="669" t="str">
+      <c r="C42" s="668" t="str">
         <f>Fluoro!C340</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50546,7 +50551,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="10"/>
-      <c r="C43" s="669">
+      <c r="C43" s="668">
         <f>Fluoro!C341</f>
         <v>0</v>
       </c>
@@ -50596,7 +50601,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="10"/>
-      <c r="C44" s="669">
+      <c r="C44" s="668">
         <f>Fluoro!C342</f>
         <v>0</v>
       </c>
@@ -50646,7 +50651,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="10"/>
-      <c r="C45" s="669" t="str">
+      <c r="C45" s="668" t="str">
         <f>Fluoro!C343</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50696,7 +50701,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="10"/>
-      <c r="C46" s="669">
+      <c r="C46" s="668">
         <f>Fluoro!C344</f>
         <v>0</v>
       </c>
@@ -50746,7 +50751,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="10"/>
-      <c r="C47" s="669">
+      <c r="C47" s="668">
         <f>Fluoro!C345</f>
         <v>0</v>
       </c>
@@ -50796,7 +50801,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="10"/>
-      <c r="C48" s="669" t="str">
+      <c r="C48" s="668" t="str">
         <f>Fluoro!C346</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50846,7 +50851,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="10"/>
-      <c r="C49" s="669">
+      <c r="C49" s="668">
         <f>Fluoro!C347</f>
         <v>0</v>
       </c>
@@ -50896,7 +50901,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="10"/>
-      <c r="C50" s="669">
+      <c r="C50" s="668">
         <f>Fluoro!C348</f>
         <v>0</v>
       </c>
@@ -50946,7 +50951,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="10"/>
-      <c r="C51" s="669" t="str">
+      <c r="C51" s="668" t="str">
         <f>Fluoro!C349</f>
         <v xml:space="preserve"> cm</v>
       </c>
@@ -50996,7 +51001,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="10"/>
-      <c r="C52" s="669">
+      <c r="C52" s="668">
         <f>Fluoro!C350</f>
         <v>0</v>
       </c>
@@ -51046,7 +51051,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="10"/>
-      <c r="C53" s="669">
+      <c r="C53" s="668">
         <f>Fluoro!C351</f>
         <v>0</v>
       </c>
@@ -51240,7 +51245,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="10"/>
-      <c r="C60" s="668"/>
+      <c r="C60" s="669"/>
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60"/>
@@ -51257,7 +51262,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="10"/>
-      <c r="C61" s="668"/>
+      <c r="C61" s="669"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>
@@ -51392,23 +51397,23 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="17">
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C51:C53"/>
     <mergeCell ref="E37:G37"/>
     <mergeCell ref="H37:J37"/>
     <mergeCell ref="K37:M37"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.88611111111111096" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup scale="68" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -51437,29 +51442,29 @@
       </c>
       <c r="B1" s="670"/>
       <c r="N1" s="275"/>
-      <c r="O1" s="649" t="str">
+      <c r="O1" s="644" t="str">
         <f>Fluoro!O105</f>
         <v>Patient Entrance Exposure Rate (Fluoroscopy)*</v>
       </c>
-      <c r="P1" s="649"/>
-      <c r="Q1" s="649"/>
-      <c r="R1" s="649" t="s">
+      <c r="P1" s="644"/>
+      <c r="Q1" s="644"/>
+      <c r="R1" s="644" t="s">
         <v>406</v>
       </c>
-      <c r="S1" s="649"/>
-      <c r="T1" s="649"/>
+      <c r="S1" s="644"/>
+      <c r="T1" s="644"/>
       <c r="V1" s="275"/>
-      <c r="W1" s="649" t="str">
+      <c r="W1" s="644" t="str">
         <f>Fluoro!O137</f>
         <v>Patient Entrance Exposure Rate – Digital Acquisition</v>
       </c>
-      <c r="X1" s="649"/>
-      <c r="Y1" s="649"/>
-      <c r="Z1" s="649" t="s">
+      <c r="X1" s="644"/>
+      <c r="Y1" s="644"/>
+      <c r="Z1" s="644" t="s">
         <v>406</v>
       </c>
-      <c r="AA1" s="649"/>
-      <c r="AB1" s="649"/>
+      <c r="AA1" s="644"/>
+      <c r="AB1" s="644"/>
     </row>
     <row r="2" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="276">
@@ -55452,14 +55457,14 @@
       <c r="B75" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="E75" s="649" t="s">
+      <c r="E75" s="644" t="s">
         <v>419</v>
       </c>
-      <c r="F75" s="649"/>
-      <c r="I75" s="649" t="s">
+      <c r="F75" s="644"/>
+      <c r="I75" s="644" t="s">
         <v>420</v>
       </c>
-      <c r="J75" s="649"/>
+      <c r="J75" s="644"/>
     </row>
     <row r="76" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">

</xml_diff>